<commit_message>
updated rule to text & formatting for individual rules
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,36 +540,36 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>58.2</v>
+        <v>52.8</v>
       </c>
       <c r="K2" t="n">
-        <v>40740</v>
+        <v>36960</v>
       </c>
       <c r="L2" t="n">
         <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>29260</v>
+        <v>33040</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>2587.2</v>
       </c>
     </row>
     <row r="3">
@@ -624,11 +624,11 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="4">
@@ -654,32 +654,32 @@
         <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>497042.2392</v>
+        <v>624000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>77.59999999999999</v>
+        <v>69.3</v>
       </c>
       <c r="K4" t="n">
-        <v>247246.65232</v>
+        <v>277200</v>
       </c>
       <c r="L4" t="n">
-        <v>3186.1682</v>
+        <v>4000</v>
       </c>
       <c r="M4" t="n">
-        <v>249795.58688</v>
+        <v>346800</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -692,11 +692,11 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -706,52 +706,52 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>156</v>
+        <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>126957.75768</v>
+        <v>253800</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>69.3</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K5" t="n">
-        <v>56398.542354</v>
+        <v>34560</v>
       </c>
       <c r="L5" t="n">
-        <v>813.83178</v>
+        <v>600</v>
       </c>
       <c r="M5" t="n">
-        <v>70559.21532600001</v>
+        <v>219240</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>2419.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility1</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>253799.577</v>
+        <v>1359000</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -788,29 +788,29 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>57.59999999999999</v>
+        <v>18.24</v>
       </c>
       <c r="K6" t="n">
-        <v>34559.9424</v>
+        <v>54719.99999999999</v>
       </c>
       <c r="L6" t="n">
-        <v>599.999</v>
+        <v>3000</v>
       </c>
       <c r="M6" t="n">
-        <v>219239.6346</v>
+        <v>1304280</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>3830.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility1</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,35 +828,35 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4229997462</v>
+        <v>1209510</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>63.05</v>
+        <v>22.77</v>
       </c>
       <c r="K7" t="n">
-        <v>0.06304996217</v>
+        <v>60795.9</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0009999994</v>
+        <v>2670</v>
       </c>
       <c r="M7" t="n">
-        <v>0.35994978403</v>
+        <v>1148714.1</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -869,7 +869,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -887,35 +887,35 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F8" t="n">
-        <v>1812000</v>
+        <v>15390</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>72.75</v>
+        <v>53.46</v>
       </c>
       <c r="K8" t="n">
-        <v>291000</v>
+        <v>2405.7</v>
       </c>
       <c r="L8" t="n">
-        <v>4000</v>
+        <v>45</v>
       </c>
       <c r="M8" t="n">
-        <v>1521000</v>
+        <v>12984.3</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -928,32 +928,32 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>653</v>
+      </c>
+      <c r="F9" t="n">
+        <v>158026</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>B</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>453</v>
-      </c>
-      <c r="F9" t="n">
-        <v>530010</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>C</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -961,20 +961,20 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>23.04</v>
+        <v>24</v>
       </c>
       <c r="K9" t="n">
-        <v>26956.8</v>
+        <v>5808</v>
       </c>
       <c r="L9" t="n">
-        <v>1170</v>
+        <v>242</v>
       </c>
       <c r="M9" t="n">
-        <v>503053.2</v>
+        <v>152218</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -987,11 +987,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>453</v>
+        <v>432</v>
       </c>
       <c r="F10" t="n">
-        <v>226500</v>
+        <v>286848</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1027,13 +1027,13 @@
         <v>22.77</v>
       </c>
       <c r="K10" t="n">
-        <v>11385</v>
+        <v>15119.28</v>
       </c>
       <c r="L10" t="n">
-        <v>500</v>
+        <v>664</v>
       </c>
       <c r="M10" t="n">
-        <v>215115</v>
+        <v>271728.72</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility3</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1064,10 +1064,10 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>342</v>
+        <v>456</v>
       </c>
       <c r="F11" t="n">
-        <v>15390</v>
+        <v>10944</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1075,24 +1075,24 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>32.98</v>
+        <v>13</v>
       </c>
       <c r="K11" t="n">
-        <v>1484.1</v>
+        <v>312</v>
       </c>
       <c r="L11" t="n">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="M11" t="n">
-        <v>13905.9</v>
+        <v>10632</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility4</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>653</v>
+        <v>234</v>
       </c>
       <c r="F12" t="n">
-        <v>158025.347</v>
+        <v>54288</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1134,7 +1134,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1142,75 +1142,75 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>61.44</v>
+        <v>12.48</v>
       </c>
       <c r="K12" t="n">
-        <v>14868.41856</v>
+        <v>2895.36</v>
       </c>
       <c r="L12" t="n">
-        <v>241.999</v>
+        <v>232</v>
       </c>
       <c r="M12" t="n">
-        <v>143156.92844</v>
+        <v>51392.64</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>202.6752</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>231</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>653</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.6529998432799999</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="H13" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>23.28</v>
+        <v>13</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0232799944128</v>
+        <v>169</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0009999997599999999</v>
+        <v>13</v>
       </c>
       <c r="M13" t="n">
-        <v>0.6297198488671999</v>
+        <v>2834</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1218,419 +1218,6 @@
         </is>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>7</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>432</v>
-      </c>
-      <c r="F14" t="n">
-        <v>206423.32896</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>86</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J14" t="n">
-        <v>82.56</v>
-      </c>
-      <c r="K14" t="n">
-        <v>39449.7917568</v>
-      </c>
-      <c r="L14" t="n">
-        <v>477.83178</v>
-      </c>
-      <c r="M14" t="n">
-        <v>166973.5372032</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>7</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>432</v>
-      </c>
-      <c r="F15" t="n">
-        <v>80424.23904</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>23</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>1%</t>
-        </is>
-      </c>
-      <c r="J15" t="n">
-        <v>22.77</v>
-      </c>
-      <c r="K15" t="n">
-        <v>4239.027599399999</v>
-      </c>
-      <c r="L15" t="n">
-        <v>186.16722</v>
-      </c>
-      <c r="M15" t="n">
-        <v>76185.2114406</v>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>7</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>432</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.43199971488</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>53</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J16" t="n">
-        <v>51.41</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.0514099660694</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.0009999993400000001</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.3805897488106</v>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>8</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Facility3</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>456</v>
-      </c>
-      <c r="F17" t="n">
-        <v>10943.544</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>24</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
-        <v>23.04</v>
-      </c>
-      <c r="K17" t="n">
-        <v>552.93696</v>
-      </c>
-      <c r="L17" t="n">
-        <v>23.999</v>
-      </c>
-      <c r="M17" t="n">
-        <v>10390.60704</v>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>8</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Facility3</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>456</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.45599999088</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>75</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>1%</t>
-        </is>
-      </c>
-      <c r="J18" t="n">
-        <v>74.25</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.07424999851500001</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.0009999999800000001</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0.381749992365</v>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>9</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Facility4</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>234</v>
-      </c>
-      <c r="F19" t="n">
-        <v>54288</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>56</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J19" t="n">
-        <v>54.32</v>
-      </c>
-      <c r="K19" t="n">
-        <v>12602.24</v>
-      </c>
-      <c r="L19" t="n">
-        <v>232</v>
-      </c>
-      <c r="M19" t="n">
-        <v>41685.76</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>10</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Facility5</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>231</v>
-      </c>
-      <c r="F20" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>13</v>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J20" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K20" t="n">
-        <v>163.93</v>
-      </c>
-      <c r="L20" t="n">
-        <v>13</v>
-      </c>
-      <c r="M20" t="n">
-        <v>2839.07</v>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1663,20 +1250,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model is infeasible. Likely causes include:
- - Insufficient supplier capacity relative to demand.
- - Custom rule constraints conflicting with overall volume/demand.
-  Bid 1: demand = 700, capacities: Supplier A (BusinessUnit=A capacity): 500; Supplier B (Bid ID capacity): 4000; Supplier C (Bid ID capacity): 3000; 
-  Bid 2: demand = 9000, capacities: Supplier A (BusinessUnit=B capacity): 1000; Supplier B (Bid ID capacity): 8000; Supplier C (Bid ID capacity): 5000; 
-  Bid 3: demand = 600, capacities: Supplier A (BusinessUnit=A capacity): 500; Supplier B (Bid ID capacity): 6000; Supplier C (Bid ID capacity): 7000; 
-  Bid 4: demand = 5670, capacities: Supplier A (BusinessUnit=A capacity): 500; Supplier B (Bid ID capacity): 4000; Supplier C (Bid ID capacity): 3000; 
-  Bid 5: demand = 45, capacities: Supplier A (BusinessUnit=A capacity): 500; Supplier B (Bid ID capacity): 8000; Supplier C (Bid ID capacity): 5000; 
-  Bid 6: demand = 242, capacities: Supplier A (BusinessUnit=B capacity): 1000; Supplier B (Bid ID capacity): 6000; Supplier C (Bid ID capacity): 7000; 
-  Bid 7: demand = 664, capacities: Supplier A (BusinessUnit=B capacity): 1000; Supplier B (Bid ID capacity): 4000; Supplier C (Bid ID capacity): 3000; 
-  Bid 8: demand = 24, capacities: Supplier A (BusinessUnit=B capacity): 1000; Supplier B (Bid ID capacity): 8000; Supplier C (Bid ID capacity): 5000; 
-  Bid 9: demand = 232, capacities: Supplier A (BusinessUnit=A capacity): 500; Supplier B (Bid ID capacity): 6000; Supplier C (Bid ID capacity): 7000; 
-  Bid 10: demand = 13, capacities: Supplier A (BusinessUnit=A capacity): 500; Supplier B (Bid ID capacity): 5000; Supplier C (Bid ID capacity): 7000; 
-Please review supplier capacities, demand, and custom rule constraints.</t>
+          <t>Model is optimal.</t>
         </is>
       </c>
     </row>
@@ -1717,11 +1291,20 @@
  - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
 BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 80 x_B_2 - 65 x_B_3 - 75 x_B_4
  - 34 x_B_5 - 24 x_B_6 - 53 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
-BaseSpend_C: S0_C - 55 x_C_1 - 75 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
+BaseSpend_C: S0_C - 55 x_C_1 - 75 x_C_10 - 75 x_C_2 - 60 x_C_3 - 19 x_C_4
  - 24 x_C_5 - 64 x_C_6 - 86 x_C_7 - 24 x_C_8 - 13 x_C_9 = 0
-Capacity_A_BusinessUnit_A: x_A_1 + x_A_10 + x_A_3 + x_A_4 + x_A_5 + x_A_9
- &lt;= 500
-Capacity_A_BusinessUnit_B: x_A_2 + x_A_6 + x_A_7 + x_A_8 &lt;= 1000
+BidExclusion_0_5_B: x_B_5 = 0
+BidExclusion_0_5_C: x_C_5 = 0
+Capacity_A_Bid_ID_1: x_A_1 &lt;= 5000
+Capacity_A_Bid_ID_10: x_A_10 &lt;= 3000
+Capacity_A_Bid_ID_2: x_A_2 &lt;= 4000
+Capacity_A_Bid_ID_3: x_A_3 &lt;= 3000
+Capacity_A_Bid_ID_4: x_A_4 &lt;= 5000
+Capacity_A_Bid_ID_5: x_A_5 &lt;= 4000
+Capacity_A_Bid_ID_6: x_A_6 &lt;= 3000
+Capacity_A_Bid_ID_7: x_A_7 &lt;= 5000
+Capacity_A_Bid_ID_8: x_A_8 &lt;= 4000
+Capacity_A_Bid_ID_9: x_A_9 &lt;= 3000
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 4000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 5000
 Capacity_B_Bid_ID_2: x_B_2 &lt;= 8000
@@ -1752,13 +1335,13 @@
 Demand_7: x_A_7 + x_B_7 + x_C_7 = 664
 Demand_8: x_A_8 + x_B_8 + x_C_8 = 24
 Demand_9: x_A_9 + x_B_9 + x_C_9 = 232
-DiscountTierLower_A_0: d_A - 145500 z_discount_A_0 &gt;= -145500
-DiscountTierLower_A_1: - 0.01 S0_A + d_A - 145500 z_discount_A_1 &gt;= -145500
+DiscountTierLower_A_0: d_A - 3783000 z_discount_A_0 &gt;= -3783000
+DiscountTierLower_A_1: - 0.01 S0_A + d_A - 3783000 z_discount_A_1 &gt;= -3783000
 DiscountTierLower_B_0: d_B - 5723000 z_discount_B_0 &gt;= -5723000
 DiscountTierLower_B_1: - 0.03 S0_B + d_B - 5723000 z_discount_B_1 &gt;= -5723000
 DiscountTierLower_C_0: d_C - 5044000 z_discount_C_0 &gt;= -5044000
 DiscountTierLower_C_1: - 0.04 S0_C + d_C - 5044000 z_discount_C_1 &gt;= -5044000
-DiscountTierMax_A_0: 145500 z_discount_A_0 &lt;= 146500
+DiscountTierMax_A_0: 3783000 z_discount_A_0 &lt;= 3784000
 DiscountTierMax_B_0: 5723000 z_discount_B_0 &lt;= 5723500
 DiscountTierMax_C_0: 5044000 z_discount_C_0 &lt;= 5044500
 _dummy: __dummy = 0
@@ -1773,8 +1356,8 @@
 DiscountTierSelect_A: z_discount_A_0 + z_discount_A_1 = 1
 DiscountTierSelect_B: z_discount_B_0 + z_discount_B_1 = 1
 DiscountTierSelect_C: z_discount_C_0 + z_discount_C_1 = 1
-DiscountTierUpper_A_0: d_A + 145500 z_discount_A_0 &lt;= 145500
-DiscountTierUpper_A_1: - 0.01 S0_A + d_A + 145500 z_discount_A_1 &lt;= 145500
+DiscountTierUpper_A_0: d_A + 3783000 z_discount_A_0 &lt;= 3783000
+DiscountTierUpper_A_1: - 0.01 S0_A + d_A + 3783000 z_discount_A_1 &lt;= 3783000
 DiscountTierUpper_B_0: d_B + 5723000 z_discount_B_0 &lt;= 5723000
 DiscountTierUpper_B_1: - 0.03 S0_B + d_B + 5723000 z_discount_B_1 &lt;= 5723000
 DiscountTierUpper_C_0: d_C + 5044000 z_discount_C_0 &lt;= 5044000
@@ -1782,13 +1365,13 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
-RebateTierLower_A_0: rebate_A - 145500 y_rebate_A_0 &gt;= -145500
-RebateTierLower_A_1: - 0.1 S_A + rebate_A - 145500 y_rebate_A_1 &gt;= -145500
+RebateTierLower_A_0: rebate_A - 3783000 y_rebate_A_0 &gt;= -3783000
+RebateTierLower_A_1: - 0.1 S_A + rebate_A - 3783000 y_rebate_A_1 &gt;= -3783000
 RebateTierLower_B_0: rebate_B - 5723000 y_rebate_B_0 &gt;= -5723000
 RebateTierLower_B_1: - 0.05 S_B + rebate_B - 5723000 y_rebate_B_1 &gt;= -5723000
 RebateTierLower_C_0: rebate_C - 5044000 y_rebate_C_0 &gt;= -5044000
 RebateTierLower_C_1: - 0.07 S_C + rebate_C - 5044000 y_rebate_C_1 &gt;= -5044000
-RebateTierMax_A_0: 145500 y_rebate_A_0 &lt;= 146000
+RebateTierMax_A_0: 3783000 y_rebate_A_0 &lt;= 3783500
 RebateTierMax_B_0: 5723000 y_rebate_B_0 &lt;= 5723500
 RebateTierMax_C_0: 5044000 y_rebate_C_0 &lt;= 5044700
 RebateTierMin_A_0: __dummy &gt;= 0
@@ -1801,82 +1384,12 @@
 RebateTierSelect_A: y_rebate_A_0 + y_rebate_A_1 = 1
 RebateTierSelect_B: y_rebate_B_0 + y_rebate_B_1 = 1
 RebateTierSelect_C: y_rebate_C_0 + y_rebate_C_1 = 1
-RebateTierUpper_A_0: rebate_A + 145500 y_rebate_A_0 &lt;= 145500
-RebateTierUpper_A_1: - 0.1 S_A + rebate_A + 145500 y_rebate_A_1 &lt;= 145500
+RebateTierUpper_A_0: rebate_A + 3783000 y_rebate_A_0 &lt;= 3783000
+RebateTierUpper_A_1: - 0.1 S_A + rebate_A + 3783000 y_rebate_A_1 &lt;= 3783000
 RebateTierUpper_B_0: rebate_B + 5723000 y_rebate_B_0 &lt;= 5723000
 RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 5723000 y_rebate_B_1 &lt;= 5723000
 RebateTierUpper_C_0: rebate_C + 5044000 y_rebate_C_0 &lt;= 5044000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 5044000 y_rebate_C_1 &lt;= 5044000
-RuleSingleSupplier_0_1: w_0_1_A + w_0_1_B + w_0_1_C = 1
-RuleSingleSupplier_1_2: w_1_2_A + w_1_2_B + w_1_2_C = 1
-RuleSingleSupplier_2_10: w_2_10_A + w_2_10_B + w_2_10_C = 1
-RuleSingleSupplier_3_3: w_3_3_A + w_3_3_B + w_3_3_C = 1
-RuleSingleSupplier_4_4: w_4_4_A + w_4_4_B + w_4_4_C = 1
-RuleSingleSupplier_5_5: w_5_5_A + w_5_5_B + w_5_5_C = 1
-RuleSingleSupplier_6_6: w_6_6_A + w_6_6_B + w_6_6_C = 1
-RuleSingleSupplier_7_7: w_7_7_A + w_7_7_B + w_7_7_C = 1
-RuleSingleSupplier_8_8: w_8_8_A + w_8_8_B + w_8_8_C = 1
-RuleSingleSupplier_9_9: w_9_9_A + w_9_9_B + w_9_9_C = 1
-RuleSupplierIndicatorLB_0_1_A: - 0.001 w_0_1_A + x_A_1 &gt;= 0
-RuleSupplierIndicatorLB_0_1_B: - 0.001 w_0_1_B + x_B_1 &gt;= 0
-RuleSupplierIndicatorLB_0_1_C: - 0.001 w_0_1_C + x_C_1 &gt;= 0
-RuleSupplierIndicatorLB_1_2_A: - 0.001 w_1_2_A + x_A_2 &gt;= 0
-RuleSupplierIndicatorLB_1_2_B: - 0.001 w_1_2_B + x_B_2 &gt;= 0
-RuleSupplierIndicatorLB_1_2_C: - 0.001 w_1_2_C + x_C_2 &gt;= 0
-RuleSupplierIndicatorLB_2_10_A: - 0.001 w_2_10_A + x_A_10 &gt;= 0
-RuleSupplierIndicatorLB_2_10_B: - 0.001 w_2_10_B + x_B_10 &gt;= 0
-RuleSupplierIndicatorLB_2_10_C: - 0.001 w_2_10_C + x_C_10 &gt;= 0
-RuleSupplierIndicatorLB_3_3_A: - 0.001 w_3_3_A + x_A_3 &gt;= 0
-RuleSupplierIndicatorLB_3_3_B: - 0.001 w_3_3_B + x_B_3 &gt;= 0
-RuleSupplierIndicatorLB_3_3_C: - 0.001 w_3_3_C + x_C_3 &gt;= 0
-RuleSupplierIndicatorLB_4_4_A: - 0.001 w_4_4_A + x_A_4 &gt;= 0
-RuleSupplierIndicatorLB_4_4_B: - 0.001 w_4_4_B + x_B_4 &gt;= 0
-RuleSupplierIndicatorLB_4_4_C: - 0.001 w_4_4_C + x_C_4 &gt;= 0
-RuleSupplierIndicatorLB_5_5_A: - 0.001 w_5_5_A + x_A_5 &gt;= 0
-RuleSupplierIndicatorLB_5_5_B: - 0.001 w_5_5_B + x_B_5 &gt;= 0
-RuleSupplierIndicatorLB_5_5_C: - 0.001 w_5_5_C + x_C_5 &gt;= 0
-RuleSupplierIndicatorLB_6_6_A: - 0.001 w_6_6_A + x_A_6 &gt;= 0
-RuleSupplierIndicatorLB_6_6_B: - 0.001 w_6_6_B + x_B_6 &gt;= 0
-RuleSupplierIndicatorLB_6_6_C: - 0.001 w_6_6_C + x_C_6 &gt;= 0
-RuleSupplierIndicatorLB_7_7_A: - 0.001 w_7_7_A + x_A_7 &gt;= 0
-RuleSupplierIndicatorLB_7_7_B: - 0.001 w_7_7_B + x_B_7 &gt;= 0
-RuleSupplierIndicatorLB_7_7_C: - 0.001 w_7_7_C + x_C_7 &gt;= 0
-RuleSupplierIndicatorLB_8_8_A: - 0.001 w_8_8_A + x_A_8 &gt;= 0
-RuleSupplierIndicatorLB_8_8_B: - 0.001 w_8_8_B + x_B_8 &gt;= 0
-RuleSupplierIndicatorLB_8_8_C: - 0.001 w_8_8_C + x_C_8 &gt;= 0
-RuleSupplierIndicatorLB_9_9_A: - 0.001 w_9_9_A + x_A_9 &gt;= 0
-RuleSupplierIndicatorLB_9_9_B: - 0.001 w_9_9_B + x_B_9 &gt;= 0
-RuleSupplierIndicatorLB_9_9_C: - 0.001 w_9_9_C + x_C_9 &gt;= 0
-RuleSupplierIndicator_0_1_A: - 1000000000 w_0_1_A + x_A_1 &lt;= 0
-RuleSupplierIndicator_0_1_B: - 1000000000 w_0_1_B + x_B_1 &lt;= 0
-RuleSupplierIndicator_0_1_C: - 1000000000 w_0_1_C + x_C_1 &lt;= 0
-RuleSupplierIndicator_1_2_A: - 1000000000 w_1_2_A + x_A_2 &lt;= 0
-RuleSupplierIndicator_1_2_B: - 1000000000 w_1_2_B + x_B_2 &lt;= 0
-RuleSupplierIndicator_1_2_C: - 1000000000 w_1_2_C + x_C_2 &lt;= 0
-RuleSupplierIndicator_2_10_A: - 1000000000 w_2_10_A + x_A_10 &lt;= 0
-RuleSupplierIndicator_2_10_B: - 1000000000 w_2_10_B + x_B_10 &lt;= 0
-RuleSupplierIndicator_2_10_C: - 1000000000 w_2_10_C + x_C_10 &lt;= 0
-RuleSupplierIndicator_3_3_A: - 1000000000 w_3_3_A + x_A_3 &lt;= 0
-RuleSupplierIndicator_3_3_B: - 1000000000 w_3_3_B + x_B_3 &lt;= 0
-RuleSupplierIndicator_3_3_C: - 1000000000 w_3_3_C + x_C_3 &lt;= 0
-RuleSupplierIndicator_4_4_A: - 1000000000 w_4_4_A + x_A_4 &lt;= 0
-RuleSupplierIndicator_4_4_B: - 1000000000 w_4_4_B + x_B_4 &lt;= 0
-RuleSupplierIndicator_4_4_C: - 1000000000 w_4_4_C + x_C_4 &lt;= 0
-RuleSupplierIndicator_5_5_A: - 1000000000 w_5_5_A + x_A_5 &lt;= 0
-RuleSupplierIndicator_5_5_B: - 1000000000 w_5_5_B + x_B_5 &lt;= 0
-RuleSupplierIndicator_5_5_C: - 1000000000 w_5_5_C + x_C_5 &lt;= 0
-RuleSupplierIndicator_6_6_A: - 1000000000 w_6_6_A + x_A_6 &lt;= 0
-RuleSupplierIndicator_6_6_B: - 1000000000 w_6_6_B + x_B_6 &lt;= 0
-RuleSupplierIndicator_6_6_C: - 1000000000 w_6_6_C + x_C_6 &lt;= 0
-RuleSupplierIndicator_7_7_A: - 1000000000 w_7_7_A + x_A_7 &lt;= 0
-RuleSupplierIndicator_7_7_B: - 1000000000 w_7_7_B + x_B_7 &lt;= 0
-RuleSupplierIndicator_7_7_C: - 1000000000 w_7_7_C + x_C_7 &lt;= 0
-RuleSupplierIndicator_8_8_A: - 1000000000 w_8_8_A + x_A_8 &lt;= 0
-RuleSupplierIndicator_8_8_B: - 1000000000 w_8_8_B + x_B_8 &lt;= 0
-RuleSupplierIndicator_8_8_C: - 1000000000 w_8_8_C + x_C_8 &lt;= 0
-RuleSupplierIndicator_9_9_A: - 1000000000 w_9_9_A + x_A_9 &lt;= 0
-RuleSupplierIndicator_9_9_B: - 1000000000 w_9_9_B + x_B_9 &lt;= 0
-RuleSupplierIndicator_9_9_C: - 1000000000 w_9_9_C + x_C_9 &lt;= 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1903,8 +1416,6 @@
  - x_B_8 - x_B_9 = 0
 Volume_C: V_C - x_C_1 - x_C_10 - x_C_2 - x_C_3 - x_C_4 - x_C_5 - x_C_6 - x_C_7
  - x_C_8 - x_C_9 = 0
-Bounds
- __dummy = 0
 Binaries
 T_10_A
 T_10_B
@@ -1926,36 +1437,6 @@
 T_8_B
 T_9_A
 T_9_B
-w_0_1_A
-w_0_1_B
-w_0_1_C
-w_1_2_A
-w_1_2_B
-w_1_2_C
-w_2_10_A
-w_2_10_B
-w_2_10_C
-w_3_3_A
-w_3_3_B
-w_3_3_C
-w_4_4_A
-w_4_4_B
-w_4_4_C
-w_5_5_A
-w_5_5_B
-w_5_5_C
-w_6_6_A
-w_6_6_B
-w_6_6_C
-w_7_7_A
-w_7_7_B
-w_7_7_C
-w_8_8_A
-w_8_8_B
-w_8_8_C
-w_9_9_A
-w_9_9_B
-w_9_9_C
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0
@@ -1984,7 +1465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2022,16 +1503,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BusinessUnit</t>
+          <t>Bid ID</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3">
@@ -2042,22 +1523,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BusinessUnit</t>
+          <t>Bid ID</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2067,17 +1548,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2087,17 +1568,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>8000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2107,17 +1588,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>6000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2127,17 +1608,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2147,17 +1628,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2167,17 +1648,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>6000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2187,17 +1668,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2207,11 +1688,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>8000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="12">
@@ -2227,11 +1708,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="13">
@@ -2247,17 +1728,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2267,17 +1748,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2287,17 +1768,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2307,17 +1788,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>7000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2327,17 +1808,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2347,17 +1828,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>5000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2367,17 +1848,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2387,17 +1868,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>3000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2407,7 +1888,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -2427,11 +1908,11 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>7000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="23">
@@ -2447,10 +1928,170 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D31" t="n">
         <v>7000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to and correction to liveapp, only thing not working is apply to all
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>70000</v>
+        <v>50000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -555,13 +555,13 @@
         <v>52.8</v>
       </c>
       <c r="K2" t="n">
-        <v>36960</v>
+        <v>26400</v>
       </c>
       <c r="L2" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="M2" t="n">
-        <v>33040</v>
+        <v>23600</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -569,16 +569,16 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>2587.2</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -588,47 +588,47 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>780000</v>
+        <v>20000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>72</v>
+        <v>19.8</v>
       </c>
       <c r="K3" t="n">
-        <v>360000</v>
+        <v>3960</v>
       </c>
       <c r="L3" t="n">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="M3" t="n">
-        <v>420000</v>
+        <v>16040</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>25200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -637,7 +637,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -654,49 +654,49 @@
         <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>624000</v>
+        <v>780000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>69.3</v>
+        <v>72</v>
       </c>
       <c r="K4" t="n">
-        <v>277200</v>
+        <v>360000</v>
       </c>
       <c r="L4" t="n">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="M4" t="n">
-        <v>346800</v>
+        <v>420000</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -706,52 +706,52 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>423</v>
+        <v>156</v>
       </c>
       <c r="F5" t="n">
-        <v>253800</v>
+        <v>624000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>57.59999999999999</v>
+        <v>69.3</v>
       </c>
       <c r="K5" t="n">
-        <v>34560</v>
+        <v>277200</v>
       </c>
       <c r="L5" t="n">
-        <v>600</v>
+        <v>4000</v>
       </c>
       <c r="M5" t="n">
-        <v>219240</v>
+        <v>346800</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>2419.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="F6" t="n">
-        <v>1359000</v>
+        <v>253800</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -788,16 +788,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>18.24</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K6" t="n">
-        <v>54719.99999999999</v>
+        <v>34560</v>
       </c>
       <c r="L6" t="n">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="M6" t="n">
-        <v>1304280</v>
+        <v>219240</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>3830.4</v>
+        <v>2419.2</v>
       </c>
     </row>
     <row r="7">
@@ -814,7 +814,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -831,49 +831,49 @@
         <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>1209510</v>
+        <v>1359000</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>22.77</v>
+        <v>18.24</v>
       </c>
       <c r="K7" t="n">
-        <v>60795.9</v>
+        <v>54719.99999999999</v>
       </c>
       <c r="L7" t="n">
-        <v>2670</v>
+        <v>3000</v>
       </c>
       <c r="M7" t="n">
-        <v>1148714.1</v>
+        <v>1304280</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>3830.4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -887,10 +887,10 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="F8" t="n">
-        <v>15390</v>
+        <v>1209510</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -906,16 +906,16 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>53.46</v>
+        <v>22.77</v>
       </c>
       <c r="K8" t="n">
-        <v>2405.7</v>
+        <v>60795.9</v>
       </c>
       <c r="L8" t="n">
-        <v>45</v>
+        <v>2670</v>
       </c>
       <c r="M8" t="n">
-        <v>12984.3</v>
+        <v>1148714.1</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,14 +946,14 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>653</v>
+        <v>342</v>
       </c>
       <c r="F9" t="n">
-        <v>158026</v>
+        <v>15390</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -961,33 +961,33 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>24</v>
+        <v>23.04</v>
       </c>
       <c r="K9" t="n">
-        <v>5808</v>
+        <v>1036.8</v>
       </c>
       <c r="L9" t="n">
-        <v>242</v>
+        <v>45</v>
       </c>
       <c r="M9" t="n">
-        <v>152218</v>
+        <v>14353.2</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>72.57600000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1005,35 +1005,35 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>432</v>
+        <v>653</v>
       </c>
       <c r="F10" t="n">
-        <v>286848</v>
+        <v>158026</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>22.77</v>
+        <v>24</v>
       </c>
       <c r="K10" t="n">
-        <v>15119.28</v>
+        <v>5808</v>
       </c>
       <c r="L10" t="n">
-        <v>664</v>
+        <v>242</v>
       </c>
       <c r="M10" t="n">
-        <v>271728.72</v>
+        <v>152218</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Facility3</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1064,35 +1064,35 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F11" t="n">
-        <v>10944</v>
+        <v>286848</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>13</v>
+        <v>22.77</v>
       </c>
       <c r="K11" t="n">
-        <v>312</v>
+        <v>15119.28</v>
       </c>
       <c r="L11" t="n">
-        <v>24</v>
+        <v>664</v>
       </c>
       <c r="M11" t="n">
-        <v>10632</v>
+        <v>271728.72</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Facility4</t>
+          <t>Facility3</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1123,14 +1123,14 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>234</v>
+        <v>456</v>
       </c>
       <c r="F12" t="n">
-        <v>54288</v>
+        <v>10944</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -1138,33 +1138,33 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>12.48</v>
+        <v>13</v>
       </c>
       <c r="K12" t="n">
-        <v>2895.36</v>
+        <v>312</v>
       </c>
       <c r="L12" t="n">
-        <v>232</v>
+        <v>24</v>
       </c>
       <c r="M12" t="n">
-        <v>51392.64</v>
+        <v>10632</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>202.6752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Facility5</t>
+          <t>Facility4</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1182,14 +1182,14 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F13" t="n">
-        <v>3003</v>
+        <v>54288</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -1197,27 +1197,86 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2895.36</v>
+      </c>
+      <c r="L13" t="n">
+        <v>232</v>
+      </c>
+      <c r="M13" t="n">
+        <v>51392.64</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>202.6752</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>231</v>
+      </c>
+      <c r="F14" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>13</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="J14" t="n">
         <v>13</v>
       </c>
-      <c r="K13" t="n">
+      <c r="K14" t="n">
         <v>169</v>
       </c>
-      <c r="L13" t="n">
+      <c r="L14" t="n">
         <v>13</v>
       </c>
-      <c r="M13" t="n">
+      <c r="M14" t="n">
         <v>2834</v>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O13" t="n">
+      <c r="O14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1287,14 +1346,12 @@
 Minimize
 OBJ: S_A + S_B + S_C - rebate_A - rebate_B - rebate_C
 Subject To
-BaseSpend_A: S0_A - 50 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
+BaseSpend_A: S0_A - 20 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
  - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
 BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 80 x_B_2 - 65 x_B_3 - 75 x_B_4
  - 34 x_B_5 - 24 x_B_6 - 53 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
 BaseSpend_C: S0_C - 55 x_C_1 - 75 x_C_10 - 75 x_C_2 - 60 x_C_3 - 19 x_C_4
  - 24 x_C_5 - 64 x_C_6 - 86 x_C_7 - 24 x_C_8 - 13 x_C_9 = 0
-BidExclusion_0_5_B: x_B_5 = 0
-BidExclusion_0_5_C: x_C_5 = 0
 Capacity_A_Bid_ID_1: x_A_1 &lt;= 5000
 Capacity_A_Bid_ID_10: x_A_10 &lt;= 3000
 Capacity_A_Bid_ID_2: x_A_2 &lt;= 4000
@@ -1390,6 +1447,7 @@
 RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 5723000 y_rebate_B_1 &lt;= 5723000
 RebateTierUpper_C_0: rebate_C + 5044000 y_rebate_C_0 &lt;= 5044000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 5044000 y_rebate_C_1 &lt;= 5044000
+Rule_0_1: x_B_1 + x_C_1 &gt;= 500
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
force commit changes from last commit
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,40 +536,40 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>50000</v>
+        <v>35000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>52.8</v>
+        <v>19.8</v>
       </c>
       <c r="K2" t="n">
-        <v>26400</v>
+        <v>6930</v>
       </c>
       <c r="L2" t="n">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="M2" t="n">
-        <v>23600</v>
+        <v>28070</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>1848</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -595,40 +595,40 @@
         <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>20000</v>
+        <v>35000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>19.8</v>
+        <v>58.2</v>
       </c>
       <c r="K3" t="n">
-        <v>3960</v>
+        <v>20370</v>
       </c>
       <c r="L3" t="n">
-        <v>200</v>
+        <v>350</v>
       </c>
       <c r="M3" t="n">
-        <v>16040</v>
+        <v>14630</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>1018.5</v>
       </c>
     </row>
     <row r="4">
@@ -713,7 +713,7 @@
         <v>156</v>
       </c>
       <c r="F5" t="n">
-        <v>624000</v>
+        <v>583752</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -732,13 +732,13 @@
         <v>69.3</v>
       </c>
       <c r="K5" t="n">
-        <v>277200</v>
+        <v>259320.6</v>
       </c>
       <c r="L5" t="n">
-        <v>4000</v>
+        <v>3742</v>
       </c>
       <c r="M5" t="n">
-        <v>346800</v>
+        <v>324431.4</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -751,11 +751,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -765,52 +765,52 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>423</v>
+        <v>156</v>
       </c>
       <c r="F6" t="n">
-        <v>253800</v>
+        <v>40248</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>57.59999999999999</v>
+        <v>77.59999999999999</v>
       </c>
       <c r="K6" t="n">
-        <v>34560</v>
+        <v>20020.8</v>
       </c>
       <c r="L6" t="n">
-        <v>600</v>
+        <v>258</v>
       </c>
       <c r="M6" t="n">
-        <v>219240</v>
+        <v>20227.2</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>2419.2</v>
+        <v>1001.04</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="F7" t="n">
-        <v>1359000</v>
+        <v>253800</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -839,7 +839,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>18.24</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K7" t="n">
-        <v>54719.99999999999</v>
+        <v>34560</v>
       </c>
       <c r="L7" t="n">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="M7" t="n">
-        <v>1304280</v>
+        <v>219240</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -864,7 +864,7 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>3830.4</v>
+        <v>2419.2</v>
       </c>
     </row>
     <row r="8">
@@ -873,7 +873,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -890,49 +890,49 @@
         <v>453</v>
       </c>
       <c r="F8" t="n">
-        <v>1209510</v>
+        <v>1359000</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>22.77</v>
+        <v>18.24</v>
       </c>
       <c r="K8" t="n">
-        <v>60795.9</v>
+        <v>54719.99999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>2670</v>
+        <v>3000</v>
       </c>
       <c r="M8" t="n">
-        <v>1148714.1</v>
+        <v>1304280</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>3830.4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -946,48 +946,48 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="F9" t="n">
-        <v>15390</v>
+        <v>1209510</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>23.04</v>
+        <v>22.77</v>
       </c>
       <c r="K9" t="n">
-        <v>1036.8</v>
+        <v>60795.9</v>
       </c>
       <c r="L9" t="n">
-        <v>45</v>
+        <v>2670</v>
       </c>
       <c r="M9" t="n">
-        <v>14353.2</v>
+        <v>1148714.1</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>72.57600000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1005,14 +1005,14 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>653</v>
+        <v>342</v>
       </c>
       <c r="F10" t="n">
-        <v>158026</v>
+        <v>15390</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -1020,33 +1020,33 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>24</v>
+        <v>23.04</v>
       </c>
       <c r="K10" t="n">
-        <v>5808</v>
+        <v>1036.8</v>
       </c>
       <c r="L10" t="n">
-        <v>242</v>
+        <v>45</v>
       </c>
       <c r="M10" t="n">
-        <v>152218</v>
+        <v>14353.2</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>72.57600000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1064,48 +1064,48 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>432</v>
+        <v>653</v>
       </c>
       <c r="F11" t="n">
-        <v>286848</v>
+        <v>158026</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>22.77</v>
+        <v>23.28</v>
       </c>
       <c r="K11" t="n">
-        <v>15119.28</v>
+        <v>5633.76</v>
       </c>
       <c r="L11" t="n">
-        <v>664</v>
+        <v>242</v>
       </c>
       <c r="M11" t="n">
-        <v>271728.72</v>
+        <v>152392.24</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>281.688</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Facility3</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1123,35 +1123,35 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F12" t="n">
-        <v>10944</v>
+        <v>286848</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>13</v>
+        <v>22.77</v>
       </c>
       <c r="K12" t="n">
-        <v>312</v>
+        <v>15119.28</v>
       </c>
       <c r="L12" t="n">
-        <v>24</v>
+        <v>664</v>
       </c>
       <c r="M12" t="n">
-        <v>10632</v>
+        <v>271728.72</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Facility4</t>
+          <t>Facility3</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1182,14 +1182,14 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>234</v>
+        <v>456</v>
       </c>
       <c r="F13" t="n">
-        <v>54288</v>
+        <v>10944</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -1197,33 +1197,33 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>12.48</v>
+        <v>12.61</v>
       </c>
       <c r="K13" t="n">
-        <v>2895.36</v>
+        <v>302.64</v>
       </c>
       <c r="L13" t="n">
-        <v>232</v>
+        <v>24</v>
       </c>
       <c r="M13" t="n">
-        <v>51392.64</v>
+        <v>10641.36</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>202.6752</v>
+        <v>15.132</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Facility5</t>
+          <t>Facility4</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1241,14 +1241,14 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F14" t="n">
-        <v>3003</v>
+        <v>54288</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1256,28 +1256,87 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J14" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2895.36</v>
+      </c>
+      <c r="L14" t="n">
+        <v>232</v>
+      </c>
+      <c r="M14" t="n">
+        <v>51392.64</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>202.6752</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>10</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>231</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
         <v>13</v>
       </c>
-      <c r="K14" t="n">
-        <v>169</v>
-      </c>
-      <c r="L14" t="n">
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>12.61</v>
+      </c>
+      <c r="K15" t="n">
+        <v>163.93</v>
+      </c>
+      <c r="L15" t="n">
         <v>13</v>
       </c>
-      <c r="M14" t="n">
-        <v>2834</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
+      <c r="M15" t="n">
+        <v>2839.07</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>8.1965</v>
       </c>
     </row>
   </sheetData>
@@ -1447,7 +1506,7 @@
 RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 5723000 y_rebate_B_1 &lt;= 5723000
 RebateTierUpper_C_0: rebate_C + 5044000 y_rebate_C_0 &lt;= 5044000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 5044000 y_rebate_C_1 &lt;= 5044000
-Rule_0_1: x_B_1 + x_C_1 &gt;= 500
+Rule_0_1: - 0.5 x_A_1 + 0.5 x_B_1 - 0.5 x_C_1 &gt;= 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
updated apply to all to be working now, additionally disabled supplier scope in exclude supplier
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,36 +599,36 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>58.2</v>
+        <v>52.8</v>
       </c>
       <c r="K3" t="n">
-        <v>20370</v>
+        <v>18480</v>
       </c>
       <c r="L3" t="n">
         <v>350</v>
       </c>
       <c r="M3" t="n">
-        <v>14630</v>
+        <v>16520</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>1018.5</v>
+        <v>1293.6</v>
       </c>
     </row>
     <row r="4">
@@ -654,7 +654,7 @@
         <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>780000</v>
+        <v>1404000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -673,13 +673,13 @@
         <v>72</v>
       </c>
       <c r="K4" t="n">
-        <v>360000</v>
+        <v>648000</v>
       </c>
       <c r="L4" t="n">
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="M4" t="n">
-        <v>420000</v>
+        <v>756000</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -687,16 +687,16 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>25200</v>
+        <v>45360.00000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -706,14 +706,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>156</v>
+        <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>583752</v>
+        <v>126900</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>69.3</v>
+        <v>54.45</v>
       </c>
       <c r="K5" t="n">
-        <v>259320.6</v>
+        <v>16335</v>
       </c>
       <c r="L5" t="n">
-        <v>3742</v>
+        <v>300</v>
       </c>
       <c r="M5" t="n">
-        <v>324431.4</v>
+        <v>110565</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -751,11 +751,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -765,52 +765,52 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>156</v>
+        <v>423</v>
       </c>
       <c r="F6" t="n">
-        <v>40248</v>
+        <v>126900</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>77.59999999999999</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K6" t="n">
-        <v>20020.8</v>
+        <v>17280</v>
       </c>
       <c r="L6" t="n">
-        <v>258</v>
+        <v>300</v>
       </c>
       <c r="M6" t="n">
-        <v>20227.2</v>
+        <v>109620</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>1001.04</v>
+        <v>1209.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility1</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,43 +828,43 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>253800</v>
+        <v>1284255</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>57.59999999999999</v>
+        <v>22.77</v>
       </c>
       <c r="K7" t="n">
-        <v>34560</v>
+        <v>64552.95</v>
       </c>
       <c r="L7" t="n">
-        <v>600</v>
+        <v>2835</v>
       </c>
       <c r="M7" t="n">
-        <v>219240</v>
+        <v>1219702.05</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>2419.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -873,7 +873,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -890,7 +890,7 @@
         <v>453</v>
       </c>
       <c r="F8" t="n">
-        <v>1359000</v>
+        <v>1284255</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>18.24</v>
       </c>
       <c r="K8" t="n">
-        <v>54719.99999999999</v>
+        <v>51710.39999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>3000</v>
+        <v>2835</v>
       </c>
       <c r="M8" t="n">
-        <v>1304280</v>
+        <v>1232544.6</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -923,58 +923,58 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>3830.4</v>
+        <v>3619.728</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>342</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7695</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>453</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1209510</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>22.77</v>
+        <v>34</v>
       </c>
       <c r="K9" t="n">
-        <v>60795.9</v>
+        <v>765</v>
       </c>
       <c r="L9" t="n">
-        <v>2670</v>
+        <v>22.5</v>
       </c>
       <c r="M9" t="n">
-        <v>1148714.1</v>
+        <v>6930</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1008,7 +1008,7 @@
         <v>342</v>
       </c>
       <c r="F10" t="n">
-        <v>15390</v>
+        <v>7695</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1027,13 +1027,13 @@
         <v>23.04</v>
       </c>
       <c r="K10" t="n">
-        <v>1036.8</v>
+        <v>518.4</v>
       </c>
       <c r="L10" t="n">
-        <v>45</v>
+        <v>22.5</v>
       </c>
       <c r="M10" t="n">
-        <v>14353.2</v>
+        <v>7176.6</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1041,7 +1041,7 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>72.57600000000001</v>
+        <v>36.288</v>
       </c>
     </row>
     <row r="11">
@@ -1067,7 +1067,7 @@
         <v>653</v>
       </c>
       <c r="F11" t="n">
-        <v>158026</v>
+        <v>144966</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1079,37 +1079,37 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>23.28</v>
+        <v>24</v>
       </c>
       <c r="K11" t="n">
-        <v>5633.76</v>
+        <v>5328</v>
       </c>
       <c r="L11" t="n">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="M11" t="n">
-        <v>152392.24</v>
+        <v>139638</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>281.688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>432</v>
+        <v>653</v>
       </c>
       <c r="F12" t="n">
-        <v>286848</v>
+        <v>13060</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1134,7 +1134,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1142,16 +1142,16 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>22.77</v>
+        <v>41.58</v>
       </c>
       <c r="K12" t="n">
-        <v>15119.28</v>
+        <v>831.5999999999999</v>
       </c>
       <c r="L12" t="n">
-        <v>664</v>
+        <v>20</v>
       </c>
       <c r="M12" t="n">
-        <v>271728.72</v>
+        <v>12228.4</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Facility3</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1182,48 +1182,48 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F13" t="n">
-        <v>10944</v>
+        <v>286848</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>12.61</v>
+        <v>22.77</v>
       </c>
       <c r="K13" t="n">
-        <v>302.64</v>
+        <v>15119.28</v>
       </c>
       <c r="L13" t="n">
-        <v>24</v>
+        <v>664</v>
       </c>
       <c r="M13" t="n">
-        <v>10641.36</v>
+        <v>271728.72</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>15.132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Facility4</t>
+          <t>Facility3</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1241,14 +1241,14 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>234</v>
+        <v>456</v>
       </c>
       <c r="F14" t="n">
-        <v>54288</v>
+        <v>10944</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1256,87 +1256,205 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>12.48</v>
+        <v>13</v>
       </c>
       <c r="K14" t="n">
-        <v>2895.36</v>
+        <v>312</v>
       </c>
       <c r="L14" t="n">
-        <v>232</v>
+        <v>24</v>
       </c>
       <c r="M14" t="n">
-        <v>51392.64</v>
+        <v>10632</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>202.6752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
+        <v>9</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Facility4</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>234</v>
+      </c>
+      <c r="F15" t="n">
+        <v>27144</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>56</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>56</v>
+      </c>
+      <c r="K15" t="n">
+        <v>6496</v>
+      </c>
+      <c r="L15" t="n">
+        <v>116</v>
+      </c>
+      <c r="M15" t="n">
+        <v>20648</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>9</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Facility4</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F16" t="n">
+        <v>27144</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>13</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1447.68</v>
+      </c>
+      <c r="L16" t="n">
+        <v>116</v>
+      </c>
+      <c r="M16" t="n">
+        <v>25696.32</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>101.3376</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>10</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>Facility5</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>231</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F17" t="n">
         <v>3003</v>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="H15" t="n">
+      <c r="H17" t="n">
         <v>13</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J15" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K15" t="n">
-        <v>163.93</v>
-      </c>
-      <c r="L15" t="n">
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
         <v>13</v>
       </c>
-      <c r="M15" t="n">
-        <v>2839.07</v>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O15" t="n">
-        <v>8.1965</v>
+      <c r="K17" t="n">
+        <v>169</v>
+      </c>
+      <c r="L17" t="n">
+        <v>13</v>
+      </c>
+      <c r="M17" t="n">
+        <v>2834</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1411,36 +1529,36 @@
  - 34 x_B_5 - 24 x_B_6 - 53 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
 BaseSpend_C: S0_C - 55 x_C_1 - 75 x_C_10 - 75 x_C_2 - 60 x_C_3 - 19 x_C_4
  - 24 x_C_5 - 64 x_C_6 - 86 x_C_7 - 24 x_C_8 - 13 x_C_9 = 0
-Capacity_A_Bid_ID_1: x_A_1 &lt;= 5000
-Capacity_A_Bid_ID_10: x_A_10 &lt;= 3000
-Capacity_A_Bid_ID_2: x_A_2 &lt;= 4000
-Capacity_A_Bid_ID_3: x_A_3 &lt;= 3000
-Capacity_A_Bid_ID_4: x_A_4 &lt;= 5000
-Capacity_A_Bid_ID_5: x_A_5 &lt;= 4000
-Capacity_A_Bid_ID_6: x_A_6 &lt;= 3000
-Capacity_A_Bid_ID_7: x_A_7 &lt;= 5000
-Capacity_A_Bid_ID_8: x_A_8 &lt;= 4000
-Capacity_A_Bid_ID_9: x_A_9 &lt;= 3000
-Capacity_B_Bid_ID_1: x_B_1 &lt;= 4000
-Capacity_B_Bid_ID_10: x_B_10 &lt;= 5000
-Capacity_B_Bid_ID_2: x_B_2 &lt;= 8000
-Capacity_B_Bid_ID_3: x_B_3 &lt;= 6000
-Capacity_B_Bid_ID_4: x_B_4 &lt;= 4000
-Capacity_B_Bid_ID_5: x_B_5 &lt;= 8000
-Capacity_B_Bid_ID_6: x_B_6 &lt;= 6000
-Capacity_B_Bid_ID_7: x_B_7 &lt;= 4000
-Capacity_B_Bid_ID_8: x_B_8 &lt;= 8000
-Capacity_B_Bid_ID_9: x_B_9 &lt;= 6000
-Capacity_C_Bid_ID_1: x_C_1 &lt;= 3000
-Capacity_C_Bid_ID_10: x_C_10 &lt;= 7000
-Capacity_C_Bid_ID_2: x_C_2 &lt;= 5000
-Capacity_C_Bid_ID_3: x_C_3 &lt;= 7000
-Capacity_C_Bid_ID_4: x_C_4 &lt;= 3000
-Capacity_C_Bid_ID_5: x_C_5 &lt;= 5000
-Capacity_C_Bid_ID_6: x_C_6 &lt;= 7000
-Capacity_C_Bid_ID_7: x_C_7 &lt;= 3000
-Capacity_C_Bid_ID_8: x_C_8 &lt;= 5000
-Capacity_C_Bid_ID_9: x_C_9 &lt;= 7000
+Capacity_A_Bid_ID_1: x_A_1 &lt;= 10000
+Capacity_A_Bid_ID_10: x_A_10 &lt;= 30002
+Capacity_A_Bid_ID_2: x_A_2 &lt;= 13000
+Capacity_A_Bid_ID_3: x_A_3 &lt;= 14000
+Capacity_A_Bid_ID_4: x_A_4 &lt;= 21111
+Capacity_A_Bid_ID_5: x_A_5 &lt;= 23132
+Capacity_A_Bid_ID_6: x_A_6 &lt;= 20242
+Capacity_A_Bid_ID_7: x_A_7 &lt;= 22212
+Capacity_A_Bid_ID_8: x_A_8 &lt;= 19999
+Capacity_A_Bid_ID_9: x_A_9 &lt;= 2321
+Capacity_B_Bid_ID_1: x_B_1 &lt;= 20002
+Capacity_B_Bid_ID_10: x_B_10 &lt;= 40001
+Capacity_B_Bid_ID_2: x_B_2 &lt;= 24214
+Capacity_B_Bid_ID_3: x_B_3 &lt;= 19232
+Capacity_B_Bid_ID_4: x_B_4 &lt;= 1992
+Capacity_B_Bid_ID_5: x_B_5 &lt;= 42410
+Capacity_B_Bid_ID_6: x_B_6 &lt;= 222
+Capacity_B_Bid_ID_7: x_B_7 &lt;= 2131
+Capacity_B_Bid_ID_8: x_B_8 &lt;= 3000
+Capacity_B_Bid_ID_9: x_B_9 &lt;= 4000
+Capacity_C_Bid_ID_1: x_C_1 &lt;= 2192
+Capacity_C_Bid_ID_10: x_C_10 &lt;= 8005
+Capacity_C_Bid_ID_2: x_C_2 &lt;= 20203
+Capacity_C_Bid_ID_3: x_C_3 &lt;= 32313
+Capacity_C_Bid_ID_4: x_C_4 &lt;= 22131
+Capacity_C_Bid_ID_5: x_C_5 &lt;= 14151
+Capacity_C_Bid_ID_6: x_C_6 &lt;= 19962
+Capacity_C_Bid_ID_7: x_C_7 &lt;= 11821
+Capacity_C_Bid_ID_8: x_C_8 &lt;= 2131
+Capacity_C_Bid_ID_9: x_C_9 &lt;= 40201
 Demand_1: x_A_1 + x_B_1 + x_C_1 = 700
 Demand_10: x_A_10 + x_B_10 + x_C_10 = 13
 Demand_2: x_A_2 + x_B_2 + x_C_2 = 9000
@@ -1451,15 +1569,18 @@
 Demand_7: x_A_7 + x_B_7 + x_C_7 = 664
 Demand_8: x_A_8 + x_B_8 + x_C_8 = 24
 Demand_9: x_A_9 + x_B_9 + x_C_9 = 232
-DiscountTierLower_A_0: d_A - 3783000 z_discount_A_0 &gt;= -3783000
-DiscountTierLower_A_1: - 0.01 S0_A + d_A - 3783000 z_discount_A_1 &gt;= -3783000
-DiscountTierLower_B_0: d_B - 5723000 z_discount_B_0 &gt;= -5723000
-DiscountTierLower_B_1: - 0.03 S0_B + d_B - 5723000 z_discount_B_1 &gt;= -5723000
-DiscountTierLower_C_0: d_C - 5044000 z_discount_C_0 &gt;= -5044000
-DiscountTierLower_C_1: - 0.04 S0_C + d_C - 5044000 z_discount_C_1 &gt;= -5044000
-DiscountTierMax_A_0: 3783000 z_discount_A_0 &lt;= 3784000
-DiscountTierMax_B_0: 5723000 z_discount_B_0 &lt;= 5723500
-DiscountTierMax_C_0: 5044000 z_discount_C_0 &lt;= 5044500
+DiscountTierLower_A_0: d_A - 17073843 z_discount_A_0 &gt;= -17073843
+DiscountTierLower_A_1: - 0.01 S0_A + d_A - 17073843 z_discount_A_1
+ &gt;= -17073843
+DiscountTierLower_B_0: d_B - 15248788 z_discount_B_0 &gt;= -15248788
+DiscountTierLower_B_1: - 0.03 S0_B + d_B - 15248788 z_discount_B_1
+ &gt;= -15248788
+DiscountTierLower_C_0: d_C - 16791670 z_discount_C_0 &gt;= -16791670
+DiscountTierLower_C_1: - 0.04 S0_C + d_C - 16791670 z_discount_C_1
+ &gt;= -16791670
+DiscountTierMax_A_0: 17073843 z_discount_A_0 &lt;= 17074843
+DiscountTierMax_B_0: 15248788 z_discount_B_0 &lt;= 15249288
+DiscountTierMax_C_0: 16791670 z_discount_C_0 &lt;= 16792170
 _dummy: __dummy = 0
 DiscountTierMin_A_0: __dummy &gt;= 0
 DiscountTierMin_A_1: x_A_1 + x_A_10 + x_A_3 + x_A_4 + x_A_8 + x_A_9
@@ -1472,24 +1593,26 @@
 DiscountTierSelect_A: z_discount_A_0 + z_discount_A_1 = 1
 DiscountTierSelect_B: z_discount_B_0 + z_discount_B_1 = 1
 DiscountTierSelect_C: z_discount_C_0 + z_discount_C_1 = 1
-DiscountTierUpper_A_0: d_A + 3783000 z_discount_A_0 &lt;= 3783000
-DiscountTierUpper_A_1: - 0.01 S0_A + d_A + 3783000 z_discount_A_1 &lt;= 3783000
-DiscountTierUpper_B_0: d_B + 5723000 z_discount_B_0 &lt;= 5723000
-DiscountTierUpper_B_1: - 0.03 S0_B + d_B + 5723000 z_discount_B_1 &lt;= 5723000
-DiscountTierUpper_C_0: d_C + 5044000 z_discount_C_0 &lt;= 5044000
-DiscountTierUpper_C_1: - 0.04 S0_C + d_C + 5044000 z_discount_C_1 &lt;= 5044000
+DiscountTierUpper_A_0: d_A + 17073843 z_discount_A_0 &lt;= 17073843
+DiscountTierUpper_A_1: - 0.01 S0_A + d_A + 17073843 z_discount_A_1 &lt;= 17073843
+DiscountTierUpper_B_0: d_B + 15248788 z_discount_B_0 &lt;= 15248788
+DiscountTierUpper_B_1: - 0.03 S0_B + d_B + 15248788 z_discount_B_1 &lt;= 15248788
+DiscountTierUpper_C_0: d_C + 16791670 z_discount_C_0 &lt;= 16791670
+DiscountTierUpper_C_1: - 0.04 S0_C + d_C + 16791670 z_discount_C_1 &lt;= 16791670
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
-RebateTierLower_A_0: rebate_A - 3783000 y_rebate_A_0 &gt;= -3783000
-RebateTierLower_A_1: - 0.1 S_A + rebate_A - 3783000 y_rebate_A_1 &gt;= -3783000
-RebateTierLower_B_0: rebate_B - 5723000 y_rebate_B_0 &gt;= -5723000
-RebateTierLower_B_1: - 0.05 S_B + rebate_B - 5723000 y_rebate_B_1 &gt;= -5723000
-RebateTierLower_C_0: rebate_C - 5044000 y_rebate_C_0 &gt;= -5044000
-RebateTierLower_C_1: - 0.07 S_C + rebate_C - 5044000 y_rebate_C_1 &gt;= -5044000
-RebateTierMax_A_0: 3783000 y_rebate_A_0 &lt;= 3783500
-RebateTierMax_B_0: 5723000 y_rebate_B_0 &lt;= 5723500
-RebateTierMax_C_0: 5044000 y_rebate_C_0 &lt;= 5044700
+RebateTierLower_A_0: rebate_A - 17073843 y_rebate_A_0 &gt;= -17073843
+RebateTierLower_A_1: - 0.1 S_A + rebate_A - 17073843 y_rebate_A_1 &gt;= -17073843
+RebateTierLower_B_0: rebate_B - 15248788 y_rebate_B_0 &gt;= -15248788
+RebateTierLower_B_1: - 0.05 S_B + rebate_B - 15248788 y_rebate_B_1
+ &gt;= -15248788
+RebateTierLower_C_0: rebate_C - 16791670 y_rebate_C_0 &gt;= -16791670
+RebateTierLower_C_1: - 0.07 S_C + rebate_C - 16791670 y_rebate_C_1
+ &gt;= -16791670
+RebateTierMax_A_0: 17073843 y_rebate_A_0 &lt;= 17074343
+RebateTierMax_B_0: 15248788 y_rebate_B_0 &lt;= 15249288
+RebateTierMax_C_0: 16791670 y_rebate_C_0 &lt;= 16792370
 RebateTierMin_A_0: __dummy &gt;= 0
 RebateTierMin_A_1: - 500 y_rebate_A_1 &gt;= 0
 RebateTierMin_B_0: __dummy &gt;= 0
@@ -1500,13 +1623,22 @@
 RebateTierSelect_A: y_rebate_A_0 + y_rebate_A_1 = 1
 RebateTierSelect_B: y_rebate_B_0 + y_rebate_B_1 = 1
 RebateTierSelect_C: y_rebate_C_0 + y_rebate_C_1 = 1
-RebateTierUpper_A_0: rebate_A + 3783000 y_rebate_A_0 &lt;= 3783000
-RebateTierUpper_A_1: - 0.1 S_A + rebate_A + 3783000 y_rebate_A_1 &lt;= 3783000
-RebateTierUpper_B_0: rebate_B + 5723000 y_rebate_B_0 &lt;= 5723000
-RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 5723000 y_rebate_B_1 &lt;= 5723000
-RebateTierUpper_C_0: rebate_C + 5044000 y_rebate_C_0 &lt;= 5044000
-RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 5044000 y_rebate_C_1 &lt;= 5044000
-Rule_0_1: - 0.5 x_A_1 + 0.5 x_B_1 - 0.5 x_C_1 &gt;= 0
+RebateTierUpper_A_0: rebate_A + 17073843 y_rebate_A_0 &lt;= 17073843
+RebateTierUpper_A_1: - 0.1 S_A + rebate_A + 17073843 y_rebate_A_1 &lt;= 17073843
+RebateTierUpper_B_0: rebate_B + 15248788 y_rebate_B_0 &lt;= 15248788
+RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 15248788 y_rebate_B_1 &lt;= 15248788
+RebateTierUpper_C_0: rebate_C + 16791670 y_rebate_C_0 &lt;= 16791670
+RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 16791670 y_rebate_C_1 &lt;= 16791670
+Rule_0_1: - 0.5 x_A_1 + 0.5 x_B_1 + 0.5 x_C_1 &gt;= 0
+Rule_0_10: 0.5 x_A_10 + 0.5 x_B_10 - 0.5 x_C_10 &gt;= 0
+Rule_0_2: 0.5 x_A_2 - 0.5 x_B_2 + 0.5 x_C_2 &gt;= 0
+Rule_0_3: 0.5 x_A_3 + 0.5 x_B_3 - 0.5 x_C_3 &gt;= 0
+Rule_0_4: 0.5 x_A_4 + 0.5 x_B_4 - 0.5 x_C_4 &gt;= 0
+Rule_0_5: 0.5 x_A_5 + 0.5 x_B_5 - 0.5 x_C_5 &gt;= 0
+Rule_0_6: 0.5 x_A_6 + 0.5 x_B_6 - 0.5 x_C_6 &gt;= 0
+Rule_0_7: 0.5 x_A_7 + 0.5 x_B_7 - 0.5 x_C_7 &gt;= 0
+Rule_0_8: 0.5 x_A_8 + 0.5 x_B_8 - 0.5 x_C_8 &gt;= 0
+Rule_0_9: 0.5 x_A_9 + 0.5 x_B_9 - 0.5 x_C_9 &gt;= 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1629,7 +1761,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="3">
@@ -1649,7 +1781,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4000</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="4">
@@ -1669,7 +1801,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3000</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="5">
@@ -1689,7 +1821,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>5000</v>
+        <v>21111</v>
       </c>
     </row>
     <row r="6">
@@ -1709,7 +1841,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4000</v>
+        <v>23132</v>
       </c>
     </row>
     <row r="7">
@@ -1729,7 +1861,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3000</v>
+        <v>20242</v>
       </c>
     </row>
     <row r="8">
@@ -1749,7 +1881,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5000</v>
+        <v>22212</v>
       </c>
     </row>
     <row r="9">
@@ -1769,7 +1901,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4000</v>
+        <v>19999</v>
       </c>
     </row>
     <row r="10">
@@ -1789,7 +1921,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3000</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="11">
@@ -1809,7 +1941,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3000</v>
+        <v>30002</v>
       </c>
     </row>
     <row r="12">
@@ -1829,7 +1961,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4000</v>
+        <v>20002</v>
       </c>
     </row>
     <row r="13">
@@ -1849,7 +1981,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>8000</v>
+        <v>24214</v>
       </c>
     </row>
     <row r="14">
@@ -1869,7 +2001,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6000</v>
+        <v>19232</v>
       </c>
     </row>
     <row r="15">
@@ -1889,7 +2021,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4000</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="16">
@@ -1909,7 +2041,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8000</v>
+        <v>42410</v>
       </c>
     </row>
     <row r="17">
@@ -1929,7 +2061,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>6000</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18">
@@ -1949,7 +2081,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4000</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="19">
@@ -1969,7 +2101,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>8000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="20">
@@ -1989,7 +2121,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>6000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="21">
@@ -2009,7 +2141,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>5000</v>
+        <v>40001</v>
       </c>
     </row>
     <row r="22">
@@ -2029,7 +2161,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3000</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="23">
@@ -2049,7 +2181,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>5000</v>
+        <v>20203</v>
       </c>
     </row>
     <row r="24">
@@ -2069,7 +2201,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7000</v>
+        <v>32313</v>
       </c>
     </row>
     <row r="25">
@@ -2089,7 +2221,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3000</v>
+        <v>22131</v>
       </c>
     </row>
     <row r="26">
@@ -2109,7 +2241,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5000</v>
+        <v>14151</v>
       </c>
     </row>
     <row r="27">
@@ -2129,7 +2261,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>7000</v>
+        <v>19962</v>
       </c>
     </row>
     <row r="28">
@@ -2149,7 +2281,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3000</v>
+        <v>11821</v>
       </c>
     </row>
     <row r="29">
@@ -2169,7 +2301,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>5000</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="30">
@@ -2189,7 +2321,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>7000</v>
+        <v>40201</v>
       </c>
     </row>
     <row r="31">
@@ -2209,7 +2341,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7000</v>
+        <v>8005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated rule type to have description in expander
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -654,49 +654,49 @@
         <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>1404000</v>
+        <v>702000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>72</v>
+        <v>77.59999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>648000</v>
+        <v>349200</v>
       </c>
       <c r="L4" t="n">
-        <v>9000</v>
+        <v>4500</v>
       </c>
       <c r="M4" t="n">
-        <v>756000</v>
+        <v>352800</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>45360.00000000001</v>
+        <v>17460</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -706,47 +706,47 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>423</v>
+        <v>156</v>
       </c>
       <c r="F5" t="n">
-        <v>126900</v>
+        <v>702000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>54.45</v>
+        <v>72</v>
       </c>
       <c r="K5" t="n">
-        <v>16335</v>
+        <v>324000</v>
       </c>
       <c r="L5" t="n">
-        <v>300</v>
+        <v>4500</v>
       </c>
       <c r="M5" t="n">
-        <v>110565</v>
+        <v>378000</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>22680</v>
       </c>
     </row>
     <row r="6">
@@ -755,7 +755,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -776,50 +776,50 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>57.59999999999999</v>
+        <v>54.45</v>
       </c>
       <c r="K6" t="n">
-        <v>17280</v>
+        <v>16335</v>
       </c>
       <c r="L6" t="n">
         <v>300</v>
       </c>
       <c r="M6" t="n">
-        <v>109620</v>
+        <v>110565</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>1209.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,43 +828,43 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="F7" t="n">
-        <v>1284255</v>
+        <v>126900</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>22.77</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K7" t="n">
-        <v>64552.95</v>
+        <v>17280</v>
       </c>
       <c r="L7" t="n">
-        <v>2835</v>
+        <v>300</v>
       </c>
       <c r="M7" t="n">
-        <v>1219702.05</v>
+        <v>109620</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>1209.6</v>
       </c>
     </row>
     <row r="8">
@@ -873,7 +873,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -894,45 +894,45 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>18.24</v>
+        <v>22.77</v>
       </c>
       <c r="K8" t="n">
-        <v>51710.39999999999</v>
+        <v>64552.95</v>
       </c>
       <c r="L8" t="n">
         <v>2835</v>
       </c>
       <c r="M8" t="n">
-        <v>1232544.6</v>
+        <v>1219702.05</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>3619.728</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -946,43 +946,43 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="F9" t="n">
-        <v>7695</v>
+        <v>1284255</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>34</v>
+        <v>18.24</v>
       </c>
       <c r="K9" t="n">
-        <v>765</v>
+        <v>51710.39999999999</v>
       </c>
       <c r="L9" t="n">
-        <v>22.5</v>
+        <v>2835</v>
       </c>
       <c r="M9" t="n">
-        <v>6930</v>
+        <v>1232544.6</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>3619.728</v>
       </c>
     </row>
     <row r="10">
@@ -991,7 +991,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1012,45 +1012,45 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>23.04</v>
+        <v>32.98</v>
       </c>
       <c r="K10" t="n">
-        <v>518.4</v>
+        <v>742.05</v>
       </c>
       <c r="L10" t="n">
         <v>22.5</v>
       </c>
       <c r="M10" t="n">
-        <v>7176.6</v>
+        <v>6952.95</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>36.288</v>
+        <v>37.1025</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1064,14 +1064,14 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>653</v>
+        <v>342</v>
       </c>
       <c r="F11" t="n">
-        <v>144966</v>
+        <v>7695</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -1079,28 +1079,28 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>24</v>
+        <v>23.04</v>
       </c>
       <c r="K11" t="n">
-        <v>5328</v>
+        <v>518.4</v>
       </c>
       <c r="L11" t="n">
-        <v>222</v>
+        <v>22.5</v>
       </c>
       <c r="M11" t="n">
-        <v>139638</v>
+        <v>7176.6</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>36.288</v>
       </c>
     </row>
     <row r="12">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1126,49 +1126,49 @@
         <v>653</v>
       </c>
       <c r="F12" t="n">
-        <v>13060</v>
+        <v>79013</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>41.58</v>
+        <v>23.28</v>
       </c>
       <c r="K12" t="n">
-        <v>831.5999999999999</v>
+        <v>2816.88</v>
       </c>
       <c r="L12" t="n">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="M12" t="n">
-        <v>12228.4</v>
+        <v>76196.12</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>140.844</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1182,48 +1182,48 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>432</v>
+        <v>653</v>
       </c>
       <c r="F13" t="n">
-        <v>286848</v>
+        <v>79013</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>22.77</v>
+        <v>61.44</v>
       </c>
       <c r="K13" t="n">
-        <v>15119.28</v>
+        <v>7434.24</v>
       </c>
       <c r="L13" t="n">
-        <v>664</v>
+        <v>121</v>
       </c>
       <c r="M13" t="n">
-        <v>271728.72</v>
+        <v>71578.75999999999</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>520.3968</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Facility3</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1241,35 +1241,35 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F14" t="n">
-        <v>10944</v>
+        <v>143424</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>13</v>
+        <v>22.77</v>
       </c>
       <c r="K14" t="n">
-        <v>312</v>
+        <v>7559.639999999999</v>
       </c>
       <c r="L14" t="n">
-        <v>24</v>
+        <v>332</v>
       </c>
       <c r="M14" t="n">
-        <v>10632</v>
+        <v>135864.36</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1282,16 +1282,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Facility4</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1300,57 +1300,57 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>234</v>
+        <v>432</v>
       </c>
       <c r="F15" t="n">
-        <v>27144</v>
+        <v>143424</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>56</v>
+        <v>82.56</v>
       </c>
       <c r="K15" t="n">
-        <v>6496</v>
+        <v>27409.92</v>
       </c>
       <c r="L15" t="n">
-        <v>116</v>
+        <v>332</v>
       </c>
       <c r="M15" t="n">
-        <v>20648</v>
+        <v>116014.08</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>1918.6944</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Facility4</t>
+          <t>Facility3</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1359,14 +1359,14 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>234</v>
+        <v>456</v>
       </c>
       <c r="F16" t="n">
-        <v>27144</v>
+        <v>5472</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1374,87 +1374,323 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>12.48</v>
+        <v>12.61</v>
       </c>
       <c r="K16" t="n">
-        <v>1447.68</v>
+        <v>151.32</v>
       </c>
       <c r="L16" t="n">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="M16" t="n">
-        <v>25696.32</v>
+        <v>5320.68</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O16" t="n">
-        <v>101.3376</v>
+        <v>7.566</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
+        <v>8</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Facility3</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>456</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5472</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>24</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="K17" t="n">
+        <v>276.48</v>
+      </c>
+      <c r="L17" t="n">
+        <v>12</v>
+      </c>
+      <c r="M17" t="n">
+        <v>5195.52</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>19.3536</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>9</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Facility4</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>234</v>
+      </c>
+      <c r="F18" t="n">
+        <v>27144</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>56</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>54.32</v>
+      </c>
+      <c r="K18" t="n">
+        <v>6301.12</v>
+      </c>
+      <c r="L18" t="n">
+        <v>116</v>
+      </c>
+      <c r="M18" t="n">
+        <v>20842.88</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>315.056</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Facility4</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>234</v>
+      </c>
+      <c r="F19" t="n">
+        <v>27144</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>13</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1447.68</v>
+      </c>
+      <c r="L19" t="n">
+        <v>116</v>
+      </c>
+      <c r="M19" t="n">
+        <v>25696.32</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>101.3376</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
         <v>10</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>Facility5</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
         <v>231</v>
       </c>
-      <c r="F17" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
+      <c r="F20" t="n">
+        <v>1501.5</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
         <v>13</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
-        <v>13</v>
-      </c>
-      <c r="K17" t="n">
-        <v>169</v>
-      </c>
-      <c r="L17" t="n">
-        <v>13</v>
-      </c>
-      <c r="M17" t="n">
-        <v>2834</v>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>12.61</v>
+      </c>
+      <c r="K20" t="n">
+        <v>81.965</v>
+      </c>
+      <c r="L20" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1419.535</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>4.09825</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>10</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>231</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1501.5</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>75</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>72</v>
+      </c>
+      <c r="K21" t="n">
+        <v>468</v>
+      </c>
+      <c r="L21" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1033.5</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>32.76000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1639,6 +1875,16 @@
 Rule_0_7: 0.5 x_A_7 + 0.5 x_B_7 - 0.5 x_C_7 &gt;= 0
 Rule_0_8: 0.5 x_A_8 + 0.5 x_B_8 - 0.5 x_C_8 &gt;= 0
 Rule_0_9: 0.5 x_A_9 + 0.5 x_B_9 - 0.5 x_C_9 &gt;= 0
+Rule_1_1: 0.5 x_A_1 - 0.5 x_B_1 - 0.5 x_C_1 &gt;= 0
+Rule_1_10: - 0.5 x_A_10 - 0.5 x_B_10 + 0.5 x_C_10 &gt;= 0
+Rule_1_2: - 0.5 x_A_2 + 0.5 x_B_2 - 0.5 x_C_2 &gt;= 0
+Rule_1_3: - 0.5 x_A_3 - 0.5 x_B_3 + 0.5 x_C_3 &gt;= 0
+Rule_1_4: - 0.5 x_A_4 - 0.5 x_B_4 + 0.5 x_C_4 &gt;= 0
+Rule_1_5: - 0.5 x_A_5 - 0.5 x_B_5 + 0.5 x_C_5 &gt;= 0
+Rule_1_6: - 0.5 x_A_6 - 0.5 x_B_6 + 0.5 x_C_6 &gt;= 0
+Rule_1_7: - 0.5 x_A_7 - 0.5 x_B_7 + 0.5 x_C_7 &gt;= 0
+Rule_1_8: - 0.5 x_A_8 - 0.5 x_B_8 + 0.5 x_C_8 &gt;= 0
+Rule_1_9: - 0.5 x_A_9 - 0.5 x_B_9 + 0.5 x_C_9 &gt;= 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
updated rule: # of volume, fixed all setting
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,40 +536,40 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>19.8</v>
+        <v>52.8</v>
       </c>
       <c r="K2" t="n">
-        <v>6930</v>
+        <v>21120</v>
       </c>
       <c r="L2" t="n">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="M2" t="n">
-        <v>28070</v>
+        <v>18880</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>1478.4</v>
       </c>
     </row>
     <row r="3">
@@ -595,40 +595,40 @@
         <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>35000</v>
+        <v>30000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>52.8</v>
+        <v>19.8</v>
       </c>
       <c r="K3" t="n">
-        <v>18480</v>
+        <v>5940</v>
       </c>
       <c r="L3" t="n">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="M3" t="n">
-        <v>16520</v>
+        <v>24060</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>1293.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -654,49 +654,49 @@
         <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>702000</v>
+        <v>1404000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>77.59999999999999</v>
+        <v>72</v>
       </c>
       <c r="K4" t="n">
-        <v>349200</v>
+        <v>648000</v>
       </c>
       <c r="L4" t="n">
-        <v>4500</v>
+        <v>9000</v>
       </c>
       <c r="M4" t="n">
-        <v>352800</v>
+        <v>756000</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>17460</v>
+        <v>45360.00000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -706,47 +706,47 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>156</v>
+        <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>702000</v>
+        <v>126900</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>72</v>
+        <v>54.45</v>
       </c>
       <c r="K5" t="n">
-        <v>324000</v>
+        <v>16335</v>
       </c>
       <c r="L5" t="n">
-        <v>4500</v>
+        <v>300</v>
       </c>
       <c r="M5" t="n">
-        <v>378000</v>
+        <v>110565</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>22680</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -755,7 +755,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -776,50 +776,50 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>54.45</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K6" t="n">
-        <v>16335</v>
+        <v>17280</v>
       </c>
       <c r="L6" t="n">
         <v>300</v>
       </c>
       <c r="M6" t="n">
-        <v>110565</v>
+        <v>109620</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>1209.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility1</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,43 +828,43 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>126900</v>
+        <v>2432610</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>57.59999999999999</v>
+        <v>22.77</v>
       </c>
       <c r="K7" t="n">
-        <v>17280</v>
+        <v>122274.9</v>
       </c>
       <c r="L7" t="n">
-        <v>300</v>
+        <v>5370</v>
       </c>
       <c r="M7" t="n">
-        <v>109620</v>
+        <v>2310335.1</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>1209.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -873,7 +873,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -890,49 +890,49 @@
         <v>453</v>
       </c>
       <c r="F8" t="n">
-        <v>1284255</v>
+        <v>135900</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>22.77</v>
+        <v>18.24</v>
       </c>
       <c r="K8" t="n">
-        <v>64552.95</v>
+        <v>5471.999999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>2835</v>
+        <v>300</v>
       </c>
       <c r="M8" t="n">
-        <v>1219702.05</v>
+        <v>130428</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>383.04</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F9" t="n">
-        <v>1284255</v>
+        <v>15390</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>18.24</v>
+        <v>23.04</v>
       </c>
       <c r="K9" t="n">
-        <v>51710.39999999999</v>
+        <v>1036.8</v>
       </c>
       <c r="L9" t="n">
-        <v>2835</v>
+        <v>45</v>
       </c>
       <c r="M9" t="n">
-        <v>1232544.6</v>
+        <v>14353.2</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -982,12 +982,12 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>3619.728</v>
+        <v>72.57600000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>342</v>
+        <v>653</v>
       </c>
       <c r="F10" t="n">
-        <v>7695</v>
+        <v>144966</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1016,37 +1016,37 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>32.98</v>
+        <v>24</v>
       </c>
       <c r="K10" t="n">
-        <v>742.05</v>
+        <v>5328</v>
       </c>
       <c r="L10" t="n">
-        <v>22.5</v>
+        <v>222</v>
       </c>
       <c r="M10" t="n">
-        <v>6952.95</v>
+        <v>139638</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>37.1025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1064,48 +1064,48 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>342</v>
+        <v>653</v>
       </c>
       <c r="F11" t="n">
-        <v>7695</v>
+        <v>13060</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>23.04</v>
+        <v>41.58</v>
       </c>
       <c r="K11" t="n">
-        <v>518.4</v>
+        <v>831.5999999999999</v>
       </c>
       <c r="L11" t="n">
-        <v>22.5</v>
+        <v>20</v>
       </c>
       <c r="M11" t="n">
-        <v>7176.6</v>
+        <v>12228.4</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>36.288</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1123,107 +1123,107 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>653</v>
+        <v>432</v>
       </c>
       <c r="F12" t="n">
-        <v>79013</v>
+        <v>286848</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>23.28</v>
+        <v>22.77</v>
       </c>
       <c r="K12" t="n">
-        <v>2816.88</v>
+        <v>15119.28</v>
       </c>
       <c r="L12" t="n">
-        <v>121</v>
+        <v>664</v>
       </c>
       <c r="M12" t="n">
-        <v>76196.12</v>
+        <v>271728.72</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>140.844</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Facility3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>456</v>
+      </c>
+      <c r="F13" t="n">
+        <v>10944</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>653</v>
-      </c>
-      <c r="F13" t="n">
-        <v>79013</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
       <c r="H13" t="n">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>61.44</v>
+        <v>13</v>
       </c>
       <c r="K13" t="n">
-        <v>7434.24</v>
+        <v>312</v>
       </c>
       <c r="L13" t="n">
-        <v>121</v>
+        <v>24</v>
       </c>
       <c r="M13" t="n">
-        <v>71578.75999999999</v>
+        <v>10632</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>520.3968</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility4</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1241,456 +1241,102 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>432</v>
+        <v>234</v>
       </c>
       <c r="F14" t="n">
-        <v>143424</v>
+        <v>54288</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>22.77</v>
+        <v>12.48</v>
       </c>
       <c r="K14" t="n">
-        <v>7559.639999999999</v>
+        <v>2895.36</v>
       </c>
       <c r="L14" t="n">
-        <v>332</v>
+        <v>232</v>
       </c>
       <c r="M14" t="n">
-        <v>135864.36</v>
+        <v>51392.64</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>202.6752</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>231</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>432</v>
-      </c>
-      <c r="F15" t="n">
-        <v>143424</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
       <c r="H15" t="n">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>82.56</v>
+        <v>13</v>
       </c>
       <c r="K15" t="n">
-        <v>27409.92</v>
+        <v>169</v>
       </c>
       <c r="L15" t="n">
-        <v>332</v>
+        <v>13</v>
       </c>
       <c r="M15" t="n">
-        <v>116014.08</v>
+        <v>2834</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>1918.6944</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>8</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Facility3</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>456</v>
-      </c>
-      <c r="F16" t="n">
-        <v>5472</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>13</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J16" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K16" t="n">
-        <v>151.32</v>
-      </c>
-      <c r="L16" t="n">
-        <v>12</v>
-      </c>
-      <c r="M16" t="n">
-        <v>5320.68</v>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O16" t="n">
-        <v>7.566</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>8</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Facility3</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>456</v>
-      </c>
-      <c r="F17" t="n">
-        <v>5472</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>24</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
-        <v>23.04</v>
-      </c>
-      <c r="K17" t="n">
-        <v>276.48</v>
-      </c>
-      <c r="L17" t="n">
-        <v>12</v>
-      </c>
-      <c r="M17" t="n">
-        <v>5195.52</v>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>19.3536</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>9</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Facility4</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>234</v>
-      </c>
-      <c r="F18" t="n">
-        <v>27144</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>56</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J18" t="n">
-        <v>54.32</v>
-      </c>
-      <c r="K18" t="n">
-        <v>6301.12</v>
-      </c>
-      <c r="L18" t="n">
-        <v>116</v>
-      </c>
-      <c r="M18" t="n">
-        <v>20842.88</v>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O18" t="n">
-        <v>315.056</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>9</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Facility4</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>234</v>
-      </c>
-      <c r="F19" t="n">
-        <v>27144</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>13</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J19" t="n">
-        <v>12.48</v>
-      </c>
-      <c r="K19" t="n">
-        <v>1447.68</v>
-      </c>
-      <c r="L19" t="n">
-        <v>116</v>
-      </c>
-      <c r="M19" t="n">
-        <v>25696.32</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="O19" t="n">
-        <v>101.3376</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>10</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Facility5</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>231</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1501.5</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>13</v>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J20" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K20" t="n">
-        <v>81.965</v>
-      </c>
-      <c r="L20" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="M20" t="n">
-        <v>1419.535</v>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O20" t="n">
-        <v>4.09825</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>10</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Facility5</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>231</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1501.5</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>75</v>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J21" t="n">
-        <v>72</v>
-      </c>
-      <c r="K21" t="n">
-        <v>468</v>
-      </c>
-      <c r="L21" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="M21" t="n">
-        <v>1033.5</v>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="O21" t="n">
-        <v>32.76000000000001</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1865,26 +1511,16 @@
 RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 15248788 y_rebate_B_1 &lt;= 15248788
 RebateTierUpper_C_0: rebate_C + 16791670 y_rebate_C_0 &lt;= 16791670
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 16791670 y_rebate_C_1 &lt;= 16791670
-Rule_0_1: - 0.5 x_A_1 + 0.5 x_B_1 + 0.5 x_C_1 &gt;= 0
-Rule_0_10: 0.5 x_A_10 + 0.5 x_B_10 - 0.5 x_C_10 &gt;= 0
-Rule_0_2: 0.5 x_A_2 - 0.5 x_B_2 + 0.5 x_C_2 &gt;= 0
-Rule_0_3: 0.5 x_A_3 + 0.5 x_B_3 - 0.5 x_C_3 &gt;= 0
-Rule_0_4: 0.5 x_A_4 + 0.5 x_B_4 - 0.5 x_C_4 &gt;= 0
-Rule_0_5: 0.5 x_A_5 + 0.5 x_B_5 - 0.5 x_C_5 &gt;= 0
-Rule_0_6: 0.5 x_A_6 + 0.5 x_B_6 - 0.5 x_C_6 &gt;= 0
-Rule_0_7: 0.5 x_A_7 + 0.5 x_B_7 - 0.5 x_C_7 &gt;= 0
-Rule_0_8: 0.5 x_A_8 + 0.5 x_B_8 - 0.5 x_C_8 &gt;= 0
-Rule_0_9: 0.5 x_A_9 + 0.5 x_B_9 - 0.5 x_C_9 &gt;= 0
-Rule_1_1: 0.5 x_A_1 - 0.5 x_B_1 - 0.5 x_C_1 &gt;= 0
-Rule_1_10: - 0.5 x_A_10 - 0.5 x_B_10 + 0.5 x_C_10 &gt;= 0
-Rule_1_2: - 0.5 x_A_2 + 0.5 x_B_2 - 0.5 x_C_2 &gt;= 0
-Rule_1_3: - 0.5 x_A_3 - 0.5 x_B_3 + 0.5 x_C_3 &gt;= 0
-Rule_1_4: - 0.5 x_A_4 - 0.5 x_B_4 + 0.5 x_C_4 &gt;= 0
-Rule_1_5: - 0.5 x_A_5 - 0.5 x_B_5 + 0.5 x_C_5 &gt;= 0
-Rule_1_6: - 0.5 x_A_6 - 0.5 x_B_6 + 0.5 x_C_6 &gt;= 0
-Rule_1_7: - 0.5 x_A_7 - 0.5 x_B_7 + 0.5 x_C_7 &gt;= 0
-Rule_1_8: - 0.5 x_A_8 - 0.5 x_B_8 + 0.5 x_C_8 &gt;= 0
-Rule_1_9: - 0.5 x_A_9 - 0.5 x_B_9 + 0.5 x_C_9 &gt;= 0
+Rule_0_1: x_A_1 &lt;= 300
+Rule_0_10: x_C_10 &lt;= 300
+Rule_0_2: x_B_2 &lt;= 300
+Rule_0_3: x_C_3 &lt;= 300
+Rule_0_4: x_C_4 &lt;= 300
+Rule_0_5: x_C_5 &lt;= 300
+Rule_0_6: x_C_6 &lt;= 300
+Rule_0_7: x_C_7 &lt;= 300
+Rule_0_8: x_C_8 &lt;= 300
+Rule_0_9: x_C_9 &lt;= 300
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
updated extended rule to text
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,40 +536,40 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>40000</v>
+        <v>68700</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>52.8</v>
+        <v>19.8</v>
       </c>
       <c r="K2" t="n">
-        <v>21120</v>
+        <v>13602.6</v>
       </c>
       <c r="L2" t="n">
-        <v>400</v>
+        <v>687</v>
       </c>
       <c r="M2" t="n">
-        <v>18880</v>
+        <v>55097.4</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>1478.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -595,40 +595,40 @@
         <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>30000</v>
+        <v>1300</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>19.8</v>
+        <v>52.8</v>
       </c>
       <c r="K3" t="n">
-        <v>5940</v>
+        <v>686.4</v>
       </c>
       <c r="L3" t="n">
-        <v>300</v>
+        <v>13</v>
       </c>
       <c r="M3" t="n">
-        <v>24060</v>
+        <v>613.6</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>48.048</v>
       </c>
     </row>
     <row r="4">
@@ -831,40 +831,40 @@
         <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>2432610</v>
+        <v>2562621</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>22.77</v>
+        <v>18.24</v>
       </c>
       <c r="K7" t="n">
-        <v>122274.9</v>
+        <v>103183.68</v>
       </c>
       <c r="L7" t="n">
-        <v>5370</v>
+        <v>5657</v>
       </c>
       <c r="M7" t="n">
-        <v>2310335.1</v>
+        <v>2459437.32</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>7222.8576</v>
       </c>
     </row>
     <row r="8">
@@ -890,40 +890,40 @@
         <v>453</v>
       </c>
       <c r="F8" t="n">
-        <v>135900</v>
+        <v>5889</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>18.24</v>
+        <v>22.77</v>
       </c>
       <c r="K8" t="n">
-        <v>5471.999999999999</v>
+        <v>296.01</v>
       </c>
       <c r="L8" t="n">
-        <v>300</v>
+        <v>13</v>
       </c>
       <c r="M8" t="n">
-        <v>130428</v>
+        <v>5592.99</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>383.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -949,7 +949,7 @@
         <v>342</v>
       </c>
       <c r="F9" t="n">
-        <v>15390</v>
+        <v>10944</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -968,13 +968,13 @@
         <v>23.04</v>
       </c>
       <c r="K9" t="n">
-        <v>1036.8</v>
+        <v>737.28</v>
       </c>
       <c r="L9" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="M9" t="n">
-        <v>14353.2</v>
+        <v>10206.72</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -982,16 +982,16 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>72.57600000000001</v>
+        <v>51.6096</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>653</v>
+        <v>342</v>
       </c>
       <c r="F10" t="n">
-        <v>144966</v>
+        <v>4446</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="K10" t="n">
-        <v>5328</v>
+        <v>442</v>
       </c>
       <c r="L10" t="n">
-        <v>222</v>
+        <v>13</v>
       </c>
       <c r="M10" t="n">
-        <v>139638</v>
+        <v>4004</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1067,32 +1067,32 @@
         <v>653</v>
       </c>
       <c r="F11" t="n">
-        <v>13060</v>
+        <v>144966</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>41.58</v>
+        <v>24</v>
       </c>
       <c r="K11" t="n">
-        <v>831.5999999999999</v>
+        <v>5328</v>
       </c>
       <c r="L11" t="n">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="M11" t="n">
-        <v>12228.4</v>
+        <v>139638</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1105,11 +1105,11 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>432</v>
+        <v>653</v>
       </c>
       <c r="F12" t="n">
-        <v>286848</v>
+        <v>13060</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1134,7 +1134,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1142,16 +1142,16 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>22.77</v>
+        <v>41.58</v>
       </c>
       <c r="K12" t="n">
-        <v>15119.28</v>
+        <v>831.5999999999999</v>
       </c>
       <c r="L12" t="n">
-        <v>664</v>
+        <v>20</v>
       </c>
       <c r="M12" t="n">
-        <v>271728.72</v>
+        <v>12228.4</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Facility3</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1182,35 +1182,35 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F13" t="n">
-        <v>10944</v>
+        <v>286848</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>13</v>
+        <v>22.77</v>
       </c>
       <c r="K13" t="n">
-        <v>312</v>
+        <v>15119.28</v>
       </c>
       <c r="L13" t="n">
-        <v>24</v>
+        <v>664</v>
       </c>
       <c r="M13" t="n">
-        <v>10632</v>
+        <v>271728.72</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Facility4</t>
+          <t>Facility3</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1241,14 +1241,14 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>234</v>
+        <v>456</v>
       </c>
       <c r="F14" t="n">
-        <v>54288</v>
+        <v>10944</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1256,33 +1256,33 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>12.48</v>
+        <v>13</v>
       </c>
       <c r="K14" t="n">
-        <v>2895.36</v>
+        <v>312</v>
       </c>
       <c r="L14" t="n">
-        <v>232</v>
+        <v>24</v>
       </c>
       <c r="M14" t="n">
-        <v>51392.64</v>
+        <v>10632</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>202.6752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Facility5</t>
+          <t>Facility4</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1300,14 +1300,14 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F15" t="n">
-        <v>3003</v>
+        <v>51246</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1315,27 +1315,145 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2733.12</v>
+      </c>
+      <c r="L15" t="n">
+        <v>219</v>
+      </c>
+      <c r="M15" t="n">
+        <v>48512.88</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>191.3184</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>9</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Facility4</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>234</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3042</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>56</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="J16" t="n">
+        <v>56</v>
+      </c>
+      <c r="K16" t="n">
+        <v>728</v>
+      </c>
+      <c r="L16" t="n">
         <v>13</v>
       </c>
-      <c r="K15" t="n">
+      <c r="M16" t="n">
+        <v>2314</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>231</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>13</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>13</v>
+      </c>
+      <c r="K17" t="n">
         <v>169</v>
       </c>
-      <c r="L15" t="n">
+      <c r="L17" t="n">
         <v>13</v>
       </c>
-      <c r="M15" t="n">
+      <c r="M17" t="n">
         <v>2834</v>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="N17" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O15" t="n">
+      <c r="O17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1511,16 +1629,16 @@
 RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 15248788 y_rebate_B_1 &lt;= 15248788
 RebateTierUpper_C_0: rebate_C + 16791670 y_rebate_C_0 &lt;= 16791670
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 16791670 y_rebate_C_1 &lt;= 16791670
-Rule_0_1: x_A_1 &lt;= 300
-Rule_0_10: x_C_10 &lt;= 300
-Rule_0_2: x_B_2 &lt;= 300
-Rule_0_3: x_C_3 &lt;= 300
-Rule_0_4: x_C_4 &lt;= 300
-Rule_0_5: x_C_5 &lt;= 300
-Rule_0_6: x_C_6 &lt;= 300
-Rule_0_7: x_C_7 &lt;= 300
-Rule_0_8: x_C_8 &lt;= 300
-Rule_0_9: x_C_9 &lt;= 300
+Rule_0_1: x_B_1 + x_C_1 &gt;= 13
+Rule_0_10: x_A_10 + x_B_10 &gt;= 13
+Rule_0_2: x_A_2 + x_C_2 &gt;= 13
+Rule_0_3: x_A_3 + x_B_3 &gt;= 13
+Rule_0_4: x_A_4 + x_B_4 &gt;= 13
+Rule_0_5: x_A_5 + x_B_5 &gt;= 13
+Rule_0_6: x_A_6 + x_B_6 &gt;= 13
+Rule_0_7: x_A_7 + x_B_7 &gt;= 13
+Rule_0_8: x_A_8 + x_B_8 &gt;= 13
+Rule_0_9: x_A_9 + x_B_9 &gt;= 13
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
Supplier Exclusions now corrected and updated on webapp
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,66 +536,66 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>68700</v>
+        <v>70000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>19.8</v>
+        <v>52.8</v>
       </c>
       <c r="K2" t="n">
-        <v>13602.6</v>
+        <v>36960</v>
       </c>
       <c r="L2" t="n">
-        <v>687</v>
+        <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>55097.4</v>
+        <v>33040</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>2587.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Facility1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Facility1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="F3" t="n">
-        <v>1300</v>
+        <v>1404000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -611,16 +611,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>52.8</v>
+        <v>72</v>
       </c>
       <c r="K3" t="n">
-        <v>686.4</v>
+        <v>648000</v>
       </c>
       <c r="L3" t="n">
-        <v>13</v>
+        <v>9000</v>
       </c>
       <c r="M3" t="n">
-        <v>613.6</v>
+        <v>756000</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -628,12 +628,12 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>48.048</v>
+        <v>45360.00000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -647,52 +647,52 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>156</v>
+        <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>1404000</v>
+        <v>253800</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>72</v>
+        <v>54.45</v>
       </c>
       <c r="K4" t="n">
-        <v>648000</v>
+        <v>32670</v>
       </c>
       <c r="L4" t="n">
-        <v>9000</v>
+        <v>600</v>
       </c>
       <c r="M4" t="n">
-        <v>756000</v>
+        <v>221130</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>45360.00000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -701,7 +701,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Facility1</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -710,10 +710,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F5" t="n">
-        <v>126900</v>
+        <v>2568510</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>54.45</v>
+        <v>22.77</v>
       </c>
       <c r="K5" t="n">
-        <v>16335</v>
+        <v>129105.9</v>
       </c>
       <c r="L5" t="n">
-        <v>300</v>
+        <v>5670</v>
       </c>
       <c r="M5" t="n">
-        <v>110565</v>
+        <v>2439404.1</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -751,16 +751,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility1</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>423</v>
+        <v>342</v>
       </c>
       <c r="F6" t="n">
-        <v>126900</v>
+        <v>15390</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -788,16 +788,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>57.59999999999999</v>
+        <v>23.04</v>
       </c>
       <c r="K6" t="n">
-        <v>17280</v>
+        <v>1036.8</v>
       </c>
       <c r="L6" t="n">
-        <v>300</v>
+        <v>45</v>
       </c>
       <c r="M6" t="n">
-        <v>109620</v>
+        <v>14353.2</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -805,12 +805,12 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>1209.6</v>
+        <v>72.57600000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -828,48 +828,48 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>453</v>
+        <v>653</v>
       </c>
       <c r="F7" t="n">
-        <v>2562621</v>
+        <v>144966</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>18.24</v>
+        <v>24</v>
       </c>
       <c r="K7" t="n">
-        <v>103183.68</v>
+        <v>5328</v>
       </c>
       <c r="L7" t="n">
-        <v>5657</v>
+        <v>222</v>
       </c>
       <c r="M7" t="n">
-        <v>2459437.32</v>
+        <v>139638</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>7222.8576</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -887,10 +887,10 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>453</v>
+        <v>653</v>
       </c>
       <c r="F8" t="n">
-        <v>5889</v>
+        <v>13060</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -906,16 +906,16 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>22.77</v>
+        <v>41.58</v>
       </c>
       <c r="K8" t="n">
-        <v>296.01</v>
+        <v>831.5999999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="M8" t="n">
-        <v>5592.99</v>
+        <v>12228.4</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,77 +946,77 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>342</v>
+        <v>432</v>
       </c>
       <c r="F9" t="n">
-        <v>10944</v>
+        <v>286848</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>23.04</v>
+        <v>22.77</v>
       </c>
       <c r="K9" t="n">
-        <v>737.28</v>
+        <v>15119.28</v>
       </c>
       <c r="L9" t="n">
-        <v>32</v>
+        <v>664</v>
       </c>
       <c r="M9" t="n">
-        <v>10206.72</v>
+        <v>271728.72</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>51.6096</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Facility3</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>456</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10944</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>342</v>
-      </c>
-      <c r="F10" t="n">
-        <v>4446</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="H10" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="K10" t="n">
-        <v>442</v>
+        <v>312</v>
       </c>
       <c r="L10" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="M10" t="n">
-        <v>4004</v>
+        <v>10632</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility4</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1064,10 +1064,10 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>653</v>
+        <v>234</v>
       </c>
       <c r="F11" t="n">
-        <v>144966</v>
+        <v>54288</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1083,16 +1083,16 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="K11" t="n">
-        <v>5328</v>
+        <v>12992</v>
       </c>
       <c r="L11" t="n">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="M11" t="n">
-        <v>139638</v>
+        <v>41296</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1105,53 +1105,53 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>231</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>653</v>
-      </c>
-      <c r="F12" t="n">
-        <v>13060</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H12" t="n">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>41.58</v>
+        <v>13</v>
       </c>
       <c r="K12" t="n">
-        <v>831.5999999999999</v>
+        <v>169</v>
       </c>
       <c r="L12" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="M12" t="n">
-        <v>12228.4</v>
+        <v>2834</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1159,301 +1159,6 @@
         </is>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>7</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>432</v>
-      </c>
-      <c r="F13" t="n">
-        <v>286848</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>23</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>1%</t>
-        </is>
-      </c>
-      <c r="J13" t="n">
-        <v>22.77</v>
-      </c>
-      <c r="K13" t="n">
-        <v>15119.28</v>
-      </c>
-      <c r="L13" t="n">
-        <v>664</v>
-      </c>
-      <c r="M13" t="n">
-        <v>271728.72</v>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>8</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Facility3</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>456</v>
-      </c>
-      <c r="F14" t="n">
-        <v>10944</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>13</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J14" t="n">
-        <v>13</v>
-      </c>
-      <c r="K14" t="n">
-        <v>312</v>
-      </c>
-      <c r="L14" t="n">
-        <v>24</v>
-      </c>
-      <c r="M14" t="n">
-        <v>10632</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>9</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Facility4</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>234</v>
-      </c>
-      <c r="F15" t="n">
-        <v>51246</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>13</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J15" t="n">
-        <v>12.48</v>
-      </c>
-      <c r="K15" t="n">
-        <v>2733.12</v>
-      </c>
-      <c r="L15" t="n">
-        <v>219</v>
-      </c>
-      <c r="M15" t="n">
-        <v>48512.88</v>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="O15" t="n">
-        <v>191.3184</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>9</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Facility4</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>234</v>
-      </c>
-      <c r="F16" t="n">
-        <v>3042</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>56</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J16" t="n">
-        <v>56</v>
-      </c>
-      <c r="K16" t="n">
-        <v>728</v>
-      </c>
-      <c r="L16" t="n">
-        <v>13</v>
-      </c>
-      <c r="M16" t="n">
-        <v>2314</v>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>10</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Facility5</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>231</v>
-      </c>
-      <c r="F17" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>13</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
-        <v>13</v>
-      </c>
-      <c r="K17" t="n">
-        <v>169</v>
-      </c>
-      <c r="L17" t="n">
-        <v>13</v>
-      </c>
-      <c r="M17" t="n">
-        <v>2834</v>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1629,16 +1334,12 @@
 RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 15248788 y_rebate_B_1 &lt;= 15248788
 RebateTierUpper_C_0: rebate_C + 16791670 y_rebate_C_0 &lt;= 16791670
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 16791670 y_rebate_C_1 &lt;= 16791670
-Rule_0_1: x_B_1 + x_C_1 &gt;= 13
-Rule_0_10: x_A_10 + x_B_10 &gt;= 13
-Rule_0_2: x_A_2 + x_C_2 &gt;= 13
-Rule_0_3: x_A_3 + x_B_3 &gt;= 13
-Rule_0_4: x_A_4 + x_B_4 &gt;= 13
-Rule_0_5: x_A_5 + x_B_5 &gt;= 13
-Rule_0_6: x_A_6 + x_B_6 &gt;= 13
-Rule_0_7: x_A_7 + x_B_7 &gt;= 13
-Rule_0_8: x_A_8 + x_B_8 &gt;= 13
-Rule_0_9: x_A_9 + x_B_9 &gt;= 13
+SupplierExclusion_0_1: x_A_1 = 0
+SupplierExclusion_0_10: x_C_10 = 0
+SupplierExclusion_0_3: x_C_3 = 0
+SupplierExclusion_0_4: x_C_4 = 0
+SupplierExclusion_0_8: x_C_8 = 0
+SupplierExclusion_0_9: x_C_9 = 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
updates to # of Suppliers
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,129 +536,129 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>70000</v>
+        <v>69800</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>52.8</v>
+        <v>19.8</v>
       </c>
       <c r="K2" t="n">
-        <v>36960</v>
+        <v>13820.4</v>
       </c>
       <c r="L2" t="n">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="M2" t="n">
-        <v>33040</v>
+        <v>55979.6</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>2587.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Facility1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Facility1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>156</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1404000</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
       <c r="H3" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="K3" t="n">
-        <v>648000</v>
+        <v>60</v>
       </c>
       <c r="L3" t="n">
-        <v>9000</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>756000</v>
+        <v>40</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>45360.00000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Facility1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Facility1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
       <c r="E4" t="n">
-        <v>423</v>
+        <v>100</v>
       </c>
       <c r="F4" t="n">
-        <v>253800</v>
+        <v>100</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -666,33 +666,33 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>54.45</v>
+        <v>52.8</v>
       </c>
       <c r="K4" t="n">
-        <v>32670</v>
+        <v>52.8</v>
       </c>
       <c r="L4" t="n">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>221130</v>
+        <v>47.2</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>3.696</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -701,137 +701,137 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>453</v>
+        <v>156</v>
       </c>
       <c r="F5" t="n">
-        <v>2568510</v>
+        <v>1403688</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>22.77</v>
+        <v>72</v>
       </c>
       <c r="K5" t="n">
-        <v>129105.9</v>
+        <v>647856</v>
       </c>
       <c r="L5" t="n">
-        <v>5670</v>
+        <v>8998</v>
       </c>
       <c r="M5" t="n">
-        <v>2439404.1</v>
+        <v>755832</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>45349.92000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Facility1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>156</v>
+      </c>
+      <c r="F6" t="n">
+        <v>156</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>342</v>
-      </c>
-      <c r="F6" t="n">
-        <v>15390</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>23.04</v>
+        <v>69.3</v>
       </c>
       <c r="K6" t="n">
-        <v>1036.8</v>
+        <v>69.3</v>
       </c>
       <c r="L6" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>14353.2</v>
+        <v>86.7</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>72.57600000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>653</v>
+        <v>156</v>
       </c>
       <c r="F7" t="n">
-        <v>144966</v>
+        <v>156</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -839,7 +839,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="K7" t="n">
-        <v>5328</v>
+        <v>80</v>
       </c>
       <c r="L7" t="n">
-        <v>222</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>139638</v>
+        <v>76</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -869,16 +869,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Facility2</t>
+          <t>Facility1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -887,77 +887,77 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>653</v>
+        <v>423</v>
       </c>
       <c r="F8" t="n">
-        <v>13060</v>
+        <v>127323</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>41.58</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K8" t="n">
-        <v>831.5999999999999</v>
+        <v>17337.6</v>
       </c>
       <c r="L8" t="n">
-        <v>20</v>
+        <v>301</v>
       </c>
       <c r="M8" t="n">
-        <v>12228.4</v>
+        <v>109985.4</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>1213.632</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Facility1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>423</v>
+      </c>
+      <c r="F9" t="n">
+        <v>126054</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Facility2</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>432</v>
-      </c>
-      <c r="F9" t="n">
-        <v>286848</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>22.77</v>
+        <v>54.45</v>
       </c>
       <c r="K9" t="n">
-        <v>15119.28</v>
+        <v>16226.1</v>
       </c>
       <c r="L9" t="n">
-        <v>664</v>
+        <v>298</v>
       </c>
       <c r="M9" t="n">
-        <v>271728.72</v>
+        <v>109827.9</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -987,16 +987,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility3</t>
+          <t>Facility1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>456</v>
+        <v>423</v>
       </c>
       <c r="F10" t="n">
-        <v>10944</v>
+        <v>423</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="K10" t="n">
-        <v>312</v>
+        <v>65</v>
       </c>
       <c r="L10" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>10632</v>
+        <v>358</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Facility4</t>
+          <t>Facility2</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1064,94 +1064,94 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>234</v>
+        <v>453</v>
       </c>
       <c r="F11" t="n">
-        <v>54288</v>
+        <v>2567604</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>56</v>
+        <v>18.24</v>
       </c>
       <c r="K11" t="n">
-        <v>12992</v>
+        <v>103384.32</v>
       </c>
       <c r="L11" t="n">
-        <v>232</v>
+        <v>5668</v>
       </c>
       <c r="M11" t="n">
-        <v>41296</v>
+        <v>2464219.68</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>7236.9024</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>453</v>
+      </c>
+      <c r="F12" t="n">
+        <v>453</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Facility5</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>231</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="H12" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>13</v>
+        <v>22.77</v>
       </c>
       <c r="K12" t="n">
-        <v>169</v>
+        <v>22.77</v>
       </c>
       <c r="L12" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>2834</v>
+        <v>430.23</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1160,6 +1160,1127 @@
       </c>
       <c r="O12" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>453</v>
+      </c>
+      <c r="F13" t="n">
+        <v>453</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>75</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>75</v>
+      </c>
+      <c r="K13" t="n">
+        <v>75</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>378</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>5</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>342</v>
+      </c>
+      <c r="F14" t="n">
+        <v>14706</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>24</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="K14" t="n">
+        <v>990.7199999999999</v>
+      </c>
+      <c r="L14" t="n">
+        <v>43</v>
+      </c>
+      <c r="M14" t="n">
+        <v>13715.28</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>69.35040000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>342</v>
+      </c>
+      <c r="F15" t="n">
+        <v>342</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>54</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>53.46</v>
+      </c>
+      <c r="K15" t="n">
+        <v>53.46</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>288.54</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>5</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>342</v>
+      </c>
+      <c r="F16" t="n">
+        <v>342</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>34</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>34</v>
+      </c>
+      <c r="K16" t="n">
+        <v>34</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" t="n">
+        <v>308</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>653</v>
+      </c>
+      <c r="F17" t="n">
+        <v>144966</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>24</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>24</v>
+      </c>
+      <c r="K17" t="n">
+        <v>5328</v>
+      </c>
+      <c r="L17" t="n">
+        <v>222</v>
+      </c>
+      <c r="M17" t="n">
+        <v>139638</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>6</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>653</v>
+      </c>
+      <c r="F18" t="n">
+        <v>12407</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>42</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>41.58</v>
+      </c>
+      <c r="K18" t="n">
+        <v>790.02</v>
+      </c>
+      <c r="L18" t="n">
+        <v>19</v>
+      </c>
+      <c r="M18" t="n">
+        <v>11616.98</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>6</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>653</v>
+      </c>
+      <c r="F19" t="n">
+        <v>653</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>64</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>61.44</v>
+      </c>
+      <c r="K19" t="n">
+        <v>61.44</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" t="n">
+        <v>591.5599999999999</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>4.300800000000001</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>7</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>432</v>
+      </c>
+      <c r="F20" t="n">
+        <v>285984</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>23</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>22.77</v>
+      </c>
+      <c r="K20" t="n">
+        <v>15073.74</v>
+      </c>
+      <c r="L20" t="n">
+        <v>662</v>
+      </c>
+      <c r="M20" t="n">
+        <v>270910.26</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>7</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>432</v>
+      </c>
+      <c r="F21" t="n">
+        <v>432</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>53</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>53</v>
+      </c>
+      <c r="K21" t="n">
+        <v>53</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="n">
+        <v>379</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>7</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Facility2</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>432</v>
+      </c>
+      <c r="F22" t="n">
+        <v>432</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>86</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>82.56</v>
+      </c>
+      <c r="K22" t="n">
+        <v>82.56</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" t="n">
+        <v>349.44</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>5.7792</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>8</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Facility3</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>456</v>
+      </c>
+      <c r="F23" t="n">
+        <v>10032</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>13</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>13</v>
+      </c>
+      <c r="K23" t="n">
+        <v>286</v>
+      </c>
+      <c r="L23" t="n">
+        <v>22</v>
+      </c>
+      <c r="M23" t="n">
+        <v>9746</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>8</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Facility3</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>456</v>
+      </c>
+      <c r="F24" t="n">
+        <v>456</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>75</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>74.25</v>
+      </c>
+      <c r="K24" t="n">
+        <v>74.25</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1</v>
+      </c>
+      <c r="M24" t="n">
+        <v>381.75</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>8</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Facility3</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>456</v>
+      </c>
+      <c r="F25" t="n">
+        <v>456</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>24</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="K25" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M25" t="n">
+        <v>432.96</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O25" t="n">
+        <v>1.6128</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>9</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Facility4</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>234</v>
+      </c>
+      <c r="F26" t="n">
+        <v>53820</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>13</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="K26" t="n">
+        <v>2870.4</v>
+      </c>
+      <c r="L26" t="n">
+        <v>230</v>
+      </c>
+      <c r="M26" t="n">
+        <v>50949.6</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O26" t="n">
+        <v>200.928</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>9</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Facility4</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>234</v>
+      </c>
+      <c r="F27" t="n">
+        <v>234</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>97</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>96.03</v>
+      </c>
+      <c r="K27" t="n">
+        <v>96.03</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="n">
+        <v>137.97</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>9</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Facility4</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>234</v>
+      </c>
+      <c r="F28" t="n">
+        <v>234</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>56</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>56</v>
+      </c>
+      <c r="K28" t="n">
+        <v>56</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1</v>
+      </c>
+      <c r="M28" t="n">
+        <v>178</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>10</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>231</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2541</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>13</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>13</v>
+      </c>
+      <c r="K29" t="n">
+        <v>143</v>
+      </c>
+      <c r="L29" t="n">
+        <v>11</v>
+      </c>
+      <c r="M29" t="n">
+        <v>2398</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>10</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>231</v>
+      </c>
+      <c r="F30" t="n">
+        <v>231</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>64</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>63.36</v>
+      </c>
+      <c r="K30" t="n">
+        <v>63.36</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" t="n">
+        <v>167.64</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>10</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Facility5</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>231</v>
+      </c>
+      <c r="F31" t="n">
+        <v>231</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>75</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>72</v>
+      </c>
+      <c r="K31" t="n">
+        <v>72</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1</v>
+      </c>
+      <c r="M31" t="n">
+        <v>159</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>5.040000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1334,12 +2455,76 @@
 RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 15248788 y_rebate_B_1 &lt;= 15248788
 RebateTierUpper_C_0: rebate_C + 16791670 y_rebate_C_0 &lt;= 16791670
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 16791670 y_rebate_C_1 &lt;= 16791670
-SupplierExclusion_0_1: x_A_1 = 0
-SupplierExclusion_0_10: x_C_10 = 0
-SupplierExclusion_0_3: x_C_3 = 0
-SupplierExclusion_0_4: x_C_4 = 0
-SupplierExclusion_0_8: x_C_8 = 0
-SupplierExclusion_0_9: x_C_9 = 0
+SupplIndicatorLB_0_A_1: - w_0_A_1 + x_A_1 &gt;= 0
+SupplIndicatorLB_0_A_10: - w_0_A_10 + x_A_10 &gt;= 0
+SupplIndicatorLB_0_A_2: - w_0_A_2 + x_A_2 &gt;= 0
+SupplIndicatorLB_0_A_3: - w_0_A_3 + x_A_3 &gt;= 0
+SupplIndicatorLB_0_A_4: - w_0_A_4 + x_A_4 &gt;= 0
+SupplIndicatorLB_0_A_5: - w_0_A_5 + x_A_5 &gt;= 0
+SupplIndicatorLB_0_A_6: - w_0_A_6 + x_A_6 &gt;= 0
+SupplIndicatorLB_0_A_7: - w_0_A_7 + x_A_7 &gt;= 0
+SupplIndicatorLB_0_A_8: - w_0_A_8 + x_A_8 &gt;= 0
+SupplIndicatorLB_0_A_9: - w_0_A_9 + x_A_9 &gt;= 0
+SupplIndicatorLB_0_B_1: - w_0_B_1 + x_B_1 &gt;= 0
+SupplIndicatorLB_0_B_10: - w_0_B_10 + x_B_10 &gt;= 0
+SupplIndicatorLB_0_B_2: - w_0_B_2 + x_B_2 &gt;= 0
+SupplIndicatorLB_0_B_3: - w_0_B_3 + x_B_3 &gt;= 0
+SupplIndicatorLB_0_B_4: - w_0_B_4 + x_B_4 &gt;= 0
+SupplIndicatorLB_0_B_5: - w_0_B_5 + x_B_5 &gt;= 0
+SupplIndicatorLB_0_B_6: - w_0_B_6 + x_B_6 &gt;= 0
+SupplIndicatorLB_0_B_7: - w_0_B_7 + x_B_7 &gt;= 0
+SupplIndicatorLB_0_B_8: - w_0_B_8 + x_B_8 &gt;= 0
+SupplIndicatorLB_0_B_9: - w_0_B_9 + x_B_9 &gt;= 0
+SupplIndicatorLB_0_C_1: - w_0_C_1 + x_C_1 &gt;= 0
+SupplIndicatorLB_0_C_10: - w_0_C_10 + x_C_10 &gt;= 0
+SupplIndicatorLB_0_C_2: - w_0_C_2 + x_C_2 &gt;= 0
+SupplIndicatorLB_0_C_3: - w_0_C_3 + x_C_3 &gt;= 0
+SupplIndicatorLB_0_C_4: - w_0_C_4 + x_C_4 &gt;= 0
+SupplIndicatorLB_0_C_5: - w_0_C_5 + x_C_5 &gt;= 0
+SupplIndicatorLB_0_C_6: - w_0_C_6 + x_C_6 &gt;= 0
+SupplIndicatorLB_0_C_7: - w_0_C_7 + x_C_7 &gt;= 0
+SupplIndicatorLB_0_C_8: - w_0_C_8 + x_C_8 &gt;= 0
+SupplIndicatorLB_0_C_9: - w_0_C_9 + x_C_9 &gt;= 0
+SupplIndicator_0_A_1: - 1000000000 w_0_A_1 + x_A_1 &lt;= 0
+SupplIndicator_0_A_10: - 1000000000 w_0_A_10 + x_A_10 &lt;= 0
+SupplIndicator_0_A_2: - 1000000000 w_0_A_2 + x_A_2 &lt;= 0
+SupplIndicator_0_A_3: - 1000000000 w_0_A_3 + x_A_3 &lt;= 0
+SupplIndicator_0_A_4: - 1000000000 w_0_A_4 + x_A_4 &lt;= 0
+SupplIndicator_0_A_5: - 1000000000 w_0_A_5 + x_A_5 &lt;= 0
+SupplIndicator_0_A_6: - 1000000000 w_0_A_6 + x_A_6 &lt;= 0
+SupplIndicator_0_A_7: - 1000000000 w_0_A_7 + x_A_7 &lt;= 0
+SupplIndicator_0_A_8: - 1000000000 w_0_A_8 + x_A_8 &lt;= 0
+SupplIndicator_0_A_9: - 1000000000 w_0_A_9 + x_A_9 &lt;= 0
+SupplIndicator_0_B_1: - 1000000000 w_0_B_1 + x_B_1 &lt;= 0
+SupplIndicator_0_B_10: - 1000000000 w_0_B_10 + x_B_10 &lt;= 0
+SupplIndicator_0_B_2: - 1000000000 w_0_B_2 + x_B_2 &lt;= 0
+SupplIndicator_0_B_3: - 1000000000 w_0_B_3 + x_B_3 &lt;= 0
+SupplIndicator_0_B_4: - 1000000000 w_0_B_4 + x_B_4 &lt;= 0
+SupplIndicator_0_B_5: - 1000000000 w_0_B_5 + x_B_5 &lt;= 0
+SupplIndicator_0_B_6: - 1000000000 w_0_B_6 + x_B_6 &lt;= 0
+SupplIndicator_0_B_7: - 1000000000 w_0_B_7 + x_B_7 &lt;= 0
+SupplIndicator_0_B_8: - 1000000000 w_0_B_8 + x_B_8 &lt;= 0
+SupplIndicator_0_B_9: - 1000000000 w_0_B_9 + x_B_9 &lt;= 0
+SupplIndicator_0_C_1: - 1000000000 w_0_C_1 + x_C_1 &lt;= 0
+SupplIndicator_0_C_10: - 1000000000 w_0_C_10 + x_C_10 &lt;= 0
+SupplIndicator_0_C_2: - 1000000000 w_0_C_2 + x_C_2 &lt;= 0
+SupplIndicator_0_C_3: - 1000000000 w_0_C_3 + x_C_3 &lt;= 0
+SupplIndicator_0_C_4: - 1000000000 w_0_C_4 + x_C_4 &lt;= 0
+SupplIndicator_0_C_5: - 1000000000 w_0_C_5 + x_C_5 &lt;= 0
+SupplIndicator_0_C_6: - 1000000000 w_0_C_6 + x_C_6 &lt;= 0
+SupplIndicator_0_C_7: - 1000000000 w_0_C_7 + x_C_7 &lt;= 0
+SupplIndicator_0_C_8: - 1000000000 w_0_C_8 + x_C_8 &lt;= 0
+SupplIndicator_0_C_9: - 1000000000 w_0_C_9 + x_C_9 &lt;= 0
+SupplierCount_0_1: w_0_A_1 + w_0_B_1 + w_0_C_1 = 3
+SupplierCount_0_10: w_0_A_10 + w_0_B_10 + w_0_C_10 = 3
+SupplierCount_0_2: w_0_A_2 + w_0_B_2 + w_0_C_2 = 3
+SupplierCount_0_3: w_0_A_3 + w_0_B_3 + w_0_C_3 = 3
+SupplierCount_0_4: w_0_A_4 + w_0_B_4 + w_0_C_4 = 3
+SupplierCount_0_5: w_0_A_5 + w_0_B_5 + w_0_C_5 = 3
+SupplierCount_0_6: w_0_A_6 + w_0_B_6 + w_0_C_6 = 3
+SupplierCount_0_7: w_0_A_7 + w_0_B_7 + w_0_C_7 = 3
+SupplierCount_0_8: w_0_A_8 + w_0_B_8 + w_0_C_8 = 3
+SupplierCount_0_9: w_0_A_9 + w_0_B_9 + w_0_C_9 = 3
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1387,6 +2572,36 @@
 T_8_B
 T_9_A
 T_9_B
+w_0_A_1
+w_0_A_10
+w_0_A_2
+w_0_A_3
+w_0_A_4
+w_0_A_5
+w_0_A_6
+w_0_A_7
+w_0_A_8
+w_0_A_9
+w_0_B_1
+w_0_B_10
+w_0_B_2
+w_0_B_3
+w_0_B_4
+w_0_B_5
+w_0_B_6
+w_0_B_7
+w_0_B_8
+w_0_B_9
+w_0_C_1
+w_0_C_10
+w_0_C_2
+w_0_C_3
+w_0_C_4
+w_0_C_5
+w_0_C_6
+w_0_C_7
+w_0_C_8
+w_0_C_9
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
%min volume confirmed working
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,36 +540,36 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>52.8</v>
+        <v>49.5</v>
       </c>
       <c r="K2" t="n">
-        <v>36960</v>
+        <v>34650</v>
       </c>
       <c r="L2" t="n">
         <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>33040</v>
+        <v>35350</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>2587.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -595,7 +595,7 @@
         <v>156</v>
       </c>
       <c r="F3" t="n">
-        <v>1404000</v>
+        <v>1224600</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -614,13 +614,13 @@
         <v>72</v>
       </c>
       <c r="K3" t="n">
-        <v>648000</v>
+        <v>565200</v>
       </c>
       <c r="L3" t="n">
-        <v>9000</v>
+        <v>7850</v>
       </c>
       <c r="M3" t="n">
-        <v>756000</v>
+        <v>659400</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -628,71 +628,71 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>45360.00000000001</v>
+        <v>39564.00000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Facility 1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>156</v>
+      </c>
+      <c r="F4" t="n">
+        <v>179400</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Facility 4</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>423</v>
-      </c>
-      <c r="F4" t="n">
-        <v>253800</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
       <c r="H4" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>57.59999999999999</v>
+        <v>69.3</v>
       </c>
       <c r="K4" t="n">
-        <v>34560</v>
+        <v>79695</v>
       </c>
       <c r="L4" t="n">
-        <v>600</v>
+        <v>1150</v>
       </c>
       <c r="M4" t="n">
-        <v>219240</v>
+        <v>99705</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>2419.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -710,48 +710,48 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>2568510</v>
+        <v>253800</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>23.04</v>
+        <v>54.45</v>
       </c>
       <c r="K5" t="n">
-        <v>130636.8</v>
+        <v>32670</v>
       </c>
       <c r="L5" t="n">
-        <v>5670</v>
+        <v>600</v>
       </c>
       <c r="M5" t="n">
-        <v>2437873.2</v>
+        <v>221130</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>9144.576000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,57 +769,57 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>15390</v>
+        <v>2373267</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>23.04</v>
+        <v>22.77</v>
       </c>
       <c r="K6" t="n">
-        <v>1036.8</v>
+        <v>119292.03</v>
       </c>
       <c r="L6" t="n">
-        <v>45</v>
+        <v>5239</v>
       </c>
       <c r="M6" t="n">
-        <v>14353.2</v>
+        <v>2253974.97</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>72.57600000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,14 +828,14 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>653</v>
+        <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>158026</v>
+        <v>195243</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -843,33 +843,33 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>24</v>
+        <v>23.04</v>
       </c>
       <c r="K7" t="n">
-        <v>5808</v>
+        <v>9930.24</v>
       </c>
       <c r="L7" t="n">
-        <v>242</v>
+        <v>431</v>
       </c>
       <c r="M7" t="n">
-        <v>152218</v>
+        <v>185312.76</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>695.1168</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -887,48 +887,48 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>432</v>
+        <v>342</v>
       </c>
       <c r="F8" t="n">
-        <v>286848</v>
+        <v>15390</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>23</v>
+        <v>23.04</v>
       </c>
       <c r="K8" t="n">
-        <v>15272</v>
+        <v>1036.8</v>
       </c>
       <c r="L8" t="n">
-        <v>664</v>
+        <v>45</v>
       </c>
       <c r="M8" t="n">
-        <v>271576</v>
+        <v>14353.2</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>72.57600000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,35 +946,35 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>456</v>
+        <v>653</v>
       </c>
       <c r="F9" t="n">
-        <v>10944</v>
+        <v>158026</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>13</v>
+        <v>41.58</v>
       </c>
       <c r="K9" t="n">
-        <v>312</v>
+        <v>10062.36</v>
       </c>
       <c r="L9" t="n">
-        <v>24</v>
+        <v>242</v>
       </c>
       <c r="M9" t="n">
-        <v>10632</v>
+        <v>147963.64</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,102 +1005,220 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>234</v>
+        <v>432</v>
       </c>
       <c r="F10" t="n">
-        <v>54288</v>
+        <v>286848</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>12.48</v>
+        <v>22.77</v>
       </c>
       <c r="K10" t="n">
-        <v>2895.36</v>
+        <v>15119.28</v>
       </c>
       <c r="L10" t="n">
-        <v>232</v>
+        <v>664</v>
       </c>
       <c r="M10" t="n">
-        <v>51392.64</v>
+        <v>271728.72</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>202.6752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Facility 9</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>456</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10944</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>24</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="K11" t="n">
+        <v>552.96</v>
+      </c>
+      <c r="L11" t="n">
+        <v>24</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10391.04</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>38.70720000000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>234</v>
+      </c>
+      <c r="F12" t="n">
+        <v>54288</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>13</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2895.36</v>
+      </c>
+      <c r="L12" t="n">
+        <v>232</v>
+      </c>
+      <c r="M12" t="n">
+        <v>51392.64</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>202.6752</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>Facility 10</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
         <v>231</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F13" t="n">
         <v>3003</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>12</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>11.52</v>
+      </c>
+      <c r="K13" t="n">
+        <v>149.76</v>
+      </c>
+      <c r="L13" t="n">
         <v>13</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
-        <v>13</v>
-      </c>
-      <c r="K11" t="n">
-        <v>169</v>
-      </c>
-      <c r="L11" t="n">
-        <v>13</v>
-      </c>
-      <c r="M11" t="n">
-        <v>2834</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
+      <c r="M13" t="n">
+        <v>2853.24</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>10.4832</v>
       </c>
     </row>
   </sheetData>
@@ -1173,7 +1291,7 @@
  - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
 BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 80 x_B_2 - 65 x_B_3 - 75 x_B_4
  - 34 x_B_5 - 24 x_B_6 - 53 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
-BaseSpend_C: S0_C - 55 x_C_1 - 75 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
+BaseSpend_C: S0_C - 55 x_C_1 - 12 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
  - 24 x_C_5 - 64 x_C_6 - 86 x_C_7 - 24 x_C_8 - 13 x_C_9 = 0
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
@@ -1241,6 +1359,24 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
+MinVolPct_LB_0_A_216520528749813870: - 8595 MinVolPct_0_A_216520528749813870
+ + x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7 + x_A_8
+ + x_A_9 &gt;= 0
+MinVolPct_LB_0_B_216520528749813870: - 8595 MinVolPct_0_B_216520528749813870
+ + x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7 + x_B_8
+ + x_B_9 &gt;= 0
+MinVolPct_LB_0_C_216520528749813870: - 8595 MinVolPct_0_C_216520528749813870
+ + x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7 + x_C_8
+ + x_C_9 &gt;= 0
+MinVolPct_UB_0_A_216520528749813870: - 17190 MinVolPct_0_A_216520528749813870
+ + x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7 + x_A_8
+ + x_A_9 &lt;= 0
+MinVolPct_UB_0_B_216520528749813870: - 17190 MinVolPct_0_B_216520528749813870
+ + x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7 + x_B_8
+ + x_B_9 &lt;= 0
+MinVolPct_UB_0_C_216520528749813870: - 17190 MinVolPct_0_C_216520528749813870
+ + x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7 + x_C_8
+ + x_C_9 &lt;= 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
  &gt;= -19400000000
@@ -1299,6 +1435,9 @@
 Volume_C: V_C - x_C_1 - x_C_10 - x_C_2 - x_C_3 - x_C_4 - x_C_5 - x_C_6 - x_C_7
  - x_C_8 - x_C_9 = 0
 Binaries
+MinVolPct_0_A_216520528749813870
+MinVolPct_0_B_216520528749813870
+MinVolPct_0_C_216520528749813870
 T_10_A
 T_10_B
 T_1_B

</xml_diff>

<commit_message>
all rules should be working correctly now
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,36 +540,36 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>49.5</v>
+        <v>52.8</v>
       </c>
       <c r="K2" t="n">
-        <v>34650</v>
+        <v>36960</v>
       </c>
       <c r="L2" t="n">
         <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>35350</v>
+        <v>33040</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>2587.2</v>
       </c>
     </row>
     <row r="3">
@@ -595,7 +595,7 @@
         <v>156</v>
       </c>
       <c r="F3" t="n">
-        <v>1224600</v>
+        <v>1396200</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -614,13 +614,13 @@
         <v>72</v>
       </c>
       <c r="K3" t="n">
-        <v>565200</v>
+        <v>644400</v>
       </c>
       <c r="L3" t="n">
-        <v>7850</v>
+        <v>8950</v>
       </c>
       <c r="M3" t="n">
-        <v>659400</v>
+        <v>751800</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>39564.00000000001</v>
+        <v>45108.00000000001</v>
       </c>
     </row>
     <row r="4">
@@ -654,40 +654,40 @@
         <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>179400</v>
+        <v>7800</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>69.3</v>
+        <v>77.59999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>79695</v>
+        <v>3880</v>
       </c>
       <c r="L4" t="n">
-        <v>1150</v>
+        <v>50</v>
       </c>
       <c r="M4" t="n">
-        <v>99705</v>
+        <v>3920</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5">
@@ -717,36 +717,36 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>54.45</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K5" t="n">
-        <v>32670</v>
+        <v>34560</v>
       </c>
       <c r="L5" t="n">
         <v>600</v>
       </c>
       <c r="M5" t="n">
-        <v>221130</v>
+        <v>219240</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>2419.2</v>
       </c>
     </row>
     <row r="6">
@@ -772,54 +772,54 @@
         <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>2373267</v>
+        <v>2568510</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>22.77</v>
+        <v>23.04</v>
       </c>
       <c r="K6" t="n">
-        <v>119292.03</v>
+        <v>130636.8</v>
       </c>
       <c r="L6" t="n">
-        <v>5239</v>
+        <v>5670</v>
       </c>
       <c r="M6" t="n">
-        <v>2253974.97</v>
+        <v>2437873.2</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>9144.576000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F7" t="n">
-        <v>195243</v>
+        <v>15390</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -850,13 +850,13 @@
         <v>23.04</v>
       </c>
       <c r="K7" t="n">
-        <v>9930.24</v>
+        <v>1036.8</v>
       </c>
       <c r="L7" t="n">
-        <v>431</v>
+        <v>45</v>
       </c>
       <c r="M7" t="n">
-        <v>185312.76</v>
+        <v>14353.2</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -864,12 +864,12 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>695.1168</v>
+        <v>72.57600000000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -887,14 +887,14 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>342</v>
+        <v>653</v>
       </c>
       <c r="F8" t="n">
-        <v>15390</v>
+        <v>157373</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -902,28 +902,28 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>23.04</v>
+        <v>23.28</v>
       </c>
       <c r="K8" t="n">
-        <v>1036.8</v>
+        <v>5610.48</v>
       </c>
       <c r="L8" t="n">
-        <v>45</v>
+        <v>241</v>
       </c>
       <c r="M8" t="n">
-        <v>14353.2</v>
+        <v>151762.52</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>72.57600000000001</v>
+        <v>280.5240000000001</v>
       </c>
     </row>
     <row r="9">
@@ -932,7 +932,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -949,7 +949,7 @@
         <v>653</v>
       </c>
       <c r="F9" t="n">
-        <v>158026</v>
+        <v>653</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -961,20 +961,20 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>41.58</v>
+        <v>42</v>
       </c>
       <c r="K9" t="n">
-        <v>10062.36</v>
+        <v>42</v>
       </c>
       <c r="L9" t="n">
-        <v>242</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>147963.64</v>
+        <v>611</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1008,7 +1008,7 @@
         <v>432</v>
       </c>
       <c r="F10" t="n">
-        <v>286848</v>
+        <v>196560</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1020,20 +1020,20 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>22.77</v>
+        <v>23</v>
       </c>
       <c r="K10" t="n">
-        <v>15119.28</v>
+        <v>10465</v>
       </c>
       <c r="L10" t="n">
-        <v>664</v>
+        <v>455</v>
       </c>
       <c r="M10" t="n">
-        <v>271728.72</v>
+        <v>186095</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1046,11 +1046,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1064,48 +1064,48 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F11" t="n">
-        <v>10944</v>
+        <v>90288</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>23.04</v>
+        <v>51.41</v>
       </c>
       <c r="K11" t="n">
-        <v>552.96</v>
+        <v>10744.69</v>
       </c>
       <c r="L11" t="n">
-        <v>24</v>
+        <v>209</v>
       </c>
       <c r="M11" t="n">
-        <v>10391.04</v>
+        <v>79543.31</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>38.70720000000001</v>
+        <v>537.2344999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1123,14 +1123,14 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>234</v>
+        <v>456</v>
       </c>
       <c r="F12" t="n">
-        <v>54288</v>
+        <v>10944</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -1138,86 +1138,145 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>12.48</v>
+        <v>12.61</v>
       </c>
       <c r="K12" t="n">
-        <v>2895.36</v>
+        <v>302.64</v>
       </c>
       <c r="L12" t="n">
-        <v>232</v>
+        <v>24</v>
       </c>
       <c r="M12" t="n">
-        <v>51392.64</v>
+        <v>10641.36</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>202.6752</v>
+        <v>15.132</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>234</v>
+      </c>
+      <c r="F13" t="n">
+        <v>54288</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>13</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2895.36</v>
+      </c>
+      <c r="L13" t="n">
+        <v>232</v>
+      </c>
+      <c r="M13" t="n">
+        <v>51392.64</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>202.6752</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>10</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Facility 10</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
         <v>231</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F14" t="n">
         <v>3003</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
         <v>12</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>4%</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="J14" t="n">
         <v>11.52</v>
       </c>
-      <c r="K13" t="n">
+      <c r="K14" t="n">
         <v>149.76</v>
       </c>
-      <c r="L13" t="n">
+      <c r="L14" t="n">
         <v>13</v>
       </c>
-      <c r="M13" t="n">
+      <c r="M14" t="n">
         <v>2853.24</v>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>7%</t>
         </is>
       </c>
-      <c r="O13" t="n">
+      <c r="O14" t="n">
         <v>10.4832</v>
       </c>
     </row>
@@ -1359,24 +1418,15 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
-MinVolPct_LB_0_A_216520528749813870: - 8595 MinVolPct_0_A_216520528749813870
- + x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7 + x_A_8
- + x_A_9 &gt;= 0
-MinVolPct_LB_0_B_216520528749813870: - 8595 MinVolPct_0_B_216520528749813870
- + x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7 + x_B_8
- + x_B_9 &gt;= 0
-MinVolPct_LB_0_C_216520528749813870: - 8595 MinVolPct_0_C_216520528749813870
- + x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7 + x_C_8
- + x_C_9 &gt;= 0
-MinVolPct_UB_0_A_216520528749813870: - 17190 MinVolPct_0_A_216520528749813870
- + x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7 + x_A_8
- + x_A_9 &lt;= 0
-MinVolPct_UB_0_B_216520528749813870: - 17190 MinVolPct_0_B_216520528749813870
- + x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7 + x_B_8
- + x_B_9 &lt;= 0
-MinVolPct_UB_0_C_216520528749813870: - 17190 MinVolPct_0_C_216520528749813870
- + x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7 + x_C_8
- + x_C_9 &lt;= 0
+MinVol_LB_1_A_Large_Gadget: - 1000000000 MinVol_1_A_Large_Gadget + x_A_6
+ + x_A_7 &gt;= -999999550
+MinVol_LB_1_B_Large_Gadget: - 1000000000 MinVol_1_B_Large_Gadget + x_B_6
+ + x_B_7 &gt;= -999999550
+MinVol_LB_1_C_Large_Gadget: - 1000000000 MinVol_1_C_Large_Gadget + x_C_6
+ + x_C_7 &gt;= -999999550
+MinVol_UB_1_A_Large_Gadget: - 906 MinVol_1_A_Large_Gadget + x_A_6 + x_A_7 &lt;= 0
+MinVol_UB_1_B_Large_Gadget: - 906 MinVol_1_B_Large_Gadget + x_B_6 + x_B_7 &lt;= 0
+MinVol_UB_1_C_Large_Gadget: - 906 MinVol_1_C_Large_Gadget + x_C_6 + x_C_7 &lt;= 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
  &gt;= -19400000000
@@ -1408,6 +1458,20 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
+SupplIndicatorLB_0_A_6: - w_0_A_6 + x_A_6 &gt;= 0
+SupplIndicatorLB_0_A_7: - w_0_A_7 + x_A_7 &gt;= 0
+SupplIndicatorLB_0_B_6: - w_0_B_6 + x_B_6 &gt;= 0
+SupplIndicatorLB_0_B_7: - w_0_B_7 + x_B_7 &gt;= 0
+SupplIndicatorLB_0_C_6: - w_0_C_6 + x_C_6 &gt;= 0
+SupplIndicatorLB_0_C_7: - w_0_C_7 + x_C_7 &gt;= 0
+SupplIndicator_0_A_6: - 1000000000 w_0_A_6 + x_A_6 &lt;= 0
+SupplIndicator_0_A_7: - 1000000000 w_0_A_7 + x_A_7 &lt;= 0
+SupplIndicator_0_B_6: - 1000000000 w_0_B_6 + x_B_6 &lt;= 0
+SupplIndicator_0_B_7: - 1000000000 w_0_B_7 + x_B_7 &lt;= 0
+SupplIndicator_0_C_6: - 1000000000 w_0_C_6 + x_C_6 &lt;= 0
+SupplIndicator_0_C_7: - 1000000000 w_0_C_7 + x_C_7 &lt;= 0
+SupplierCount_0_6: w_0_A_6 + w_0_B_6 + w_0_C_6 = 2
+SupplierCount_0_7: w_0_A_7 + w_0_B_7 + w_0_C_7 = 2
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1435,9 +1499,9 @@
 Volume_C: V_C - x_C_1 - x_C_10 - x_C_2 - x_C_3 - x_C_4 - x_C_5 - x_C_6 - x_C_7
  - x_C_8 - x_C_9 = 0
 Binaries
-MinVolPct_0_A_216520528749813870
-MinVolPct_0_B_216520528749813870
-MinVolPct_0_C_216520528749813870
+MinVol_1_A_Large_Gadget
+MinVol_1_B_Large_Gadget
+MinVol_1_C_Large_Gadget
 T_10_A
 T_10_B
 T_1_B
@@ -1458,6 +1522,12 @@
 T_8_B
 T_9_A
 T_9_B
+w_0_A_6
+w_0_A_7
+w_0_B_6
+w_0_B_7
+w_0_C_6
+w_0_C_7
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
# of volume awarded fixed
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>70000</v>
+        <v>40000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -555,13 +555,13 @@
         <v>52.8</v>
       </c>
       <c r="K2" t="n">
-        <v>36960</v>
+        <v>21120</v>
       </c>
       <c r="L2" t="n">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="M2" t="n">
-        <v>33040</v>
+        <v>18880</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -569,66 +569,66 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>2587.2</v>
+        <v>1478.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Facility 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Facility 1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="E3" t="n">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>1396200</v>
+        <v>30000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="K3" t="n">
-        <v>644400</v>
+        <v>15000</v>
       </c>
       <c r="L3" t="n">
-        <v>8950</v>
+        <v>300</v>
       </c>
       <c r="M3" t="n">
-        <v>751800</v>
+        <v>15000</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>45108.00000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -637,7 +637,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -654,7 +654,7 @@
         <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>7800</v>
+        <v>1404000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>77.59999999999999</v>
+        <v>67.89999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>3880</v>
+        <v>611099.9999999999</v>
       </c>
       <c r="L4" t="n">
-        <v>50</v>
+        <v>9000</v>
       </c>
       <c r="M4" t="n">
-        <v>3920</v>
+        <v>792900.0000000001</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>194</v>
+        <v>30555</v>
       </c>
     </row>
     <row r="5">
@@ -890,7 +890,7 @@
         <v>653</v>
       </c>
       <c r="F8" t="n">
-        <v>157373</v>
+        <v>158026</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>23.28</v>
       </c>
       <c r="K8" t="n">
-        <v>5610.48</v>
+        <v>5633.76</v>
       </c>
       <c r="L8" t="n">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M8" t="n">
-        <v>151762.52</v>
+        <v>152392.24</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -923,16 +923,16 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>280.5240000000001</v>
+        <v>281.688</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -946,48 +946,48 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>653</v>
+        <v>432</v>
       </c>
       <c r="F9" t="n">
-        <v>653</v>
+        <v>286848</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>42</v>
+        <v>22.08</v>
       </c>
       <c r="K9" t="n">
-        <v>42</v>
+        <v>14661.12</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>664</v>
       </c>
       <c r="M9" t="n">
-        <v>611</v>
+        <v>272186.88</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>1026.2784</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1005,57 +1005,57 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="F10" t="n">
-        <v>196560</v>
+        <v>10944</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>23</v>
+        <v>12.61</v>
       </c>
       <c r="K10" t="n">
-        <v>10465</v>
+        <v>302.64</v>
       </c>
       <c r="L10" t="n">
-        <v>455</v>
+        <v>24</v>
       </c>
       <c r="M10" t="n">
-        <v>186095</v>
+        <v>10641.36</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>15.132</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1064,48 +1064,48 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>432</v>
+        <v>234</v>
       </c>
       <c r="F11" t="n">
-        <v>90288</v>
+        <v>54288</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>51.41</v>
+        <v>12.48</v>
       </c>
       <c r="K11" t="n">
-        <v>10744.69</v>
+        <v>2895.36</v>
       </c>
       <c r="L11" t="n">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="M11" t="n">
-        <v>79543.31</v>
+        <v>51392.64</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>537.2344999999999</v>
+        <v>202.6752</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>456</v>
+        <v>231</v>
       </c>
       <c r="F12" t="n">
-        <v>10944</v>
+        <v>3003</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1145,13 +1145,13 @@
         <v>12.61</v>
       </c>
       <c r="K12" t="n">
-        <v>302.64</v>
+        <v>163.93</v>
       </c>
       <c r="L12" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="M12" t="n">
-        <v>10641.36</v>
+        <v>2839.07</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1159,125 +1159,7 @@
         </is>
       </c>
       <c r="O12" t="n">
-        <v>15.132</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>234</v>
-      </c>
-      <c r="F13" t="n">
-        <v>54288</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>13</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J13" t="n">
-        <v>12.48</v>
-      </c>
-      <c r="K13" t="n">
-        <v>2895.36</v>
-      </c>
-      <c r="L13" t="n">
-        <v>232</v>
-      </c>
-      <c r="M13" t="n">
-        <v>51392.64</v>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="O13" t="n">
-        <v>202.6752</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>231</v>
-      </c>
-      <c r="F14" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>12</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J14" t="n">
-        <v>11.52</v>
-      </c>
-      <c r="K14" t="n">
-        <v>149.76</v>
-      </c>
-      <c r="L14" t="n">
-        <v>13</v>
-      </c>
-      <c r="M14" t="n">
-        <v>2853.24</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>10.4832</v>
+        <v>8.1965</v>
       </c>
     </row>
   </sheetData>
@@ -1348,10 +1230,10 @@
 Subject To
 BaseSpend_A: S0_A - 50 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
  - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
-BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 80 x_B_2 - 65 x_B_3 - 75 x_B_4
- - 34 x_B_5 - 24 x_B_6 - 53 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
-BaseSpend_C: S0_C - 55 x_C_1 - 12 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
- - 24 x_C_5 - 64 x_C_6 - 86 x_C_7 - 24 x_C_8 - 13 x_C_9 = 0
+BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 70 x_B_2 - 65 x_B_3 - 75 x_B_4
+ - 34 x_B_5 - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
+BaseSpend_C: S0_C - 55 x_C_1 - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
+ - 24 x_C_5 - 64 x_C_6 - 23 x_C_7 - 24 x_C_8 - 13 x_C_9 = 0
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
 Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000
@@ -1418,15 +1300,12 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
-MinVol_LB_1_A_Large_Gadget: - 1000000000 MinVol_1_A_Large_Gadget + x_A_6
- + x_A_7 &gt;= -999999550
-MinVol_LB_1_B_Large_Gadget: - 1000000000 MinVol_1_B_Large_Gadget + x_B_6
- + x_B_7 &gt;= -999999550
-MinVol_LB_1_C_Large_Gadget: - 1000000000 MinVol_1_C_Large_Gadget + x_C_6
- + x_C_7 &gt;= -999999550
-MinVol_UB_1_A_Large_Gadget: - 906 MinVol_1_A_Large_Gadget + x_A_6 + x_A_7 &lt;= 0
-MinVol_UB_1_B_Large_Gadget: - 906 MinVol_1_B_Large_Gadget + x_B_6 + x_B_7 &lt;= 0
-MinVol_UB_1_C_Large_Gadget: - 906 MinVol_1_C_Large_Gadget + x_C_6 + x_C_7 &lt;= 0
+MinVolAwarded_LB_1_A_1: - 300 award_indicator_1_A_1 + x_A_1 &gt;= 0
+MinVolAwarded_LB_1_B_1: - 300 award_indicator_1_B_1 + x_B_1 &gt;= 0
+MinVolAwarded_LB_1_C_1: - 300 award_indicator_1_C_1 + x_C_1 &gt;= 0
+MinVolAwarded_UB_1_A_1: - 700 award_indicator_1_A_1 + x_A_1 &lt;= 0
+MinVolAwarded_UB_1_B_1: - 700 award_indicator_1_B_1 + x_B_1 &lt;= 0
+MinVolAwarded_UB_1_C_1: - 700 award_indicator_1_C_1 + x_C_1 &lt;= 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
  &gt;= -19400000000
@@ -1458,20 +1337,13 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-SupplIndicatorLB_0_A_6: - w_0_A_6 + x_A_6 &gt;= 0
-SupplIndicatorLB_0_A_7: - w_0_A_7 + x_A_7 &gt;= 0
-SupplIndicatorLB_0_B_6: - w_0_B_6 + x_B_6 &gt;= 0
-SupplIndicatorLB_0_B_7: - w_0_B_7 + x_B_7 &gt;= 0
-SupplIndicatorLB_0_C_6: - w_0_C_6 + x_C_6 &gt;= 0
-SupplIndicatorLB_0_C_7: - w_0_C_7 + x_C_7 &gt;= 0
-SupplIndicator_0_A_6: - 1000000000 w_0_A_6 + x_A_6 &lt;= 0
-SupplIndicator_0_A_7: - 1000000000 w_0_A_7 + x_A_7 &lt;= 0
-SupplIndicator_0_B_6: - 1000000000 w_0_B_6 + x_B_6 &lt;= 0
-SupplIndicator_0_B_7: - 1000000000 w_0_B_7 + x_B_7 &lt;= 0
-SupplIndicator_0_C_6: - 1000000000 w_0_C_6 + x_C_6 &lt;= 0
-SupplIndicator_0_C_7: - 1000000000 w_0_C_7 + x_C_7 &lt;= 0
-SupplierCount_0_6: w_0_A_6 + w_0_B_6 + w_0_C_6 = 2
-SupplierCount_0_7: w_0_A_7 + w_0_B_7 + w_0_C_7 = 2
+SupplIndicatorLB_0_A_1: - w_0_A_1 + x_A_1 &gt;= 0
+SupplIndicatorLB_0_B_1: - w_0_B_1 + x_B_1 &gt;= 0
+SupplIndicatorLB_0_C_1: - w_0_C_1 + x_C_1 &gt;= 0
+SupplIndicator_0_A_1: - 1000000000 w_0_A_1 + x_A_1 &lt;= 0
+SupplIndicator_0_B_1: - 1000000000 w_0_B_1 + x_B_1 &lt;= 0
+SupplIndicator_0_C_1: - 1000000000 w_0_C_1 + x_C_1 &lt;= 0
+SupplierCount_0_1: w_0_A_1 + w_0_B_1 + w_0_C_1 = 2
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1499,9 +1371,6 @@
 Volume_C: V_C - x_C_1 - x_C_10 - x_C_2 - x_C_3 - x_C_4 - x_C_5 - x_C_6 - x_C_7
  - x_C_8 - x_C_9 = 0
 Binaries
-MinVol_1_A_Large_Gadget
-MinVol_1_B_Large_Gadget
-MinVol_1_C_Large_Gadget
 T_10_A
 T_10_B
 T_1_B
@@ -1522,12 +1391,12 @@
 T_8_B
 T_9_A
 T_9_B
-w_0_A_6
-w_0_A_7
-w_0_B_6
-w_0_B_7
-w_0_C_6
-w_0_C_7
+award_indicator_1_A_1
+award_indicator_1_B_1
+award_indicator_1_C_1
+w_0_A_1
+w_0_B_1
+w_0_C_1
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
works with 0, blanks, and deleted lines for supplier bid in price sheet upload
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>40000</v>
+        <v>70000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -555,13 +555,13 @@
         <v>52.8</v>
       </c>
       <c r="K2" t="n">
-        <v>21120</v>
+        <v>36960</v>
       </c>
       <c r="L2" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>18880</v>
+        <v>33040</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -569,71 +569,71 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>1478.4</v>
+        <v>2587.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Facility 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Facility 1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="F3" t="n">
-        <v>30000</v>
+        <v>1404000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>50</v>
+        <v>67.89999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>15000</v>
+        <v>611099.9999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>300</v>
+        <v>9000</v>
       </c>
       <c r="M3" t="n">
-        <v>15000</v>
+        <v>792900.0000000001</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>30555</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -642,57 +642,57 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Facility 1</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>156</v>
+        <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>1404000</v>
+        <v>253800</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>67.89999999999999</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>611099.9999999999</v>
+        <v>34560</v>
       </c>
       <c r="L4" t="n">
-        <v>9000</v>
+        <v>600</v>
       </c>
       <c r="M4" t="n">
-        <v>792900.0000000001</v>
+        <v>219240</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>30555</v>
+        <v>2419.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -710,10 +710,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F5" t="n">
-        <v>253800</v>
+        <v>2568510</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>57.59999999999999</v>
+        <v>23.04</v>
       </c>
       <c r="K5" t="n">
-        <v>34560</v>
+        <v>130636.8</v>
       </c>
       <c r="L5" t="n">
-        <v>600</v>
+        <v>5670</v>
       </c>
       <c r="M5" t="n">
-        <v>219240</v>
+        <v>2437873.2</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -746,12 +746,12 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>2419.2</v>
+        <v>9144.576000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,48 +769,48 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F6" t="n">
-        <v>2568510</v>
+        <v>15390</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>23.04</v>
+        <v>32.98</v>
       </c>
       <c r="K6" t="n">
-        <v>130636.8</v>
+        <v>1484.1</v>
       </c>
       <c r="L6" t="n">
-        <v>5670</v>
+        <v>45</v>
       </c>
       <c r="M6" t="n">
-        <v>2437873.2</v>
+        <v>13905.9</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>9144.576000000001</v>
+        <v>74.205</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,14 +828,14 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>342</v>
+        <v>653</v>
       </c>
       <c r="F7" t="n">
-        <v>15390</v>
+        <v>158026</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -843,33 +843,33 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>23.04</v>
+        <v>23.28</v>
       </c>
       <c r="K7" t="n">
-        <v>1036.8</v>
+        <v>5633.76</v>
       </c>
       <c r="L7" t="n">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="M7" t="n">
-        <v>14353.2</v>
+        <v>152392.24</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>72.57600000000001</v>
+        <v>281.688</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -887,48 +887,48 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>653</v>
+        <v>432</v>
       </c>
       <c r="F8" t="n">
-        <v>158026</v>
+        <v>286848</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>23.28</v>
+        <v>23</v>
       </c>
       <c r="K8" t="n">
-        <v>5633.76</v>
+        <v>15272</v>
       </c>
       <c r="L8" t="n">
-        <v>242</v>
+        <v>664</v>
       </c>
       <c r="M8" t="n">
-        <v>152392.24</v>
+        <v>271576</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>281.688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,48 +946,48 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="F9" t="n">
-        <v>286848</v>
+        <v>10944</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>22.08</v>
+        <v>12.61</v>
       </c>
       <c r="K9" t="n">
-        <v>14661.12</v>
+        <v>302.64</v>
       </c>
       <c r="L9" t="n">
-        <v>664</v>
+        <v>24</v>
       </c>
       <c r="M9" t="n">
-        <v>272186.88</v>
+        <v>10641.36</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>1026.2784</v>
+        <v>15.132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>456</v>
+        <v>234</v>
       </c>
       <c r="F10" t="n">
-        <v>10944</v>
+        <v>54288</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>12.61</v>
+        <v>54.32</v>
       </c>
       <c r="K10" t="n">
-        <v>302.64</v>
+        <v>12602.24</v>
       </c>
       <c r="L10" t="n">
-        <v>24</v>
+        <v>232</v>
       </c>
       <c r="M10" t="n">
-        <v>10641.36</v>
+        <v>41685.76</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1041,12 +1041,12 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>15.132</v>
+        <v>630.1120000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1064,14 +1064,14 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F11" t="n">
-        <v>54288</v>
+        <v>3003</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -1079,86 +1079,27 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>12.48</v>
+        <v>12.61</v>
       </c>
       <c r="K11" t="n">
-        <v>2895.36</v>
+        <v>163.93</v>
       </c>
       <c r="L11" t="n">
-        <v>232</v>
+        <v>13</v>
       </c>
       <c r="M11" t="n">
-        <v>51392.64</v>
+        <v>2839.07</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>202.6752</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>231</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>13</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J12" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K12" t="n">
-        <v>163.93</v>
-      </c>
-      <c r="L12" t="n">
-        <v>13</v>
-      </c>
-      <c r="M12" t="n">
-        <v>2839.07</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O12" t="n">
         <v>8.1965</v>
       </c>
     </row>
@@ -1233,7 +1174,7 @@
 BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 70 x_B_2 - 65 x_B_3 - 75 x_B_4
  - 34 x_B_5 - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
 BaseSpend_C: S0_C - 55 x_C_1 - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
- - 24 x_C_5 - 64 x_C_6 - 23 x_C_7 - 24 x_C_8 - 13 x_C_9 = 0
+ - 42 x_C_7 - 24 x_C_8 = 0
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
 Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000
@@ -1300,12 +1241,9 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
-MinVolAwarded_LB_1_A_1: - 300 award_indicator_1_A_1 + x_A_1 &gt;= 0
-MinVolAwarded_LB_1_B_1: - 300 award_indicator_1_B_1 + x_B_1 &gt;= 0
-MinVolAwarded_LB_1_C_1: - 300 award_indicator_1_C_1 + x_C_1 &gt;= 0
-MinVolAwarded_UB_1_A_1: - 700 award_indicator_1_A_1 + x_A_1 &lt;= 0
-MinVolAwarded_UB_1_B_1: - 700 award_indicator_1_B_1 + x_B_1 &lt;= 0
-MinVolAwarded_UB_1_C_1: - 700 award_indicator_1_C_1 + x_C_1 &lt;= 0
+NonBid_C_5: x_C_5 = 0
+NonBid_C_6: x_C_6 = 0
+NonBid_C_9: x_C_9 = 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
  &gt;= -19400000000
@@ -1337,13 +1275,6 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-SupplIndicatorLB_0_A_1: - w_0_A_1 + x_A_1 &gt;= 0
-SupplIndicatorLB_0_B_1: - w_0_B_1 + x_B_1 &gt;= 0
-SupplIndicatorLB_0_C_1: - w_0_C_1 + x_C_1 &gt;= 0
-SupplIndicator_0_A_1: - 1000000000 w_0_A_1 + x_A_1 &lt;= 0
-SupplIndicator_0_B_1: - 1000000000 w_0_B_1 + x_B_1 &lt;= 0
-SupplIndicator_0_C_1: - 1000000000 w_0_C_1 + x_C_1 &lt;= 0
-SupplierCount_0_1: w_0_A_1 + w_0_B_1 + w_0_C_1 = 2
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1391,12 +1322,6 @@
 T_8_B
 T_9_A
 T_9_B
-award_indicator_1_A_1
-award_indicator_1_B_1
-award_indicator_1_C_1
-w_0_A_1
-w_0_B_1
-w_0_C_1
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
changes to accept 0, blank, and no line bids
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>70000</v>
+        <v>68600</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -555,13 +555,13 @@
         <v>52.8</v>
       </c>
       <c r="K2" t="n">
-        <v>36960</v>
+        <v>36220.8</v>
       </c>
       <c r="L2" t="n">
-        <v>700</v>
+        <v>686</v>
       </c>
       <c r="M2" t="n">
-        <v>33040</v>
+        <v>32379.2</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -569,71 +569,71 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>2587.2</v>
+        <v>2535.456</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Facility 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Facility 1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="E3" t="n">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>1404000</v>
+        <v>1400</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>67.89999999999999</v>
+        <v>50</v>
       </c>
       <c r="K3" t="n">
-        <v>611099.9999999999</v>
+        <v>700</v>
       </c>
       <c r="L3" t="n">
-        <v>9000</v>
+        <v>14</v>
       </c>
       <c r="M3" t="n">
-        <v>792900.0000000001</v>
+        <v>700</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>30555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -642,57 +642,57 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>423</v>
+        <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>253800</v>
+        <v>1404000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>57.59999999999999</v>
+        <v>67.89999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>34560</v>
+        <v>611099.9999999999</v>
       </c>
       <c r="L4" t="n">
-        <v>600</v>
+        <v>9000</v>
       </c>
       <c r="M4" t="n">
-        <v>219240</v>
+        <v>792900.0000000001</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>2419.2</v>
+        <v>30555</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -710,10 +710,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>2568510</v>
+        <v>253800</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>23.04</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K5" t="n">
-        <v>130636.8</v>
+        <v>34560</v>
       </c>
       <c r="L5" t="n">
-        <v>5670</v>
+        <v>600</v>
       </c>
       <c r="M5" t="n">
-        <v>2437873.2</v>
+        <v>219240</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -746,12 +746,12 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>9144.576000000001</v>
+        <v>2419.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,48 +769,48 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>15390</v>
+        <v>2568510</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>32.98</v>
+        <v>23.04</v>
       </c>
       <c r="K6" t="n">
-        <v>1484.1</v>
+        <v>130636.8</v>
       </c>
       <c r="L6" t="n">
-        <v>45</v>
+        <v>5670</v>
       </c>
       <c r="M6" t="n">
-        <v>13905.9</v>
+        <v>2437873.2</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>74.205</v>
+        <v>9144.576000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>653</v>
+        <v>342</v>
       </c>
       <c r="F7" t="n">
-        <v>158026</v>
+        <v>15390</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -839,7 +839,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>23.28</v>
+        <v>32.98</v>
       </c>
       <c r="K7" t="n">
-        <v>5633.76</v>
+        <v>1484.1</v>
       </c>
       <c r="L7" t="n">
-        <v>242</v>
+        <v>45</v>
       </c>
       <c r="M7" t="n">
-        <v>152392.24</v>
+        <v>13905.9</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -864,12 +864,12 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>281.688</v>
+        <v>74.205</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -887,48 +887,48 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>432</v>
+        <v>653</v>
       </c>
       <c r="F8" t="n">
-        <v>286848</v>
+        <v>158026</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>23</v>
+        <v>23.28</v>
       </c>
       <c r="K8" t="n">
-        <v>15272</v>
+        <v>5633.76</v>
       </c>
       <c r="L8" t="n">
-        <v>664</v>
+        <v>242</v>
       </c>
       <c r="M8" t="n">
-        <v>271576</v>
+        <v>152392.24</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>281.688</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,48 +946,48 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F9" t="n">
-        <v>10944</v>
+        <v>286848</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>12.61</v>
+        <v>23</v>
       </c>
       <c r="K9" t="n">
-        <v>302.64</v>
+        <v>15272</v>
       </c>
       <c r="L9" t="n">
-        <v>24</v>
+        <v>664</v>
       </c>
       <c r="M9" t="n">
-        <v>10641.36</v>
+        <v>271576</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>15.132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>234</v>
+        <v>456</v>
       </c>
       <c r="F10" t="n">
-        <v>54288</v>
+        <v>10944</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>54.32</v>
+        <v>12.61</v>
       </c>
       <c r="K10" t="n">
-        <v>12602.24</v>
+        <v>302.64</v>
       </c>
       <c r="L10" t="n">
-        <v>232</v>
+        <v>24</v>
       </c>
       <c r="M10" t="n">
-        <v>41685.76</v>
+        <v>10641.36</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1041,65 +1041,124 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>630.1120000000001</v>
+        <v>15.132</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>234</v>
+      </c>
+      <c r="F11" t="n">
+        <v>54288</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>56</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>54.32</v>
+      </c>
+      <c r="K11" t="n">
+        <v>12602.24</v>
+      </c>
+      <c r="L11" t="n">
+        <v>232</v>
+      </c>
+      <c r="M11" t="n">
+        <v>41685.76</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>630.1120000000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Facility 10</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
         <v>231</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F12" t="n">
         <v>3003</v>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="H12" t="n">
         <v>13</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>3%</t>
         </is>
       </c>
-      <c r="J11" t="n">
+      <c r="J12" t="n">
         <v>12.61</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K12" t="n">
         <v>163.93</v>
       </c>
-      <c r="L11" t="n">
+      <c r="L12" t="n">
         <v>13</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M12" t="n">
         <v>2839.07</v>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>5%</t>
         </is>
       </c>
-      <c r="O11" t="n">
+      <c r="O12" t="n">
         <v>8.1965</v>
       </c>
     </row>
@@ -1275,6 +1334,7 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
+Rule_0_1: 0.98 x_A_1 - 0.02 x_B_1 - 0.02 x_C_1 &gt;= 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
working with PMDI test data
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,86 +524,86 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Facility 1</t>
+          <t>Alabama River Cellulose</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>175.31</v>
       </c>
       <c r="F2" t="n">
-        <v>68600</v>
+        <v>8414880</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>55</v>
+        <v>132.8</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>52.8</v>
+        <v>132.8</v>
       </c>
       <c r="K2" t="n">
-        <v>36220.8</v>
+        <v>6374400.000000001</v>
       </c>
       <c r="L2" t="n">
-        <v>686</v>
+        <v>48000</v>
       </c>
       <c r="M2" t="n">
-        <v>32379.2</v>
+        <v>2040479.999999999</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>2535.456</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Facility 1</t>
+          <t>Alabama River Cellulose</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Southern State</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>157.73</v>
       </c>
       <c r="F3" t="n">
-        <v>1400</v>
+        <v>630920</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>SATCO</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -611,16 +611,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>14</v>
+        <v>4000</v>
       </c>
       <c r="M3" t="n">
-        <v>700</v>
+        <v>630920</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -633,7 +633,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -642,57 +642,57 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Facility 1</t>
+          <t>Brewton Bleach Board</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>156</v>
+        <v>157.54</v>
       </c>
       <c r="F4" t="n">
-        <v>1404000</v>
+        <v>2678180</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>67.89999999999999</v>
+        <v>139</v>
       </c>
       <c r="K4" t="n">
-        <v>611099.9999999999</v>
+        <v>2363000</v>
       </c>
       <c r="L4" t="n">
-        <v>9000</v>
+        <v>17000</v>
       </c>
       <c r="M4" t="n">
-        <v>792900.0000000001</v>
+        <v>315180</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>30555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -701,57 +701,57 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Brewton Bleach Board</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Southern State</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>423</v>
+        <v>157.76</v>
       </c>
       <c r="F5" t="n">
-        <v>253800</v>
+        <v>1972000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Southern State</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>60</v>
+        <v>253.46</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>57.59999999999999</v>
+        <v>253.46</v>
       </c>
       <c r="K5" t="n">
-        <v>34560</v>
+        <v>3168250</v>
       </c>
       <c r="L5" t="n">
-        <v>600</v>
+        <v>12500</v>
       </c>
       <c r="M5" t="n">
-        <v>219240</v>
+        <v>-1196250</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>2419.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,57 +760,57 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Brunswick Cellulose</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>453</v>
+        <v>130.05</v>
       </c>
       <c r="F6" t="n">
-        <v>2568510</v>
+        <v>4551750</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>131.81</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>23.04</v>
+        <v>131.81</v>
       </c>
       <c r="K6" t="n">
-        <v>130636.8</v>
+        <v>4613350</v>
       </c>
       <c r="L6" t="n">
-        <v>5670</v>
+        <v>35000</v>
       </c>
       <c r="M6" t="n">
-        <v>2437873.2</v>
+        <v>-61600</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>9144.576000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,57 +819,57 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Cedar Springs Paper</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>342</v>
+        <v>173.57</v>
       </c>
       <c r="F7" t="n">
-        <v>15390</v>
+        <v>3679684</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>34</v>
+        <v>128.8</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>32.98</v>
+        <v>128.8</v>
       </c>
       <c r="K7" t="n">
-        <v>1484.1</v>
+        <v>2730560</v>
       </c>
       <c r="L7" t="n">
-        <v>45</v>
+        <v>21200</v>
       </c>
       <c r="M7" t="n">
-        <v>13905.9</v>
+        <v>949123.9999999995</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>74.205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -878,57 +878,57 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Crossett Paper</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>SATCO</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>653</v>
+        <v>440</v>
       </c>
       <c r="F8" t="n">
-        <v>158026</v>
+        <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>None</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>23.28</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>5633.76</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>242</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>152392.24</v>
+        <v>0</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>281.688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -937,27 +937,27 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Green Bay Broadway</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Chemtrade</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>432</v>
+        <v>230.13</v>
       </c>
       <c r="F9" t="n">
-        <v>286848</v>
+        <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>None</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>15272</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>664</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>271576</v>
+        <v>0</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,57 +996,57 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Leaf River Cellulose</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Chemtrade</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>456</v>
+        <v>151.79</v>
       </c>
       <c r="F10" t="n">
-        <v>10944</v>
+        <v>2884010</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>171.8</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>12.61</v>
+        <v>171.8</v>
       </c>
       <c r="K10" t="n">
-        <v>302.64</v>
+        <v>3264200</v>
       </c>
       <c r="L10" t="n">
-        <v>24</v>
+        <v>19000</v>
       </c>
       <c r="M10" t="n">
-        <v>10641.36</v>
+        <v>-380189.9999999995</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>15.132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1055,57 +1055,57 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Leaf River Cellulose</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>234</v>
+        <v>179.03</v>
       </c>
       <c r="F11" t="n">
-        <v>54288</v>
+        <v>1879815</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>56</v>
+        <v>175.8</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>54.32</v>
+        <v>175.8</v>
       </c>
       <c r="K11" t="n">
-        <v>12602.24</v>
+        <v>1845900</v>
       </c>
       <c r="L11" t="n">
-        <v>232</v>
+        <v>10500</v>
       </c>
       <c r="M11" t="n">
-        <v>41685.76</v>
+        <v>33914.99999999977</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>630.1120000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1114,52 +1114,760 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Memphis Cellulose</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Chemtrade</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>231</v>
+        <v>174.5</v>
       </c>
       <c r="F12" t="n">
-        <v>3003</v>
+        <v>1169150</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="H12" t="n">
+        <v>160.8</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>160.8</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1077360</v>
+      </c>
+      <c r="L12" t="n">
+        <v>6700</v>
+      </c>
+      <c r="M12" t="n">
+        <v>91790</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Memphis Cellulose</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>SATCO</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>173</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J12" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K12" t="n">
-        <v>163.93</v>
-      </c>
-      <c r="L12" t="n">
-        <v>13</v>
-      </c>
-      <c r="M12" t="n">
-        <v>2839.07</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O12" t="n">
-        <v>8.1965</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Monticello Paper</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Shrieve</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>165.6</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4371840</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Shrieve</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>132.8</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>132.8</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3505920</v>
+      </c>
+      <c r="L14" t="n">
+        <v>26400</v>
+      </c>
+      <c r="M14" t="n">
+        <v>865919.9999999995</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Monticello Paper</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>SATCO</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>147.01</v>
+      </c>
+      <c r="F15" t="n">
+        <v>338123</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Chemtrade</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>2300</v>
+      </c>
+      <c r="M15" t="n">
+        <v>338123</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Muskogee Tissue</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Chemtrade</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>757.65</v>
+      </c>
+      <c r="F16" t="n">
+        <v>500049</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>SATCO</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>660</v>
+      </c>
+      <c r="M16" t="n">
+        <v>500049</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Naheola Paper</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Shrieve</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>133.75</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3477500</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Shrieve</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>135.8</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>135.8</v>
+      </c>
+      <c r="K17" t="n">
+        <v>3530800</v>
+      </c>
+      <c r="L17" t="n">
+        <v>26000</v>
+      </c>
+      <c r="M17" t="n">
+        <v>-53300.00000000047</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Naheola Paper</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>156.09</v>
+      </c>
+      <c r="F18" t="n">
+        <v>312180</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Chemtrade</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>2000</v>
+      </c>
+      <c r="M18" t="n">
+        <v>312180</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Palatka Paper</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Shrieve</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>136.05</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1836675</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Shrieve</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>164.97</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>164.97</v>
+      </c>
+      <c r="K19" t="n">
+        <v>2227095</v>
+      </c>
+      <c r="L19" t="n">
+        <v>13500</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-390419.9999999998</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Port Hudson Paper</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>SATCO</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>175.17</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Savannah River Tissue</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>114.55</v>
+      </c>
+      <c r="F21" t="n">
+        <v>76748.5</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>SATCO</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>670</v>
+      </c>
+      <c r="M21" t="n">
+        <v>76748.5</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Toledo Paper</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Chemtrade</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>153.54</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1305090</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Chemtrade</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>8500</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1305090</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Wauna Tissue</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Chemtrade</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>146.77</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1056744</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Shrieve</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>7200</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1056744</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Foley(Perry) Cellulose</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Shrieve</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>201.05</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1809450</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>131.8</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>131.8</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1186200</v>
+      </c>
+      <c r="L24" t="n">
+        <v>9000</v>
+      </c>
+      <c r="M24" t="n">
+        <v>623250</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1899,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model is optimal.</t>
+          <t>Model is infeasible. Likely causes include:
+ - Insufficient supplier capacity relative to demand.
+ - Custom rule constraints conflicting with overall volume/demand.
+  Bid 1: demand = 48000, capacities: Supplier Shrieve (Bid ID capacity): 48000; Supplier Southern State (Bid ID capacity): 48000; 
+  Bid 2: demand = 4000, capacities: Supplier Southern State (Bid ID capacity): 4000; 
+  Bid 3: demand = 17000, capacities: Supplier Shrieve (Bid ID capacity): 17000; Supplier Southern State (Bid ID capacity): 17000; 
+  Bid 4: demand = 12500, capacities: Supplier Southern State (Bid ID capacity): 12500; 
+  Bid 5: demand = 35000, capacities: Supplier Shrieve (Bid ID capacity): 35000; Supplier Southern State (Bid ID capacity): 35000; 
+  Bid 6: demand = 21200, capacities: Supplier Shrieve (Bid ID capacity): 21200; Supplier SATCO (Bid ID capacity): 21200; Supplier Southern State (Bid ID capacity): 21200; 
+  Bid 7: demand = 350, capacities: 
+  Bid 8: demand = 480, capacities: Supplier Chemtrade (Bid ID capacity): 480; 
+  Bid 9: demand = 19000, capacities: Supplier Shrieve (Bid ID capacity): 19000; Supplier Chemtrade (Bid ID capacity): 19000; 
+  Bid 10: demand = 10500, capacities: Supplier Shrieve (Bid ID capacity): 10500; 
+  Bid 11: demand = 6700, capacities: Supplier Shrieve (Bid ID capacity): 6700; Supplier Chemtrade (Bid ID capacity): 6700; Supplier SATCO (Bid ID capacity): 6700; 
+  Bid 12: demand = 900, capacities: 
+  Bid 13: demand = 26400, capacities: Supplier Shrieve (Bid ID capacity): 26400; 
+  Bid 14: demand = 2300, capacities: 
+  Bid 15: demand = 660, capacities: Supplier Chemtrade (Bid ID capacity): 660; 
+  Bid 16: demand = 26000, capacities: Supplier Shrieve (Bid ID capacity): 26000; Supplier Southern State (Bid ID capacity): 26000; 
+  Bid 17: demand = 2000, capacities: Supplier Southern State (Bid ID capacity): 2000; 
+  Bid 18: demand = 13500, capacities: Supplier Shrieve (Bid ID capacity): 13500; Supplier SATCO (Bid ID capacity): 13500; 
+  Bid 19: demand = 300, capacities: 
+  Bid 20: demand = 670, capacities: Supplier Southern State (Bid ID capacity): 670; 
+  Bid 21: demand = 8500, capacities: 
+  Bid 22: demand = 7200, capacities: 
+  Bid 23: demand = 9000, capacities: Supplier Shrieve (Bid ID capacity): 9000; Supplier SATCO (Bid ID capacity): 9000; Supplier Southern State (Bid ID capacity): 9000; 
+Please review supplier capacities, demand, and custom rule constraints.</t>
         </is>
       </c>
     </row>
@@ -1226,174 +1960,351 @@
         <is>
           <t xml:space="preserve">\* Sourcing_with_MultiTier_Rebates_Discounts *\
 Minimize
-OBJ: S_A + S_B + S_C - rebate_A - rebate_B - rebate_C
+OBJ: S_Chemtrade + S_SATCO + S_Shrieve + S_Southern_State - rebate_Chemtrade
+ - rebate_SATCO - rebate_Shrieve - rebate_Southern_State
 Subject To
-BaseSpend_A: S0_A - 50 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
- - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
-BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 70 x_B_2 - 65 x_B_3 - 75 x_B_4
- - 34 x_B_5 - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
-BaseSpend_C: S0_C - 55 x_C_1 - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
- - 42 x_C_7 - 24 x_C_8 = 0
-Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
-Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
-Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000
-Capacity_B_Bid_ID_3: x_B_3 &lt;= 100000000
-Capacity_B_Bid_ID_4: x_B_4 &lt;= 100000000
-Capacity_B_Bid_ID_5: x_B_5 &lt;= 100000000
-Capacity_B_Bid_ID_6: x_B_6 &lt;= 100000000
-Capacity_B_Bid_ID_7: x_B_7 &lt;= 100000000
-Capacity_B_Bid_ID_8: x_B_8 &lt;= 100000000
-Capacity_B_Bid_ID_9: x_B_9 &lt;= 100000000
-Capacity_C_Bid_ID_1: x_C_1 &lt;= 100000000
-Capacity_C_Bid_ID_10: x_C_10 &lt;= 100000000
-Capacity_C_Bid_ID_2: x_C_2 &lt;= 100000000
-Capacity_C_Bid_ID_3: x_C_3 &lt;= 100000000
-Capacity_C_Bid_ID_4: x_C_4 &lt;= 100000000
-Capacity_C_Bid_ID_5: x_C_5 &lt;= 100000000
-Capacity_C_Bid_ID_6: x_C_6 &lt;= 100000000
-Capacity_C_Bid_ID_7: x_C_7 &lt;= 100000000
-Capacity_C_Bid_ID_8: x_C_8 &lt;= 100000000
-Capacity_C_Bid_ID_9: x_C_9 &lt;= 100000000
-Demand_1: x_A_1 + x_B_1 + x_C_1 = 700
-Demand_10: x_A_10 + x_B_10 + x_C_10 = 13
-Demand_2: x_A_2 + x_B_2 + x_C_2 = 9000
-Demand_3: x_A_3 + x_B_3 + x_C_3 = 600
-Demand_4: x_A_4 + x_B_4 + x_C_4 = 5670
-Demand_5: x_A_5 + x_B_5 + x_C_5 = 45
-Demand_6: x_A_6 + x_B_6 + x_C_6 = 242
-Demand_7: x_A_7 + x_B_7 + x_C_7 = 664
-Demand_8: x_A_8 + x_B_8 + x_C_8 = 24
-Demand_9: x_A_9 + x_B_9 + x_C_9 = 232
-DiscountTierLower_A_0: d_A - 19400000000 z_discount_A_0 &gt;= -19400000000
-DiscountTierLower_A_1: - 0.01 S0_A + d_A - 19400000000 z_discount_A_1
- &gt;= -19400000000
-DiscountTierLower_B_0: d_B - 97000000000 z_discount_B_0 &gt;= -97000000000
-DiscountTierLower_B_1: - 0.03 S0_B + d_B - 97000000000 z_discount_B_1
- &gt;= -97000000000
-DiscountTierLower_C_0: d_C - 97000000000 z_discount_C_0 &gt;= -97000000000
-DiscountTierLower_C_1: - 0.04 S0_C + d_C - 97000000000 z_discount_C_1
- &gt;= -97000000000
-DiscountTierMax_A_0: 19400000000 z_discount_A_0 &lt;= 19400001000
-DiscountTierMax_B_0: 97000000000 z_discount_B_0 &lt;= 97000000500
-DiscountTierMax_C_0: 97000000000 z_discount_C_0 &lt;= 97000000500
-_dummy: __dummy = 0
-DiscountTierMin_A_0: __dummy &gt;= 0
-DiscountTierMin_A_1: x_A_1 + x_A_10 + x_A_3 + x_A_4 + x_A_8 + x_A_9
- - 1000 z_discount_A_1 &gt;= 0
-DiscountTierMin_B_0: __dummy &gt;= 0
-DiscountTierMin_B_1: x_B_2 + x_B_5 + x_B_6 + x_B_7 - 500 z_discount_B_1 &gt;= 0
-DiscountTierMin_C_0: __dummy &gt;= 0
-DiscountTierMin_C_1: x_C_1 + x_C_10 + x_C_3 + x_C_4 + x_C_8 + x_C_9
- - 500 z_discount_C_1 &gt;= 0
-DiscountTierSelect_A: z_discount_A_0 + z_discount_A_1 = 1
-DiscountTierSelect_B: z_discount_B_0 + z_discount_B_1 = 1
-DiscountTierSelect_C: z_discount_C_0 + z_discount_C_1 = 1
-DiscountTierUpper_A_0: d_A + 19400000000 z_discount_A_0 &lt;= 19400000000
-DiscountTierUpper_A_1: - 0.01 S0_A + d_A + 19400000000 z_discount_A_1
- &lt;= 19400000000
-DiscountTierUpper_B_0: d_B + 97000000000 z_discount_B_0 &lt;= 97000000000
-DiscountTierUpper_B_1: - 0.03 S0_B + d_B + 97000000000 z_discount_B_1
- &lt;= 97000000000
-DiscountTierUpper_C_0: d_C + 97000000000 z_discount_C_0 &lt;= 97000000000
-DiscountTierUpper_C_1: - 0.04 S0_C + d_C + 97000000000 z_discount_C_1
- &lt;= 97000000000
-EffectiveSpend_A: - S0_A + S_A + d_A = 0
-EffectiveSpend_B: - S0_B + S_B + d_B = 0
-EffectiveSpend_C: - S0_C + S_C + d_C = 0
-NonBid_C_5: x_C_5 = 0
-NonBid_C_6: x_C_6 = 0
-NonBid_C_9: x_C_9 = 0
-RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
-RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
- &gt;= -19400000000
-RebateTierLower_B_0: rebate_B - 97000000000 y_rebate_B_0 &gt;= -97000000000
-RebateTierLower_B_1: - 0.05 S_B + rebate_B - 97000000000 y_rebate_B_1
- &gt;= -97000000000
-RebateTierLower_C_0: rebate_C - 97000000000 y_rebate_C_0 &gt;= -97000000000
-RebateTierLower_C_1: - 0.07 S_C + rebate_C - 97000000000 y_rebate_C_1
- &gt;= -97000000000
-RebateTierMax_A_0: 19400000000 y_rebate_A_0 &lt;= 19400000500
-RebateTierMax_B_0: 97000000000 y_rebate_B_0 &lt;= 97000000500
-RebateTierMax_C_0: 97000000000 y_rebate_C_0 &lt;= 97000000700
-RebateTierMin_A_0: __dummy &gt;= 0
-RebateTierMin_A_1: - 500 y_rebate_A_1 &gt;= 0
-RebateTierMin_B_0: __dummy &gt;= 0
-RebateTierMin_B_1: x_B_2 + x_B_5 + x_B_6 + x_B_7 - 500 y_rebate_B_1 &gt;= 0
-RebateTierMin_C_0: __dummy &gt;= 0
-RebateTierMin_C_1: x_C_1 + x_C_10 + x_C_3 + x_C_4 + x_C_8 + x_C_9
- - 700 y_rebate_C_1 &gt;= 0
-RebateTierSelect_A: y_rebate_A_0 + y_rebate_A_1 = 1
-RebateTierSelect_B: y_rebate_B_0 + y_rebate_B_1 = 1
-RebateTierSelect_C: y_rebate_C_0 + y_rebate_C_1 = 1
-RebateTierUpper_A_0: rebate_A + 19400000000 y_rebate_A_0 &lt;= 19400000000
-RebateTierUpper_A_1: - 0.1 S_A + rebate_A + 19400000000 y_rebate_A_1
- &lt;= 19400000000
-RebateTierUpper_B_0: rebate_B + 97000000000 y_rebate_B_0 &lt;= 97000000000
-RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 97000000000 y_rebate_B_1
- &lt;= 97000000000
-RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
-RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
- &lt;= 97000000000
-Rule_0_1: 0.98 x_A_1 - 0.02 x_B_1 - 0.02 x_C_1 &gt;= 0
-Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
-Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
-Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
-Transition_1_C: - 700 T_1_C + x_C_1 &lt;= 0
-Transition_2_A: - 9000 T_2_A + x_A_2 &lt;= 0
-Transition_2_C: - 9000 T_2_C + x_C_2 &lt;= 0
-Transition_3_A: - 600 T_3_A + x_A_3 &lt;= 0
-Transition_3_B: - 600 T_3_B + x_B_3 &lt;= 0
-Transition_4_A: - 5670 T_4_A + x_A_4 &lt;= 0
-Transition_4_B: - 5670 T_4_B + x_B_4 &lt;= 0
-Transition_5_A: - 45 T_5_A + x_A_5 &lt;= 0
-Transition_5_B: - 45 T_5_B + x_B_5 &lt;= 0
-Transition_6_A: - 242 T_6_A + x_A_6 &lt;= 0
-Transition_6_B: - 242 T_6_B + x_B_6 &lt;= 0
-Transition_7_A: - 664 T_7_A + x_A_7 &lt;= 0
-Transition_7_B: - 664 T_7_B + x_B_7 &lt;= 0
-Transition_8_A: - 24 T_8_A + x_A_8 &lt;= 0
-Transition_8_B: - 24 T_8_B + x_B_8 &lt;= 0
-Transition_9_A: - 232 T_9_A + x_A_9 &lt;= 0
-Transition_9_B: - 232 T_9_B + x_B_9 &lt;= 0
-Volume_A: V_A - x_A_1 - x_A_10 - x_A_2 - x_A_3 - x_A_4 - x_A_5 - x_A_6 - x_A_7
- - x_A_8 - x_A_9 = 0
-Volume_B: V_B - x_B_1 - x_B_10 - x_B_2 - x_B_3 - x_B_4 - x_B_5 - x_B_6 - x_B_7
- - x_B_8 - x_B_9 = 0
-Volume_C: V_C - x_C_1 - x_C_10 - x_C_2 - x_C_3 - x_C_4 - x_C_5 - x_C_6 - x_C_7
- - x_C_8 - x_C_9 = 0
+BaseSpend_Chemtrade: S0_Chemtrade - 196.8 x_Chemtrade_11
+ - 343.8 x_Chemtrade_15 - 306.8 x_Chemtrade_8 - 195.8 x_Chemtrade_9 = 0
+BaseSpend_SATCO: S0_SATCO - 217.8 x_SATCO_11 - 218.8 x_SATCO_18
+ - 159.8 x_SATCO_23 - 205.8 x_SATCO_6 = 0
+BaseSpend_Shrieve: S0_Shrieve - 132.8 x_Shrieve_1 - 175.8 x_Shrieve_10
+ - 160.8 x_Shrieve_11 - 132.8 x_Shrieve_13 - 135.8 x_Shrieve_16
+ - 164.97 x_Shrieve_18 - 184.3 x_Shrieve_23 - 139 x_Shrieve_3
+ - 131.81 x_Shrieve_5 - 128.8 x_Shrieve_6 - 171.8 x_Shrieve_9 = 0
+BaseSpend_Southern_State: S0_Southern_State - 188.38 x_Southern_State_1
+ - 190.88 x_Southern_State_16 - 253.46 x_Southern_State_17
+ - 253.46 x_Southern_State_2 - 150.46 x_Southern_State_20
+ - 131.8 x_Southern_State_23 - 187.12 x_Southern_State_3
+ - 253.46 x_Southern_State_4 - 139.84 x_Southern_State_5
+ - 160.49 x_Southern_State_6 = 0
+Capacity_Chemtrade_Bid_ID_11: x_Chemtrade_11 &lt;= 6700
+Capacity_Chemtrade_Bid_ID_15: x_Chemtrade_15 &lt;= 660
+Capacity_Chemtrade_Bid_ID_8: x_Chemtrade_8 &lt;= 480
+Capacity_Chemtrade_Bid_ID_9: x_Chemtrade_9 &lt;= 19000
+Capacity_SATCO_Bid_ID_11: x_SATCO_11 &lt;= 6700
+Capacity_SATCO_Bid_ID_18: x_SATCO_18 &lt;= 13500
+Capacity_SATCO_Bid_ID_23: x_SATCO_23 &lt;= 9000
+Capacity_SATCO_Bid_ID_6: x_SATCO_6 &lt;= 21200
+Capacity_Shrieve_Bid_ID_1: x_Shrieve_1 &lt;= 48000
+Capacity_Shrieve_Bid_ID_10: x_Shrieve_10 &lt;= 10500
+Capacity_Shrieve_Bid_ID_11: x_Shrieve_11 &lt;= 6700
+Capacity_Shrieve_Bid_ID_13: x_Shrieve_13 &lt;= 26400
+Capacity_Shrieve_Bid_ID_16: x_Shrieve_16 &lt;= 26000
+Capacity_Shrieve_Bid_ID_18: x_Shrieve_18 &lt;= 13500
+Capacity_Shrieve_Bid_ID_23: x_Shrieve_23 &lt;= 9000
+Capacity_Shrieve_Bid_ID_3: x_Shrieve_3 &lt;= 17000
+Capacity_Shrieve_Bid_ID_5: x_Shrieve_5 &lt;= 35000
+Capacity_Shrieve_Bid_ID_6: x_Shrieve_6 &lt;= 21200
+Capacity_Shrieve_Bid_ID_9: x_Shrieve_9 &lt;= 19000
+Capacity_Southern_State_Bid_ID_1: x_Southern_State_1 &lt;= 48000
+Capacity_Southern_State_Bid_ID_16: x_Southern_State_16 &lt;= 26000
+Capacity_Southern_State_Bid_ID_17: x_Southern_State_17 &lt;= 2000
+Capacity_Southern_State_Bid_ID_2: x_Southern_State_2 &lt;= 4000
+Capacity_Southern_State_Bid_ID_20: x_Southern_State_20 &lt;= 670
+Capacity_Southern_State_Bid_ID_23: x_Southern_State_23 &lt;= 9000
+Capacity_Southern_State_Bid_ID_3: x_Southern_State_3 &lt;= 17000
+Capacity_Southern_State_Bid_ID_4: x_Southern_State_4 &lt;= 12500
+Capacity_Southern_State_Bid_ID_5: x_Southern_State_5 &lt;= 35000
+Capacity_Southern_State_Bid_ID_6: x_Southern_State_6 &lt;= 21200
+Demand_1: x_Chemtrade_1 + x_SATCO_1 + x_Shrieve_1 + x_Southern_State_1 = 48000
+Demand_10: x_Chemtrade_10 + x_SATCO_10 + x_Shrieve_10 + x_Southern_State_10
+ = 10500
+Demand_11: x_Chemtrade_11 + x_SATCO_11 + x_Shrieve_11 + x_Southern_State_11
+ = 6700
+Demand_12: x_Chemtrade_12 + x_SATCO_12 + x_Shrieve_12 + x_Southern_State_12
+ = 900
+Demand_13: x_Chemtrade_13 + x_SATCO_13 + x_Shrieve_13 + x_Southern_State_13
+ = 26400
+Demand_14: x_Chemtrade_14 + x_SATCO_14 + x_Shrieve_14 + x_Southern_State_14
+ = 2300
+Demand_15: x_Chemtrade_15 + x_SATCO_15 + x_Shrieve_15 + x_Southern_State_15
+ = 660
+Demand_16: x_Chemtrade_16 + x_SATCO_16 + x_Shrieve_16 + x_Southern_State_16
+ = 26000
+Demand_17: x_Chemtrade_17 + x_SATCO_17 + x_Shrieve_17 + x_Southern_State_17
+ = 2000
+Demand_18: x_Chemtrade_18 + x_SATCO_18 + x_Shrieve_18 + x_Southern_State_18
+ = 13500
+Demand_19: x_Chemtrade_19 + x_SATCO_19 + x_Shrieve_19 + x_Southern_State_19
+ = 300
+Demand_2: x_Chemtrade_2 + x_SATCO_2 + x_Shrieve_2 + x_Southern_State_2 = 4000
+Demand_20: x_Chemtrade_20 + x_SATCO_20 + x_Shrieve_20 + x_Southern_State_20
+ = 670
+Demand_21: x_Chemtrade_21 + x_SATCO_21 + x_Shrieve_21 + x_Southern_State_21
+ = 8500
+Demand_22: x_Chemtrade_22 + x_SATCO_22 + x_Shrieve_22 + x_Southern_State_22
+ = 7200
+Demand_23: x_Chemtrade_23 + x_SATCO_23 + x_Shrieve_23 + x_Southern_State_23
+ = 9000
+Demand_3: x_Chemtrade_3 + x_SATCO_3 + x_Shrieve_3 + x_Southern_State_3 = 17000
+Demand_4: x_Chemtrade_4 + x_SATCO_4 + x_Shrieve_4 + x_Southern_State_4 = 12500
+Demand_5: x_Chemtrade_5 + x_SATCO_5 + x_Shrieve_5 + x_Southern_State_5 = 35000
+Demand_6: x_Chemtrade_6 + x_SATCO_6 + x_Shrieve_6 + x_Southern_State_6 = 21200
+Demand_7: x_Chemtrade_7 + x_SATCO_7 + x_Shrieve_7 + x_Southern_State_7 = 350
+Demand_8: x_Chemtrade_8 + x_SATCO_8 + x_Shrieve_8 + x_Southern_State_8 = 480
+Demand_9: x_Chemtrade_9 + x_SATCO_9 + x_Shrieve_9 + x_Southern_State_9 = 19000
+EffectiveSpend_Chemtrade: - S0_Chemtrade + S_Chemtrade + d_Chemtrade = 0
+EffectiveSpend_SATCO: - S0_SATCO + S_SATCO + d_SATCO = 0
+EffectiveSpend_Shrieve: - S0_Shrieve + S_Shrieve + d_Shrieve = 0
+EffectiveSpend_Southern_State: - S0_Southern_State + S_Southern_State
+ + d_Southern_State = 0
+Fix_d_Chemtrade: d_Chemtrade = 0
+Fix_d_SATCO: d_SATCO = 0
+Fix_d_Shrieve: d_Shrieve = 0
+Fix_d_Southern_State: d_Southern_State = 0
+Fix_rebate_Chemtrade: rebate_Chemtrade = 0
+Fix_rebate_SATCO: rebate_SATCO = 0
+Fix_rebate_Shrieve: rebate_Shrieve = 0
+Fix_rebate_Southern_State: rebate_Southern_State = 0
+NonBid_Chemtrade_1: x_Chemtrade_1 = 0
+NonBid_Chemtrade_10: x_Chemtrade_10 = 0
+NonBid_Chemtrade_12: x_Chemtrade_12 = 0
+NonBid_Chemtrade_13: x_Chemtrade_13 = 0
+NonBid_Chemtrade_14: x_Chemtrade_14 = 0
+NonBid_Chemtrade_16: x_Chemtrade_16 = 0
+NonBid_Chemtrade_17: x_Chemtrade_17 = 0
+NonBid_Chemtrade_18: x_Chemtrade_18 = 0
+NonBid_Chemtrade_19: x_Chemtrade_19 = 0
+NonBid_Chemtrade_2: x_Chemtrade_2 = 0
+NonBid_Chemtrade_20: x_Chemtrade_20 = 0
+NonBid_Chemtrade_21: x_Chemtrade_21 = 0
+NonBid_Chemtrade_22: x_Chemtrade_22 = 0
+NonBid_Chemtrade_23: x_Chemtrade_23 = 0
+NonBid_Chemtrade_3: x_Chemtrade_3 = 0
+NonBid_Chemtrade_4: x_Chemtrade_4 = 0
+NonBid_Chemtrade_5: x_Chemtrade_5 = 0
+NonBid_Chemtrade_6: x_Chemtrade_6 = 0
+NonBid_Chemtrade_7: x_Chemtrade_7 = 0
+NonBid_SATCO_1: x_SATCO_1 = 0
+NonBid_SATCO_10: x_SATCO_10 = 0
+NonBid_SATCO_12: x_SATCO_12 = 0
+NonBid_SATCO_13: x_SATCO_13 = 0
+NonBid_SATCO_14: x_SATCO_14 = 0
+NonBid_SATCO_15: x_SATCO_15 = 0
+NonBid_SATCO_16: x_SATCO_16 = 0
+NonBid_SATCO_17: x_SATCO_17 = 0
+NonBid_SATCO_19: x_SATCO_19 = 0
+NonBid_SATCO_2: x_SATCO_2 = 0
+NonBid_SATCO_20: x_SATCO_20 = 0
+NonBid_SATCO_21: x_SATCO_21 = 0
+NonBid_SATCO_22: x_SATCO_22 = 0
+NonBid_SATCO_3: x_SATCO_3 = 0
+NonBid_SATCO_4: x_SATCO_4 = 0
+NonBid_SATCO_5: x_SATCO_5 = 0
+NonBid_SATCO_7: x_SATCO_7 = 0
+NonBid_SATCO_8: x_SATCO_8 = 0
+NonBid_SATCO_9: x_SATCO_9 = 0
+NonBid_Shrieve_12: x_Shrieve_12 = 0
+NonBid_Shrieve_14: x_Shrieve_14 = 0
+NonBid_Shrieve_15: x_Shrieve_15 = 0
+NonBid_Shrieve_17: x_Shrieve_17 = 0
+NonBid_Shrieve_19: x_Shrieve_19 = 0
+NonBid_Shrieve_2: x_Shrieve_2 = 0
+NonBid_Shrieve_20: x_Shrieve_20 = 0
+NonBid_Shrieve_21: x_Shrieve_21 = 0
+NonBid_Shrieve_22: x_Shrieve_22 = 0
+NonBid_Shrieve_4: x_Shrieve_4 = 0
+NonBid_Shrieve_7: x_Shrieve_7 = 0
+NonBid_Shrieve_8: x_Shrieve_8 = 0
+NonBid_Southern_State_10: x_Southern_State_10 = 0
+NonBid_Southern_State_11: x_Southern_State_11 = 0
+NonBid_Southern_State_12: x_Southern_State_12 = 0
+NonBid_Southern_State_13: x_Southern_State_13 = 0
+NonBid_Southern_State_14: x_Southern_State_14 = 0
+NonBid_Southern_State_15: x_Southern_State_15 = 0
+NonBid_Southern_State_18: x_Southern_State_18 = 0
+NonBid_Southern_State_19: x_Southern_State_19 = 0
+NonBid_Southern_State_21: x_Southern_State_21 = 0
+NonBid_Southern_State_22: x_Southern_State_22 = 0
+NonBid_Southern_State_7: x_Southern_State_7 = 0
+NonBid_Southern_State_8: x_Southern_State_8 = 0
+NonBid_Southern_State_9: x_Southern_State_9 = 0
+Rule_0_1: - 0.5 x_Chemtrade_1 - 0.5 x_SATCO_1 + 0.5 x_Shrieve_1
+ - 0.5 x_Southern_State_1 &gt;= 0
+Transition_10_Chemtrade: - 10500 T_10_Chemtrade + x_Chemtrade_10 &lt;= 0
+Transition_10_SATCO: - 10500 T_10_SATCO + x_SATCO_10 &lt;= 0
+Transition_10_Southern_State: - 10500 T_10_Southern_State
+ + x_Southern_State_10 &lt;= 0
+Transition_11_SATCO: - 6700 T_11_SATCO + x_SATCO_11 &lt;= 0
+Transition_11_Shrieve: - 6700 T_11_Shrieve + x_Shrieve_11 &lt;= 0
+Transition_11_Southern_State: - 6700 T_11_Southern_State + x_Southern_State_11
+ &lt;= 0
+Transition_12_Chemtrade: - 900 T_12_Chemtrade + x_Chemtrade_12 &lt;= 0
+Transition_12_Shrieve: - 900 T_12_Shrieve + x_Shrieve_12 &lt;= 0
+Transition_12_Southern_State: - 900 T_12_Southern_State + x_Southern_State_12
+ &lt;= 0
+Transition_13_Chemtrade: - 26400 T_13_Chemtrade + x_Chemtrade_13 &lt;= 0
+Transition_13_SATCO: - 26400 T_13_SATCO + x_SATCO_13 &lt;= 0
+Transition_13_Southern_State: - 26400 T_13_Southern_State
+ + x_Southern_State_13 &lt;= 0
+Transition_14_Chemtrade: - 2300 T_14_Chemtrade + x_Chemtrade_14 &lt;= 0
+Transition_14_Shrieve: - 2300 T_14_Shrieve + x_Shrieve_14 &lt;= 0
+Transition_14_Southern_State: - 2300 T_14_Southern_State + x_Southern_State_14
+ &lt;= 0
+Transition_15_SATCO: - 660 T_15_SATCO + x_SATCO_15 &lt;= 0
+Transition_15_Shrieve: - 660 T_15_Shrieve + x_Shrieve_15 &lt;= 0
+Transition_15_Southern_State: - 660 T_15_Southern_State + x_Southern_State_15
+ &lt;= 0
+Transition_16_Chemtrade: - 26000 T_16_Chemtrade + x_Chemtrade_16 &lt;= 0
+Transition_16_SATCO: - 26000 T_16_SATCO + x_SATCO_16 &lt;= 0
+Transition_16_Southern_State: - 26000 T_16_Southern_State
+ + x_Southern_State_16 &lt;= 0
+Transition_17_Chemtrade: - 2000 T_17_Chemtrade + x_Chemtrade_17 &lt;= 0
+Transition_17_SATCO: - 2000 T_17_SATCO + x_SATCO_17 &lt;= 0
+Transition_17_Shrieve: - 2000 T_17_Shrieve + x_Shrieve_17 &lt;= 0
+Transition_18_Chemtrade: - 13500 T_18_Chemtrade + x_Chemtrade_18 &lt;= 0
+Transition_18_SATCO: - 13500 T_18_SATCO + x_SATCO_18 &lt;= 0
+Transition_18_Southern_State: - 13500 T_18_Southern_State
+ + x_Southern_State_18 &lt;= 0
+Transition_19_Chemtrade: - 300 T_19_Chemtrade + x_Chemtrade_19 &lt;= 0
+Transition_19_Shrieve: - 300 T_19_Shrieve + x_Shrieve_19 &lt;= 0
+Transition_19_Southern_State: - 300 T_19_Southern_State + x_Southern_State_19
+ &lt;= 0
+Transition_1_Chemtrade: - 48000 T_1_Chemtrade + x_Chemtrade_1 &lt;= 0
+Transition_1_SATCO: - 48000 T_1_SATCO + x_SATCO_1 &lt;= 0
+Transition_1_Southern_State: - 48000 T_1_Southern_State + x_Southern_State_1
+ &lt;= 0
+Transition_20_Chemtrade: - 670 T_20_Chemtrade + x_Chemtrade_20 &lt;= 0
+Transition_20_SATCO: - 670 T_20_SATCO + x_SATCO_20 &lt;= 0
+Transition_20_Shrieve: - 670 T_20_Shrieve + x_Shrieve_20 &lt;= 0
+Transition_21_SATCO: - 8500 T_21_SATCO + x_SATCO_21 &lt;= 0
+Transition_21_Shrieve: - 8500 T_21_Shrieve + x_Shrieve_21 &lt;= 0
+Transition_21_Southern_State: - 8500 T_21_Southern_State + x_Southern_State_21
+ &lt;= 0
+Transition_22_SATCO: - 7200 T_22_SATCO + x_SATCO_22 &lt;= 0
+Transition_22_Shrieve: - 7200 T_22_Shrieve + x_Shrieve_22 &lt;= 0
+Transition_22_Southern_State: - 7200 T_22_Southern_State + x_Southern_State_22
+ &lt;= 0
+Transition_23_Chemtrade: - 9000 T_23_Chemtrade + x_Chemtrade_23 &lt;= 0
+Transition_23_SATCO: - 9000 T_23_SATCO + x_SATCO_23 &lt;= 0
+Transition_23_Southern_State: - 9000 T_23_Southern_State + x_Southern_State_23
+ &lt;= 0
+Transition_2_Chemtrade: - 4000 T_2_Chemtrade + x_Chemtrade_2 &lt;= 0
+Transition_2_SATCO: - 4000 T_2_SATCO + x_SATCO_2 &lt;= 0
+Transition_2_Shrieve: - 4000 T_2_Shrieve + x_Shrieve_2 &lt;= 0
+Transition_3_Chemtrade: - 17000 T_3_Chemtrade + x_Chemtrade_3 &lt;= 0
+Transition_3_SATCO: - 17000 T_3_SATCO + x_SATCO_3 &lt;= 0
+Transition_3_Southern_State: - 17000 T_3_Southern_State + x_Southern_State_3
+ &lt;= 0
+Transition_4_Chemtrade: - 12500 T_4_Chemtrade + x_Chemtrade_4 &lt;= 0
+Transition_4_SATCO: - 12500 T_4_SATCO + x_SATCO_4 &lt;= 0
+Transition_4_Shrieve: - 12500 T_4_Shrieve + x_Shrieve_4 &lt;= 0
+Transition_5_Chemtrade: - 35000 T_5_Chemtrade + x_Chemtrade_5 &lt;= 0
+Transition_5_SATCO: - 35000 T_5_SATCO + x_SATCO_5 &lt;= 0
+Transition_5_Southern_State: - 35000 T_5_Southern_State + x_Southern_State_5
+ &lt;= 0
+Transition_6_Chemtrade: - 21200 T_6_Chemtrade + x_Chemtrade_6 &lt;= 0
+Transition_6_SATCO: - 21200 T_6_SATCO + x_SATCO_6 &lt;= 0
+Transition_6_Southern_State: - 21200 T_6_Southern_State + x_Southern_State_6
+ &lt;= 0
+Transition_7_Chemtrade: - 350 T_7_Chemtrade + x_Chemtrade_7 &lt;= 0
+Transition_7_Shrieve: - 350 T_7_Shrieve + x_Shrieve_7 &lt;= 0
+Transition_7_Southern_State: - 350 T_7_Southern_State + x_Southern_State_7
+ &lt;= 0
+Transition_8_SATCO: - 480 T_8_SATCO + x_SATCO_8 &lt;= 0
+Transition_8_Shrieve: - 480 T_8_Shrieve + x_Shrieve_8 &lt;= 0
+Transition_8_Southern_State: - 480 T_8_Southern_State + x_Southern_State_8
+ &lt;= 0
+Transition_9_SATCO: - 19000 T_9_SATCO + x_SATCO_9 &lt;= 0
+Transition_9_Shrieve: - 19000 T_9_Shrieve + x_Shrieve_9 &lt;= 0
+Transition_9_Southern_State: - 19000 T_9_Southern_State + x_Southern_State_9
+ &lt;= 0
+Volume_Chemtrade: V_Chemtrade - x_Chemtrade_1 - x_Chemtrade_10
+ - x_Chemtrade_11 - x_Chemtrade_12 - x_Chemtrade_13 - x_Chemtrade_14
+ - x_Chemtrade_15 - x_Chemtrade_16 - x_Chemtrade_17 - x_Chemtrade_18
+ - x_Chemtrade_19 - x_Chemtrade_2 - x_Chemtrade_20 - x_Chemtrade_21
+ - x_Chemtrade_22 - x_Chemtrade_23 - x_Chemtrade_3 - x_Chemtrade_4
+ - x_Chemtrade_5 - x_Chemtrade_6 - x_Chemtrade_7 - x_Chemtrade_8
+ - x_Chemtrade_9 = 0
+Volume_SATCO: V_SATCO - x_SATCO_1 - x_SATCO_10 - x_SATCO_11 - x_SATCO_12
+ - x_SATCO_13 - x_SATCO_14 - x_SATCO_15 - x_SATCO_16 - x_SATCO_17 - x_SATCO_18
+ - x_SATCO_19 - x_SATCO_2 - x_SATCO_20 - x_SATCO_21 - x_SATCO_22 - x_SATCO_23
+ - x_SATCO_3 - x_SATCO_4 - x_SATCO_5 - x_SATCO_6 - x_SATCO_7 - x_SATCO_8
+ - x_SATCO_9 = 0
+Volume_Shrieve: V_Shrieve - x_Shrieve_1 - x_Shrieve_10 - x_Shrieve_11
+ - x_Shrieve_12 - x_Shrieve_13 - x_Shrieve_14 - x_Shrieve_15 - x_Shrieve_16
+ - x_Shrieve_17 - x_Shrieve_18 - x_Shrieve_19 - x_Shrieve_2 - x_Shrieve_20
+ - x_Shrieve_21 - x_Shrieve_22 - x_Shrieve_23 - x_Shrieve_3 - x_Shrieve_4
+ - x_Shrieve_5 - x_Shrieve_6 - x_Shrieve_7 - x_Shrieve_8 - x_Shrieve_9 = 0
+Volume_Southern_State: V_Southern_State - x_Southern_State_1
+ - x_Southern_State_10 - x_Southern_State_11 - x_Southern_State_12
+ - x_Southern_State_13 - x_Southern_State_14 - x_Southern_State_15
+ - x_Southern_State_16 - x_Southern_State_17 - x_Southern_State_18
+ - x_Southern_State_19 - x_Southern_State_2 - x_Southern_State_20
+ - x_Southern_State_21 - x_Southern_State_22 - x_Southern_State_23
+ - x_Southern_State_3 - x_Southern_State_4 - x_Southern_State_5
+ - x_Southern_State_6 - x_Southern_State_7 - x_Southern_State_8
+ - x_Southern_State_9 = 0
 Binaries
-T_10_A
-T_10_B
-T_1_B
-T_1_C
-T_2_A
-T_2_C
-T_3_A
-T_3_B
-T_4_A
-T_4_B
-T_5_A
-T_5_B
-T_6_A
-T_6_B
-T_7_A
-T_7_B
-T_8_A
-T_8_B
-T_9_A
-T_9_B
-y_rebate_A_0
-y_rebate_A_1
-y_rebate_B_0
-y_rebate_B_1
-y_rebate_C_0
-y_rebate_C_1
-z_discount_A_0
-z_discount_A_1
-z_discount_B_0
-z_discount_B_1
-z_discount_C_0
-z_discount_C_1
+T_10_Chemtrade
+T_10_SATCO
+T_10_Southern_State
+T_11_SATCO
+T_11_Shrieve
+T_11_Southern_State
+T_12_Chemtrade
+T_12_Shrieve
+T_12_Southern_State
+T_13_Chemtrade
+T_13_SATCO
+T_13_Southern_State
+T_14_Chemtrade
+T_14_Shrieve
+T_14_Southern_State
+T_15_SATCO
+T_15_Shrieve
+T_15_Southern_State
+T_16_Chemtrade
+T_16_SATCO
+T_16_Southern_State
+T_17_Chemtrade
+T_17_SATCO
+T_17_Shrieve
+T_18_Chemtrade
+T_18_SATCO
+T_18_Southern_State
+T_19_Chemtrade
+T_19_Shrieve
+T_19_Southern_State
+T_1_Chemtrade
+T_1_SATCO
+T_1_Southern_State
+T_20_Chemtrade
+T_20_SATCO
+T_20_Shrieve
+T_21_SATCO
+T_21_Shrieve
+T_21_Southern_State
+T_22_SATCO
+T_22_Shrieve
+T_22_Southern_State
+T_23_Chemtrade
+T_23_SATCO
+T_23_Southern_State
+T_2_Chemtrade
+T_2_SATCO
+T_2_Shrieve
+T_3_Chemtrade
+T_3_SATCO
+T_3_Southern_State
+T_4_Chemtrade
+T_4_SATCO
+T_4_Shrieve
+T_5_Chemtrade
+T_5_SATCO
+T_5_Southern_State
+T_6_Chemtrade
+T_6_SATCO
+T_6_Southern_State
+T_7_Chemtrade
+T_7_Shrieve
+T_7_Southern_State
+T_8_SATCO
+T_8_Shrieve
+T_8_Southern_State
+T_9_SATCO
+T_9_Shrieve
+T_9_Southern_State
 End
 </t>
         </is>
@@ -1410,7 +2321,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1443,47 +2354,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BusinessUnit</t>
+          <t>Bid ID</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>100000000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BusinessUnit</t>
+          <t>Bid ID</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>100000000</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1493,17 +2404,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>100000000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1513,17 +2424,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>100000000</v>
+        <v>21200</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1533,17 +2444,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>100000000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1553,17 +2464,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>100000000</v>
+        <v>10500</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1573,17 +2484,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>100000000</v>
+        <v>6700</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1593,17 +2504,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>100000000</v>
+        <v>26400</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1613,17 +2524,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>16</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>100000000</v>
+        <v>26000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1633,17 +2544,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>100000000</v>
+        <v>13500</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Shrieve</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1653,17 +2564,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>100000000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Chemtrade</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1673,17 +2584,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>100000000</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Chemtrade</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1693,17 +2604,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>100000000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Chemtrade</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1713,17 +2624,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>100000000</v>
+        <v>6700</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Chemtrade</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1733,17 +2644,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>100000000</v>
+        <v>660</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>SATCO</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1753,17 +2664,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>100000000</v>
+        <v>21200</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>SATCO</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1773,17 +2684,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>100000000</v>
+        <v>6700</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>SATCO</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1793,17 +2704,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>100000000</v>
+        <v>13500</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>SATCO</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1813,17 +2724,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>100000000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Southern State</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1833,17 +2744,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>100000000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Southern State</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1853,17 +2764,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>100000000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Southern State</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1873,11 +2784,151 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>100000000</v>
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>21200</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Southern State</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>9000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code can now recognize no bid bids - transitions not working correctly
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,32 +536,32 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>49.5</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>34650</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>35350</v>
+        <v>0</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -654,49 +654,49 @@
         <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>126900</v>
+        <v>253800</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>54.45</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>16335</v>
+        <v>34560</v>
       </c>
       <c r="L4" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="M4" t="n">
-        <v>110565</v>
+        <v>219240</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>2419.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -710,10 +710,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F5" t="n">
-        <v>126900</v>
+        <v>2568510</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>57.59999999999999</v>
+        <v>23.04</v>
       </c>
       <c r="K5" t="n">
-        <v>17280</v>
+        <v>130636.8</v>
       </c>
       <c r="L5" t="n">
-        <v>300</v>
+        <v>5670</v>
       </c>
       <c r="M5" t="n">
-        <v>109620</v>
+        <v>2437873.2</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -746,12 +746,12 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>1209.6</v>
+        <v>9144.576000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,48 +769,48 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F6" t="n">
-        <v>2568510</v>
+        <v>15390</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>23.04</v>
+        <v>32.98</v>
       </c>
       <c r="K6" t="n">
-        <v>130636.8</v>
+        <v>1484.1</v>
       </c>
       <c r="L6" t="n">
-        <v>5670</v>
+        <v>45</v>
       </c>
       <c r="M6" t="n">
-        <v>2437873.2</v>
+        <v>13905.9</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>9144.576000000001</v>
+        <v>74.205</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>342</v>
+        <v>653</v>
       </c>
       <c r="F7" t="n">
-        <v>15390</v>
+        <v>158026</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -839,7 +839,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>32.98</v>
+        <v>23.28</v>
       </c>
       <c r="K7" t="n">
-        <v>1484.1</v>
+        <v>5633.76</v>
       </c>
       <c r="L7" t="n">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="M7" t="n">
-        <v>13905.9</v>
+        <v>152392.24</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -864,12 +864,12 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>74.205</v>
+        <v>281.688</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -887,48 +887,48 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>653</v>
+        <v>432</v>
       </c>
       <c r="F8" t="n">
-        <v>158026</v>
+        <v>286848</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>23.28</v>
+        <v>23</v>
       </c>
       <c r="K8" t="n">
-        <v>5633.76</v>
+        <v>15272</v>
       </c>
       <c r="L8" t="n">
-        <v>242</v>
+        <v>664</v>
       </c>
       <c r="M8" t="n">
-        <v>152392.24</v>
+        <v>271576</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>281.688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,48 +946,48 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="F9" t="n">
-        <v>286848</v>
+        <v>10944</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>22.77</v>
+        <v>12.61</v>
       </c>
       <c r="K9" t="n">
-        <v>15119.28</v>
+        <v>302.64</v>
       </c>
       <c r="L9" t="n">
-        <v>664</v>
+        <v>24</v>
       </c>
       <c r="M9" t="n">
-        <v>271728.72</v>
+        <v>10641.36</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>15.132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,48 +1005,48 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>456</v>
+        <v>234</v>
       </c>
       <c r="F10" t="n">
-        <v>10944</v>
+        <v>54288</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>12.61</v>
+        <v>30.72</v>
       </c>
       <c r="K10" t="n">
-        <v>302.64</v>
+        <v>7127.04</v>
       </c>
       <c r="L10" t="n">
-        <v>24</v>
+        <v>232</v>
       </c>
       <c r="M10" t="n">
-        <v>10641.36</v>
+        <v>47160.96</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>15.132</v>
+        <v>498.8928</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1064,10 +1064,10 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F11" t="n">
-        <v>54288</v>
+        <v>3003</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1083,16 +1083,16 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>54.32</v>
+        <v>12.61</v>
       </c>
       <c r="K11" t="n">
-        <v>12602.24</v>
+        <v>163.93</v>
       </c>
       <c r="L11" t="n">
-        <v>232</v>
+        <v>13</v>
       </c>
       <c r="M11" t="n">
-        <v>41685.76</v>
+        <v>2839.07</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1100,65 +1100,6 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>630.1120000000001</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>231</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>13</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J12" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K12" t="n">
-        <v>163.93</v>
-      </c>
-      <c r="L12" t="n">
-        <v>13</v>
-      </c>
-      <c r="M12" t="n">
-        <v>2839.07</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O12" t="n">
         <v>8.1965</v>
       </c>
     </row>
@@ -1191,7 +1132,8 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model is optimal.</t>
+          <t>Model is optimal.
+Note: The following Bid ID(s) were excluded because no supplier bids were found: 1.</t>
         </is>
       </c>
     </row>
@@ -1228,14 +1170,12 @@
 Minimize
 OBJ: S_A + S_B + S_C - rebate_A - rebate_B - rebate_C
 Subject To
-BaseSpend_A: S0_A - 50 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
- - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
-BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 70 x_B_2 - 65 x_B_3 - 75 x_B_4
- - 34 x_B_5 - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
-BaseSpend_C: S0_C - 55 x_C_1 - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
- - 42 x_C_7 - 24 x_C_8 = 0
-BidExclusion_0_1_B: x_B_1 = 0
-BidExclusion_0_1_C: x_C_1 = 0
+BaseSpend_A: S0_A - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4 - 54 x_A_5
+ - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
+BaseSpend_B: S0_B - 13 x_B_10 - 70 x_B_2 - 65 x_B_3 - 75 x_B_4 - 34 x_B_5
+ - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
+BaseSpend_C: S0_C - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4 - 44 x_C_6
+ - 42 x_C_7 - 24 x_C_8 - 32 x_C_9 = 0
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
 Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000
@@ -1256,7 +1196,7 @@
 Capacity_C_Bid_ID_7: x_C_7 &lt;= 100000000
 Capacity_C_Bid_ID_8: x_C_8 &lt;= 100000000
 Capacity_C_Bid_ID_9: x_C_9 &lt;= 100000000
-Demand_1: x_A_1 + x_B_1 + x_C_1 = 700
+Demand_1: x_A_1 + x_B_1 + x_C_1 = 0
 Demand_10: x_A_10 + x_B_10 + x_C_10 = 13
 Demand_2: x_A_2 + x_B_2 + x_C_2 = 9000
 Demand_3: x_A_3 + x_B_3 + x_C_3 = 600
@@ -1302,9 +1242,10 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
+NonBid_A_1: x_A_1 = 0
+NonBid_B_1: x_B_1 = 0
+NonBid_C_1: x_C_1 = 0
 NonBid_C_5: x_C_5 = 0
-NonBid_C_6: x_C_6 = 0
-NonBid_C_9: x_C_9 = 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
  &gt;= -19400000000
@@ -1338,8 +1279,8 @@
  &lt;= 97000000000
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
-Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
-Transition_1_C: - 700 T_1_C + x_C_1 &lt;= 0
+Transition_1_B: x_B_1 &lt;= 0
+Transition_1_C: x_C_1 &lt;= 0
 Transition_2_A: - 9000 T_2_A + x_A_2 &lt;= 0
 Transition_2_C: - 9000 T_2_C + x_C_2 &lt;= 0
 Transition_3_A: - 600 T_3_A + x_A_3 &lt;= 0
@@ -1365,8 +1306,6 @@
 Binaries
 T_10_A
 T_10_B
-T_1_B
-T_1_C
 T_2_A
 T_2_C
 T_3_A

</xml_diff>

<commit_message>
code can now recognize no bids - transitions not working correctly
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -1277,26 +1277,26 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
-Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
-Transition_1_B: x_B_1 &lt;= 0
-Transition_1_C: x_C_1 &lt;= 0
-Transition_2_A: - 9000 T_2_A + x_A_2 &lt;= 0
-Transition_2_C: - 9000 T_2_C + x_C_2 &lt;= 0
-Transition_3_A: - 600 T_3_A + x_A_3 &lt;= 0
-Transition_3_B: - 600 T_3_B + x_B_3 &lt;= 0
-Transition_4_A: - 5670 T_4_A + x_A_4 &lt;= 0
-Transition_4_B: - 5670 T_4_B + x_B_4 &lt;= 0
-Transition_5_A: - 45 T_5_A + x_A_5 &lt;= 0
-Transition_5_B: - 45 T_5_B + x_B_5 &lt;= 0
-Transition_6_A: - 242 T_6_A + x_A_6 &lt;= 0
-Transition_6_B: - 242 T_6_B + x_B_6 &lt;= 0
-Transition_7_A: - 664 T_7_A + x_A_7 &lt;= 0
-Transition_7_B: - 664 T_7_B + x_B_7 &lt;= 0
-Transition_8_A: - 24 T_8_A + x_A_8 &lt;= 0
-Transition_8_B: - 24 T_8_B + x_B_8 &lt;= 0
-Transition_9_A: - 232 T_9_A + x_A_9 &lt;= 0
-Transition_9_B: - 232 T_9_B + x_B_9 &lt;= 0
+Transition_lb_1: - 0.001 T_bid_1 + x_B_1 + x_C_1 &gt;= 0
+Transition_lb_10: - 0.001 T_bid_10 + x_A_10 + x_B_10 &gt;= 0
+Transition_lb_2: - 0.001 T_bid_2 + x_A_2 + x_C_2 &gt;= 0
+Transition_lb_3: - 0.001 T_bid_3 + x_A_3 + x_B_3 &gt;= 0
+Transition_lb_4: - 0.001 T_bid_4 + x_A_4 + x_B_4 &gt;= 0
+Transition_lb_5: - 0.001 T_bid_5 + x_A_5 + x_B_5 &gt;= 0
+Transition_lb_6: - 0.001 T_bid_6 + x_A_6 + x_B_6 &gt;= 0
+Transition_lb_7: - 0.001 T_bid_7 + x_A_7 + x_B_7 &gt;= 0
+Transition_lb_8: - 0.001 T_bid_8 + x_A_8 + x_B_8 &gt;= 0
+Transition_lb_9: - 0.001 T_bid_9 + x_A_9 + x_B_9 &gt;= 0
+Transition_ub_1: x_B_1 + x_C_1 &lt;= 0
+Transition_ub_10: - 13 T_bid_10 + x_A_10 + x_B_10 &lt;= 0
+Transition_ub_2: - 9000 T_bid_2 + x_A_2 + x_C_2 &lt;= 0
+Transition_ub_3: - 600 T_bid_3 + x_A_3 + x_B_3 &lt;= 0
+Transition_ub_4: - 5670 T_bid_4 + x_A_4 + x_B_4 &lt;= 0
+Transition_ub_5: - 45 T_bid_5 + x_A_5 + x_B_5 &lt;= 0
+Transition_ub_6: - 242 T_bid_6 + x_A_6 + x_B_6 &lt;= 0
+Transition_ub_7: - 664 T_bid_7 + x_A_7 + x_B_7 &lt;= 0
+Transition_ub_8: - 24 T_bid_8 + x_A_8 + x_B_8 &lt;= 0
+Transition_ub_9: - 232 T_bid_9 + x_A_9 + x_B_9 &lt;= 0
 Volume_A: V_A - x_A_1 - x_A_10 - x_A_2 - x_A_3 - x_A_4 - x_A_5 - x_A_6 - x_A_7
  - x_A_8 - x_A_9 = 0
 Volume_B: V_B - x_B_1 - x_B_10 - x_B_2 - x_B_3 - x_B_4 - x_B_5 - x_B_6 - x_B_7
@@ -1304,24 +1304,16 @@
 Volume_C: V_C - x_C_1 - x_C_10 - x_C_2 - x_C_3 - x_C_4 - x_C_5 - x_C_6 - x_C_7
  - x_C_8 - x_C_9 = 0
 Binaries
-T_10_A
-T_10_B
-T_2_A
-T_2_C
-T_3_A
-T_3_B
-T_4_A
-T_4_B
-T_5_A
-T_5_B
-T_6_A
-T_6_B
-T_7_A
-T_7_B
-T_8_A
-T_8_B
-T_9_A
-T_9_B
+T_bid_1
+T_bid_10
+T_bid_2
+T_bid_3
+T_bid_4
+T_bid_5
+T_bid_6
+T_bid_7
+T_bid_8
+T_bid_9
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
code can not recognize no bids - transitions still not working
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -1277,26 +1277,26 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-Transition_lb_1: - 0.001 T_bid_1 + x_B_1 + x_C_1 &gt;= 0
-Transition_lb_10: - 0.001 T_bid_10 + x_A_10 + x_B_10 &gt;= 0
-Transition_lb_2: - 0.001 T_bid_2 + x_A_2 + x_C_2 &gt;= 0
-Transition_lb_3: - 0.001 T_bid_3 + x_A_3 + x_B_3 &gt;= 0
-Transition_lb_4: - 0.001 T_bid_4 + x_A_4 + x_B_4 &gt;= 0
-Transition_lb_5: - 0.001 T_bid_5 + x_A_5 + x_B_5 &gt;= 0
-Transition_lb_6: - 0.001 T_bid_6 + x_A_6 + x_B_6 &gt;= 0
-Transition_lb_7: - 0.001 T_bid_7 + x_A_7 + x_B_7 &gt;= 0
-Transition_lb_8: - 0.001 T_bid_8 + x_A_8 + x_B_8 &gt;= 0
-Transition_lb_9: - 0.001 T_bid_9 + x_A_9 + x_B_9 &gt;= 0
-Transition_ub_1: x_B_1 + x_C_1 &lt;= 0
-Transition_ub_10: - 13 T_bid_10 + x_A_10 + x_B_10 &lt;= 0
-Transition_ub_2: - 9000 T_bid_2 + x_A_2 + x_C_2 &lt;= 0
-Transition_ub_3: - 600 T_bid_3 + x_A_3 + x_B_3 &lt;= 0
-Transition_ub_4: - 5670 T_bid_4 + x_A_4 + x_B_4 &lt;= 0
-Transition_ub_5: - 45 T_bid_5 + x_A_5 + x_B_5 &lt;= 0
-Transition_ub_6: - 242 T_bid_6 + x_A_6 + x_B_6 &lt;= 0
-Transition_ub_7: - 664 T_bid_7 + x_A_7 + x_B_7 &lt;= 0
-Transition_ub_8: - 24 T_bid_8 + x_A_8 + x_B_8 &lt;= 0
-Transition_ub_9: - 232 T_bid_9 + x_A_9 + x_B_9 &lt;= 0
+Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
+Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
+Transition_1_B: x_B_1 &lt;= 0
+Transition_1_C: x_C_1 &lt;= 0
+Transition_2_A: - 9000 T_2_A + x_A_2 &lt;= 0
+Transition_2_C: - 9000 T_2_C + x_C_2 &lt;= 0
+Transition_3_A: - 600 T_3_A + x_A_3 &lt;= 0
+Transition_3_B: - 600 T_3_B + x_B_3 &lt;= 0
+Transition_4_A: - 5670 T_4_A + x_A_4 &lt;= 0
+Transition_4_B: - 5670 T_4_B + x_B_4 &lt;= 0
+Transition_5_A: - 45 T_5_A + x_A_5 &lt;= 0
+Transition_5_B: - 45 T_5_B + x_B_5 &lt;= 0
+Transition_6_A: - 242 T_6_A + x_A_6 &lt;= 0
+Transition_6_B: - 242 T_6_B + x_B_6 &lt;= 0
+Transition_7_A: - 664 T_7_A + x_A_7 &lt;= 0
+Transition_7_B: - 664 T_7_B + x_B_7 &lt;= 0
+Transition_8_A: - 24 T_8_A + x_A_8 &lt;= 0
+Transition_8_B: - 24 T_8_B + x_B_8 &lt;= 0
+Transition_9_A: - 232 T_9_A + x_A_9 &lt;= 0
+Transition_9_B: - 232 T_9_B + x_B_9 &lt;= 0
 Volume_A: V_A - x_A_1 - x_A_10 - x_A_2 - x_A_3 - x_A_4 - x_A_5 - x_A_6 - x_A_7
  - x_A_8 - x_A_9 = 0
 Volume_B: V_B - x_B_1 - x_B_10 - x_B_2 - x_B_3 - x_B_4 - x_B_5 - x_B_6 - x_B_7
@@ -1304,16 +1304,24 @@
 Volume_C: V_C - x_C_1 - x_C_10 - x_C_2 - x_C_3 - x_C_4 - x_C_5 - x_C_6 - x_C_7
  - x_C_8 - x_C_9 = 0
 Binaries
-T_bid_1
-T_bid_10
-T_bid_2
-T_bid_3
-T_bid_4
-T_bid_5
-T_bid_6
-T_bid_7
-T_bid_8
-T_bid_9
+T_10_A
+T_10_B
+T_2_A
+T_2_C
+T_3_A
+T_3_B
+T_4_A
+T_4_B
+T_5_A
+T_5_B
+T_6_A
+T_6_B
+T_7_A
+T_7_B
+T_8_A
+T_8_B
+T_9_A
+T_9_B
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
transitions is now working correctly
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -1071,36 +1071,36 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>12.61</v>
+        <v>14.4</v>
       </c>
       <c r="K11" t="n">
-        <v>163.93</v>
+        <v>187.2</v>
       </c>
       <c r="L11" t="n">
         <v>13</v>
       </c>
       <c r="M11" t="n">
-        <v>2839.07</v>
+        <v>2815.8</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>8.1965</v>
+        <v>13.104</v>
       </c>
     </row>
   </sheetData>
@@ -1277,6 +1277,9 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
+Rule_0: T_10_A + T_10_B + T_1_B + T_1_C + T_2_A + T_2_C + T_3_A + T_3_B
+ + T_4_A + T_4_B + T_5_A + T_5_B + T_6_A + T_6_B + T_7_A + T_7_B + T_8_A
+ + T_8_B + T_9_A + T_9_B = 4
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: x_B_1 &lt;= 0
@@ -1306,6 +1309,8 @@
 Binaries
 T_10_A
 T_10_B
+T_1_B
+T_1_C
 T_2_A
 T_2_C
 T_3_A

</xml_diff>

<commit_message>
finalized ALL option changes in supplier scope for exclude bids
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>45000</v>
+        <v>70000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -548,20 +548,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.5252</v>
+        <v>0.519948</v>
       </c>
       <c r="K2" t="n">
-        <v>236.34</v>
+        <v>363.9636</v>
       </c>
       <c r="L2" t="n">
-        <v>450</v>
+        <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>44763.66</v>
+        <v>69636.0364</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -574,66 +574,66 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Facility 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Facility 1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="F3" t="n">
-        <v>25000</v>
+        <v>1404000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>9.699999999999999</v>
+        <v>69.3</v>
       </c>
       <c r="K3" t="n">
-        <v>2425</v>
+        <v>623700</v>
       </c>
       <c r="L3" t="n">
-        <v>250</v>
+        <v>9000</v>
       </c>
       <c r="M3" t="n">
-        <v>22575</v>
+        <v>780300</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>121.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -642,57 +642,57 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Facility 1</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>156</v>
+        <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>1404000</v>
+        <v>253800</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>67.89999999999999</v>
+        <v>54.45</v>
       </c>
       <c r="K4" t="n">
-        <v>611099.9999999999</v>
+        <v>32670</v>
       </c>
       <c r="L4" t="n">
-        <v>9000</v>
+        <v>600</v>
       </c>
       <c r="M4" t="n">
-        <v>792900.0000000001</v>
+        <v>221130</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>30555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -710,48 +710,48 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F5" t="n">
-        <v>253800</v>
+        <v>2568510</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>57.59999999999999</v>
+        <v>22.77</v>
       </c>
       <c r="K5" t="n">
-        <v>34560</v>
+        <v>129105.9</v>
       </c>
       <c r="L5" t="n">
-        <v>600</v>
+        <v>5670</v>
       </c>
       <c r="M5" t="n">
-        <v>219240</v>
+        <v>2439404.1</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>2419.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,48 +769,48 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F6" t="n">
-        <v>2568510</v>
+        <v>15390</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>23.04</v>
+        <v>53.46</v>
       </c>
       <c r="K6" t="n">
-        <v>130636.8</v>
+        <v>2405.7</v>
       </c>
       <c r="L6" t="n">
-        <v>5670</v>
+        <v>45</v>
       </c>
       <c r="M6" t="n">
-        <v>2437873.2</v>
+        <v>12984.3</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>9144.576000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,48 +828,48 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>342</v>
+        <v>653</v>
       </c>
       <c r="F7" t="n">
-        <v>15390</v>
+        <v>158026</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>32.98</v>
+        <v>41.58</v>
       </c>
       <c r="K7" t="n">
-        <v>1484.1</v>
+        <v>10062.36</v>
       </c>
       <c r="L7" t="n">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="M7" t="n">
-        <v>13905.9</v>
+        <v>147963.64</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>74.205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -887,48 +887,48 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>653</v>
+        <v>432</v>
       </c>
       <c r="F8" t="n">
-        <v>158026</v>
+        <v>286848</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>23.28</v>
+        <v>22.77</v>
       </c>
       <c r="K8" t="n">
-        <v>5633.76</v>
+        <v>15119.28</v>
       </c>
       <c r="L8" t="n">
-        <v>242</v>
+        <v>664</v>
       </c>
       <c r="M8" t="n">
-        <v>152392.24</v>
+        <v>271728.72</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>281.688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="F9" t="n">
-        <v>286848</v>
+        <v>10944</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -957,24 +957,24 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>23</v>
+        <v>74.25</v>
       </c>
       <c r="K9" t="n">
-        <v>15272</v>
+        <v>1782</v>
       </c>
       <c r="L9" t="n">
-        <v>664</v>
+        <v>24</v>
       </c>
       <c r="M9" t="n">
-        <v>271576</v>
+        <v>9162</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,48 +1005,48 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>456</v>
+        <v>234</v>
       </c>
       <c r="F10" t="n">
-        <v>10944</v>
+        <v>54288</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>12.61</v>
+        <v>96.03</v>
       </c>
       <c r="K10" t="n">
-        <v>302.64</v>
+        <v>22278.96</v>
       </c>
       <c r="L10" t="n">
-        <v>24</v>
+        <v>232</v>
       </c>
       <c r="M10" t="n">
-        <v>10641.36</v>
+        <v>32009.04</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>15.132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1064,102 +1064,43 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F11" t="n">
-        <v>54288</v>
+        <v>3003</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>30.72</v>
+        <v>63.36</v>
       </c>
       <c r="K11" t="n">
-        <v>7127.04</v>
+        <v>823.6799999999999</v>
       </c>
       <c r="L11" t="n">
-        <v>232</v>
+        <v>13</v>
       </c>
       <c r="M11" t="n">
-        <v>47160.96</v>
+        <v>2179.32</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>498.8928</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>231</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>13</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J12" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K12" t="n">
-        <v>163.93</v>
-      </c>
-      <c r="L12" t="n">
-        <v>13</v>
-      </c>
-      <c r="M12" t="n">
-        <v>2839.07</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O12" t="n">
-        <v>8.1965</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1234,6 +1175,24 @@
  - 34 x_B_5 - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
 BaseSpend_C: S0_C - 24 x_C_1 - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
  - 44 x_C_6 - 42 x_C_7 - 24 x_C_8 - 32 x_C_9 = 0
+BidExclusion_0_10_B: x_B_10 = 0
+BidExclusion_0_10_C: x_C_10 = 0
+BidExclusion_0_2_B: x_B_2 = 0
+BidExclusion_0_2_C: x_C_2 = 0
+BidExclusion_0_3_B: x_B_3 = 0
+BidExclusion_0_3_C: x_C_3 = 0
+BidExclusion_0_4_B: x_B_4 = 0
+BidExclusion_0_4_C: x_C_4 = 0
+BidExclusion_0_5_B: x_B_5 = 0
+BidExclusion_0_5_C: x_C_5 = 0
+BidExclusion_0_6_B: x_B_6 = 0
+BidExclusion_0_6_C: x_C_6 = 0
+BidExclusion_0_7_B: x_B_7 = 0
+BidExclusion_0_7_C: x_C_7 = 0
+BidExclusion_0_8_B: x_B_8 = 0
+BidExclusion_0_8_C: x_C_8 = 0
+BidExclusion_0_9_B: x_B_9 = 0
+BidExclusion_0_9_C: x_C_9 = 0
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
 Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000
@@ -1300,7 +1259,6 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
-MinVolAwarded_0_Second_Lowest_Cost_Supplier_1_Exact: x_B_1 = 250
 NonBid_C_5: x_C_5 = 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1

</xml_diff>

<commit_message>
added feasibility notes and corrected an issue with apply to all in exclude bids
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -536,32 +536,32 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.5252</v>
+        <v>0</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.519948</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>363.9636</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>69636.0364</v>
+        <v>0</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -607,20 +607,20 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>69.3</v>
+        <v>70</v>
       </c>
       <c r="K3" t="n">
-        <v>623700</v>
+        <v>630000</v>
       </c>
       <c r="L3" t="n">
         <v>9000</v>
       </c>
       <c r="M3" t="n">
-        <v>780300</v>
+        <v>774000</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -654,32 +654,32 @@
         <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>253800</v>
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>54.45</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>32670</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>221130</v>
+        <v>0</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -713,32 +713,32 @@
         <v>453</v>
       </c>
       <c r="F5" t="n">
-        <v>2568510</v>
+        <v>0</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>22.77</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>129105.9</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>5670</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>2439404.1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -772,32 +772,32 @@
         <v>342</v>
       </c>
       <c r="F6" t="n">
-        <v>15390</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>53.46</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>2405.7</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>12984.3</v>
+        <v>0</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -831,32 +831,32 @@
         <v>653</v>
       </c>
       <c r="F7" t="n">
-        <v>158026</v>
+        <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>41.58</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>10062.36</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>242</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>147963.64</v>
+        <v>0</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -890,32 +890,32 @@
         <v>432</v>
       </c>
       <c r="F8" t="n">
-        <v>286848</v>
+        <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>22.77</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>15119.28</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>664</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>271728.72</v>
+        <v>0</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -949,32 +949,32 @@
         <v>456</v>
       </c>
       <c r="F9" t="n">
-        <v>10944</v>
+        <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>74.25</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>1782</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>9162</v>
+        <v>0</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1008,32 +1008,32 @@
         <v>234</v>
       </c>
       <c r="F10" t="n">
-        <v>54288</v>
+        <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>96.03</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>22278.96</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>232</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>32009.04</v>
+        <v>0</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1067,32 +1067,32 @@
         <v>231</v>
       </c>
       <c r="F11" t="n">
-        <v>3003</v>
+        <v>0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>63.36</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>823.6799999999999</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>2179.32</v>
+        <v>0</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1132,7 +1132,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model is optimal.</t>
+          <t>Model is infeasible. Likely causes include:
+ - Insufficient supplier capacity relative to demand.
+ - Custom rule constraints conflicting with overall volume/demand.
+Detailed Rule Evaluations:
+Rule 1 ('Exclude Bids'): The exclusion criteria might be too broad, removing all valid bids needed to satisfy demand for a Bid ID or grouping.
+Please review supplier capacities, demand figures, and custom rule constraints for adjustments.</t>
         </is>
       </c>
     </row>
@@ -1175,24 +1180,9 @@
  - 34 x_B_5 - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
 BaseSpend_C: S0_C - 24 x_C_1 - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
  - 44 x_C_6 - 42 x_C_7 - 24 x_C_8 - 32 x_C_9 = 0
-BidExclusion_0_10_B: x_B_10 = 0
-BidExclusion_0_10_C: x_C_10 = 0
+BidExclusion_0_2_A: x_A_2 = 0
 BidExclusion_0_2_B: x_B_2 = 0
 BidExclusion_0_2_C: x_C_2 = 0
-BidExclusion_0_3_B: x_B_3 = 0
-BidExclusion_0_3_C: x_C_3 = 0
-BidExclusion_0_4_B: x_B_4 = 0
-BidExclusion_0_4_C: x_C_4 = 0
-BidExclusion_0_5_B: x_B_5 = 0
-BidExclusion_0_5_C: x_C_5 = 0
-BidExclusion_0_6_B: x_B_6 = 0
-BidExclusion_0_6_C: x_C_6 = 0
-BidExclusion_0_7_B: x_B_7 = 0
-BidExclusion_0_7_C: x_C_7 = 0
-BidExclusion_0_8_B: x_B_8 = 0
-BidExclusion_0_8_C: x_C_8 = 0
-BidExclusion_0_9_B: x_B_9 = 0
-BidExclusion_0_9_C: x_C_9 = 0
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
 Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000

</xml_diff>

<commit_message>
created advanced feasibility notes with more specific guidelines
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,15 +536,15 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.5252</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -552,16 +552,16 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>0.5252</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>367.64</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>69632.36</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -599,7 +599,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -654,15 +654,15 @@
         <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>219537</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>33735</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>519</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>185802</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -692,11 +692,11 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -710,18 +710,18 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>34263</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>4860</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>29403</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -751,7 +751,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,18 +769,18 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>2568510</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -788,16 +788,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>130410</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>5670</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>2438100</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -810,7 +810,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,18 +828,18 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>653</v>
+        <v>342</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>15390</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>1530</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>13860</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -869,7 +869,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -887,18 +887,18 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>432</v>
+        <v>653</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>158026</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -906,16 +906,16 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>5808</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>152218</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,18 +946,18 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>286848</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>15272</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>664</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>271576</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,18 +1005,18 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>234</v>
+        <v>456</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>10944</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>576</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>10368</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1046,60 +1046,119 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>234</v>
+      </c>
+      <c r="F11" t="n">
+        <v>54288</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>32</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>32</v>
+      </c>
+      <c r="K11" t="n">
+        <v>7424</v>
+      </c>
+      <c r="L11" t="n">
+        <v>232</v>
+      </c>
+      <c r="M11" t="n">
+        <v>46864</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Facility 10</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
         <v>231</v>
       </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>No Bid</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O11" t="n">
+      <c r="F12" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>15</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>15</v>
+      </c>
+      <c r="K12" t="n">
+        <v>195</v>
+      </c>
+      <c r="L12" t="n">
+        <v>13</v>
+      </c>
+      <c r="M12" t="n">
+        <v>2808</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1136,7 +1195,7 @@
  - Insufficient supplier capacity relative to demand.
  - Custom rule constraints conflicting with overall volume/demand.
 Detailed Rule Evaluations:
-Rule 1 ('Exclude Bids'): The exclusion criteria might be too broad, removing all valid bids needed to satisfy demand for a Bid ID or grouping.
+Rule 1 ('# of Transitions'): The rule requires at least 1 transition for Bid ID 1. Note: Requiring at least one transition on an individual Bid ID is a very strict requirement; it forces a non-incumbent allocation even when data or economic factors might not support a transition. Consider applying this rule conditionally or relaxing the requirement to improve feasibility.
 Please review supplier capacities, demand figures, and custom rule constraints for adjustments.</t>
         </is>
       </c>
@@ -1180,9 +1239,6 @@
  - 34 x_B_5 - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
 BaseSpend_C: S0_C - 24 x_C_1 - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
  - 44 x_C_6 - 42 x_C_7 - 24 x_C_8 - 32 x_C_9 = 0
-BidExclusion_0_2_A: x_A_2 = 0
-BidExclusion_0_2_B: x_B_2 = 0
-BidExclusion_0_2_C: x_C_2 = 0
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
 Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000
@@ -1281,6 +1337,7 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
+Rule_0: __dummy &gt;= 1
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
changes to how apply to all works in supplier exclusion rule
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -654,15 +654,15 @@
         <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>219537</v>
+        <v>253800</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K4" t="n">
-        <v>33735</v>
+        <v>36000</v>
       </c>
       <c r="L4" t="n">
-        <v>519</v>
+        <v>600</v>
       </c>
       <c r="M4" t="n">
-        <v>185802</v>
+        <v>217800</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -692,11 +692,11 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -710,10 +710,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F5" t="n">
-        <v>34263</v>
+        <v>2568510</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="K5" t="n">
-        <v>4860</v>
+        <v>136080</v>
       </c>
       <c r="L5" t="n">
-        <v>81</v>
+        <v>5670</v>
       </c>
       <c r="M5" t="n">
-        <v>29403</v>
+        <v>2432430</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -751,7 +751,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,18 +769,18 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F6" t="n">
-        <v>2568510</v>
+        <v>15390</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -788,16 +788,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>130410</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>5670</v>
+        <v>45</v>
       </c>
       <c r="M6" t="n">
-        <v>2438100</v>
+        <v>15390</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -810,7 +810,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,18 +828,18 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>342</v>
+        <v>653</v>
       </c>
       <c r="F7" t="n">
-        <v>15390</v>
+        <v>158026</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="K7" t="n">
-        <v>1530</v>
+        <v>10648</v>
       </c>
       <c r="L7" t="n">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="M7" t="n">
-        <v>13860</v>
+        <v>147378</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -869,7 +869,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -887,18 +887,18 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>653</v>
+        <v>432</v>
       </c>
       <c r="F8" t="n">
-        <v>158026</v>
+        <v>286848</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -906,16 +906,16 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="K8" t="n">
-        <v>5808</v>
+        <v>27888</v>
       </c>
       <c r="L8" t="n">
-        <v>242</v>
+        <v>664</v>
       </c>
       <c r="M8" t="n">
-        <v>152218</v>
+        <v>258960</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,18 +946,18 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="F9" t="n">
-        <v>286848</v>
+        <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>15272</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>664</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>271576</v>
+        <v>0</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>456</v>
+        <v>234</v>
       </c>
       <c r="F10" t="n">
-        <v>10944</v>
+        <v>54288</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="K10" t="n">
-        <v>576</v>
+        <v>7424</v>
       </c>
       <c r="L10" t="n">
-        <v>24</v>
+        <v>232</v>
       </c>
       <c r="M10" t="n">
-        <v>10368</v>
+        <v>46864</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1064,18 +1064,18 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F11" t="n">
-        <v>54288</v>
+        <v>0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1083,16 +1083,16 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>7424</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>232</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>46864</v>
+        <v>0</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1100,65 +1100,6 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>231</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>15</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J12" t="n">
-        <v>15</v>
-      </c>
-      <c r="K12" t="n">
-        <v>195</v>
-      </c>
-      <c r="L12" t="n">
-        <v>13</v>
-      </c>
-      <c r="M12" t="n">
-        <v>2808</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1195,7 +1136,7 @@
  - Insufficient supplier capacity relative to demand.
  - Custom rule constraints conflicting with overall volume/demand.
 Detailed Rule Evaluations:
-Rule 1 ('# of Transitions'): The rule requires at least 1 transition for Bid ID 1. Note: Requiring at least one transition on an individual Bid ID is a very strict requirement; it forces a non-incumbent allocation even when data or economic factors might not support a transition. Consider applying this rule conditionally or relaxing the requirement to improve feasibility.
+Rule 1 ('Supplier Exclusion'): For Bid ID Apply to all items individually, supplier New Suppliers is excluded, and it is the only supplier with a valid bid.
 Please review supplier capacities, demand figures, and custom rule constraints for adjustments.</t>
         </is>
       </c>
@@ -1337,7 +1278,36 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-Rule_0: __dummy &gt;= 1
+SupplierExclusion_10_A: x_A_10 = 0
+SupplierExclusion_10_B: x_B_10 = 0
+SupplierExclusion_1_B: x_B_1 = 0
+SupplierExclusion_1_C: x_C_1 = 0
+SupplierExclusion_2_A: x_A_2 = 0
+SupplierExclusion_2_C: x_C_2 = 0
+SupplierExclusion_3_A: x_A_3 = 0
+SupplierExclusion_3_B: x_B_3 = 0
+SupplierExclusion_4_A: x_A_4 = 0
+SupplierExclusion_4_B: x_B_4 = 0
+SupplierExclusion_5_A: x_A_5 = 0
+SupplierExclusion_5_B: x_B_5 = 0
+SupplierExclusion_6_A: x_A_6 = 0
+SupplierExclusion_6_B: x_B_6 = 0
+SupplierExclusion_7_A: x_A_7 = 0
+SupplierExclusion_7_B: x_B_7 = 0
+SupplierExclusion_8_A: x_A_8 = 0
+SupplierExclusion_8_B: x_B_8 = 0
+SupplierExclusion_9_A: x_A_9 = 0
+SupplierExclusion_9_B: x_B_9 = 0
+SupplierExclusion_Full_1: x_A_1 = 700
+SupplierExclusion_Full_10: x_C_10 = 13
+SupplierExclusion_Full_2: x_B_2 = 9000
+SupplierExclusion_Full_3: x_C_3 = 600
+SupplierExclusion_Full_4: x_C_4 = 5670
+SupplierExclusion_Full_5: x_C_5 = 45
+SupplierExclusion_Full_6: x_C_6 = 242
+SupplierExclusion_Full_7: x_C_7 = 664
+SupplierExclusion_Full_8: x_C_8 = 24
+SupplierExclusion_Full_9: x_C_9 = 232
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
updated feasibility notes for uxp
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -1136,7 +1136,16 @@
  - Insufficient supplier capacity relative to demand.
  - Custom rule constraints conflicting with overall volume/demand.
 Detailed Rule Evaluations:
-Rule 1 ('Supplier Exclusion'): For Bid ID Apply to all items individually, supplier New Suppliers is excluded, and it is the only supplier with a valid bid.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 1, total demand is 700 units; a 100% allocation requires 700.0 units for Incumbent. Supplier capacity is not available.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 2, total demand is 9000 units; a 100% allocation requires 9000.0 units for Incumbent. Supplier capacity is 100000000.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 3, total demand is 600 units; a 100% allocation requires 600.0 units for Incumbent. Supplier capacity is 100000000.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 4, total demand is 5670 units; a 100% allocation requires 5670.0 units for Incumbent. Supplier capacity is 100000000.
+Rule 1 ('% of Volume Awarded'): ❌ For Bid ID 5, the incumbent (C) did not submit a bid.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 6, total demand is 242 units; a 100% allocation requires 242.0 units for Incumbent. Supplier capacity is 100000000.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 7, total demand is 664 units; a 100% allocation requires 664.0 units for Incumbent. Supplier capacity is 100000000.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 8, total demand is 24 units; a 100% allocation requires 24.0 units for Incumbent. Supplier capacity is 100000000.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 9, total demand is 232 units; a 100% allocation requires 232.0 units for Incumbent. Supplier capacity is 100000000.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 10, total demand is 13 units; a 100% allocation requires 13.0 units for Incumbent. Supplier capacity is 100000000.
 Please review supplier capacities, demand figures, and custom rule constraints for adjustments.</t>
         </is>
       </c>
@@ -1278,36 +1287,16 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-SupplierExclusion_10_A: x_A_10 = 0
-SupplierExclusion_10_B: x_B_10 = 0
-SupplierExclusion_1_B: x_B_1 = 0
-SupplierExclusion_1_C: x_C_1 = 0
-SupplierExclusion_2_A: x_A_2 = 0
-SupplierExclusion_2_C: x_C_2 = 0
-SupplierExclusion_3_A: x_A_3 = 0
-SupplierExclusion_3_B: x_B_3 = 0
-SupplierExclusion_4_A: x_A_4 = 0
-SupplierExclusion_4_B: x_B_4 = 0
-SupplierExclusion_5_A: x_A_5 = 0
-SupplierExclusion_5_B: x_B_5 = 0
-SupplierExclusion_6_A: x_A_6 = 0
-SupplierExclusion_6_B: x_B_6 = 0
-SupplierExclusion_7_A: x_A_7 = 0
-SupplierExclusion_7_B: x_B_7 = 0
-SupplierExclusion_8_A: x_A_8 = 0
-SupplierExclusion_8_B: x_B_8 = 0
-SupplierExclusion_9_A: x_A_9 = 0
-SupplierExclusion_9_B: x_B_9 = 0
-SupplierExclusion_Full_1: x_A_1 = 700
-SupplierExclusion_Full_10: x_C_10 = 13
-SupplierExclusion_Full_2: x_B_2 = 9000
-SupplierExclusion_Full_3: x_C_3 = 600
-SupplierExclusion_Full_4: x_C_4 = 5670
-SupplierExclusion_Full_5: x_C_5 = 45
-SupplierExclusion_Full_6: x_C_6 = 242
-SupplierExclusion_Full_7: x_C_7 = 664
-SupplierExclusion_Full_8: x_C_8 = 24
-SupplierExclusion_Full_9: x_C_9 = 232
+Rule_0_1: 0 x_A_1 - x_B_1 - x_C_1 &gt;= 0
+Rule_0_10: - x_A_10 - x_B_10 + 0 x_C_10 &gt;= 0
+Rule_0_2: - x_A_2 + 0 x_B_2 - x_C_2 &gt;= 0
+Rule_0_3: - x_A_3 - x_B_3 + 0 x_C_3 &gt;= 0
+Rule_0_4: - x_A_4 - x_B_4 + 0 x_C_4 &gt;= 0
+Rule_0_5: - x_A_5 - x_B_5 + 0 x_C_5 &gt;= 0
+Rule_0_6: - x_A_6 - x_B_6 + 0 x_C_6 &gt;= 0
+Rule_0_7: - x_A_7 - x_B_7 + 0 x_C_7 &gt;= 0
+Rule_0_8: - x_A_8 - x_B_8 + 0 x_C_8 &gt;= 0
+Rule_0_9: - x_A_9 - x_B_9 + 0 x_C_9 &gt;= 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
updates to % and # of volume awarded
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,20 +548,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.5252</v>
+        <v>0.519948</v>
       </c>
       <c r="K2" t="n">
-        <v>367.64</v>
+        <v>363.9636</v>
       </c>
       <c r="L2" t="n">
         <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>69632.36</v>
+        <v>69636.0364</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -607,28 +607,28 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>70</v>
+        <v>67.89999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>630000</v>
+        <v>611099.9999999999</v>
       </c>
       <c r="L3" t="n">
         <v>9000</v>
       </c>
       <c r="M3" t="n">
-        <v>774000</v>
+        <v>792900.0000000001</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>30555</v>
       </c>
     </row>
     <row r="4">
@@ -654,91 +654,91 @@
         <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>253800</v>
+        <v>195849</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>60</v>
+        <v>63.05</v>
       </c>
       <c r="K4" t="n">
-        <v>36000</v>
+        <v>29192.15</v>
       </c>
       <c r="L4" t="n">
-        <v>600</v>
+        <v>463</v>
       </c>
       <c r="M4" t="n">
-        <v>217800</v>
+        <v>166656.85</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>1459.6075</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Facility 4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>423</v>
+      </c>
+      <c r="F5" t="n">
+        <v>57951</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Facility 4</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>453</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2568510</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
       <c r="H5" t="n">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>24</v>
+        <v>54.45</v>
       </c>
       <c r="K5" t="n">
-        <v>136080</v>
+        <v>7459.650000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>5670</v>
+        <v>137</v>
       </c>
       <c r="M5" t="n">
-        <v>2432430</v>
+        <v>50491.35</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -751,7 +751,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,35 +769,35 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>15390</v>
+        <v>2447106</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>22.77</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>123003.54</v>
       </c>
       <c r="L6" t="n">
-        <v>45</v>
+        <v>5402</v>
       </c>
       <c r="M6" t="n">
-        <v>15390</v>
+        <v>2324102.46</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -810,16 +810,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>653</v>
+        <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>158026</v>
+        <v>121404</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -839,24 +839,24 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>44</v>
+        <v>23.04</v>
       </c>
       <c r="K7" t="n">
-        <v>10648</v>
+        <v>6174.719999999999</v>
       </c>
       <c r="L7" t="n">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="M7" t="n">
-        <v>147378</v>
+        <v>115229.28</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -869,7 +869,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -887,94 +887,94 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>432</v>
+        <v>342</v>
       </c>
       <c r="F8" t="n">
-        <v>286848</v>
+        <v>8550</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>42</v>
+        <v>32.98</v>
       </c>
       <c r="K8" t="n">
-        <v>27888</v>
+        <v>824.4999999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>664</v>
+        <v>25</v>
       </c>
       <c r="M8" t="n">
-        <v>258960</v>
+        <v>7725.5</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>41.22499999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Facility 5</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>342</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6840</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>456</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>No Bid</t>
-        </is>
-      </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>53.46</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>1069.2</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>5770.8</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,48 +1005,48 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>234</v>
+        <v>653</v>
       </c>
       <c r="F10" t="n">
-        <v>54288</v>
+        <v>158026</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>32</v>
+        <v>23.28</v>
       </c>
       <c r="K10" t="n">
-        <v>7424</v>
+        <v>5633.76</v>
       </c>
       <c r="L10" t="n">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="M10" t="n">
-        <v>46864</v>
+        <v>152392.24</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>281.688</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1064,35 +1064,35 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>231</v>
+        <v>432</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>286848</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>22.77</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>15119.28</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>664</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>271728.72</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1101,6 +1101,183 @@
       </c>
       <c r="O11" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Facility 9</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>456</v>
+      </c>
+      <c r="F12" t="n">
+        <v>10944</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>13</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>12.61</v>
+      </c>
+      <c r="K12" t="n">
+        <v>302.64</v>
+      </c>
+      <c r="L12" t="n">
+        <v>24</v>
+      </c>
+      <c r="M12" t="n">
+        <v>10641.36</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>15.132</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>234</v>
+      </c>
+      <c r="F13" t="n">
+        <v>54288</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>32</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>30.72</v>
+      </c>
+      <c r="K13" t="n">
+        <v>7127.04</v>
+      </c>
+      <c r="L13" t="n">
+        <v>232</v>
+      </c>
+      <c r="M13" t="n">
+        <v>47160.96</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>231</v>
+      </c>
+      <c r="F14" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>13</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>12.61</v>
+      </c>
+      <c r="K14" t="n">
+        <v>163.93</v>
+      </c>
+      <c r="L14" t="n">
+        <v>13</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2839.07</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>8.1965</v>
       </c>
     </row>
   </sheetData>
@@ -1132,21 +1309,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model is infeasible. Likely causes include:
- - Insufficient supplier capacity relative to demand.
- - Custom rule constraints conflicting with overall volume/demand.
-Detailed Rule Evaluations:
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 1, total demand is 700 units; a 100% allocation requires 700.0 units for Incumbent. Supplier capacity is not available.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 2, total demand is 9000 units; a 100% allocation requires 9000.0 units for Incumbent. Supplier capacity is 100000000.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 3, total demand is 600 units; a 100% allocation requires 600.0 units for Incumbent. Supplier capacity is 100000000.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 4, total demand is 5670 units; a 100% allocation requires 5670.0 units for Incumbent. Supplier capacity is 100000000.
-Rule 1 ('% of Volume Awarded'): ❌ For Bid ID 5, the incumbent (C) did not submit a bid.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 6, total demand is 242 units; a 100% allocation requires 242.0 units for Incumbent. Supplier capacity is 100000000.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 7, total demand is 664 units; a 100% allocation requires 664.0 units for Incumbent. Supplier capacity is 100000000.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 8, total demand is 24 units; a 100% allocation requires 24.0 units for Incumbent. Supplier capacity is 100000000.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 9, total demand is 232 units; a 100% allocation requires 232.0 units for Incumbent. Supplier capacity is 100000000.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 10, total demand is 13 units; a 100% allocation requires 13.0 units for Incumbent. Supplier capacity is 100000000.
-Please review supplier capacities, demand figures, and custom rule constraints for adjustments.</t>
+          <t>Model is optimal.</t>
         </is>
       </c>
     </row>
@@ -1271,10 +1434,10 @@
 RebateTierMin_A_0: __dummy &gt;= 0
 RebateTierMin_A_1: - 500 y_rebate_A_1 &gt;= 0
 RebateTierMin_B_0: __dummy &gt;= 0
-RebateTierMin_B_1: x_B_2 + x_B_5 + x_B_6 + x_B_7 - 500 y_rebate_B_1 &gt;= 0
+RebateTierMin_B_1: x_B_1 + x_B_10 + x_B_3 + x_B_4 + x_B_8 + x_B_9
+ - 500 y_rebate_B_1 &gt;= 0
 RebateTierMin_C_0: __dummy &gt;= 0
-RebateTierMin_C_1: x_C_1 + x_C_10 + x_C_3 + x_C_4 + x_C_8 + x_C_9
- - 700 y_rebate_C_1 &gt;= 0
+RebateTierMin_C_1: - 700 y_rebate_C_1 &gt;= 0
 RebateTierSelect_A: y_rebate_A_0 + y_rebate_A_1 = 1
 RebateTierSelect_B: y_rebate_B_0 + y_rebate_B_1 = 1
 RebateTierSelect_C: y_rebate_C_0 + y_rebate_C_1 = 1
@@ -1287,16 +1450,13 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-Rule_0_1: 0 x_A_1 - x_B_1 - x_C_1 &gt;= 0
-Rule_0_10: - x_A_10 - x_B_10 + 0 x_C_10 &gt;= 0
-Rule_0_2: - x_A_2 + 0 x_B_2 - x_C_2 &gt;= 0
-Rule_0_3: - x_A_3 - x_B_3 + 0 x_C_3 &gt;= 0
-Rule_0_4: - x_A_4 - x_B_4 + 0 x_C_4 &gt;= 0
-Rule_0_5: - x_A_5 - x_B_5 + 0 x_C_5 &gt;= 0
-Rule_0_6: - x_A_6 - x_B_6 + 0 x_C_6 &gt;= 0
-Rule_0_7: - x_A_7 - x_B_7 + 0 x_C_7 &gt;= 0
-Rule_0_8: - x_A_8 - x_B_8 + 0 x_C_8 &gt;= 0
-Rule_0_9: - x_A_9 - x_B_9 + 0 x_C_9 &gt;= 0
+SupplIndicatorLB_0_A_5: - w_0_A_5 + x_A_5 &gt;= 0
+SupplIndicatorLB_0_B_5: - w_0_B_5 + x_B_5 &gt;= 0
+SupplIndicatorLB_0_C_5: - w_0_C_5 + x_C_5 &gt;= 0
+SupplIndicator_0_A_5: - 1000000000 w_0_A_5 + x_A_5 &lt;= 0
+SupplIndicator_0_B_5: - 1000000000 w_0_B_5 + x_B_5 &lt;= 0
+SupplIndicator_0_C_5: - 1000000000 w_0_C_5 + x_C_5 &lt;= 0
+SupplierCount_0_5: w_0_A_5 + w_0_B_5 + w_0_C_5 &gt;= 2
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1317,6 +1477,15 @@
 Transition_8_B: - 24 T_8_B + x_B_8 &lt;= 0
 Transition_9_A: - 232 T_9_A + x_A_9 &lt;= 0
 Transition_9_B: - 232 T_9_B + x_B_9 &lt;= 0
+VolRule_1_A_5_LB: - 1000000000 w_vol_1_A_5 + x_A_5 &gt;= -999999980
+VolRule_1_B_5_LB: - 1000000000 w_vol_1_B_5 + x_B_5 &gt;= -999999980
+VolRule_1_C_5_LB: - 1000000000 w_vol_1_C_5 + x_C_5 &gt;= -999999980
+VolSupplIndicatorLB_1_A_5: - w_vol_1_A_5 + x_A_5 &gt;= 0
+VolSupplIndicatorLB_1_B_5: - w_vol_1_B_5 + x_B_5 &gt;= 0
+VolSupplIndicatorLB_1_C_5: - w_vol_1_C_5 + x_C_5 &gt;= 0
+VolSupplIndicator_1_A_5: - 1000000000 w_vol_1_A_5 + x_A_5 &lt;= 0
+VolSupplIndicator_1_B_5: - 1000000000 w_vol_1_B_5 + x_B_5 &lt;= 0
+VolSupplIndicator_1_C_5: - 1000000000 w_vol_1_C_5 + x_C_5 &lt;= 0
 Volume_A: V_A - x_A_1 - x_A_10 - x_A_2 - x_A_3 - x_A_4 - x_A_5 - x_A_6 - x_A_7
  - x_A_8 - x_A_9 = 0
 Volume_B: V_B - x_B_1 - x_B_10 - x_B_2 - x_B_3 - x_B_4 - x_B_5 - x_B_6 - x_B_7
@@ -1344,6 +1513,12 @@
 T_8_B
 T_9_A
 T_9_B
+w_0_A_5
+w_0_B_5
+w_0_C_5
+w_vol_1_A_5
+w_vol_1_B_5
+w_vol_1_C_5
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
updates to # of transitions
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -654,7 +654,7 @@
         <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>195849</v>
+        <v>211500</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -673,13 +673,13 @@
         <v>63.05</v>
       </c>
       <c r="K4" t="n">
-        <v>29192.15</v>
+        <v>31525</v>
       </c>
       <c r="L4" t="n">
-        <v>463</v>
+        <v>500</v>
       </c>
       <c r="M4" t="n">
-        <v>166656.85</v>
+        <v>179975</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>1459.6075</v>
+        <v>1576.25</v>
       </c>
     </row>
     <row r="5">
@@ -713,7 +713,7 @@
         <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>57951</v>
+        <v>42300</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -732,13 +732,13 @@
         <v>54.45</v>
       </c>
       <c r="K5" t="n">
-        <v>7459.650000000001</v>
+        <v>5445</v>
       </c>
       <c r="L5" t="n">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="M5" t="n">
-        <v>50491.35</v>
+        <v>36855</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -772,7 +772,7 @@
         <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>2447106</v>
+        <v>2463867</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -791,13 +791,13 @@
         <v>22.77</v>
       </c>
       <c r="K6" t="n">
-        <v>123003.54</v>
+        <v>123846.03</v>
       </c>
       <c r="L6" t="n">
-        <v>5402</v>
+        <v>5439</v>
       </c>
       <c r="M6" t="n">
-        <v>2324102.46</v>
+        <v>2340020.97</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -831,7 +831,7 @@
         <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>121404</v>
+        <v>104643</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -850,13 +850,13 @@
         <v>23.04</v>
       </c>
       <c r="K7" t="n">
-        <v>6174.719999999999</v>
+        <v>5322.24</v>
       </c>
       <c r="L7" t="n">
-        <v>268</v>
+        <v>231</v>
       </c>
       <c r="M7" t="n">
-        <v>115229.28</v>
+        <v>99320.75999999999</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -890,7 +890,7 @@
         <v>342</v>
       </c>
       <c r="F8" t="n">
-        <v>8550</v>
+        <v>15390</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -909,13 +909,13 @@
         <v>32.98</v>
       </c>
       <c r="K8" t="n">
-        <v>824.4999999999999</v>
+        <v>1484.1</v>
       </c>
       <c r="L8" t="n">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="M8" t="n">
-        <v>7725.5</v>
+        <v>13905.9</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -923,71 +923,71 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>41.22499999999999</v>
+        <v>74.205</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Facility 9</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>653</v>
+      </c>
+      <c r="F9" t="n">
+        <v>158026</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Facility 5</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>342</v>
-      </c>
-      <c r="F9" t="n">
-        <v>6840</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H9" t="n">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>53.46</v>
+        <v>23.28</v>
       </c>
       <c r="K9" t="n">
-        <v>1069.2</v>
+        <v>5633.76</v>
       </c>
       <c r="L9" t="n">
-        <v>20</v>
+        <v>242</v>
       </c>
       <c r="M9" t="n">
-        <v>5770.8</v>
+        <v>152392.24</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>281.688</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1005,48 +1005,48 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>653</v>
+        <v>432</v>
       </c>
       <c r="F10" t="n">
-        <v>158026</v>
+        <v>286848</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>23.28</v>
+        <v>22.77</v>
       </c>
       <c r="K10" t="n">
-        <v>5633.76</v>
+        <v>15119.28</v>
       </c>
       <c r="L10" t="n">
-        <v>242</v>
+        <v>664</v>
       </c>
       <c r="M10" t="n">
-        <v>152392.24</v>
+        <v>271728.72</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>281.688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1064,35 +1064,35 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="F11" t="n">
-        <v>286848</v>
+        <v>10944</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>22.77</v>
+        <v>23.04</v>
       </c>
       <c r="K11" t="n">
-        <v>15119.28</v>
+        <v>552.96</v>
       </c>
       <c r="L11" t="n">
-        <v>664</v>
+        <v>24</v>
       </c>
       <c r="M11" t="n">
-        <v>271728.72</v>
+        <v>10391.04</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1123,48 +1123,48 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>456</v>
+        <v>234</v>
       </c>
       <c r="F12" t="n">
-        <v>10944</v>
+        <v>54288</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>12.61</v>
+        <v>30.72</v>
       </c>
       <c r="K12" t="n">
-        <v>302.64</v>
+        <v>7127.04</v>
       </c>
       <c r="L12" t="n">
-        <v>24</v>
+        <v>232</v>
       </c>
       <c r="M12" t="n">
-        <v>10641.36</v>
+        <v>47160.96</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>15.132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1182,10 +1182,10 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F13" t="n">
-        <v>54288</v>
+        <v>3003</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1201,16 +1201,16 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>30.72</v>
+        <v>14.4</v>
       </c>
       <c r="K13" t="n">
-        <v>7127.04</v>
+        <v>187.2</v>
       </c>
       <c r="L13" t="n">
-        <v>232</v>
+        <v>13</v>
       </c>
       <c r="M13" t="n">
-        <v>47160.96</v>
+        <v>2815.8</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1219,65 +1219,6 @@
       </c>
       <c r="O13" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>231</v>
-      </c>
-      <c r="F14" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>13</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J14" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K14" t="n">
-        <v>163.93</v>
-      </c>
-      <c r="L14" t="n">
-        <v>13</v>
-      </c>
-      <c r="M14" t="n">
-        <v>2839.07</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>8.1965</v>
       </c>
     </row>
   </sheetData>
@@ -1418,6 +1359,36 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
+Link_Y_lower_10_A: - T_10_A + Y_10 &gt;= 0
+Link_Y_lower_10_B: - T_10_B + Y_10 &gt;= 0
+Link_Y_lower_1_B: - T_1_B + Y_1 &gt;= 0
+Link_Y_lower_1_C: - T_1_C + Y_1 &gt;= 0
+Link_Y_lower_2_A: - T_2_A + Y_2 &gt;= 0
+Link_Y_lower_2_C: - T_2_C + Y_2 &gt;= 0
+Link_Y_lower_3_A: - T_3_A + Y_3 &gt;= 0
+Link_Y_lower_3_B: - T_3_B + Y_3 &gt;= 0
+Link_Y_lower_4_A: - T_4_A + Y_4 &gt;= 0
+Link_Y_lower_4_B: - T_4_B + Y_4 &gt;= 0
+Link_Y_lower_5_A: - T_5_A + Y_5 &gt;= 0
+Link_Y_lower_5_B: - T_5_B + Y_5 &gt;= 0
+Link_Y_lower_6_A: - T_6_A + Y_6 &gt;= 0
+Link_Y_lower_6_B: - T_6_B + Y_6 &gt;= 0
+Link_Y_lower_7_A: - T_7_A + Y_7 &gt;= 0
+Link_Y_lower_7_B: - T_7_B + Y_7 &gt;= 0
+Link_Y_lower_8_A: - T_8_A + Y_8 &gt;= 0
+Link_Y_lower_8_B: - T_8_B + Y_8 &gt;= 0
+Link_Y_lower_9_A: - T_9_A + Y_9 &gt;= 0
+Link_Y_lower_9_B: - T_9_B + Y_9 &gt;= 0
+Link_Y_upper_1: - T_1_B - T_1_C + Y_1 &lt;= 0
+Link_Y_upper_10: - T_10_A - T_10_B + Y_10 &lt;= 0
+Link_Y_upper_2: - T_2_A - T_2_C + Y_2 &lt;= 0
+Link_Y_upper_3: - T_3_A - T_3_B + Y_3 &lt;= 0
+Link_Y_upper_4: - T_4_A - T_4_B + Y_4 &lt;= 0
+Link_Y_upper_5: - T_5_A - T_5_B + Y_5 &lt;= 0
+Link_Y_upper_6: - T_6_A - T_6_B + Y_6 &lt;= 0
+Link_Y_upper_7: - T_7_A - T_7_B + Y_7 &lt;= 0
+Link_Y_upper_8: - T_8_A - T_8_B + Y_8 &lt;= 0
+Link_Y_upper_9: - T_9_A - T_9_B + Y_9 &lt;= 0
 NonBid_C_5: x_C_5 = 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
@@ -1450,13 +1421,7 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-SupplIndicatorLB_0_A_5: - w_0_A_5 + x_A_5 &gt;= 0
-SupplIndicatorLB_0_B_5: - w_0_B_5 + x_B_5 &gt;= 0
-SupplIndicatorLB_0_C_5: - w_0_C_5 + x_C_5 &gt;= 0
-SupplIndicator_0_A_5: - 1000000000 w_0_A_5 + x_A_5 &lt;= 0
-SupplIndicator_0_B_5: - 1000000000 w_0_B_5 + x_B_5 &lt;= 0
-SupplIndicator_0_C_5: - 1000000000 w_0_C_5 + x_C_5 &lt;= 0
-SupplierCount_0_5: w_0_A_5 + w_0_B_5 + w_0_C_5 &gt;= 2
+TransRule_0: Y_1 + Y_10 + Y_2 + Y_3 + Y_4 + Y_5 + Y_6 + Y_7 + Y_8 + Y_9 = 5
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1477,15 +1442,6 @@
 Transition_8_B: - 24 T_8_B + x_B_8 &lt;= 0
 Transition_9_A: - 232 T_9_A + x_A_9 &lt;= 0
 Transition_9_B: - 232 T_9_B + x_B_9 &lt;= 0
-VolRule_1_A_5_LB: - 1000000000 w_vol_1_A_5 + x_A_5 &gt;= -999999980
-VolRule_1_B_5_LB: - 1000000000 w_vol_1_B_5 + x_B_5 &gt;= -999999980
-VolRule_1_C_5_LB: - 1000000000 w_vol_1_C_5 + x_C_5 &gt;= -999999980
-VolSupplIndicatorLB_1_A_5: - w_vol_1_A_5 + x_A_5 &gt;= 0
-VolSupplIndicatorLB_1_B_5: - w_vol_1_B_5 + x_B_5 &gt;= 0
-VolSupplIndicatorLB_1_C_5: - w_vol_1_C_5 + x_C_5 &gt;= 0
-VolSupplIndicator_1_A_5: - 1000000000 w_vol_1_A_5 + x_A_5 &lt;= 0
-VolSupplIndicator_1_B_5: - 1000000000 w_vol_1_B_5 + x_B_5 &lt;= 0
-VolSupplIndicator_1_C_5: - 1000000000 w_vol_1_C_5 + x_C_5 &lt;= 0
 Volume_A: V_A - x_A_1 - x_A_10 - x_A_2 - x_A_3 - x_A_4 - x_A_5 - x_A_6 - x_A_7
  - x_A_8 - x_A_9 = 0
 Volume_B: V_B - x_B_1 - x_B_10 - x_B_2 - x_B_3 - x_B_4 - x_B_5 - x_B_6 - x_B_7
@@ -1513,12 +1469,16 @@
 T_8_B
 T_9_A
 T_9_B
-w_0_A_5
-w_0_B_5
-w_0_C_5
-w_vol_1_A_5
-w_vol_1_B_5
-w_vol_1_C_5
+Y_1
+Y_10
+Y_2
+Y_3
+Y_4
+Y_5
+Y_6
+Y_7
+Y_8
+Y_9
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
updates to # of Suppliers logic
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>70000</v>
+        <v>69900</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -555,13 +555,13 @@
         <v>0.519948</v>
       </c>
       <c r="K2" t="n">
-        <v>363.9636</v>
+        <v>363.443652</v>
       </c>
       <c r="L2" t="n">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="M2" t="n">
-        <v>69636.0364</v>
+        <v>69536.556348</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -574,28 +574,28 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Facility 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Facility 1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="E3" t="n">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>1404000</v>
+        <v>100</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -611,16 +611,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>67.89999999999999</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>611099.9999999999</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>9000</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>792900.0000000001</v>
+        <v>90.3</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -628,12 +628,12 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>30555</v>
+        <v>0.485</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -642,19 +642,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>423</v>
+        <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>211500</v>
+        <v>1404000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>63.05</v>
+        <v>67.89999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>31525</v>
+        <v>611099.9999999999</v>
       </c>
       <c r="L4" t="n">
-        <v>500</v>
+        <v>9000</v>
       </c>
       <c r="M4" t="n">
-        <v>179975</v>
+        <v>792900.0000000001</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>1576.25</v>
+        <v>30555</v>
       </c>
     </row>
     <row r="5">
@@ -696,7 +696,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -713,74 +713,74 @@
         <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>42300</v>
+        <v>195849</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>54.45</v>
+        <v>63.05</v>
       </c>
       <c r="K5" t="n">
-        <v>5445</v>
+        <v>29192.15</v>
       </c>
       <c r="L5" t="n">
-        <v>100</v>
+        <v>463</v>
       </c>
       <c r="M5" t="n">
-        <v>36855</v>
+        <v>166656.85</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>1459.6075</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Facility 4</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>423</v>
+      </c>
+      <c r="F6" t="n">
+        <v>57951</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Facility 4</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>453</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2463867</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H6" t="n">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -788,16 +788,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>22.77</v>
+        <v>54.45</v>
       </c>
       <c r="K6" t="n">
-        <v>123846.03</v>
+        <v>7459.650000000001</v>
       </c>
       <c r="L6" t="n">
-        <v>5439</v>
+        <v>137</v>
       </c>
       <c r="M6" t="n">
-        <v>2340020.97</v>
+        <v>50491.35</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -814,7 +814,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -831,32 +831,32 @@
         <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>104643</v>
+        <v>2447559</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>23.04</v>
+        <v>22.77</v>
       </c>
       <c r="K7" t="n">
-        <v>5322.24</v>
+        <v>123026.31</v>
       </c>
       <c r="L7" t="n">
-        <v>231</v>
+        <v>5403</v>
       </c>
       <c r="M7" t="n">
-        <v>99320.75999999999</v>
+        <v>2324532.69</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -869,16 +869,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -887,48 +887,48 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="F8" t="n">
-        <v>15390</v>
+        <v>120951</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>32.98</v>
+        <v>23.04</v>
       </c>
       <c r="K8" t="n">
-        <v>1484.1</v>
+        <v>6151.679999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="M8" t="n">
-        <v>13905.9</v>
+        <v>114799.32</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>74.205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>653</v>
+        <v>342</v>
       </c>
       <c r="F9" t="n">
-        <v>158026</v>
+        <v>15390</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>23.28</v>
+        <v>32.98</v>
       </c>
       <c r="K9" t="n">
-        <v>5633.76</v>
+        <v>1484.1</v>
       </c>
       <c r="L9" t="n">
-        <v>242</v>
+        <v>45</v>
       </c>
       <c r="M9" t="n">
-        <v>152392.24</v>
+        <v>13905.9</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -982,12 +982,12 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>281.688</v>
+        <v>74.205</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1005,48 +1005,48 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>432</v>
+        <v>653</v>
       </c>
       <c r="F10" t="n">
-        <v>286848</v>
+        <v>158026</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>22.77</v>
+        <v>23.28</v>
       </c>
       <c r="K10" t="n">
-        <v>15119.28</v>
+        <v>5633.76</v>
       </c>
       <c r="L10" t="n">
-        <v>664</v>
+        <v>242</v>
       </c>
       <c r="M10" t="n">
-        <v>271728.72</v>
+        <v>152392.24</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>281.688</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1064,35 +1064,35 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F11" t="n">
-        <v>10944</v>
+        <v>286848</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>23.04</v>
+        <v>22.77</v>
       </c>
       <c r="K11" t="n">
-        <v>552.96</v>
+        <v>15119.28</v>
       </c>
       <c r="L11" t="n">
-        <v>24</v>
+        <v>664</v>
       </c>
       <c r="M11" t="n">
-        <v>10391.04</v>
+        <v>271728.72</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1123,101 +1123,337 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>234</v>
+        <v>456</v>
       </c>
       <c r="F12" t="n">
-        <v>54288</v>
+        <v>10488</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>30.72</v>
+        <v>12.61</v>
       </c>
       <c r="K12" t="n">
-        <v>7127.04</v>
+        <v>290.03</v>
       </c>
       <c r="L12" t="n">
-        <v>232</v>
+        <v>23</v>
       </c>
       <c r="M12" t="n">
-        <v>47160.96</v>
+        <v>10197.97</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>14.5015</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>8</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Facility 9</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>456</v>
+      </c>
+      <c r="F13" t="n">
+        <v>456</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>24</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="K13" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>432.96</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>9</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>234</v>
+      </c>
+      <c r="F14" t="n">
+        <v>54054</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>32</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>30.72</v>
+      </c>
+      <c r="K14" t="n">
+        <v>7096.32</v>
+      </c>
+      <c r="L14" t="n">
+        <v>231</v>
+      </c>
+      <c r="M14" t="n">
+        <v>46957.68</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>9</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>234</v>
+      </c>
+      <c r="F15" t="n">
+        <v>234</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>56</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>54.32</v>
+      </c>
+      <c r="K15" t="n">
+        <v>54.32</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>179.68</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>2.716</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>10</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Facility 10</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
         <v>231</v>
       </c>
-      <c r="F13" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
+      <c r="F16" t="n">
+        <v>2772</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>13</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>12.61</v>
+      </c>
+      <c r="K16" t="n">
+        <v>151.32</v>
+      </c>
+      <c r="L16" t="n">
+        <v>12</v>
+      </c>
+      <c r="M16" t="n">
+        <v>2620.68</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>7.566</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>231</v>
+      </c>
+      <c r="F17" t="n">
+        <v>231</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
         <v>15</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>4%</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="J17" t="n">
         <v>14.4</v>
       </c>
-      <c r="K13" t="n">
-        <v>187.2</v>
-      </c>
-      <c r="L13" t="n">
-        <v>13</v>
-      </c>
-      <c r="M13" t="n">
-        <v>2815.8</v>
-      </c>
-      <c r="N13" t="inlineStr">
+      <c r="K17" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" t="n">
+        <v>216.6</v>
+      </c>
+      <c r="N17" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O13" t="n">
+      <c r="O17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1359,36 +1595,6 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
-Link_Y_lower_10_A: - T_10_A + Y_10 &gt;= 0
-Link_Y_lower_10_B: - T_10_B + Y_10 &gt;= 0
-Link_Y_lower_1_B: - T_1_B + Y_1 &gt;= 0
-Link_Y_lower_1_C: - T_1_C + Y_1 &gt;= 0
-Link_Y_lower_2_A: - T_2_A + Y_2 &gt;= 0
-Link_Y_lower_2_C: - T_2_C + Y_2 &gt;= 0
-Link_Y_lower_3_A: - T_3_A + Y_3 &gt;= 0
-Link_Y_lower_3_B: - T_3_B + Y_3 &gt;= 0
-Link_Y_lower_4_A: - T_4_A + Y_4 &gt;= 0
-Link_Y_lower_4_B: - T_4_B + Y_4 &gt;= 0
-Link_Y_lower_5_A: - T_5_A + Y_5 &gt;= 0
-Link_Y_lower_5_B: - T_5_B + Y_5 &gt;= 0
-Link_Y_lower_6_A: - T_6_A + Y_6 &gt;= 0
-Link_Y_lower_6_B: - T_6_B + Y_6 &gt;= 0
-Link_Y_lower_7_A: - T_7_A + Y_7 &gt;= 0
-Link_Y_lower_7_B: - T_7_B + Y_7 &gt;= 0
-Link_Y_lower_8_A: - T_8_A + Y_8 &gt;= 0
-Link_Y_lower_8_B: - T_8_B + Y_8 &gt;= 0
-Link_Y_lower_9_A: - T_9_A + Y_9 &gt;= 0
-Link_Y_lower_9_B: - T_9_B + Y_9 &gt;= 0
-Link_Y_upper_1: - T_1_B - T_1_C + Y_1 &lt;= 0
-Link_Y_upper_10: - T_10_A - T_10_B + Y_10 &lt;= 0
-Link_Y_upper_2: - T_2_A - T_2_C + Y_2 &lt;= 0
-Link_Y_upper_3: - T_3_A - T_3_B + Y_3 &lt;= 0
-Link_Y_upper_4: - T_4_A - T_4_B + Y_4 &lt;= 0
-Link_Y_upper_5: - T_5_A - T_5_B + Y_5 &lt;= 0
-Link_Y_upper_6: - T_6_A - T_6_B + Y_6 &lt;= 0
-Link_Y_upper_7: - T_7_A - T_7_B + Y_7 &lt;= 0
-Link_Y_upper_8: - T_8_A - T_8_B + Y_8 &lt;= 0
-Link_Y_upper_9: - T_9_A - T_9_B + Y_9 &lt;= 0
 NonBid_C_5: x_C_5 = 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
@@ -1421,7 +1627,48 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-TransRule_0: Y_1 + Y_10 + Y_2 + Y_3 + Y_4 + Y_5 + Y_6 + Y_7 + Y_8 + Y_9 = 5
+SupplIndicatorLB_0_A_1: - w_0_A_1 + x_A_1 &gt;= 0
+SupplIndicatorLB_0_A_10: - w_0_A_10 + x_A_10 &gt;= 0
+SupplIndicatorLB_0_A_3: - w_0_A_3 + x_A_3 &gt;= 0
+SupplIndicatorLB_0_A_4: - w_0_A_4 + x_A_4 &gt;= 0
+SupplIndicatorLB_0_A_8: - w_0_A_8 + x_A_8 &gt;= 0
+SupplIndicatorLB_0_A_9: - w_0_A_9 + x_A_9 &gt;= 0
+SupplIndicatorLB_0_B_1: - w_0_B_1 + x_B_1 &gt;= 0
+SupplIndicatorLB_0_B_10: - w_0_B_10 + x_B_10 &gt;= 0
+SupplIndicatorLB_0_B_3: - w_0_B_3 + x_B_3 &gt;= 0
+SupplIndicatorLB_0_B_4: - w_0_B_4 + x_B_4 &gt;= 0
+SupplIndicatorLB_0_B_8: - w_0_B_8 + x_B_8 &gt;= 0
+SupplIndicatorLB_0_B_9: - w_0_B_9 + x_B_9 &gt;= 0
+SupplIndicatorLB_0_C_1: - w_0_C_1 + x_C_1 &gt;= 0
+SupplIndicatorLB_0_C_10: - w_0_C_10 + x_C_10 &gt;= 0
+SupplIndicatorLB_0_C_3: - w_0_C_3 + x_C_3 &gt;= 0
+SupplIndicatorLB_0_C_4: - w_0_C_4 + x_C_4 &gt;= 0
+SupplIndicatorLB_0_C_8: - w_0_C_8 + x_C_8 &gt;= 0
+SupplIndicatorLB_0_C_9: - w_0_C_9 + x_C_9 &gt;= 0
+SupplIndicator_0_A_1: - 1000000000 w_0_A_1 + x_A_1 &lt;= 0
+SupplIndicator_0_A_10: - 1000000000 w_0_A_10 + x_A_10 &lt;= 0
+SupplIndicator_0_A_3: - 1000000000 w_0_A_3 + x_A_3 &lt;= 0
+SupplIndicator_0_A_4: - 1000000000 w_0_A_4 + x_A_4 &lt;= 0
+SupplIndicator_0_A_8: - 1000000000 w_0_A_8 + x_A_8 &lt;= 0
+SupplIndicator_0_A_9: - 1000000000 w_0_A_9 + x_A_9 &lt;= 0
+SupplIndicator_0_B_1: - 1000000000 w_0_B_1 + x_B_1 &lt;= 0
+SupplIndicator_0_B_10: - 1000000000 w_0_B_10 + x_B_10 &lt;= 0
+SupplIndicator_0_B_3: - 1000000000 w_0_B_3 + x_B_3 &lt;= 0
+SupplIndicator_0_B_4: - 1000000000 w_0_B_4 + x_B_4 &lt;= 0
+SupplIndicator_0_B_8: - 1000000000 w_0_B_8 + x_B_8 &lt;= 0
+SupplIndicator_0_B_9: - 1000000000 w_0_B_9 + x_B_9 &lt;= 0
+SupplIndicator_0_C_1: - 1000000000 w_0_C_1 + x_C_1 &lt;= 0
+SupplIndicator_0_C_10: - 1000000000 w_0_C_10 + x_C_10 &lt;= 0
+SupplIndicator_0_C_3: - 1000000000 w_0_C_3 + x_C_3 &lt;= 0
+SupplIndicator_0_C_4: - 1000000000 w_0_C_4 + x_C_4 &lt;= 0
+SupplIndicator_0_C_8: - 1000000000 w_0_C_8 + x_C_8 &lt;= 0
+SupplIndicator_0_C_9: - 1000000000 w_0_C_9 + x_C_9 &lt;= 0
+SupplierCount_0_1: w_0_A_1 + w_0_B_1 + w_0_C_1 &gt;= 2
+SupplierCount_0_10: w_0_A_10 + w_0_B_10 + w_0_C_10 &gt;= 2
+SupplierCount_0_3: w_0_A_3 + w_0_B_3 + w_0_C_3 &gt;= 2
+SupplierCount_0_4: w_0_A_4 + w_0_B_4 + w_0_C_4 &gt;= 2
+SupplierCount_0_8: w_0_A_8 + w_0_B_8 + w_0_C_8 &gt;= 2
+SupplierCount_0_9: w_0_A_9 + w_0_B_9 + w_0_C_9 &gt;= 2
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1469,16 +1716,24 @@
 T_8_B
 T_9_A
 T_9_B
-Y_1
-Y_10
-Y_2
-Y_3
-Y_4
-Y_5
-Y_6
-Y_7
-Y_8
-Y_9
+w_0_A_1
+w_0_A_10
+w_0_A_3
+w_0_A_4
+w_0_A_8
+w_0_A_9
+w_0_B_1
+w_0_B_10
+w_0_B_3
+w_0_B_4
+w_0_B_8
+w_0_B_9
+w_0_C_1
+w_0_C_10
+w_0_C_3
+w_0_C_4
+w_0_C_8
+w_0_C_9
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
final updates and removed % min vol award and # min vol award
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -654,7 +654,7 @@
         <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>1404000</v>
+        <v>1403844</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -673,13 +673,13 @@
         <v>67.89999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>611099.9999999999</v>
+        <v>611032.1</v>
       </c>
       <c r="L4" t="n">
-        <v>9000</v>
+        <v>8999</v>
       </c>
       <c r="M4" t="n">
-        <v>792900.0000000001</v>
+        <v>792811.9</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -687,66 +687,66 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>30555</v>
+        <v>30551.605</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Facility 1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>156</v>
+      </c>
+      <c r="F5" t="n">
+        <v>156</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Facility 4</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>423</v>
-      </c>
-      <c r="F5" t="n">
-        <v>195849</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="H5" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>63.05</v>
+        <v>69.3</v>
       </c>
       <c r="K5" t="n">
-        <v>29192.15</v>
+        <v>69.3</v>
       </c>
       <c r="L5" t="n">
-        <v>463</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>166656.85</v>
+        <v>86.7</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>1459.6075</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -755,7 +755,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -772,74 +772,74 @@
         <v>423</v>
       </c>
       <c r="F6" t="n">
-        <v>57951</v>
+        <v>195849</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>54.45</v>
+        <v>63.05</v>
       </c>
       <c r="K6" t="n">
-        <v>7459.650000000001</v>
+        <v>29192.15</v>
       </c>
       <c r="L6" t="n">
-        <v>137</v>
+        <v>463</v>
       </c>
       <c r="M6" t="n">
-        <v>50491.35</v>
+        <v>166656.85</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>1459.6075</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Facility 4</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>423</v>
+      </c>
+      <c r="F7" t="n">
+        <v>57951</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Facility 4</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>453</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2447559</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H7" t="n">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>22.77</v>
+        <v>54.45</v>
       </c>
       <c r="K7" t="n">
-        <v>123026.31</v>
+        <v>7459.650000000001</v>
       </c>
       <c r="L7" t="n">
-        <v>5403</v>
+        <v>137</v>
       </c>
       <c r="M7" t="n">
-        <v>2324532.69</v>
+        <v>50491.35</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -873,7 +873,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -890,32 +890,32 @@
         <v>453</v>
       </c>
       <c r="F8" t="n">
-        <v>120951</v>
+        <v>2447559</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>23.04</v>
+        <v>22.77</v>
       </c>
       <c r="K8" t="n">
-        <v>6151.679999999999</v>
+        <v>123026.31</v>
       </c>
       <c r="L8" t="n">
-        <v>267</v>
+        <v>5403</v>
       </c>
       <c r="M8" t="n">
-        <v>114799.32</v>
+        <v>2324532.69</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -928,16 +928,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -946,48 +946,48 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="F9" t="n">
-        <v>15390</v>
+        <v>120951</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>32.98</v>
+        <v>23.04</v>
       </c>
       <c r="K9" t="n">
-        <v>1484.1</v>
+        <v>6151.679999999999</v>
       </c>
       <c r="L9" t="n">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="M9" t="n">
-        <v>13905.9</v>
+        <v>114799.32</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>74.205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>653</v>
+        <v>342</v>
       </c>
       <c r="F10" t="n">
-        <v>158026</v>
+        <v>15048</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>23.28</v>
+        <v>32.98</v>
       </c>
       <c r="K10" t="n">
-        <v>5633.76</v>
+        <v>1451.12</v>
       </c>
       <c r="L10" t="n">
-        <v>242</v>
+        <v>44</v>
       </c>
       <c r="M10" t="n">
-        <v>152392.24</v>
+        <v>13596.88</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1041,41 +1041,41 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>281.688</v>
+        <v>72.556</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Facility 5</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>342</v>
+      </c>
+      <c r="F11" t="n">
+        <v>342</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>432</v>
-      </c>
-      <c r="F11" t="n">
-        <v>286848</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H11" t="n">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1083,16 +1083,16 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>22.77</v>
+        <v>53.46</v>
       </c>
       <c r="K11" t="n">
-        <v>15119.28</v>
+        <v>53.46</v>
       </c>
       <c r="L11" t="n">
-        <v>664</v>
+        <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>271728.72</v>
+        <v>288.54</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>456</v>
+        <v>653</v>
       </c>
       <c r="F12" t="n">
-        <v>10488</v>
+        <v>157373</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1134,7 +1134,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1142,16 +1142,16 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>12.61</v>
+        <v>23.28</v>
       </c>
       <c r="K12" t="n">
-        <v>290.03</v>
+        <v>5610.48</v>
       </c>
       <c r="L12" t="n">
-        <v>23</v>
+        <v>241</v>
       </c>
       <c r="M12" t="n">
-        <v>10197.97</v>
+        <v>151762.52</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1159,12 +1159,12 @@
         </is>
       </c>
       <c r="O12" t="n">
-        <v>14.5015</v>
+        <v>280.5240000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1182,35 +1182,35 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>456</v>
+        <v>653</v>
       </c>
       <c r="F13" t="n">
-        <v>456</v>
+        <v>653</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>23.04</v>
+        <v>41.58</v>
       </c>
       <c r="K13" t="n">
-        <v>23.04</v>
+        <v>41.58</v>
       </c>
       <c r="L13" t="n">
         <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>432.96</v>
+        <v>611.42</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1241,35 +1241,35 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>234</v>
+        <v>432</v>
       </c>
       <c r="F14" t="n">
-        <v>54054</v>
+        <v>286416</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>30.72</v>
+        <v>22.77</v>
       </c>
       <c r="K14" t="n">
-        <v>7096.32</v>
+        <v>15096.51</v>
       </c>
       <c r="L14" t="n">
-        <v>231</v>
+        <v>663</v>
       </c>
       <c r="M14" t="n">
-        <v>46957.68</v>
+        <v>271319.49</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1300,48 +1300,48 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>234</v>
+        <v>432</v>
       </c>
       <c r="F15" t="n">
-        <v>234</v>
+        <v>432</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>54.32</v>
+        <v>40.32</v>
       </c>
       <c r="K15" t="n">
-        <v>54.32</v>
+        <v>40.32</v>
       </c>
       <c r="L15" t="n">
         <v>1</v>
       </c>
       <c r="M15" t="n">
-        <v>179.68</v>
+        <v>391.68</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>2.716</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1359,10 +1359,10 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>231</v>
+        <v>456</v>
       </c>
       <c r="F16" t="n">
-        <v>2772</v>
+        <v>10488</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1381,13 +1381,13 @@
         <v>12.61</v>
       </c>
       <c r="K16" t="n">
-        <v>151.32</v>
+        <v>290.03</v>
       </c>
       <c r="L16" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="M16" t="n">
-        <v>2620.68</v>
+        <v>10197.97</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -1395,12 +1395,12 @@
         </is>
       </c>
       <c r="O16" t="n">
-        <v>7.566</v>
+        <v>14.5015</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Facility 10</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1418,10 +1418,10 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>231</v>
+        <v>456</v>
       </c>
       <c r="F17" t="n">
-        <v>231</v>
+        <v>456</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1437,23 +1437,259 @@
         </is>
       </c>
       <c r="J17" t="n">
-        <v>14.4</v>
+        <v>23.04</v>
       </c>
       <c r="K17" t="n">
-        <v>14.4</v>
+        <v>23.04</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
       </c>
       <c r="M17" t="n">
+        <v>432.96</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>9</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>234</v>
+      </c>
+      <c r="F18" t="n">
+        <v>54054</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>32</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>30.72</v>
+      </c>
+      <c r="K18" t="n">
+        <v>7096.32</v>
+      </c>
+      <c r="L18" t="n">
+        <v>231</v>
+      </c>
+      <c r="M18" t="n">
+        <v>46957.68</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>234</v>
+      </c>
+      <c r="F19" t="n">
+        <v>234</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>56</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>54.32</v>
+      </c>
+      <c r="K19" t="n">
+        <v>54.32</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" t="n">
+        <v>179.68</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>2.716</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>10</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>231</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2772</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>13</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>12.61</v>
+      </c>
+      <c r="K20" t="n">
+        <v>151.32</v>
+      </c>
+      <c r="L20" t="n">
+        <v>12</v>
+      </c>
+      <c r="M20" t="n">
+        <v>2620.68</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>7.566</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>10</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>231</v>
+      </c>
+      <c r="F21" t="n">
+        <v>231</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>15</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="K21" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="n">
         <v>216.6</v>
       </c>
-      <c r="N17" t="inlineStr">
+      <c r="N21" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O17" t="n">
+      <c r="O21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1629,44 +1865,72 @@
  &lt;= 97000000000
 SupplIndicatorLB_0_A_1: - w_0_A_1 + x_A_1 &gt;= 0
 SupplIndicatorLB_0_A_10: - w_0_A_10 + x_A_10 &gt;= 0
+SupplIndicatorLB_0_A_2: - w_0_A_2 + x_A_2 &gt;= 0
 SupplIndicatorLB_0_A_3: - w_0_A_3 + x_A_3 &gt;= 0
 SupplIndicatorLB_0_A_4: - w_0_A_4 + x_A_4 &gt;= 0
+SupplIndicatorLB_0_A_5: - w_0_A_5 + x_A_5 &gt;= 0
+SupplIndicatorLB_0_A_6: - w_0_A_6 + x_A_6 &gt;= 0
+SupplIndicatorLB_0_A_7: - w_0_A_7 + x_A_7 &gt;= 0
 SupplIndicatorLB_0_A_8: - w_0_A_8 + x_A_8 &gt;= 0
 SupplIndicatorLB_0_A_9: - w_0_A_9 + x_A_9 &gt;= 0
 SupplIndicatorLB_0_B_1: - w_0_B_1 + x_B_1 &gt;= 0
 SupplIndicatorLB_0_B_10: - w_0_B_10 + x_B_10 &gt;= 0
+SupplIndicatorLB_0_B_2: - w_0_B_2 + x_B_2 &gt;= 0
 SupplIndicatorLB_0_B_3: - w_0_B_3 + x_B_3 &gt;= 0
 SupplIndicatorLB_0_B_4: - w_0_B_4 + x_B_4 &gt;= 0
+SupplIndicatorLB_0_B_5: - w_0_B_5 + x_B_5 &gt;= 0
+SupplIndicatorLB_0_B_6: - w_0_B_6 + x_B_6 &gt;= 0
+SupplIndicatorLB_0_B_7: - w_0_B_7 + x_B_7 &gt;= 0
 SupplIndicatorLB_0_B_8: - w_0_B_8 + x_B_8 &gt;= 0
 SupplIndicatorLB_0_B_9: - w_0_B_9 + x_B_9 &gt;= 0
 SupplIndicatorLB_0_C_1: - w_0_C_1 + x_C_1 &gt;= 0
 SupplIndicatorLB_0_C_10: - w_0_C_10 + x_C_10 &gt;= 0
+SupplIndicatorLB_0_C_2: - w_0_C_2 + x_C_2 &gt;= 0
 SupplIndicatorLB_0_C_3: - w_0_C_3 + x_C_3 &gt;= 0
 SupplIndicatorLB_0_C_4: - w_0_C_4 + x_C_4 &gt;= 0
+SupplIndicatorLB_0_C_5: - w_0_C_5 + x_C_5 &gt;= 0
+SupplIndicatorLB_0_C_6: - w_0_C_6 + x_C_6 &gt;= 0
+SupplIndicatorLB_0_C_7: - w_0_C_7 + x_C_7 &gt;= 0
 SupplIndicatorLB_0_C_8: - w_0_C_8 + x_C_8 &gt;= 0
 SupplIndicatorLB_0_C_9: - w_0_C_9 + x_C_9 &gt;= 0
 SupplIndicator_0_A_1: - 1000000000 w_0_A_1 + x_A_1 &lt;= 0
 SupplIndicator_0_A_10: - 1000000000 w_0_A_10 + x_A_10 &lt;= 0
+SupplIndicator_0_A_2: - 1000000000 w_0_A_2 + x_A_2 &lt;= 0
 SupplIndicator_0_A_3: - 1000000000 w_0_A_3 + x_A_3 &lt;= 0
 SupplIndicator_0_A_4: - 1000000000 w_0_A_4 + x_A_4 &lt;= 0
+SupplIndicator_0_A_5: - 1000000000 w_0_A_5 + x_A_5 &lt;= 0
+SupplIndicator_0_A_6: - 1000000000 w_0_A_6 + x_A_6 &lt;= 0
+SupplIndicator_0_A_7: - 1000000000 w_0_A_7 + x_A_7 &lt;= 0
 SupplIndicator_0_A_8: - 1000000000 w_0_A_8 + x_A_8 &lt;= 0
 SupplIndicator_0_A_9: - 1000000000 w_0_A_9 + x_A_9 &lt;= 0
 SupplIndicator_0_B_1: - 1000000000 w_0_B_1 + x_B_1 &lt;= 0
 SupplIndicator_0_B_10: - 1000000000 w_0_B_10 + x_B_10 &lt;= 0
+SupplIndicator_0_B_2: - 1000000000 w_0_B_2 + x_B_2 &lt;= 0
 SupplIndicator_0_B_3: - 1000000000 w_0_B_3 + x_B_3 &lt;= 0
 SupplIndicator_0_B_4: - 1000000000 w_0_B_4 + x_B_4 &lt;= 0
+SupplIndicator_0_B_5: - 1000000000 w_0_B_5 + x_B_5 &lt;= 0
+SupplIndicator_0_B_6: - 1000000000 w_0_B_6 + x_B_6 &lt;= 0
+SupplIndicator_0_B_7: - 1000000000 w_0_B_7 + x_B_7 &lt;= 0
 SupplIndicator_0_B_8: - 1000000000 w_0_B_8 + x_B_8 &lt;= 0
 SupplIndicator_0_B_9: - 1000000000 w_0_B_9 + x_B_9 &lt;= 0
 SupplIndicator_0_C_1: - 1000000000 w_0_C_1 + x_C_1 &lt;= 0
 SupplIndicator_0_C_10: - 1000000000 w_0_C_10 + x_C_10 &lt;= 0
+SupplIndicator_0_C_2: - 1000000000 w_0_C_2 + x_C_2 &lt;= 0
 SupplIndicator_0_C_3: - 1000000000 w_0_C_3 + x_C_3 &lt;= 0
 SupplIndicator_0_C_4: - 1000000000 w_0_C_4 + x_C_4 &lt;= 0
+SupplIndicator_0_C_5: - 1000000000 w_0_C_5 + x_C_5 &lt;= 0
+SupplIndicator_0_C_6: - 1000000000 w_0_C_6 + x_C_6 &lt;= 0
+SupplIndicator_0_C_7: - 1000000000 w_0_C_7 + x_C_7 &lt;= 0
 SupplIndicator_0_C_8: - 1000000000 w_0_C_8 + x_C_8 &lt;= 0
 SupplIndicator_0_C_9: - 1000000000 w_0_C_9 + x_C_9 &lt;= 0
 SupplierCount_0_1: w_0_A_1 + w_0_B_1 + w_0_C_1 &gt;= 2
 SupplierCount_0_10: w_0_A_10 + w_0_B_10 + w_0_C_10 &gt;= 2
+SupplierCount_0_2: w_0_A_2 + w_0_B_2 + w_0_C_2 &gt;= 2
 SupplierCount_0_3: w_0_A_3 + w_0_B_3 + w_0_C_3 &gt;= 2
 SupplierCount_0_4: w_0_A_4 + w_0_B_4 + w_0_C_4 &gt;= 2
+SupplierCount_0_5: w_0_A_5 + w_0_B_5 + w_0_C_5 &gt;= 2
+SupplierCount_0_6: w_0_A_6 + w_0_B_6 + w_0_C_6 &gt;= 2
+SupplierCount_0_7: w_0_A_7 + w_0_B_7 + w_0_C_7 &gt;= 2
 SupplierCount_0_8: w_0_A_8 + w_0_B_8 + w_0_C_8 &gt;= 2
 SupplierCount_0_9: w_0_A_9 + w_0_B_9 + w_0_C_9 &gt;= 2
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
@@ -1718,20 +1982,32 @@
 T_9_B
 w_0_A_1
 w_0_A_10
+w_0_A_2
 w_0_A_3
 w_0_A_4
+w_0_A_5
+w_0_A_6
+w_0_A_7
 w_0_A_8
 w_0_A_9
 w_0_B_1
 w_0_B_10
+w_0_B_2
 w_0_B_3
 w_0_B_4
+w_0_B_5
+w_0_B_6
+w_0_B_7
 w_0_B_8
 w_0_B_9
 w_0_C_1
 w_0_C_10
+w_0_C_2
 w_0_C_3
 w_0_C_4
+w_0_C_5
+w_0_C_6
+w_0_C_7
 w_0_C_8
 w_0_C_9
 y_rebate_A_0

</xml_diff>

<commit_message>
logic changes to discount and rebate tiers
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>69900</v>
+        <v>70000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -555,47 +555,47 @@
         <v>0.519948</v>
       </c>
       <c r="K2" t="n">
-        <v>363.443652</v>
+        <v>363.9636</v>
       </c>
       <c r="L2" t="n">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>69536.556348</v>
+        <v>69636.0364</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>9%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>32.756724</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Facility 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Facility 1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="F3" t="n">
-        <v>100</v>
+        <v>1404000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -611,29 +611,29 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>9.699999999999999</v>
+        <v>67.89999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>9.699999999999999</v>
+        <v>611099.9999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>9000</v>
       </c>
       <c r="M3" t="n">
-        <v>90.3</v>
+        <v>792900.0000000001</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0.485</v>
+        <v>91664.99999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -642,27 +642,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Facility 1</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>423</v>
+      </c>
+      <c r="F4" t="n">
+        <v>195849</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>156</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1403844</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="H4" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -670,29 +670,29 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>67.89999999999999</v>
+        <v>63.05</v>
       </c>
       <c r="K4" t="n">
-        <v>611032.1</v>
+        <v>29192.15</v>
       </c>
       <c r="L4" t="n">
-        <v>8999</v>
+        <v>463</v>
       </c>
       <c r="M4" t="n">
-        <v>792811.9</v>
+        <v>166656.85</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>30551.605</v>
+        <v>4378.822499999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -701,19 +701,19 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Facility 1</t>
+          <t>Facility 4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>156</v>
+        <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>156</v>
+        <v>57951</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,29 +729,29 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>69.3</v>
+        <v>54.45</v>
       </c>
       <c r="K5" t="n">
-        <v>69.3</v>
+        <v>7459.650000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="M5" t="n">
-        <v>86.7</v>
+        <v>50491.35</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>9%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>671.3685</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -769,48 +769,48 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>195849</v>
+        <v>2356506</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>63.05</v>
+        <v>22.77</v>
       </c>
       <c r="K6" t="n">
-        <v>29192.15</v>
+        <v>118449.54</v>
       </c>
       <c r="L6" t="n">
-        <v>463</v>
+        <v>5202</v>
       </c>
       <c r="M6" t="n">
-        <v>166656.85</v>
+        <v>2238056.46</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>9%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>1459.6075</v>
+        <v>10660.4586</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -828,48 +828,48 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F7" t="n">
-        <v>57951</v>
+        <v>212004</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>54.45</v>
+        <v>23.04</v>
       </c>
       <c r="K7" t="n">
-        <v>7459.650000000001</v>
+        <v>10782.72</v>
       </c>
       <c r="L7" t="n">
-        <v>137</v>
+        <v>468</v>
       </c>
       <c r="M7" t="n">
-        <v>50491.35</v>
+        <v>201221.28</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>754.7904</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -887,73 +887,73 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F8" t="n">
-        <v>2447559</v>
+        <v>15390</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>22.77</v>
+        <v>32.98</v>
       </c>
       <c r="K8" t="n">
-        <v>123026.31</v>
+        <v>1484.1</v>
       </c>
       <c r="L8" t="n">
-        <v>5403</v>
+        <v>45</v>
       </c>
       <c r="M8" t="n">
-        <v>2324532.69</v>
+        <v>13905.9</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>222.615</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Facility 9</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>653</v>
+      </c>
+      <c r="F9" t="n">
+        <v>158026</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>B</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Facility 4</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>453</v>
-      </c>
-      <c r="F9" t="n">
-        <v>120951</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>C</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -961,33 +961,33 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>23.04</v>
+        <v>23.28</v>
       </c>
       <c r="K9" t="n">
-        <v>6151.679999999999</v>
+        <v>5633.76</v>
       </c>
       <c r="L9" t="n">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="M9" t="n">
-        <v>114799.32</v>
+        <v>152392.24</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>845.064</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,107 +1005,107 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>342</v>
+        <v>432</v>
       </c>
       <c r="F10" t="n">
-        <v>15048</v>
+        <v>286848</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>32.98</v>
+        <v>22.77</v>
       </c>
       <c r="K10" t="n">
-        <v>1451.12</v>
+        <v>15119.28</v>
       </c>
       <c r="L10" t="n">
-        <v>44</v>
+        <v>664</v>
       </c>
       <c r="M10" t="n">
-        <v>13596.88</v>
+        <v>271728.72</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>9%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>72.556</v>
+        <v>1360.7352</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Facility 9</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>456</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10944</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Facility 5</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>342</v>
-      </c>
-      <c r="F11" t="n">
-        <v>342</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H11" t="n">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>53.46</v>
+        <v>12.61</v>
       </c>
       <c r="K11" t="n">
-        <v>53.46</v>
+        <v>302.64</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="M11" t="n">
-        <v>288.54</v>
+        <v>10641.36</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>45.39599999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1123,574 +1123,102 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>653</v>
+        <v>234</v>
       </c>
       <c r="F12" t="n">
-        <v>157373</v>
+        <v>54288</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>23.28</v>
+        <v>30.72</v>
       </c>
       <c r="K12" t="n">
-        <v>5610.48</v>
+        <v>7127.04</v>
       </c>
       <c r="L12" t="n">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="M12" t="n">
-        <v>151762.52</v>
+        <v>47160.96</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>280.5240000000001</v>
+        <v>498.8928</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Facility 10</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>231</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3003</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>653</v>
-      </c>
-      <c r="F13" t="n">
-        <v>653</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H13" t="n">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>41.58</v>
+        <v>12.61</v>
       </c>
       <c r="K13" t="n">
-        <v>41.58</v>
+        <v>163.93</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="M13" t="n">
-        <v>611.42</v>
+        <v>2839.07</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>7</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>432</v>
-      </c>
-      <c r="F14" t="n">
-        <v>286416</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>23</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>1%</t>
-        </is>
-      </c>
-      <c r="J14" t="n">
-        <v>22.77</v>
-      </c>
-      <c r="K14" t="n">
-        <v>15096.51</v>
-      </c>
-      <c r="L14" t="n">
-        <v>663</v>
-      </c>
-      <c r="M14" t="n">
-        <v>271319.49</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>7</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>432</v>
-      </c>
-      <c r="F15" t="n">
-        <v>432</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>42</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J15" t="n">
-        <v>40.32</v>
-      </c>
-      <c r="K15" t="n">
-        <v>40.32</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" t="n">
-        <v>391.68</v>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>8</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>456</v>
-      </c>
-      <c r="F16" t="n">
-        <v>10488</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>13</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J16" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K16" t="n">
-        <v>290.03</v>
-      </c>
-      <c r="L16" t="n">
-        <v>23</v>
-      </c>
-      <c r="M16" t="n">
-        <v>10197.97</v>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O16" t="n">
-        <v>14.5015</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>8</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>456</v>
-      </c>
-      <c r="F17" t="n">
-        <v>456</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>24</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
-        <v>23.04</v>
-      </c>
-      <c r="K17" t="n">
-        <v>23.04</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" t="n">
-        <v>432.96</v>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>9</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>234</v>
-      </c>
-      <c r="F18" t="n">
-        <v>54054</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>32</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J18" t="n">
-        <v>30.72</v>
-      </c>
-      <c r="K18" t="n">
-        <v>7096.32</v>
-      </c>
-      <c r="L18" t="n">
-        <v>231</v>
-      </c>
-      <c r="M18" t="n">
-        <v>46957.68</v>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>9</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>234</v>
-      </c>
-      <c r="F19" t="n">
-        <v>234</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>56</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J19" t="n">
-        <v>54.32</v>
-      </c>
-      <c r="K19" t="n">
-        <v>54.32</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1</v>
-      </c>
-      <c r="M19" t="n">
-        <v>179.68</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O19" t="n">
-        <v>2.716</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>10</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>231</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2772</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>13</v>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J20" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K20" t="n">
-        <v>151.32</v>
-      </c>
-      <c r="L20" t="n">
-        <v>12</v>
-      </c>
-      <c r="M20" t="n">
-        <v>2620.68</v>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="O20" t="n">
-        <v>7.566</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>10</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>231</v>
-      </c>
-      <c r="F21" t="n">
-        <v>231</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>15</v>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J21" t="n">
-        <v>14.4</v>
-      </c>
-      <c r="K21" t="n">
-        <v>14.4</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1</v>
-      </c>
-      <c r="M21" t="n">
-        <v>216.6</v>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O21" t="n">
-        <v>0</v>
+        <v>24.5895</v>
       </c>
     </row>
   </sheetData>
@@ -1804,18 +1332,24 @@
 DiscountTierLower_C_0: d_C - 97000000000 z_discount_C_0 &gt;= -97000000000
 DiscountTierLower_C_1: - 0.04 S0_C + d_C - 97000000000 z_discount_C_1
  &gt;= -97000000000
-DiscountTierMax_A_0: 19400000000 z_discount_A_0 &lt;= 19400001000
-DiscountTierMax_B_0: 97000000000 z_discount_B_0 &lt;= 97000000500
-DiscountTierMax_C_0: 97000000000 z_discount_C_0 &lt;= 97000000500
-_dummy: __dummy = 0
-DiscountTierMin_A_0: __dummy &gt;= 0
-DiscountTierMin_A_1: x_A_1 + x_A_10 + x_A_3 + x_A_4 + x_A_8 + x_A_9
- - 1000 z_discount_A_1 &gt;= 0
-DiscountTierMin_B_0: __dummy &gt;= 0
-DiscountTierMin_B_1: x_B_2 + x_B_5 + x_B_6 + x_B_7 - 500 z_discount_B_1 &gt;= 0
-DiscountTierMin_C_0: __dummy &gt;= 0
-DiscountTierMin_C_1: x_C_1 + x_C_10 + x_C_3 + x_C_4 + x_C_8 + x_C_9
- - 500 z_discount_C_1 &gt;= 0
+DiscountTierMax_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
+ + x_A_7 + x_A_8 + x_A_9 + 19400000000 z_discount_A_0 &lt;= 19400001000
+DiscountTierMax_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
+ + x_B_7 + x_B_8 + x_B_9 + 97000000000 z_discount_B_0 &lt;= 97000000500
+DiscountTierMax_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
+ + x_C_7 + x_C_8 + x_C_9 + 97000000000 z_discount_C_0 &lt;= 97000000500
+DiscountTierMin_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
+ + x_A_7 + x_A_8 + x_A_9 &gt;= 0
+DiscountTierMin_A_1: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
+ + x_A_7 + x_A_8 + x_A_9 - 1000 z_discount_A_1 &gt;= 0
+DiscountTierMin_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
+ + x_B_7 + x_B_8 + x_B_9 &gt;= 0
+DiscountTierMin_B_1: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
+ + x_B_7 + x_B_8 + x_B_9 - 500 z_discount_B_1 &gt;= 0
+DiscountTierMin_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
+ + x_C_7 + x_C_8 + x_C_9 &gt;= 0
+DiscountTierMin_C_1: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
+ + x_C_7 + x_C_8 + x_C_9 - 500 z_discount_C_1 &gt;= 0
 DiscountTierSelect_A: z_discount_A_0 + z_discount_A_1 = 1
 DiscountTierSelect_B: z_discount_B_0 + z_discount_B_1 = 1
 DiscountTierSelect_C: z_discount_C_0 + z_discount_C_1 = 1
@@ -1833,106 +1367,44 @@
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
 NonBid_C_5: x_C_5 = 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
-RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
+RebateTierLower_A_1: - 0.09 S_A + rebate_A - 19400000000 y_rebate_A_1
  &gt;= -19400000000
 RebateTierLower_B_0: rebate_B - 97000000000 y_rebate_B_0 &gt;= -97000000000
-RebateTierLower_B_1: - 0.05 S_B + rebate_B - 97000000000 y_rebate_B_1
+RebateTierLower_B_1: - 0.15 S_B + rebate_B - 97000000000 y_rebate_B_1
  &gt;= -97000000000
 RebateTierLower_C_0: rebate_C - 97000000000 y_rebate_C_0 &gt;= -97000000000
 RebateTierLower_C_1: - 0.07 S_C + rebate_C - 97000000000 y_rebate_C_1
  &gt;= -97000000000
-RebateTierMax_A_0: 19400000000 y_rebate_A_0 &lt;= 19400000500
-RebateTierMax_B_0: 97000000000 y_rebate_B_0 &lt;= 97000000500
-RebateTierMax_C_0: 97000000000 y_rebate_C_0 &lt;= 97000000700
-RebateTierMin_A_0: __dummy &gt;= 0
-RebateTierMin_A_1: - 500 y_rebate_A_1 &gt;= 0
-RebateTierMin_B_0: __dummy &gt;= 0
+RebateTierMax_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
+ + x_A_7 + x_A_8 + x_A_9 + 19400000000 y_rebate_A_0 &lt;= 19400000500
+RebateTierMax_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
+ + x_B_7 + x_B_8 + x_B_9 + 97000000000 y_rebate_B_0 &lt;= 97000000300
+RebateTierMax_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
+ + x_C_7 + x_C_8 + x_C_9 + 97000000000 y_rebate_C_0 &lt;= 97000000700
+RebateTierMin_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
+ + x_A_7 + x_A_8 + x_A_9 &gt;= 0
+RebateTierMin_A_1: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
+ + x_A_7 + x_A_8 + x_A_9 - 500 y_rebate_A_1 &gt;= 0
+RebateTierMin_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
+ + x_B_7 + x_B_8 + x_B_9 &gt;= 0
 RebateTierMin_B_1: x_B_1 + x_B_10 + x_B_3 + x_B_4 + x_B_8 + x_B_9
  - 500 y_rebate_B_1 &gt;= 0
-RebateTierMin_C_0: __dummy &gt;= 0
-RebateTierMin_C_1: - 700 y_rebate_C_1 &gt;= 0
+RebateTierMin_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
+ + x_C_7 + x_C_8 + x_C_9 &gt;= 0
+RebateTierMin_C_1: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
+ + x_C_7 + x_C_8 + x_C_9 - 700 y_rebate_C_1 &gt;= 0
 RebateTierSelect_A: y_rebate_A_0 + y_rebate_A_1 = 1
 RebateTierSelect_B: y_rebate_B_0 + y_rebate_B_1 = 1
 RebateTierSelect_C: y_rebate_C_0 + y_rebate_C_1 = 1
 RebateTierUpper_A_0: rebate_A + 19400000000 y_rebate_A_0 &lt;= 19400000000
-RebateTierUpper_A_1: - 0.1 S_A + rebate_A + 19400000000 y_rebate_A_1
+RebateTierUpper_A_1: - 0.09 S_A + rebate_A + 19400000000 y_rebate_A_1
  &lt;= 19400000000
 RebateTierUpper_B_0: rebate_B + 97000000000 y_rebate_B_0 &lt;= 97000000000
-RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 97000000000 y_rebate_B_1
+RebateTierUpper_B_1: - 0.15 S_B + rebate_B + 97000000000 y_rebate_B_1
  &lt;= 97000000000
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-SupplIndicatorLB_0_A_1: - w_0_A_1 + x_A_1 &gt;= 0
-SupplIndicatorLB_0_A_10: - w_0_A_10 + x_A_10 &gt;= 0
-SupplIndicatorLB_0_A_2: - w_0_A_2 + x_A_2 &gt;= 0
-SupplIndicatorLB_0_A_3: - w_0_A_3 + x_A_3 &gt;= 0
-SupplIndicatorLB_0_A_4: - w_0_A_4 + x_A_4 &gt;= 0
-SupplIndicatorLB_0_A_5: - w_0_A_5 + x_A_5 &gt;= 0
-SupplIndicatorLB_0_A_6: - w_0_A_6 + x_A_6 &gt;= 0
-SupplIndicatorLB_0_A_7: - w_0_A_7 + x_A_7 &gt;= 0
-SupplIndicatorLB_0_A_8: - w_0_A_8 + x_A_8 &gt;= 0
-SupplIndicatorLB_0_A_9: - w_0_A_9 + x_A_9 &gt;= 0
-SupplIndicatorLB_0_B_1: - w_0_B_1 + x_B_1 &gt;= 0
-SupplIndicatorLB_0_B_10: - w_0_B_10 + x_B_10 &gt;= 0
-SupplIndicatorLB_0_B_2: - w_0_B_2 + x_B_2 &gt;= 0
-SupplIndicatorLB_0_B_3: - w_0_B_3 + x_B_3 &gt;= 0
-SupplIndicatorLB_0_B_4: - w_0_B_4 + x_B_4 &gt;= 0
-SupplIndicatorLB_0_B_5: - w_0_B_5 + x_B_5 &gt;= 0
-SupplIndicatorLB_0_B_6: - w_0_B_6 + x_B_6 &gt;= 0
-SupplIndicatorLB_0_B_7: - w_0_B_7 + x_B_7 &gt;= 0
-SupplIndicatorLB_0_B_8: - w_0_B_8 + x_B_8 &gt;= 0
-SupplIndicatorLB_0_B_9: - w_0_B_9 + x_B_9 &gt;= 0
-SupplIndicatorLB_0_C_1: - w_0_C_1 + x_C_1 &gt;= 0
-SupplIndicatorLB_0_C_10: - w_0_C_10 + x_C_10 &gt;= 0
-SupplIndicatorLB_0_C_2: - w_0_C_2 + x_C_2 &gt;= 0
-SupplIndicatorLB_0_C_3: - w_0_C_3 + x_C_3 &gt;= 0
-SupplIndicatorLB_0_C_4: - w_0_C_4 + x_C_4 &gt;= 0
-SupplIndicatorLB_0_C_5: - w_0_C_5 + x_C_5 &gt;= 0
-SupplIndicatorLB_0_C_6: - w_0_C_6 + x_C_6 &gt;= 0
-SupplIndicatorLB_0_C_7: - w_0_C_7 + x_C_7 &gt;= 0
-SupplIndicatorLB_0_C_8: - w_0_C_8 + x_C_8 &gt;= 0
-SupplIndicatorLB_0_C_9: - w_0_C_9 + x_C_9 &gt;= 0
-SupplIndicator_0_A_1: - 1000000000 w_0_A_1 + x_A_1 &lt;= 0
-SupplIndicator_0_A_10: - 1000000000 w_0_A_10 + x_A_10 &lt;= 0
-SupplIndicator_0_A_2: - 1000000000 w_0_A_2 + x_A_2 &lt;= 0
-SupplIndicator_0_A_3: - 1000000000 w_0_A_3 + x_A_3 &lt;= 0
-SupplIndicator_0_A_4: - 1000000000 w_0_A_4 + x_A_4 &lt;= 0
-SupplIndicator_0_A_5: - 1000000000 w_0_A_5 + x_A_5 &lt;= 0
-SupplIndicator_0_A_6: - 1000000000 w_0_A_6 + x_A_6 &lt;= 0
-SupplIndicator_0_A_7: - 1000000000 w_0_A_7 + x_A_7 &lt;= 0
-SupplIndicator_0_A_8: - 1000000000 w_0_A_8 + x_A_8 &lt;= 0
-SupplIndicator_0_A_9: - 1000000000 w_0_A_9 + x_A_9 &lt;= 0
-SupplIndicator_0_B_1: - 1000000000 w_0_B_1 + x_B_1 &lt;= 0
-SupplIndicator_0_B_10: - 1000000000 w_0_B_10 + x_B_10 &lt;= 0
-SupplIndicator_0_B_2: - 1000000000 w_0_B_2 + x_B_2 &lt;= 0
-SupplIndicator_0_B_3: - 1000000000 w_0_B_3 + x_B_3 &lt;= 0
-SupplIndicator_0_B_4: - 1000000000 w_0_B_4 + x_B_4 &lt;= 0
-SupplIndicator_0_B_5: - 1000000000 w_0_B_5 + x_B_5 &lt;= 0
-SupplIndicator_0_B_6: - 1000000000 w_0_B_6 + x_B_6 &lt;= 0
-SupplIndicator_0_B_7: - 1000000000 w_0_B_7 + x_B_7 &lt;= 0
-SupplIndicator_0_B_8: - 1000000000 w_0_B_8 + x_B_8 &lt;= 0
-SupplIndicator_0_B_9: - 1000000000 w_0_B_9 + x_B_9 &lt;= 0
-SupplIndicator_0_C_1: - 1000000000 w_0_C_1 + x_C_1 &lt;= 0
-SupplIndicator_0_C_10: - 1000000000 w_0_C_10 + x_C_10 &lt;= 0
-SupplIndicator_0_C_2: - 1000000000 w_0_C_2 + x_C_2 &lt;= 0
-SupplIndicator_0_C_3: - 1000000000 w_0_C_3 + x_C_3 &lt;= 0
-SupplIndicator_0_C_4: - 1000000000 w_0_C_4 + x_C_4 &lt;= 0
-SupplIndicator_0_C_5: - 1000000000 w_0_C_5 + x_C_5 &lt;= 0
-SupplIndicator_0_C_6: - 1000000000 w_0_C_6 + x_C_6 &lt;= 0
-SupplIndicator_0_C_7: - 1000000000 w_0_C_7 + x_C_7 &lt;= 0
-SupplIndicator_0_C_8: - 1000000000 w_0_C_8 + x_C_8 &lt;= 0
-SupplIndicator_0_C_9: - 1000000000 w_0_C_9 + x_C_9 &lt;= 0
-SupplierCount_0_1: w_0_A_1 + w_0_B_1 + w_0_C_1 &gt;= 2
-SupplierCount_0_10: w_0_A_10 + w_0_B_10 + w_0_C_10 &gt;= 2
-SupplierCount_0_2: w_0_A_2 + w_0_B_2 + w_0_C_2 &gt;= 2
-SupplierCount_0_3: w_0_A_3 + w_0_B_3 + w_0_C_3 &gt;= 2
-SupplierCount_0_4: w_0_A_4 + w_0_B_4 + w_0_C_4 &gt;= 2
-SupplierCount_0_5: w_0_A_5 + w_0_B_5 + w_0_C_5 &gt;= 2
-SupplierCount_0_6: w_0_A_6 + w_0_B_6 + w_0_C_6 &gt;= 2
-SupplierCount_0_7: w_0_A_7 + w_0_B_7 + w_0_C_7 &gt;= 2
-SupplierCount_0_8: w_0_A_8 + w_0_B_8 + w_0_C_8 &gt;= 2
-SupplierCount_0_9: w_0_A_9 + w_0_B_9 + w_0_C_9 &gt;= 2
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1980,36 +1452,6 @@
 T_8_B
 T_9_A
 T_9_B
-w_0_A_1
-w_0_A_10
-w_0_A_2
-w_0_A_3
-w_0_A_4
-w_0_A_5
-w_0_A_6
-w_0_A_7
-w_0_A_8
-w_0_A_9
-w_0_B_1
-w_0_B_10
-w_0_B_2
-w_0_B_3
-w_0_B_4
-w_0_B_5
-w_0_B_6
-w_0_B_7
-w_0_B_8
-w_0_B_9
-w_0_C_1
-w_0_C_10
-w_0_C_2
-w_0_C_3
-w_0_C_4
-w_0_C_5
-w_0_C_6
-w_0_C_7
-w_0_C_8
-w_0_C_9
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
updates to % of volume awarded rule
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -599,7 +599,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -607,28 +607,28 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>69.3</v>
+        <v>67.89999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>623700</v>
+        <v>611099.9999999999</v>
       </c>
       <c r="L3" t="n">
         <v>9000</v>
       </c>
       <c r="M3" t="n">
-        <v>780300</v>
+        <v>792900.0000000001</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>56133</v>
+        <v>91664.99999999999</v>
       </c>
     </row>
     <row r="4">
@@ -654,74 +654,74 @@
         <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>253800</v>
+        <v>195849</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>54.45</v>
+        <v>63.05</v>
       </c>
       <c r="K4" t="n">
-        <v>32670</v>
+        <v>29192.15</v>
       </c>
       <c r="L4" t="n">
-        <v>600</v>
+        <v>463</v>
       </c>
       <c r="M4" t="n">
-        <v>221130</v>
+        <v>166656.85</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>2940.3</v>
+        <v>4378.822499999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Facility 4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>423</v>
+      </c>
+      <c r="F5" t="n">
+        <v>57951</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Facility 4</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>453</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2367378</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="H5" t="n">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>22.77</v>
+        <v>54.45</v>
       </c>
       <c r="K5" t="n">
-        <v>118996.02</v>
+        <v>7459.650000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>5226</v>
+        <v>137</v>
       </c>
       <c r="M5" t="n">
-        <v>2248381.98</v>
+        <v>50491.35</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>10709.6418</v>
+        <v>671.3685</v>
       </c>
     </row>
     <row r="6">
@@ -755,7 +755,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -772,7 +772,7 @@
         <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>201132</v>
+        <v>2231025</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -791,13 +791,13 @@
         <v>23.04</v>
       </c>
       <c r="K6" t="n">
-        <v>10229.76</v>
+        <v>113472</v>
       </c>
       <c r="L6" t="n">
-        <v>444</v>
+        <v>4925</v>
       </c>
       <c r="M6" t="n">
-        <v>190902.24</v>
+        <v>2117553</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -805,71 +805,71 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>716.0832</v>
+        <v>7943.040000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Facility 4</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>453</v>
+      </c>
+      <c r="F7" t="n">
+        <v>337485</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Facility 5</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>342</v>
-      </c>
-      <c r="F7" t="n">
-        <v>15390</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
       <c r="H7" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>34</v>
+        <v>22.77</v>
       </c>
       <c r="K7" t="n">
-        <v>1530</v>
+        <v>16963.65</v>
       </c>
       <c r="L7" t="n">
-        <v>45</v>
+        <v>745</v>
       </c>
       <c r="M7" t="n">
-        <v>13860</v>
+        <v>320521.35</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>9%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>1526.7285</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -887,10 +887,10 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>653</v>
+        <v>342</v>
       </c>
       <c r="F8" t="n">
-        <v>158026</v>
+        <v>15390</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -898,37 +898,37 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>24</v>
+        <v>32.98</v>
       </c>
       <c r="K8" t="n">
-        <v>5808</v>
+        <v>1484.1</v>
       </c>
       <c r="L8" t="n">
-        <v>242</v>
+        <v>45</v>
       </c>
       <c r="M8" t="n">
-        <v>152218</v>
+        <v>13905.9</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>222.615</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,48 +946,48 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>432</v>
+        <v>653</v>
       </c>
       <c r="F9" t="n">
-        <v>286848</v>
+        <v>158026</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>22.77</v>
+        <v>23.28</v>
       </c>
       <c r="K9" t="n">
-        <v>15119.28</v>
+        <v>5633.76</v>
       </c>
       <c r="L9" t="n">
-        <v>664</v>
+        <v>242</v>
       </c>
       <c r="M9" t="n">
-        <v>271728.72</v>
+        <v>152392.24</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>1360.7352</v>
+        <v>845.064</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1005,43 +1005,43 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F10" t="n">
-        <v>5928.000456</v>
+        <v>286848</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>13</v>
+        <v>22.77</v>
       </c>
       <c r="K10" t="n">
-        <v>169.000013</v>
+        <v>15119.28</v>
       </c>
       <c r="L10" t="n">
-        <v>13.000001</v>
+        <v>664</v>
       </c>
       <c r="M10" t="n">
-        <v>5759.000443</v>
+        <v>271728.72</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>9%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>1360.7352</v>
       </c>
     </row>
     <row r="11">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1067,40 +1067,40 @@
         <v>456</v>
       </c>
       <c r="F11" t="n">
-        <v>5015.999544</v>
+        <v>10944</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H11" t="n">
+        <v>13</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>12.61</v>
+      </c>
+      <c r="K11" t="n">
+        <v>302.64</v>
+      </c>
+      <c r="L11" t="n">
         <v>24</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
-        <v>23.04</v>
-      </c>
-      <c r="K11" t="n">
-        <v>253.43997696</v>
-      </c>
-      <c r="L11" t="n">
-        <v>10.999999</v>
-      </c>
       <c r="M11" t="n">
-        <v>4762.55956704</v>
+        <v>10641.36</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>17.7407983872</v>
+        <v>45.39599999999999</v>
       </c>
     </row>
     <row r="12">
@@ -1189,36 +1189,36 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>14.4</v>
+        <v>12.61</v>
       </c>
       <c r="K13" t="n">
-        <v>187.2</v>
+        <v>163.93</v>
       </c>
       <c r="L13" t="n">
         <v>13</v>
       </c>
       <c r="M13" t="n">
-        <v>2815.8</v>
+        <v>2839.07</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>13.104</v>
+        <v>24.5895</v>
       </c>
     </row>
   </sheetData>
@@ -1293,7 +1293,6 @@
  - 34 x_B_5 - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
 BaseSpend_C: S0_C - 24 x_C_1 - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
  - 44 x_C_6 - 42 x_C_7 - 24 x_C_8 - 32 x_C_9 = 0
-BidExclusion_0_2_B: x_B_2 = 0
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
 Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000
@@ -1406,6 +1405,12 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
+Rule_0_aggregate: - 0.3 x_A_1 - 0.3 x_A_10 - 0.3 x_A_2 - 0.3 x_A_3 - 0.3 x_A_4
+ - 0.3 x_A_5 - 0.3 x_A_6 - 0.3 x_A_7 - 0.3 x_A_8 - 0.3 x_A_9 - 0.3 x_B_1
+ - 0.3 x_B_10 - 0.3 x_B_2 - 0.3 x_B_3 - 0.3 x_B_4 - 0.3 x_B_5 - 0.3 x_B_6
+ - 0.3 x_B_7 - 0.3 x_B_8 - 0.3 x_B_9 + 0.7 x_C_1 + 0.7 x_C_10 + 0.7 x_C_2
+ + 0.7 x_C_3 + 0.7 x_C_4 + 0.7 x_C_5 + 0.7 x_C_6 + 0.7 x_C_7 + 0.7 x_C_8
+ + 0.7 x_C_9 &gt;= 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0

</xml_diff>

<commit_message>
Fixed % of Volume Awarded
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,36 +540,36 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.5252</v>
+        <v>55</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.519948</v>
+        <v>52.8</v>
       </c>
       <c r="K2" t="n">
-        <v>363.9636</v>
+        <v>36960</v>
       </c>
       <c r="L2" t="n">
         <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>69636.0364</v>
+        <v>33040</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>32.756724</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -611,24 +611,24 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>67.89999999999999</v>
+        <v>77.59999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>611099.9999999999</v>
+        <v>698400</v>
       </c>
       <c r="L3" t="n">
         <v>9000</v>
       </c>
       <c r="M3" t="n">
-        <v>792900.0000000001</v>
+        <v>705600</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>15%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>91664.99999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -654,40 +654,40 @@
         <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>195849</v>
+        <v>142127.27244</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>63.05</v>
+        <v>54.45</v>
       </c>
       <c r="K4" t="n">
-        <v>29192.15</v>
+        <v>18295.106346</v>
       </c>
       <c r="L4" t="n">
-        <v>463</v>
+        <v>335.99828</v>
       </c>
       <c r="M4" t="n">
-        <v>166656.85</v>
+        <v>123832.166094</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>15%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>4378.822499999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -713,40 +713,40 @@
         <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>57951</v>
+        <v>111672.72756</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>54.45</v>
+        <v>63.05</v>
       </c>
       <c r="K5" t="n">
-        <v>7459.650000000001</v>
+        <v>16645.308446</v>
       </c>
       <c r="L5" t="n">
-        <v>137</v>
+        <v>264.00172</v>
       </c>
       <c r="M5" t="n">
-        <v>50491.35</v>
+        <v>95027.41911399999</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>671.3685</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -772,54 +772,54 @@
         <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>2231025</v>
+        <v>2568510</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>23.04</v>
+        <v>72.75</v>
       </c>
       <c r="K6" t="n">
-        <v>113472</v>
+        <v>412492.5</v>
       </c>
       <c r="L6" t="n">
-        <v>4925</v>
+        <v>5670</v>
       </c>
       <c r="M6" t="n">
-        <v>2117553</v>
+        <v>2156017.5</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>7943.040000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,48 +828,48 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F7" t="n">
-        <v>337485</v>
+        <v>15390</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>22.77</v>
+        <v>23.04</v>
       </c>
       <c r="K7" t="n">
-        <v>16963.65</v>
+        <v>1036.8</v>
       </c>
       <c r="L7" t="n">
-        <v>745</v>
+        <v>45</v>
       </c>
       <c r="M7" t="n">
-        <v>320521.35</v>
+        <v>14353.2</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>1526.7285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -887,10 +887,10 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>342</v>
+        <v>653</v>
       </c>
       <c r="F8" t="n">
-        <v>15390</v>
+        <v>158026</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -906,29 +906,29 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>32.98</v>
+        <v>23.28</v>
       </c>
       <c r="K8" t="n">
-        <v>1484.1</v>
+        <v>5633.76</v>
       </c>
       <c r="L8" t="n">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="M8" t="n">
-        <v>13905.9</v>
+        <v>152392.24</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>15%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>222.615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,48 +946,48 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>653</v>
+        <v>432</v>
       </c>
       <c r="F9" t="n">
-        <v>158026</v>
+        <v>286848</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>23.28</v>
+        <v>22.77</v>
       </c>
       <c r="K9" t="n">
-        <v>5633.76</v>
+        <v>15119.28</v>
       </c>
       <c r="L9" t="n">
-        <v>242</v>
+        <v>664</v>
       </c>
       <c r="M9" t="n">
-        <v>152392.24</v>
+        <v>271728.72</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>15%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>845.064</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1005,48 +1005,48 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="F10" t="n">
-        <v>286848</v>
+        <v>10944</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>22.77</v>
+        <v>12.61</v>
       </c>
       <c r="K10" t="n">
-        <v>15119.28</v>
+        <v>302.64</v>
       </c>
       <c r="L10" t="n">
-        <v>664</v>
+        <v>24</v>
       </c>
       <c r="M10" t="n">
-        <v>271728.72</v>
+        <v>10641.36</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>1360.7352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1064,14 +1064,14 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>456</v>
+        <v>234</v>
       </c>
       <c r="F11" t="n">
-        <v>10944</v>
+        <v>54288</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -1079,33 +1079,33 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>12.61</v>
+        <v>12.48</v>
       </c>
       <c r="K11" t="n">
-        <v>302.64</v>
+        <v>2895.36</v>
       </c>
       <c r="L11" t="n">
-        <v>24</v>
+        <v>232</v>
       </c>
       <c r="M11" t="n">
-        <v>10641.36</v>
+        <v>51392.64</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>15%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>45.39599999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1123,102 +1123,43 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F12" t="n">
-        <v>54288</v>
+        <v>3003</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>30.72</v>
+        <v>12.61</v>
       </c>
       <c r="K12" t="n">
-        <v>7127.04</v>
+        <v>163.93</v>
       </c>
       <c r="L12" t="n">
-        <v>232</v>
+        <v>13</v>
       </c>
       <c r="M12" t="n">
-        <v>47160.96</v>
+        <v>2839.07</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>498.8928</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>10</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>231</v>
-      </c>
-      <c r="F13" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>13</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>3%</t>
-        </is>
-      </c>
-      <c r="J13" t="n">
-        <v>12.61</v>
-      </c>
-      <c r="K13" t="n">
-        <v>163.93</v>
-      </c>
-      <c r="L13" t="n">
-        <v>13</v>
-      </c>
-      <c r="M13" t="n">
-        <v>2839.07</v>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>15%</t>
-        </is>
-      </c>
-      <c r="O13" t="n">
-        <v>24.5895</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1191,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model is optimal.</t>
+          <t>Model is infeasible. Likely causes include:
+ - Insufficient supplier capacity relative to demand.
+ - Custom rule constraints conflicting with overall volume/demand.
+Detailed Rule Evaluations:
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 1, total demand: 700 units; a 30% allocation requires 210.0 units for All.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 2, total demand: 9000 units; a 30% allocation requires 2700.0 units for All.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 3, total demand: 600 units; a 30% allocation requires 180.0 units for All.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 4, total demand: 5670 units; a 30% allocation requires 1701.0 units for All.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 5, total demand: 45 units; a 30% allocation requires 13.5 units for All.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 6, total demand: 242 units; a 30% allocation requires 72.6 units for All.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 7, total demand: 664 units; a 30% allocation requires 199.2 units for All.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 8, total demand: 24 units; a 30% allocation requires 7.2 units for All.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 9, total demand: 232 units; a 30% allocation requires 69.6 units for All.
+Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 10, total demand: 13 units; a 30% allocation requires 3.9 units for All.
+Review supplier capacities, demand, and custom rule constraints for adjustments.</t>
         </is>
       </c>
     </row>
@@ -1287,12 +1242,36 @@
 Minimize
 OBJ: S_A + S_B + S_C - rebate_A - rebate_B - rebate_C
 Subject To
-BaseSpend_A: S0_A - 0.5252 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
+%VolAwarded_Agg_0_A_UB: 0.7 x_A_1 + 0.7 x_A_10 + 0.7 x_A_2 + 0.7 x_A_3
+ + 0.7 x_A_4 + 0.7 x_A_5 + 0.7 x_A_6 + 0.7 x_A_7 + 0.7 x_A_8 + 0.7 x_A_9
+ - 0.3 x_B_1 - 0.3 x_B_10 - 0.3 x_B_2 - 0.3 x_B_3 - 0.3 x_B_4 - 0.3 x_B_5
+ - 0.3 x_B_6 - 0.3 x_B_7 - 0.3 x_B_8 - 0.3 x_B_9 - 0.3 x_C_1 - 0.3 x_C_10
+ - 0.3 x_C_2 - 0.3 x_C_3 - 0.3 x_C_4 - 0.3 x_C_5 - 0.3 x_C_6 - 0.3 x_C_7
+ - 0.3 x_C_8 - 0.3 x_C_9 + 1000000000 y_0_A &lt;= 1000000000
+%VolAwarded_Agg_0_B_UB: - 0.3 x_A_1 - 0.3 x_A_10 - 0.3 x_A_2 - 0.3 x_A_3
+ - 0.3 x_A_4 - 0.3 x_A_5 - 0.3 x_A_6 - 0.3 x_A_7 - 0.3 x_A_8 - 0.3 x_A_9
+ + 0.7 x_B_1 + 0.7 x_B_10 + 0.7 x_B_2 + 0.7 x_B_3 + 0.7 x_B_4 + 0.7 x_B_5
+ + 0.7 x_B_6 + 0.7 x_B_7 + 0.7 x_B_8 + 0.7 x_B_9 - 0.3 x_C_1 - 0.3 x_C_10
+ - 0.3 x_C_2 - 0.3 x_C_3 - 0.3 x_C_4 - 0.3 x_C_5 - 0.3 x_C_6 - 0.3 x_C_7
+ - 0.3 x_C_8 - 0.3 x_C_9 + 1000000000 y_0_B &lt;= 1000000000
+%VolAwarded_Agg_0_C_UB: - 0.3 x_A_1 - 0.3 x_A_10 - 0.3 x_A_2 - 0.3 x_A_3
+ - 0.3 x_A_4 - 0.3 x_A_5 - 0.3 x_A_6 - 0.3 x_A_7 - 0.3 x_A_8 - 0.3 x_A_9
+ - 0.3 x_B_1 - 0.3 x_B_10 - 0.3 x_B_2 - 0.3 x_B_3 - 0.3 x_B_4 - 0.3 x_B_5
+ - 0.3 x_B_6 - 0.3 x_B_7 - 0.3 x_B_8 - 0.3 x_B_9 + 0.7 x_C_1 + 0.7 x_C_10
+ + 0.7 x_C_2 + 0.7 x_C_3 + 0.7 x_C_4 + 0.7 x_C_5 + 0.7 x_C_6 + 0.7 x_C_7
+ + 0.7 x_C_8 + 0.7 x_C_9 + 1000000000 y_0_C &lt;= 1000000000
+Active_0_A: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7
+ + x_A_8 + x_A_9 - 1000000000 y_0_A &lt;= 0
+Active_0_B: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7
+ + x_B_8 + x_B_9 - 1000000000 y_0_B &lt;= 0
+Active_0_C: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7
+ + x_C_8 + x_C_9 - 1000000000 y_0_C &lt;= 0
+BaseSpend_A: S0_A - 50 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
  - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
-BaseSpend_B: S0_B - 10 x_B_1 - 13 x_B_10 - 70 x_B_2 - 65 x_B_3 - 75 x_B_4
- - 34 x_B_5 - 24 x_B_6 - 85 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
-BaseSpend_C: S0_C - 24 x_C_1 - 15 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
- - 44 x_C_6 - 42 x_C_7 - 24 x_C_8 - 32 x_C_9 = 0
+BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 80 x_B_2 - 65 x_B_3 - 75 x_B_4
+ - 34 x_B_5 - 24 x_B_6 - 53 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
+BaseSpend_C: S0_C - 55 x_C_1 - 75 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
+ - 24 x_C_5 - 64 x_C_6 - 86 x_C_7 - 24 x_C_8 - 13 x_C_9 = 0
 Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
 Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
 Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000
@@ -1365,12 +1344,17 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
-NonBid_C_5: x_C_5 = 0
+MinActive_0_A: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7
+ + x_A_8 + x_A_9 - 0.001 y_0_A &gt;= 0
+MinActive_0_B: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7
+ + x_B_8 + x_B_9 - 0.001 y_0_B &gt;= 0
+MinActive_0_C: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7
+ + x_C_8 + x_C_9 - 0.001 y_0_C &gt;= 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
-RebateTierLower_A_1: - 0.09 S_A + rebate_A - 19400000000 y_rebate_A_1
+RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
  &gt;= -19400000000
 RebateTierLower_B_0: rebate_B - 97000000000 y_rebate_B_0 &gt;= -97000000000
-RebateTierLower_B_1: - 0.15 S_B + rebate_B - 97000000000 y_rebate_B_1
+RebateTierLower_B_1: - 0.05 S_B + rebate_B - 97000000000 y_rebate_B_1
  &gt;= -97000000000
 RebateTierLower_C_0: rebate_C - 97000000000 y_rebate_C_0 &gt;= -97000000000
 RebateTierLower_C_1: - 0.07 S_C + rebate_C - 97000000000 y_rebate_C_1
@@ -1378,7 +1362,7 @@
 RebateTierMax_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
  + x_A_7 + x_A_8 + x_A_9 + 19400000000 y_rebate_A_0 &lt;= 19400000500
 RebateTierMax_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
- + x_B_7 + x_B_8 + x_B_9 + 97000000000 y_rebate_B_0 &lt;= 97000000300
+ + x_B_7 + x_B_8 + x_B_9 + 97000000000 y_rebate_B_0 &lt;= 97000000500
 RebateTierMax_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
  + x_C_7 + x_C_8 + x_C_9 + 97000000000 y_rebate_C_0 &lt;= 97000000700
 RebateTierMin_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
@@ -1387,8 +1371,8 @@
  + x_A_7 + x_A_8 + x_A_9 - 500 y_rebate_A_1 &gt;= 0
 RebateTierMin_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
  + x_B_7 + x_B_8 + x_B_9 &gt;= 0
-RebateTierMin_B_1: x_B_1 + x_B_10 + x_B_3 + x_B_4 + x_B_8 + x_B_9
- - 500 y_rebate_B_1 &gt;= 0
+RebateTierMin_B_1: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
+ + x_B_7 + x_B_8 + x_B_9 - 500 y_rebate_B_1 &gt;= 0
 RebateTierMin_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
  + x_C_7 + x_C_8 + x_C_9 &gt;= 0
 RebateTierMin_C_1: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
@@ -1397,20 +1381,14 @@
 RebateTierSelect_B: y_rebate_B_0 + y_rebate_B_1 = 1
 RebateTierSelect_C: y_rebate_C_0 + y_rebate_C_1 = 1
 RebateTierUpper_A_0: rebate_A + 19400000000 y_rebate_A_0 &lt;= 19400000000
-RebateTierUpper_A_1: - 0.09 S_A + rebate_A + 19400000000 y_rebate_A_1
+RebateTierUpper_A_1: - 0.1 S_A + rebate_A + 19400000000 y_rebate_A_1
  &lt;= 19400000000
 RebateTierUpper_B_0: rebate_B + 97000000000 y_rebate_B_0 &lt;= 97000000000
-RebateTierUpper_B_1: - 0.15 S_B + rebate_B + 97000000000 y_rebate_B_1
+RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 97000000000 y_rebate_B_1
  &lt;= 97000000000
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
-Rule_0_aggregate: - 0.3 x_A_1 - 0.3 x_A_10 - 0.3 x_A_2 - 0.3 x_A_3 - 0.3 x_A_4
- - 0.3 x_A_5 - 0.3 x_A_6 - 0.3 x_A_7 - 0.3 x_A_8 - 0.3 x_A_9 - 0.3 x_B_1
- - 0.3 x_B_10 - 0.3 x_B_2 - 0.3 x_B_3 - 0.3 x_B_4 - 0.3 x_B_5 - 0.3 x_B_6
- - 0.3 x_B_7 - 0.3 x_B_8 - 0.3 x_B_9 + 0.7 x_C_1 + 0.7 x_C_10 + 0.7 x_C_2
- + 0.7 x_C_3 + 0.7 x_C_4 + 0.7 x_C_5 + 0.7 x_C_6 + 0.7 x_C_7 + 0.7 x_C_8
- + 0.7 x_C_9 &gt;= 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1458,6 +1436,9 @@
 T_8_B
 T_9_A
 T_9_B
+y_0_A
+y_0_B
+y_0_C
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
Fixed # Volume Awarded rule
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -540,36 +540,36 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>52.8</v>
+        <v>49.5</v>
       </c>
       <c r="K2" t="n">
-        <v>36960</v>
+        <v>34650</v>
       </c>
       <c r="L2" t="n">
         <v>700</v>
       </c>
       <c r="M2" t="n">
-        <v>33040</v>
+        <v>35350</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="3">
@@ -599,36 +599,36 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>77.59999999999999</v>
+        <v>69.3</v>
       </c>
       <c r="K3" t="n">
-        <v>698400</v>
+        <v>623700</v>
       </c>
       <c r="L3" t="n">
         <v>9000</v>
       </c>
       <c r="M3" t="n">
-        <v>705600</v>
+        <v>780300</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>62370</v>
       </c>
     </row>
     <row r="4">
@@ -654,7 +654,7 @@
         <v>423</v>
       </c>
       <c r="F4" t="n">
-        <v>142127.27244</v>
+        <v>253800</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -673,30 +673,30 @@
         <v>54.45</v>
       </c>
       <c r="K4" t="n">
-        <v>18295.106346</v>
+        <v>32670</v>
       </c>
       <c r="L4" t="n">
-        <v>335.99828</v>
+        <v>600</v>
       </c>
       <c r="M4" t="n">
-        <v>123832.166094</v>
+        <v>221130</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>3267</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -710,43 +710,43 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="F5" t="n">
-        <v>111672.72756</v>
+        <v>2376891</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>63.05</v>
+        <v>22.77</v>
       </c>
       <c r="K5" t="n">
-        <v>16645.308446</v>
+        <v>119474.19</v>
       </c>
       <c r="L5" t="n">
-        <v>264.00172</v>
+        <v>5247</v>
       </c>
       <c r="M5" t="n">
-        <v>95027.41911399999</v>
+        <v>2257416.81</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>11947.419</v>
       </c>
     </row>
     <row r="6">
@@ -755,7 +755,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -772,40 +772,40 @@
         <v>453</v>
       </c>
       <c r="F6" t="n">
-        <v>2568510</v>
+        <v>191619</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>72.75</v>
+        <v>23.04</v>
       </c>
       <c r="K6" t="n">
-        <v>412492.5</v>
+        <v>9745.92</v>
       </c>
       <c r="L6" t="n">
-        <v>5670</v>
+        <v>423</v>
       </c>
       <c r="M6" t="n">
-        <v>2156017.5</v>
+        <v>181873.08</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>682.2144000000001</v>
       </c>
     </row>
     <row r="7">
@@ -860,11 +860,11 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>72.57600000000001</v>
       </c>
     </row>
     <row r="8">
@@ -902,20 +902,20 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>23.28</v>
+        <v>24</v>
       </c>
       <c r="K8" t="n">
-        <v>5633.76</v>
+        <v>5808</v>
       </c>
       <c r="L8" t="n">
         <v>242</v>
       </c>
       <c r="M8" t="n">
-        <v>152392.24</v>
+        <v>152218</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -978,11 +978,11 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>1511.928</v>
       </c>
     </row>
     <row r="10">
@@ -1020,20 +1020,20 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>12.61</v>
+        <v>13</v>
       </c>
       <c r="K10" t="n">
-        <v>302.64</v>
+        <v>312</v>
       </c>
       <c r="L10" t="n">
         <v>24</v>
       </c>
       <c r="M10" t="n">
-        <v>10641.36</v>
+        <v>10632</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1096,11 +1096,11 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>202.6752</v>
       </c>
     </row>
     <row r="12">
@@ -1138,20 +1138,20 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>12.61</v>
+        <v>13</v>
       </c>
       <c r="K12" t="n">
-        <v>163.93</v>
+        <v>169</v>
       </c>
       <c r="L12" t="n">
         <v>13</v>
       </c>
       <c r="M12" t="n">
-        <v>2839.07</v>
+        <v>2834</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1191,21 +1191,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model is infeasible. Likely causes include:
- - Insufficient supplier capacity relative to demand.
- - Custom rule constraints conflicting with overall volume/demand.
-Detailed Rule Evaluations:
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 1, total demand: 700 units; a 30% allocation requires 210.0 units for All.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 2, total demand: 9000 units; a 30% allocation requires 2700.0 units for All.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 3, total demand: 600 units; a 30% allocation requires 180.0 units for All.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 4, total demand: 5670 units; a 30% allocation requires 1701.0 units for All.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 5, total demand: 45 units; a 30% allocation requires 13.5 units for All.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 6, total demand: 242 units; a 30% allocation requires 72.6 units for All.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 7, total demand: 664 units; a 30% allocation requires 199.2 units for All.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 8, total demand: 24 units; a 30% allocation requires 7.2 units for All.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 9, total demand: 232 units; a 30% allocation requires 69.6 units for All.
-Rule 1 ('% of Volume Awarded'): ✅ For Bid ID 10, total demand: 13 units; a 30% allocation requires 3.9 units for All.
-Review supplier capacities, demand, and custom rule constraints for adjustments.</t>
+          <t>Model is optimal.</t>
         </is>
       </c>
     </row>
@@ -1242,30 +1228,6 @@
 Minimize
 OBJ: S_A + S_B + S_C - rebate_A - rebate_B - rebate_C
 Subject To
-%VolAwarded_Agg_0_A_UB: 0.7 x_A_1 + 0.7 x_A_10 + 0.7 x_A_2 + 0.7 x_A_3
- + 0.7 x_A_4 + 0.7 x_A_5 + 0.7 x_A_6 + 0.7 x_A_7 + 0.7 x_A_8 + 0.7 x_A_9
- - 0.3 x_B_1 - 0.3 x_B_10 - 0.3 x_B_2 - 0.3 x_B_3 - 0.3 x_B_4 - 0.3 x_B_5
- - 0.3 x_B_6 - 0.3 x_B_7 - 0.3 x_B_8 - 0.3 x_B_9 - 0.3 x_C_1 - 0.3 x_C_10
- - 0.3 x_C_2 - 0.3 x_C_3 - 0.3 x_C_4 - 0.3 x_C_5 - 0.3 x_C_6 - 0.3 x_C_7
- - 0.3 x_C_8 - 0.3 x_C_9 + 1000000000 y_0_A &lt;= 1000000000
-%VolAwarded_Agg_0_B_UB: - 0.3 x_A_1 - 0.3 x_A_10 - 0.3 x_A_2 - 0.3 x_A_3
- - 0.3 x_A_4 - 0.3 x_A_5 - 0.3 x_A_6 - 0.3 x_A_7 - 0.3 x_A_8 - 0.3 x_A_9
- + 0.7 x_B_1 + 0.7 x_B_10 + 0.7 x_B_2 + 0.7 x_B_3 + 0.7 x_B_4 + 0.7 x_B_5
- + 0.7 x_B_6 + 0.7 x_B_7 + 0.7 x_B_8 + 0.7 x_B_9 - 0.3 x_C_1 - 0.3 x_C_10
- - 0.3 x_C_2 - 0.3 x_C_3 - 0.3 x_C_4 - 0.3 x_C_5 - 0.3 x_C_6 - 0.3 x_C_7
- - 0.3 x_C_8 - 0.3 x_C_9 + 1000000000 y_0_B &lt;= 1000000000
-%VolAwarded_Agg_0_C_UB: - 0.3 x_A_1 - 0.3 x_A_10 - 0.3 x_A_2 - 0.3 x_A_3
- - 0.3 x_A_4 - 0.3 x_A_5 - 0.3 x_A_6 - 0.3 x_A_7 - 0.3 x_A_8 - 0.3 x_A_9
- - 0.3 x_B_1 - 0.3 x_B_10 - 0.3 x_B_2 - 0.3 x_B_3 - 0.3 x_B_4 - 0.3 x_B_5
- - 0.3 x_B_6 - 0.3 x_B_7 - 0.3 x_B_8 - 0.3 x_B_9 + 0.7 x_C_1 + 0.7 x_C_10
- + 0.7 x_C_2 + 0.7 x_C_3 + 0.7 x_C_4 + 0.7 x_C_5 + 0.7 x_C_6 + 0.7 x_C_7
- + 0.7 x_C_8 + 0.7 x_C_9 + 1000000000 y_0_C &lt;= 1000000000
-Active_0_A: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7
- + x_A_8 + x_A_9 - 1000000000 y_0_A &lt;= 0
-Active_0_B: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7
- + x_B_8 + x_B_9 - 1000000000 y_0_B &lt;= 0
-Active_0_C: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7
- + x_C_8 + x_C_9 - 1000000000 y_0_C &lt;= 0
 BaseSpend_A: S0_A - 50 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
  - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
 BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 80 x_B_2 - 65 x_B_3 - 75 x_B_4
@@ -1344,12 +1306,6 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
-MinActive_0_A: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7
- + x_A_8 + x_A_9 - 0.001 y_0_A &gt;= 0
-MinActive_0_B: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7
- + x_B_8 + x_B_9 - 0.001 y_0_B &gt;= 0
-MinActive_0_C: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7
- + x_C_8 + x_C_9 - 0.001 y_0_C &gt;= 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
  &gt;= -19400000000
@@ -1409,6 +1365,8 @@
 Transition_8_B: - 24 T_8_B + x_B_8 &lt;= 0
 Transition_9_A: - 232 T_9_A + x_A_9 &lt;= 0
 Transition_9_B: - 232 T_9_B + x_B_9 &lt;= 0
+VolAwarded_Agg_0_incumbent_UB: x_A_1 + x_C_10 + x_C_3 + x_C_4 + x_C_5 + x_C_9
+ &lt;= 3000
 Volume_A: V_A - x_A_1 - x_A_10 - x_A_2 - x_A_3 - x_A_4 - x_A_5 - x_A_6 - x_A_7
  - x_A_8 - x_A_9 = 0
 Volume_B: V_B - x_B_1 - x_B_10 - x_B_2 - x_B_3 - x_B_4 - x_B_5 - x_B_6 - x_B_7
@@ -1436,9 +1394,6 @@
 T_8_B
 T_9_A
 T_9_B
-y_0_A
-y_0_B
-y_0_C
 y_rebate_A_0
 y_rebate_A_1
 y_rebate_B_0

</xml_diff>

<commit_message>
Fixed # of transitions rule
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -658,36 +658,36 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>54.45</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>32670</v>
+        <v>34560</v>
       </c>
       <c r="L4" t="n">
         <v>600</v>
       </c>
       <c r="M4" t="n">
-        <v>221130</v>
+        <v>219240</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>3267</v>
+        <v>2419.2</v>
       </c>
     </row>
     <row r="5">
@@ -713,54 +713,54 @@
         <v>453</v>
       </c>
       <c r="F5" t="n">
-        <v>2376891</v>
+        <v>2568510</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>22.77</v>
+        <v>23.04</v>
       </c>
       <c r="K5" t="n">
-        <v>119474.19</v>
+        <v>130636.8</v>
       </c>
       <c r="L5" t="n">
-        <v>5247</v>
+        <v>5670</v>
       </c>
       <c r="M5" t="n">
-        <v>2257416.81</v>
+        <v>2437873.2</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>11947.419</v>
+        <v>9144.576000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Facility 5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>453</v>
+        <v>342</v>
       </c>
       <c r="F6" t="n">
-        <v>191619</v>
+        <v>15390</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -791,13 +791,13 @@
         <v>23.04</v>
       </c>
       <c r="K6" t="n">
-        <v>9745.92</v>
+        <v>1036.8</v>
       </c>
       <c r="L6" t="n">
-        <v>423</v>
+        <v>45</v>
       </c>
       <c r="M6" t="n">
-        <v>181873.08</v>
+        <v>14353.2</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -805,12 +805,12 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>682.2144000000001</v>
+        <v>72.57600000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -819,7 +819,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Facility 9</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -828,14 +828,14 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>342</v>
+        <v>653</v>
       </c>
       <c r="F7" t="n">
-        <v>15390</v>
+        <v>158026</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -843,33 +843,33 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>23.04</v>
+        <v>24</v>
       </c>
       <c r="K7" t="n">
-        <v>1036.8</v>
+        <v>5808</v>
       </c>
       <c r="L7" t="n">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="M7" t="n">
-        <v>14353.2</v>
+        <v>152218</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>72.57600000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -887,48 +887,48 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>653</v>
+        <v>432</v>
       </c>
       <c r="F8" t="n">
-        <v>158026</v>
+        <v>286848</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>24</v>
+        <v>22.77</v>
       </c>
       <c r="K8" t="n">
-        <v>5808</v>
+        <v>15119.28</v>
       </c>
       <c r="L8" t="n">
-        <v>242</v>
+        <v>664</v>
       </c>
       <c r="M8" t="n">
-        <v>152218</v>
+        <v>271728.72</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>1511.928</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -946,48 +946,48 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="F9" t="n">
-        <v>286848</v>
+        <v>10944</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>22.77</v>
+        <v>23.04</v>
       </c>
       <c r="K9" t="n">
-        <v>15119.28</v>
+        <v>552.96</v>
       </c>
       <c r="L9" t="n">
-        <v>664</v>
+        <v>24</v>
       </c>
       <c r="M9" t="n">
-        <v>271728.72</v>
+        <v>10391.04</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>1511.928</v>
+        <v>38.70720000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facility 9</t>
+          <t>Facility 10</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1005,14 +1005,14 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>456</v>
+        <v>234</v>
       </c>
       <c r="F10" t="n">
-        <v>10944</v>
+        <v>54288</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -1020,33 +1020,33 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>13</v>
+        <v>12.48</v>
       </c>
       <c r="K10" t="n">
-        <v>312</v>
+        <v>2895.36</v>
       </c>
       <c r="L10" t="n">
-        <v>24</v>
+        <v>232</v>
       </c>
       <c r="M10" t="n">
-        <v>10632</v>
+        <v>51392.64</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>202.6752</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1064,10 +1064,10 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F11" t="n">
-        <v>54288</v>
+        <v>3003</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1075,24 +1075,24 @@
         </is>
       </c>
       <c r="H11" t="n">
+        <v>75</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>72</v>
+      </c>
+      <c r="K11" t="n">
+        <v>936</v>
+      </c>
+      <c r="L11" t="n">
         <v>13</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
-        <v>12.48</v>
-      </c>
-      <c r="K11" t="n">
-        <v>2895.36</v>
-      </c>
-      <c r="L11" t="n">
-        <v>232</v>
-      </c>
       <c r="M11" t="n">
-        <v>51392.64</v>
+        <v>2067</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1100,66 +1100,7 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>202.6752</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>231</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>13</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J12" t="n">
-        <v>13</v>
-      </c>
-      <c r="K12" t="n">
-        <v>169</v>
-      </c>
-      <c r="L12" t="n">
-        <v>13</v>
-      </c>
-      <c r="M12" t="n">
-        <v>2834</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
+        <v>65.52000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1228,6 +1169,36 @@
 Minimize
 OBJ: S_A + S_B + S_C - rebate_A - rebate_B - rebate_C
 Subject To
+ActiveLink_A_1: x_A_1 - 1000000000 z_A &lt;= 0
+ActiveLink_A_10: x_A_10 - 1000000000 z_A &lt;= 0
+ActiveLink_A_2: x_A_2 - 1000000000 z_A &lt;= 0
+ActiveLink_A_3: x_A_3 - 1000000000 z_A &lt;= 0
+ActiveLink_A_4: x_A_4 - 1000000000 z_A &lt;= 0
+ActiveLink_A_5: x_A_5 - 1000000000 z_A &lt;= 0
+ActiveLink_A_6: x_A_6 - 1000000000 z_A &lt;= 0
+ActiveLink_A_7: x_A_7 - 1000000000 z_A &lt;= 0
+ActiveLink_A_8: x_A_8 - 1000000000 z_A &lt;= 0
+ActiveLink_A_9: x_A_9 - 1000000000 z_A &lt;= 0
+ActiveLink_B_1: x_B_1 - 1000000000 z_B &lt;= 0
+ActiveLink_B_10: x_B_10 - 1000000000 z_B &lt;= 0
+ActiveLink_B_2: x_B_2 - 1000000000 z_B &lt;= 0
+ActiveLink_B_3: x_B_3 - 1000000000 z_B &lt;= 0
+ActiveLink_B_4: x_B_4 - 1000000000 z_B &lt;= 0
+ActiveLink_B_5: x_B_5 - 1000000000 z_B &lt;= 0
+ActiveLink_B_6: x_B_6 - 1000000000 z_B &lt;= 0
+ActiveLink_B_7: x_B_7 - 1000000000 z_B &lt;= 0
+ActiveLink_B_8: x_B_8 - 1000000000 z_B &lt;= 0
+ActiveLink_B_9: x_B_9 - 1000000000 z_B &lt;= 0
+ActiveLink_C_1: x_C_1 - 1000000000 z_C &lt;= 0
+ActiveLink_C_10: x_C_10 - 1000000000 z_C &lt;= 0
+ActiveLink_C_2: x_C_2 - 1000000000 z_C &lt;= 0
+ActiveLink_C_3: x_C_3 - 1000000000 z_C &lt;= 0
+ActiveLink_C_4: x_C_4 - 1000000000 z_C &lt;= 0
+ActiveLink_C_5: x_C_5 - 1000000000 z_C &lt;= 0
+ActiveLink_C_6: x_C_6 - 1000000000 z_C &lt;= 0
+ActiveLink_C_7: x_C_7 - 1000000000 z_C &lt;= 0
+ActiveLink_C_8: x_C_8 - 1000000000 z_C &lt;= 0
+ActiveLink_C_9: x_C_9 - 1000000000 z_C &lt;= 0
 BaseSpend_A: S0_A - 50 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
  - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
 BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 80 x_B_2 - 65 x_B_3 - 75 x_B_4
@@ -1306,6 +1277,12 @@
 EffectiveSpend_A: - S0_A + S_A + d_A = 0
 EffectiveSpend_B: - S0_B + S_B + d_B = 0
 EffectiveSpend_C: - S0_C + S_C + d_C = 0
+MinAward_A: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7
+ + x_A_8 + x_A_9 - z_A &gt;= 0
+MinAward_B: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7
+ + x_B_8 + x_B_9 - z_B &gt;= 0
+MinAward_C: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7
+ + x_C_8 + x_C_9 - z_C &gt;= 0
 RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
 RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
  &gt;= -19400000000
@@ -1345,6 +1322,26 @@
 RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
 RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
  &lt;= 97000000000
+TransitionLower_10_A: x_A_10 &gt;= 0
+TransitionLower_10_B: x_B_10 &gt;= 0
+TransitionLower_1_B: x_B_1 &gt;= 0
+TransitionLower_1_C: x_C_1 &gt;= 0
+TransitionLower_2_A: x_A_2 &gt;= 0
+TransitionLower_2_C: x_C_2 &gt;= 0
+TransitionLower_3_A: x_A_3 &gt;= 0
+TransitionLower_3_B: x_B_3 &gt;= 0
+TransitionLower_4_A: x_A_4 &gt;= 0
+TransitionLower_4_B: x_B_4 &gt;= 0
+TransitionLower_5_A: x_A_5 &gt;= 0
+TransitionLower_5_B: x_B_5 &gt;= 0
+TransitionLower_6_A: x_A_6 &gt;= 0
+TransitionLower_6_B: x_B_6 &gt;= 0
+TransitionLower_7_A: x_A_7 &gt;= 0
+TransitionLower_7_B: x_B_7 &gt;= 0
+TransitionLower_8_A: x_A_8 &gt;= 0
+TransitionLower_8_B: x_B_8 &gt;= 0
+TransitionLower_9_A: x_A_9 &gt;= 0
+TransitionLower_9_B: x_B_9 &gt;= 0
 Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
 Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
 Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
@@ -1365,8 +1362,8 @@
 Transition_8_B: - 24 T_8_B + x_B_8 &lt;= 0
 Transition_9_A: - 232 T_9_A + x_A_9 &lt;= 0
 Transition_9_B: - 232 T_9_B + x_B_9 &lt;= 0
-VolAwarded_Agg_0_incumbent_UB: x_A_1 + x_C_10 + x_C_3 + x_C_4 + x_C_5 + x_C_9
- &lt;= 3000
+Transitions_0_UB: T_10_A + T_10_B + T_3_A + T_3_B + T_4_A + T_4_B + T_5_A
+ + T_5_B + T_6_A + T_6_B + T_7_A + T_7_B + T_8_A + T_8_B + T_9_A + T_9_B &lt;= 2
 Volume_A: V_A - x_A_1 - x_A_10 - x_A_2 - x_A_3 - x_A_4 - x_A_5 - x_A_6 - x_A_7
  - x_A_8 - x_A_9 = 0
 Volume_B: V_B - x_B_1 - x_B_10 - x_B_2 - x_B_3 - x_B_4 - x_B_5 - x_B_6 - x_B_7
@@ -1400,6 +1397,9 @@
 y_rebate_B_1
 y_rebate_C_0
 y_rebate_C_1
+z_A
+z_B
+z_C
 z_discount_A_0
 z_discount_A_1
 z_discount_B_0

</xml_diff>

<commit_message>
Mostly fixed Exlcusion rules needs validation
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,52 +524,52 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Facility 1</t>
+          <t>Diboll</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Dow</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>1.06</v>
       </c>
       <c r="F2" t="n">
-        <v>70000</v>
+        <v>9392122.58</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Dow</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>50</v>
+        <v>0.753</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>49.5</v>
+        <v>0.753</v>
       </c>
       <c r="K2" t="n">
-        <v>34650</v>
+        <v>6671951.229</v>
       </c>
       <c r="L2" t="n">
-        <v>700</v>
+        <v>8860493</v>
       </c>
       <c r="M2" t="n">
-        <v>35350</v>
+        <v>2720171.351</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>3465</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -583,52 +583,52 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Facility 1</t>
+          <t>Mt Jewett</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>156</v>
+        <v>1.16</v>
       </c>
       <c r="F3" t="n">
-        <v>1404000</v>
+        <v>8228219.880000001</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>70</v>
+        <v>0.8862</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>69.3</v>
+        <v>0.8862</v>
       </c>
       <c r="K3" t="n">
-        <v>623700</v>
+        <v>6286076.2566</v>
       </c>
       <c r="L3" t="n">
-        <v>9000</v>
+        <v>7093293</v>
       </c>
       <c r="M3" t="n">
-        <v>780300</v>
+        <v>1942143.623400001</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>62370</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -642,52 +642,52 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Clarendon</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>423</v>
+        <v>1.19</v>
       </c>
       <c r="F4" t="n">
-        <v>253800</v>
+        <v>8833477.100000001</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>60</v>
+        <v>0.8762</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>57.59999999999999</v>
+        <v>0.8762</v>
       </c>
       <c r="K4" t="n">
-        <v>34560</v>
+        <v>6504111.458</v>
       </c>
       <c r="L4" t="n">
-        <v>600</v>
+        <v>7423090</v>
       </c>
       <c r="M4" t="n">
-        <v>219240</v>
+        <v>2329365.642000002</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>2419.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -701,52 +701,52 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Facility 4</t>
+          <t>Englehart</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>453</v>
+        <v>1.1527</v>
       </c>
       <c r="F5" t="n">
-        <v>2568510</v>
+        <v>16306582.9448</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>24</v>
+        <v>0.9372</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>23.04</v>
+        <v>0.9372</v>
       </c>
       <c r="K5" t="n">
-        <v>130636.8</v>
+        <v>13258028.5728</v>
       </c>
       <c r="L5" t="n">
-        <v>5670</v>
+        <v>14146424</v>
       </c>
       <c r="M5" t="n">
-        <v>2437873.2</v>
+        <v>3048554.372</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>9144.576000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -760,347 +760,52 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facility 5</t>
+          <t>Fordyce</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Dow</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>342</v>
+        <v>1.16</v>
       </c>
       <c r="F6" t="n">
-        <v>15390</v>
+        <v>5734979.680000001</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Dow</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>0.743</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>23.04</v>
+        <v>0.743</v>
       </c>
       <c r="K6" t="n">
-        <v>1036.8</v>
+        <v>3673353.364</v>
       </c>
       <c r="L6" t="n">
-        <v>45</v>
+        <v>4943948</v>
       </c>
       <c r="M6" t="n">
-        <v>14353.2</v>
+        <v>2061626.316000001</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>72.57600000000001</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>653</v>
-      </c>
-      <c r="F7" t="n">
-        <v>158026</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>24</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J7" t="n">
-        <v>24</v>
-      </c>
-      <c r="K7" t="n">
-        <v>5808</v>
-      </c>
-      <c r="L7" t="n">
-        <v>242</v>
-      </c>
-      <c r="M7" t="n">
-        <v>152218</v>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O7" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>432</v>
-      </c>
-      <c r="F8" t="n">
-        <v>286848</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>23</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>1%</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>22.77</v>
-      </c>
-      <c r="K8" t="n">
-        <v>15119.28</v>
-      </c>
-      <c r="L8" t="n">
-        <v>664</v>
-      </c>
-      <c r="M8" t="n">
-        <v>271728.72</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="O8" t="n">
-        <v>1511.928</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Facility 9</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>456</v>
-      </c>
-      <c r="F9" t="n">
-        <v>10944</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>24</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J9" t="n">
-        <v>23.04</v>
-      </c>
-      <c r="K9" t="n">
-        <v>552.96</v>
-      </c>
-      <c r="L9" t="n">
-        <v>24</v>
-      </c>
-      <c r="M9" t="n">
-        <v>10391.04</v>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="O9" t="n">
-        <v>38.70720000000001</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>234</v>
-      </c>
-      <c r="F10" t="n">
-        <v>54288</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>13</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
-        <v>12.48</v>
-      </c>
-      <c r="K10" t="n">
-        <v>2895.36</v>
-      </c>
-      <c r="L10" t="n">
-        <v>232</v>
-      </c>
-      <c r="M10" t="n">
-        <v>51392.64</v>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="O10" t="n">
-        <v>202.6752</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Facility 10</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>231</v>
-      </c>
-      <c r="F11" t="n">
-        <v>3003</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>75</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>4%</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
-        <v>72</v>
-      </c>
-      <c r="K11" t="n">
-        <v>936</v>
-      </c>
-      <c r="L11" t="n">
-        <v>13</v>
-      </c>
-      <c r="M11" t="n">
-        <v>2067</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>7%</t>
-        </is>
-      </c>
-      <c r="O11" t="n">
-        <v>65.52000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1167,245 +872,241 @@
         <is>
           <t xml:space="preserve">\* Sourcing_with_MultiTier_Rebates_Discounts *\
 Minimize
-OBJ: S_A + S_B + S_C - rebate_A - rebate_B - rebate_C
+OBJ: S_BASF + S_Covestro + S_Dow + S_Huntsman + S_Wanhua - rebate_BASF
+ - rebate_Covestro - rebate_Dow - rebate_Huntsman - rebate_Wanhua
 Subject To
-ActiveLink_A_1: x_A_1 - 1000000000 z_A &lt;= 0
-ActiveLink_A_10: x_A_10 - 1000000000 z_A &lt;= 0
-ActiveLink_A_2: x_A_2 - 1000000000 z_A &lt;= 0
-ActiveLink_A_3: x_A_3 - 1000000000 z_A &lt;= 0
-ActiveLink_A_4: x_A_4 - 1000000000 z_A &lt;= 0
-ActiveLink_A_5: x_A_5 - 1000000000 z_A &lt;= 0
-ActiveLink_A_6: x_A_6 - 1000000000 z_A &lt;= 0
-ActiveLink_A_7: x_A_7 - 1000000000 z_A &lt;= 0
-ActiveLink_A_8: x_A_8 - 1000000000 z_A &lt;= 0
-ActiveLink_A_9: x_A_9 - 1000000000 z_A &lt;= 0
-ActiveLink_B_1: x_B_1 - 1000000000 z_B &lt;= 0
-ActiveLink_B_10: x_B_10 - 1000000000 z_B &lt;= 0
-ActiveLink_B_2: x_B_2 - 1000000000 z_B &lt;= 0
-ActiveLink_B_3: x_B_3 - 1000000000 z_B &lt;= 0
-ActiveLink_B_4: x_B_4 - 1000000000 z_B &lt;= 0
-ActiveLink_B_5: x_B_5 - 1000000000 z_B &lt;= 0
-ActiveLink_B_6: x_B_6 - 1000000000 z_B &lt;= 0
-ActiveLink_B_7: x_B_7 - 1000000000 z_B &lt;= 0
-ActiveLink_B_8: x_B_8 - 1000000000 z_B &lt;= 0
-ActiveLink_B_9: x_B_9 - 1000000000 z_B &lt;= 0
-ActiveLink_C_1: x_C_1 - 1000000000 z_C &lt;= 0
-ActiveLink_C_10: x_C_10 - 1000000000 z_C &lt;= 0
-ActiveLink_C_2: x_C_2 - 1000000000 z_C &lt;= 0
-ActiveLink_C_3: x_C_3 - 1000000000 z_C &lt;= 0
-ActiveLink_C_4: x_C_4 - 1000000000 z_C &lt;= 0
-ActiveLink_C_5: x_C_5 - 1000000000 z_C &lt;= 0
-ActiveLink_C_6: x_C_6 - 1000000000 z_C &lt;= 0
-ActiveLink_C_7: x_C_7 - 1000000000 z_C &lt;= 0
-ActiveLink_C_8: x_C_8 - 1000000000 z_C &lt;= 0
-ActiveLink_C_9: x_C_9 - 1000000000 z_C &lt;= 0
-BaseSpend_A: S0_A - 50 x_A_1 - 64 x_A_10 - 70 x_A_2 - 55 x_A_3 - 23 x_A_4
- - 54 x_A_5 - 42 x_A_6 - 23 x_A_7 - 75 x_A_8 - 97 x_A_9 = 0
-BaseSpend_B: S0_B - 60 x_B_1 - 13 x_B_10 - 80 x_B_2 - 65 x_B_3 - 75 x_B_4
- - 34 x_B_5 - 24 x_B_6 - 53 x_B_7 - 13 x_B_8 - 56 x_B_9 = 0
-BaseSpend_C: S0_C - 55 x_C_1 - 75 x_C_10 - 75 x_C_2 - 60 x_C_3 - 24 x_C_4
- - 24 x_C_5 - 64 x_C_6 - 86 x_C_7 - 24 x_C_8 - 13 x_C_9 = 0
-Capacity_B_Bid_ID_1: x_B_1 &lt;= 100000000
-Capacity_B_Bid_ID_10: x_B_10 &lt;= 100000000
-Capacity_B_Bid_ID_2: x_B_2 &lt;= 100000000
-Capacity_B_Bid_ID_3: x_B_3 &lt;= 100000000
-Capacity_B_Bid_ID_4: x_B_4 &lt;= 100000000
-Capacity_B_Bid_ID_5: x_B_5 &lt;= 100000000
-Capacity_B_Bid_ID_6: x_B_6 &lt;= 100000000
-Capacity_B_Bid_ID_7: x_B_7 &lt;= 100000000
-Capacity_B_Bid_ID_8: x_B_8 &lt;= 100000000
-Capacity_B_Bid_ID_9: x_B_9 &lt;= 100000000
-Capacity_C_Bid_ID_1: x_C_1 &lt;= 100000000
-Capacity_C_Bid_ID_10: x_C_10 &lt;= 100000000
-Capacity_C_Bid_ID_2: x_C_2 &lt;= 100000000
-Capacity_C_Bid_ID_3: x_C_3 &lt;= 100000000
-Capacity_C_Bid_ID_4: x_C_4 &lt;= 100000000
-Capacity_C_Bid_ID_5: x_C_5 &lt;= 100000000
-Capacity_C_Bid_ID_6: x_C_6 &lt;= 100000000
-Capacity_C_Bid_ID_7: x_C_7 &lt;= 100000000
-Capacity_C_Bid_ID_8: x_C_8 &lt;= 100000000
-Capacity_C_Bid_ID_9: x_C_9 &lt;= 100000000
-Demand_1: x_A_1 + x_B_1 + x_C_1 = 700
-Demand_10: x_A_10 + x_B_10 + x_C_10 = 13
-Demand_2: x_A_2 + x_B_2 + x_C_2 = 9000
-Demand_3: x_A_3 + x_B_3 + x_C_3 = 600
-Demand_4: x_A_4 + x_B_4 + x_C_4 = 5670
-Demand_5: x_A_5 + x_B_5 + x_C_5 = 45
-Demand_6: x_A_6 + x_B_6 + x_C_6 = 242
-Demand_7: x_A_7 + x_B_7 + x_C_7 = 664
-Demand_8: x_A_8 + x_B_8 + x_C_8 = 24
-Demand_9: x_A_9 + x_B_9 + x_C_9 = 232
-DiscountTierLower_A_0: d_A - 19400000000 z_discount_A_0 &gt;= -19400000000
-DiscountTierLower_A_1: - 0.01 S0_A + d_A - 19400000000 z_discount_A_1
- &gt;= -19400000000
-DiscountTierLower_B_0: d_B - 97000000000 z_discount_B_0 &gt;= -97000000000
-DiscountTierLower_B_1: - 0.03 S0_B + d_B - 97000000000 z_discount_B_1
- &gt;= -97000000000
-DiscountTierLower_C_0: d_C - 97000000000 z_discount_C_0 &gt;= -97000000000
-DiscountTierLower_C_1: - 0.04 S0_C + d_C - 97000000000 z_discount_C_1
- &gt;= -97000000000
-DiscountTierMax_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
- + x_A_7 + x_A_8 + x_A_9 + 19400000000 z_discount_A_0 &lt;= 19400001000
-DiscountTierMax_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
- + x_B_7 + x_B_8 + x_B_9 + 97000000000 z_discount_B_0 &lt;= 97000000500
-DiscountTierMax_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
- + x_C_7 + x_C_8 + x_C_9 + 97000000000 z_discount_C_0 &lt;= 97000000500
-DiscountTierMin_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
- + x_A_7 + x_A_8 + x_A_9 &gt;= 0
-DiscountTierMin_A_1: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
- + x_A_7 + x_A_8 + x_A_9 - 1000 z_discount_A_1 &gt;= 0
-DiscountTierMin_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
- + x_B_7 + x_B_8 + x_B_9 &gt;= 0
-DiscountTierMin_B_1: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
- + x_B_7 + x_B_8 + x_B_9 - 500 z_discount_B_1 &gt;= 0
-DiscountTierMin_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
- + x_C_7 + x_C_8 + x_C_9 &gt;= 0
-DiscountTierMin_C_1: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
- + x_C_7 + x_C_8 + x_C_9 - 500 z_discount_C_1 &gt;= 0
-DiscountTierSelect_A: z_discount_A_0 + z_discount_A_1 = 1
-DiscountTierSelect_B: z_discount_B_0 + z_discount_B_1 = 1
-DiscountTierSelect_C: z_discount_C_0 + z_discount_C_1 = 1
-DiscountTierUpper_A_0: d_A + 19400000000 z_discount_A_0 &lt;= 19400000000
-DiscountTierUpper_A_1: - 0.01 S0_A + d_A + 19400000000 z_discount_A_1
- &lt;= 19400000000
-DiscountTierUpper_B_0: d_B + 97000000000 z_discount_B_0 &lt;= 97000000000
-DiscountTierUpper_B_1: - 0.03 S0_B + d_B + 97000000000 z_discount_B_1
- &lt;= 97000000000
-DiscountTierUpper_C_0: d_C + 97000000000 z_discount_C_0 &lt;= 97000000000
-DiscountTierUpper_C_1: - 0.04 S0_C + d_C + 97000000000 z_discount_C_1
- &lt;= 97000000000
-EffectiveSpend_A: - S0_A + S_A + d_A = 0
-EffectiveSpend_B: - S0_B + S_B + d_B = 0
-EffectiveSpend_C: - S0_C + S_C + d_C = 0
-MinAward_A: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6 + x_A_7
- + x_A_8 + x_A_9 - z_A &gt;= 0
-MinAward_B: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6 + x_B_7
- + x_B_8 + x_B_9 - z_B &gt;= 0
-MinAward_C: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6 + x_C_7
- + x_C_8 + x_C_9 - z_C &gt;= 0
-RebateTierLower_A_0: rebate_A - 19400000000 y_rebate_A_0 &gt;= -19400000000
-RebateTierLower_A_1: - 0.1 S_A + rebate_A - 19400000000 y_rebate_A_1
- &gt;= -19400000000
-RebateTierLower_B_0: rebate_B - 97000000000 y_rebate_B_0 &gt;= -97000000000
-RebateTierLower_B_1: - 0.05 S_B + rebate_B - 97000000000 y_rebate_B_1
- &gt;= -97000000000
-RebateTierLower_C_0: rebate_C - 97000000000 y_rebate_C_0 &gt;= -97000000000
-RebateTierLower_C_1: - 0.07 S_C + rebate_C - 97000000000 y_rebate_C_1
- &gt;= -97000000000
-RebateTierMax_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
- + x_A_7 + x_A_8 + x_A_9 + 19400000000 y_rebate_A_0 &lt;= 19400000500
-RebateTierMax_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
- + x_B_7 + x_B_8 + x_B_9 + 97000000000 y_rebate_B_0 &lt;= 97000000500
-RebateTierMax_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
- + x_C_7 + x_C_8 + x_C_9 + 97000000000 y_rebate_C_0 &lt;= 97000000700
-RebateTierMin_A_0: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
- + x_A_7 + x_A_8 + x_A_9 &gt;= 0
-RebateTierMin_A_1: x_A_1 + x_A_10 + x_A_2 + x_A_3 + x_A_4 + x_A_5 + x_A_6
- + x_A_7 + x_A_8 + x_A_9 - 500 y_rebate_A_1 &gt;= 0
-RebateTierMin_B_0: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
- + x_B_7 + x_B_8 + x_B_9 &gt;= 0
-RebateTierMin_B_1: x_B_1 + x_B_10 + x_B_2 + x_B_3 + x_B_4 + x_B_5 + x_B_6
- + x_B_7 + x_B_8 + x_B_9 - 500 y_rebate_B_1 &gt;= 0
-RebateTierMin_C_0: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
- + x_C_7 + x_C_8 + x_C_9 &gt;= 0
-RebateTierMin_C_1: x_C_1 + x_C_10 + x_C_2 + x_C_3 + x_C_4 + x_C_5 + x_C_6
- + x_C_7 + x_C_8 + x_C_9 - 700 y_rebate_C_1 &gt;= 0
-RebateTierSelect_A: y_rebate_A_0 + y_rebate_A_1 = 1
-RebateTierSelect_B: y_rebate_B_0 + y_rebate_B_1 = 1
-RebateTierSelect_C: y_rebate_C_0 + y_rebate_C_1 = 1
-RebateTierUpper_A_0: rebate_A + 19400000000 y_rebate_A_0 &lt;= 19400000000
-RebateTierUpper_A_1: - 0.1 S_A + rebate_A + 19400000000 y_rebate_A_1
- &lt;= 19400000000
-RebateTierUpper_B_0: rebate_B + 97000000000 y_rebate_B_0 &lt;= 97000000000
-RebateTierUpper_B_1: - 0.05 S_B + rebate_B + 97000000000 y_rebate_B_1
- &lt;= 97000000000
-RebateTierUpper_C_0: rebate_C + 97000000000 y_rebate_C_0 &lt;= 97000000000
-RebateTierUpper_C_1: - 0.07 S_C + rebate_C + 97000000000 y_rebate_C_1
- &lt;= 97000000000
-TransitionLower_10_A: x_A_10 &gt;= 0
-TransitionLower_10_B: x_B_10 &gt;= 0
-TransitionLower_1_B: x_B_1 &gt;= 0
-TransitionLower_1_C: x_C_1 &gt;= 0
-TransitionLower_2_A: x_A_2 &gt;= 0
-TransitionLower_2_C: x_C_2 &gt;= 0
-TransitionLower_3_A: x_A_3 &gt;= 0
-TransitionLower_3_B: x_B_3 &gt;= 0
-TransitionLower_4_A: x_A_4 &gt;= 0
-TransitionLower_4_B: x_B_4 &gt;= 0
-TransitionLower_5_A: x_A_5 &gt;= 0
-TransitionLower_5_B: x_B_5 &gt;= 0
-TransitionLower_6_A: x_A_6 &gt;= 0
-TransitionLower_6_B: x_B_6 &gt;= 0
-TransitionLower_7_A: x_A_7 &gt;= 0
-TransitionLower_7_B: x_B_7 &gt;= 0
-TransitionLower_8_A: x_A_8 &gt;= 0
-TransitionLower_8_B: x_B_8 &gt;= 0
-TransitionLower_9_A: x_A_9 &gt;= 0
-TransitionLower_9_B: x_B_9 &gt;= 0
-Transition_10_A: - 13 T_10_A + x_A_10 &lt;= 0
-Transition_10_B: - 13 T_10_B + x_B_10 &lt;= 0
-Transition_1_B: - 700 T_1_B + x_B_1 &lt;= 0
-Transition_1_C: - 700 T_1_C + x_C_1 &lt;= 0
-Transition_2_A: - 9000 T_2_A + x_A_2 &lt;= 0
-Transition_2_C: - 9000 T_2_C + x_C_2 &lt;= 0
-Transition_3_A: - 600 T_3_A + x_A_3 &lt;= 0
-Transition_3_B: - 600 T_3_B + x_B_3 &lt;= 0
-Transition_4_A: - 5670 T_4_A + x_A_4 &lt;= 0
-Transition_4_B: - 5670 T_4_B + x_B_4 &lt;= 0
-Transition_5_A: - 45 T_5_A + x_A_5 &lt;= 0
-Transition_5_B: - 45 T_5_B + x_B_5 &lt;= 0
-Transition_6_A: - 242 T_6_A + x_A_6 &lt;= 0
-Transition_6_B: - 242 T_6_B + x_B_6 &lt;= 0
-Transition_7_A: - 664 T_7_A + x_A_7 &lt;= 0
-Transition_7_B: - 664 T_7_B + x_B_7 &lt;= 0
-Transition_8_A: - 24 T_8_A + x_A_8 &lt;= 0
-Transition_8_B: - 24 T_8_B + x_B_8 &lt;= 0
-Transition_9_A: - 232 T_9_A + x_A_9 &lt;= 0
-Transition_9_B: - 232 T_9_B + x_B_9 &lt;= 0
-Transitions_0_UB: T_10_A + T_10_B + T_3_A + T_3_B + T_4_A + T_4_B + T_5_A
- + T_5_B + T_6_A + T_6_B + T_7_A + T_7_B + T_8_A + T_8_B + T_9_A + T_9_B &lt;= 2
-Volume_A: V_A - x_A_1 - x_A_10 - x_A_2 - x_A_3 - x_A_4 - x_A_5 - x_A_6 - x_A_7
- - x_A_8 - x_A_9 = 0
-Volume_B: V_B - x_B_1 - x_B_10 - x_B_2 - x_B_3 - x_B_4 - x_B_5 - x_B_6 - x_B_7
- - x_B_8 - x_B_9 = 0
-Volume_C: V_C - x_C_1 - x_C_10 - x_C_2 - x_C_3 - x_C_4 - x_C_5 - x_C_6 - x_C_7
- - x_C_8 - x_C_9 = 0
+ActiveLink_BASF_1: x_BASF_1 - 1000000000 z_BASF &lt;= 0
+ActiveLink_BASF_2: x_BASF_2 - 1000000000 z_BASF &lt;= 0
+ActiveLink_BASF_3: x_BASF_3 - 1000000000 z_BASF &lt;= 0
+ActiveLink_BASF_4: x_BASF_4 - 1000000000 z_BASF &lt;= 0
+ActiveLink_BASF_5: x_BASF_5 - 1000000000 z_BASF &lt;= 0
+ActiveLink_Covestro_1: x_Covestro_1 - 1000000000 z_Covestro &lt;= 0
+ActiveLink_Covestro_2: x_Covestro_2 - 1000000000 z_Covestro &lt;= 0
+ActiveLink_Covestro_3: x_Covestro_3 - 1000000000 z_Covestro &lt;= 0
+ActiveLink_Covestro_4: x_Covestro_4 - 1000000000 z_Covestro &lt;= 0
+ActiveLink_Covestro_5: x_Covestro_5 - 1000000000 z_Covestro &lt;= 0
+ActiveLink_Dow_1: x_Dow_1 - 1000000000 z_Dow &lt;= 0
+ActiveLink_Dow_2: x_Dow_2 - 1000000000 z_Dow &lt;= 0
+ActiveLink_Dow_3: x_Dow_3 - 1000000000 z_Dow &lt;= 0
+ActiveLink_Dow_4: x_Dow_4 - 1000000000 z_Dow &lt;= 0
+ActiveLink_Dow_5: x_Dow_5 - 1000000000 z_Dow &lt;= 0
+ActiveLink_Huntsman_1: x_Huntsman_1 - 1000000000 z_Huntsman &lt;= 0
+ActiveLink_Huntsman_2: x_Huntsman_2 - 1000000000 z_Huntsman &lt;= 0
+ActiveLink_Huntsman_3: x_Huntsman_3 - 1000000000 z_Huntsman &lt;= 0
+ActiveLink_Huntsman_4: x_Huntsman_4 - 1000000000 z_Huntsman &lt;= 0
+ActiveLink_Huntsman_5: x_Huntsman_5 - 1000000000 z_Huntsman &lt;= 0
+ActiveLink_Wanhua_1: x_Wanhua_1 - 1000000000 z_Wanhua &lt;= 0
+ActiveLink_Wanhua_2: x_Wanhua_2 - 1000000000 z_Wanhua &lt;= 0
+ActiveLink_Wanhua_3: x_Wanhua_3 - 1000000000 z_Wanhua &lt;= 0
+ActiveLink_Wanhua_4: x_Wanhua_4 - 1000000000 z_Wanhua &lt;= 0
+ActiveLink_Wanhua_5: x_Wanhua_5 - 1000000000 z_Wanhua &lt;= 0
+BaseSpend_BASF: S0_BASF - 0.8762 x_BASF_1 - 0.8862 x_BASF_2 - 0.8762 x_BASF_3
+ - 0.9372 x_BASF_4 - 0.8762 x_BASF_5 = 0
+BaseSpend_Covestro: S0_Covestro - 0.788 x_Covestro_1 - 0.973 x_Covestro_2
+ - 0.863 x_Covestro_3 - 0.983 x_Covestro_4 - 0.813 x_Covestro_5 = 0
+BaseSpend_Dow: S0_Dow - 0.753 x_Dow_1 - 0.823 x_Dow_2 - 0.773 x_Dow_3
+ - 0.843 x_Dow_4 - 0.743 x_Dow_5 = 0
+BaseSpend_Huntsman: S0_Huntsman - 0.83 x_Huntsman_1 - 0.83 x_Huntsman_2
+ - 0.83 x_Huntsman_3 - 0.83 x_Huntsman_4 - 0.83 x_Huntsman_5 = 0
+BaseSpend_Wanhua: S0_Wanhua - 0.8 x_Wanhua_1 - 0.8 x_Wanhua_2 - 0.8 x_Wanhua_3
+ - 0.831 x_Wanhua_4 - 0.8 x_Wanhua_5 = 0
+Capacity_BASF_Bid_ID_1: x_BASF_1 &lt;= 10000000000
+Capacity_BASF_Bid_ID_2: x_BASF_2 &lt;= 10000000000
+Capacity_BASF_Bid_ID_3: x_BASF_3 &lt;= 10000000000
+Capacity_BASF_Bid_ID_4: x_BASF_4 &lt;= 10000000000
+Capacity_BASF_Bid_ID_5: x_BASF_5 &lt;= 10000000000
+Capacity_Covestro_Bid_ID_1: x_Covestro_1 &lt;= 10000000000
+Capacity_Covestro_Bid_ID_2: x_Covestro_2 &lt;= 10000000000
+Capacity_Covestro_Bid_ID_3: x_Covestro_3 &lt;= 10000000000
+Capacity_Covestro_Bid_ID_4: x_Covestro_4 &lt;= 10000000000
+Capacity_Covestro_Bid_ID_5: x_Covestro_5 &lt;= 10000000000
+Capacity_Dow_Bid_ID_1: x_Dow_1 &lt;= 10000000000
+Capacity_Dow_Bid_ID_2: x_Dow_2 &lt;= 10000000000
+Capacity_Dow_Bid_ID_3: x_Dow_3 &lt;= 10000000000
+Capacity_Dow_Bid_ID_4: x_Dow_4 &lt;= 10000000000
+Capacity_Dow_Bid_ID_5: x_Dow_5 &lt;= 10000000000
+Capacity_Huntsman_Bid_ID_1: x_Huntsman_1 &lt;= 10000000000
+Capacity_Huntsman_Bid_ID_2: x_Huntsman_2 &lt;= 10000000000
+Capacity_Huntsman_Bid_ID_3: x_Huntsman_3 &lt;= 10000000000
+Capacity_Huntsman_Bid_ID_4: x_Huntsman_4 &lt;= 10000000000
+Capacity_Huntsman_Bid_ID_5: x_Huntsman_5 &lt;= 10000000000
+Capacity_Wanhua_Bid_ID_1: x_Wanhua_1 &lt;= 10000000000
+Capacity_Wanhua_Bid_ID_2: x_Wanhua_2 &lt;= 10000000000
+Capacity_Wanhua_Bid_ID_3: x_Wanhua_3 &lt;= 10000000000
+Capacity_Wanhua_Bid_ID_4: x_Wanhua_4 &lt;= 10000000000
+Capacity_Wanhua_Bid_ID_5: x_Wanhua_5 &lt;= 10000000000
+Demand_1: x_BASF_1 + x_Covestro_1 + x_Dow_1 + x_Huntsman_1 + x_Wanhua_1
+ = 8860493
+Demand_2: x_BASF_2 + x_Covestro_2 + x_Dow_2 + x_Huntsman_2 + x_Wanhua_2
+ = 7093293
+Demand_3: x_BASF_3 + x_Covestro_3 + x_Dow_3 + x_Huntsman_3 + x_Wanhua_3
+ = 7423090
+Demand_4: x_BASF_4 + x_Covestro_4 + x_Dow_4 + x_Huntsman_4 + x_Wanhua_4
+ = 14146424
+Demand_5: x_BASF_5 + x_Covestro_5 + x_Dow_5 + x_Huntsman_5 + x_Wanhua_5
+ = 4943948
+EffectiveSpend_BASF: - S0_BASF + S_BASF + d_BASF = 0
+EffectiveSpend_Covestro: - S0_Covestro + S_Covestro + d_Covestro = 0
+EffectiveSpend_Dow: - S0_Dow + S_Dow + d_Dow = 0
+EffectiveSpend_Huntsman: - S0_Huntsman + S_Huntsman + d_Huntsman = 0
+EffectiveSpend_Wanhua: - S0_Wanhua + S_Wanhua + d_Wanhua = 0
+Fix_d_BASF: d_BASF = 0
+Fix_d_Covestro: d_Covestro = 0
+Fix_d_Dow: d_Dow = 0
+Fix_d_Huntsman: d_Huntsman = 0
+Fix_d_Wanhua: d_Wanhua = 0
+Fix_rebate_Dow: rebate_Dow = 0
+Fix_rebate_Wanhua: rebate_Wanhua = 0
+MinAward_BASF: x_BASF_1 + x_BASF_2 + x_BASF_3 + x_BASF_4 + x_BASF_5 - z_BASF
+ &gt;= 0
+MinAward_Covestro: x_Covestro_1 + x_Covestro_2 + x_Covestro_3 + x_Covestro_4
+ + x_Covestro_5 - z_Covestro &gt;= 0
+MinAward_Dow: x_Dow_1 + x_Dow_2 + x_Dow_3 + x_Dow_4 + x_Dow_5 - z_Dow &gt;= 0
+MinAward_Huntsman: x_Huntsman_1 + x_Huntsman_2 + x_Huntsman_3 + x_Huntsman_4
+ + x_Huntsman_5 - z_Huntsman &gt;= 0
+MinAward_Wanhua: x_Wanhua_1 + x_Wanhua_2 + x_Wanhua_3 + x_Wanhua_4
+ + x_Wanhua_5 - z_Wanhua &gt;= 0
+RebateTierLower_BASF_0: rebate_BASF - 49150000000 y_rebate_BASF_0
+ &gt;= -49150000000
+RebateTierLower_BASF_1: rebate_BASF - 49150000000 y_rebate_BASF_1
+ &gt;= -49150000000
+RebateTierLower_Covestro_0: rebate_Covestro - 49150000000 y_rebate_Covestro_0
+ &gt;= -49150000000
+RebateTierLower_Covestro_1: rebate_Covestro - 49150000000 y_rebate_Covestro_1
+ &gt;= -49150000000
+RebateTierLower_Huntsman_0: rebate_Huntsman - 49150000000 y_rebate_Huntsman_0
+ &gt;= -49150000000
+RebateTierLower_Huntsman_1: rebate_Huntsman - 49150000000 y_rebate_Huntsman_1
+ &gt;= -49150000000
+RebateTierMax_BASF_0: 49150000000 y_rebate_BASF_0 &lt;= 49150000500
+RebateTierMax_Covestro_0: 49150000000 y_rebate_Covestro_0 &lt;= 49150000500
+RebateTierMax_Huntsman_0: 49150000000 y_rebate_Huntsman_0 &lt;= 49150000700
+_dummy: __dummy = 0
+RebateTierMin_BASF_0: __dummy &gt;= 0
+RebateTierMin_BASF_1: - 500 y_rebate_BASF_1 &gt;= 0
+RebateTierMin_Covestro_0: __dummy &gt;= 0
+RebateTierMin_Covestro_1: x_Covestro_1 + x_Covestro_2 + x_Covestro_3
+ + x_Covestro_4 + x_Covestro_5 - 500 y_rebate_Covestro_1 &gt;= 0
+RebateTierMin_Huntsman_0: __dummy &gt;= 0
+RebateTierMin_Huntsman_1: x_Huntsman_1 + x_Huntsman_2 + x_Huntsman_3
+ + x_Huntsman_4 + x_Huntsman_5 - 700 y_rebate_Huntsman_1 &gt;= 0
+RebateTierSelect_BASF: y_rebate_BASF_0 + y_rebate_BASF_1 = 1
+RebateTierSelect_Covestro: y_rebate_Covestro_0 + y_rebate_Covestro_1 = 1
+RebateTierSelect_Huntsman: y_rebate_Huntsman_0 + y_rebate_Huntsman_1 = 1
+RebateTierUpper_BASF_0: rebate_BASF + 49150000000 y_rebate_BASF_0
+ &lt;= 49150000000
+RebateTierUpper_BASF_1: rebate_BASF + 49150000000 y_rebate_BASF_1
+ &lt;= 49150000000
+RebateTierUpper_Covestro_0: rebate_Covestro + 49150000000 y_rebate_Covestro_0
+ &lt;= 49150000000
+RebateTierUpper_Covestro_1: rebate_Covestro + 49150000000 y_rebate_Covestro_1
+ &lt;= 49150000000
+RebateTierUpper_Huntsman_0: rebate_Huntsman + 49150000000 y_rebate_Huntsman_0
+ &lt;= 49150000000
+RebateTierUpper_Huntsman_1: rebate_Huntsman + 49150000000 y_rebate_Huntsman_1
+ &lt;= 49150000000
+SupplierExclusion_0_1_BASF: x_BASF_1 = 0
+SupplierExclusion_0_1_Covestro: x_Covestro_1 = 0
+SupplierExclusion_0_1_Huntsman: x_Huntsman_1 = 0
+SupplierExclusion_0_1_Wanhua: x_Wanhua_1 = 0
+SupplierExclusion_0_2_Covestro: x_Covestro_2 = 0
+SupplierExclusion_0_2_Dow: x_Dow_2 = 0
+SupplierExclusion_0_2_Huntsman: x_Huntsman_2 = 0
+SupplierExclusion_0_2_Wanhua: x_Wanhua_2 = 0
+SupplierExclusion_0_3_Covestro: x_Covestro_3 = 0
+SupplierExclusion_0_3_Dow: x_Dow_3 = 0
+SupplierExclusion_0_3_Huntsman: x_Huntsman_3 = 0
+SupplierExclusion_0_3_Wanhua: x_Wanhua_3 = 0
+SupplierExclusion_0_4_Covestro: x_Covestro_4 = 0
+SupplierExclusion_0_4_Dow: x_Dow_4 = 0
+SupplierExclusion_0_4_Huntsman: x_Huntsman_4 = 0
+SupplierExclusion_0_4_Wanhua: x_Wanhua_4 = 0
+SupplierExclusion_0_5_BASF: x_BASF_5 = 0
+SupplierExclusion_0_5_Covestro: x_Covestro_5 = 0
+SupplierExclusion_0_5_Huntsman: x_Huntsman_5 = 0
+SupplierExclusion_0_5_Wanhua: x_Wanhua_5 = 0
+TransitionLower_1_BASF: x_BASF_1 &gt;= 0
+TransitionLower_1_Covestro: x_Covestro_1 &gt;= 0
+TransitionLower_1_Huntsman: x_Huntsman_1 &gt;= 0
+TransitionLower_1_Wanhua: x_Wanhua_1 &gt;= 0
+TransitionLower_2_Covestro: x_Covestro_2 &gt;= 0
+TransitionLower_2_Dow: x_Dow_2 &gt;= 0
+TransitionLower_2_Huntsman: x_Huntsman_2 &gt;= 0
+TransitionLower_2_Wanhua: x_Wanhua_2 &gt;= 0
+TransitionLower_3_Covestro: x_Covestro_3 &gt;= 0
+TransitionLower_3_Dow: x_Dow_3 &gt;= 0
+TransitionLower_3_Huntsman: x_Huntsman_3 &gt;= 0
+TransitionLower_3_Wanhua: x_Wanhua_3 &gt;= 0
+TransitionLower_4_Covestro: x_Covestro_4 &gt;= 0
+TransitionLower_4_Dow: x_Dow_4 &gt;= 0
+TransitionLower_4_Huntsman: x_Huntsman_4 &gt;= 0
+TransitionLower_4_Wanhua: x_Wanhua_4 &gt;= 0
+TransitionLower_5_BASF: x_BASF_5 &gt;= 0
+TransitionLower_5_Covestro: x_Covestro_5 &gt;= 0
+TransitionLower_5_Huntsman: x_Huntsman_5 &gt;= 0
+TransitionLower_5_Wanhua: x_Wanhua_5 &gt;= 0
+Transition_1_BASF: - 8860493 T_1_BASF + x_BASF_1 &lt;= 0
+Transition_1_Covestro: - 8860493 T_1_Covestro + x_Covestro_1 &lt;= 0
+Transition_1_Huntsman: - 8860493 T_1_Huntsman + x_Huntsman_1 &lt;= 0
+Transition_1_Wanhua: - 8860493 T_1_Wanhua + x_Wanhua_1 &lt;= 0
+Transition_2_Covestro: - 7093293 T_2_Covestro + x_Covestro_2 &lt;= 0
+Transition_2_Dow: - 7093293 T_2_Dow + x_Dow_2 &lt;= 0
+Transition_2_Huntsman: - 7093293 T_2_Huntsman + x_Huntsman_2 &lt;= 0
+Transition_2_Wanhua: - 7093293 T_2_Wanhua + x_Wanhua_2 &lt;= 0
+Transition_3_Covestro: - 7423090 T_3_Covestro + x_Covestro_3 &lt;= 0
+Transition_3_Dow: - 7423090 T_3_Dow + x_Dow_3 &lt;= 0
+Transition_3_Huntsman: - 7423090 T_3_Huntsman + x_Huntsman_3 &lt;= 0
+Transition_3_Wanhua: - 7423090 T_3_Wanhua + x_Wanhua_3 &lt;= 0
+Transition_4_Covestro: - 14146424 T_4_Covestro + x_Covestro_4 &lt;= 0
+Transition_4_Dow: - 14146424 T_4_Dow + x_Dow_4 &lt;= 0
+Transition_4_Huntsman: - 14146424 T_4_Huntsman + x_Huntsman_4 &lt;= 0
+Transition_4_Wanhua: - 14146424 T_4_Wanhua + x_Wanhua_4 &lt;= 0
+Transition_5_BASF: - 4943948 T_5_BASF + x_BASF_5 &lt;= 0
+Transition_5_Covestro: - 4943948 T_5_Covestro + x_Covestro_5 &lt;= 0
+Transition_5_Huntsman: - 4943948 T_5_Huntsman + x_Huntsman_5 &lt;= 0
+Transition_5_Wanhua: - 4943948 T_5_Wanhua + x_Wanhua_5 &lt;= 0
+Volume_BASF: V_BASF - x_BASF_1 - x_BASF_2 - x_BASF_3 - x_BASF_4 - x_BASF_5 = 0
+Volume_Covestro: V_Covestro - x_Covestro_1 - x_Covestro_2 - x_Covestro_3
+ - x_Covestro_4 - x_Covestro_5 = 0
+Volume_Dow: V_Dow - x_Dow_1 - x_Dow_2 - x_Dow_3 - x_Dow_4 - x_Dow_5 = 0
+Volume_Huntsman: V_Huntsman - x_Huntsman_1 - x_Huntsman_2 - x_Huntsman_3
+ - x_Huntsman_4 - x_Huntsman_5 = 0
+Volume_Wanhua: V_Wanhua - x_Wanhua_1 - x_Wanhua_2 - x_Wanhua_3 - x_Wanhua_4
+ - x_Wanhua_5 = 0
+Bounds
+ __dummy = 0
 Binaries
-T_10_A
-T_10_B
-T_1_B
-T_1_C
-T_2_A
-T_2_C
-T_3_A
-T_3_B
-T_4_A
-T_4_B
-T_5_A
-T_5_B
-T_6_A
-T_6_B
-T_7_A
-T_7_B
-T_8_A
-T_8_B
-T_9_A
-T_9_B
-y_rebate_A_0
-y_rebate_A_1
-y_rebate_B_0
-y_rebate_B_1
-y_rebate_C_0
-y_rebate_C_1
-z_A
-z_B
-z_C
-z_discount_A_0
-z_discount_A_1
-z_discount_B_0
-z_discount_B_1
-z_discount_C_0
-z_discount_C_1
+T_1_BASF
+T_1_Covestro
+T_1_Huntsman
+T_1_Wanhua
+T_2_Covestro
+T_2_Dow
+T_2_Huntsman
+T_2_Wanhua
+T_3_Covestro
+T_3_Dow
+T_3_Huntsman
+T_3_Wanhua
+T_4_Covestro
+T_4_Dow
+T_4_Huntsman
+T_4_Wanhua
+T_5_BASF
+T_5_Covestro
+T_5_Huntsman
+T_5_Wanhua
+y_rebate_BASF_0
+y_rebate_BASF_1
+y_rebate_Covestro_0
+y_rebate_Covestro_1
+y_rebate_Huntsman_0
+y_rebate_Huntsman_1
+z_BASF
+z_Covestro
+z_Dow
+z_Huntsman
+z_Wanhua
 End
 </t>
         </is>
@@ -1422,7 +1123,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1455,47 +1156,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BusinessUnit</t>
+          <t>Bid ID</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Covestro</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BusinessUnit</t>
+          <t>Bid ID</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Dow</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1509,13 +1210,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Huntsman</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1525,17 +1226,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Wanhua</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1545,17 +1246,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1565,17 +1266,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Covestro</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1585,17 +1286,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Dow</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1605,17 +1306,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Huntsman</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1625,17 +1326,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Wanhua</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1645,17 +1346,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1665,17 +1366,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Covestro</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1685,17 +1386,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Dow</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1705,17 +1406,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Huntsman</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1725,17 +1426,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Wanhua</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1749,13 +1450,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1769,13 +1470,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Covestro</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1785,17 +1486,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Dow</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1805,17 +1506,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Huntsman</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1825,17 +1526,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Wanhua</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1845,17 +1546,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>BASF</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1865,17 +1566,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Covestro</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1885,11 +1586,71 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>100000000</v>
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Dow</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Huntsman</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Wanhua</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>10000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue where if rebates or volume tier exceeded demand caused infeasibility
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -524,27 +524,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Diboll</t>
+          <t>Brunswick</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Dow</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1.06</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
-        <v>9392122.58</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Dow</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.753</v>
+        <v>0</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -552,16 +552,16 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.753</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>6671951.229</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>8860493</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>2720171.351</v>
+        <v>0</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -583,27 +583,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mt Jewett</t>
+          <t>Brunswick</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1.16</v>
+        <v>36</v>
       </c>
       <c r="F3" t="n">
-        <v>8228219.880000001</v>
+        <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.8862</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -611,16 +611,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0.8862</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>6286076.2566</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>7093293</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>1942143.623400001</v>
+        <v>0</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -642,27 +642,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Clarendon</t>
+          <t>Palatka</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1.19</v>
+        <v>82</v>
       </c>
       <c r="F4" t="n">
-        <v>8833477.100000001</v>
+        <v>529884</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>Supplier 5</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.8762</v>
+        <v>89</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.8762</v>
+        <v>89</v>
       </c>
       <c r="K4" t="n">
-        <v>6504111.458</v>
+        <v>575118</v>
       </c>
       <c r="L4" t="n">
-        <v>7423090</v>
+        <v>6462</v>
       </c>
       <c r="M4" t="n">
-        <v>2329365.642000002</v>
+        <v>-45234</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -701,27 +701,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Englehart</t>
+          <t>Big Island</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1.1527</v>
+        <v>32</v>
       </c>
       <c r="F5" t="n">
-        <v>16306582.9448</v>
+        <v>0</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0.9372</v>
+        <v>0</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.9372</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>13258028.5728</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>14146424</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>3048554.372</v>
+        <v>0</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -760,27 +760,27 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fordyce</t>
+          <t>Huntsville</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Dow</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1.16</v>
+        <v>75</v>
       </c>
       <c r="F6" t="n">
-        <v>5734979.680000001</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Dow</t>
+          <t>No Bid</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.743</v>
+        <v>0</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -788,16 +788,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0.743</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>3673353.364</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>4943948</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>2061626.316000001</v>
+        <v>0</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -837,7 +837,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model is optimal.</t>
+          <t xml:space="preserve">Model is infeasible. Likely causes include:
+ - Insufficient supplier capacity relative to demand.
+ - Custom rule constraints conflicting with overall volume/demand.
+Detailed Rule Evaluations:
+</t>
         </is>
       </c>
     </row>
@@ -872,241 +876,200 @@
         <is>
           <t xml:space="preserve">\* Sourcing_with_MultiTier_Rebates_Discounts *\
 Minimize
-OBJ: S_BASF + S_Covestro + S_Dow + S_Huntsman + S_Wanhua - rebate_BASF
- - rebate_Covestro - rebate_Dow - rebate_Huntsman - rebate_Wanhua
+OBJ: S_Supplier_1 + S_Supplier_2 + S_Supplier_3 + S_Supplier_4 + S_Supplier_5
+ - rebate_Supplier_1 - rebate_Supplier_2 - rebate_Supplier_3
+ - rebate_Supplier_4 - rebate_Supplier_5
 Subject To
-ActiveLink_BASF_1: x_BASF_1 - 1000000000 z_BASF &lt;= 0
-ActiveLink_BASF_2: x_BASF_2 - 1000000000 z_BASF &lt;= 0
-ActiveLink_BASF_3: x_BASF_3 - 1000000000 z_BASF &lt;= 0
-ActiveLink_BASF_4: x_BASF_4 - 1000000000 z_BASF &lt;= 0
-ActiveLink_BASF_5: x_BASF_5 - 1000000000 z_BASF &lt;= 0
-ActiveLink_Covestro_1: x_Covestro_1 - 1000000000 z_Covestro &lt;= 0
-ActiveLink_Covestro_2: x_Covestro_2 - 1000000000 z_Covestro &lt;= 0
-ActiveLink_Covestro_3: x_Covestro_3 - 1000000000 z_Covestro &lt;= 0
-ActiveLink_Covestro_4: x_Covestro_4 - 1000000000 z_Covestro &lt;= 0
-ActiveLink_Covestro_5: x_Covestro_5 - 1000000000 z_Covestro &lt;= 0
-ActiveLink_Dow_1: x_Dow_1 - 1000000000 z_Dow &lt;= 0
-ActiveLink_Dow_2: x_Dow_2 - 1000000000 z_Dow &lt;= 0
-ActiveLink_Dow_3: x_Dow_3 - 1000000000 z_Dow &lt;= 0
-ActiveLink_Dow_4: x_Dow_4 - 1000000000 z_Dow &lt;= 0
-ActiveLink_Dow_5: x_Dow_5 - 1000000000 z_Dow &lt;= 0
-ActiveLink_Huntsman_1: x_Huntsman_1 - 1000000000 z_Huntsman &lt;= 0
-ActiveLink_Huntsman_2: x_Huntsman_2 - 1000000000 z_Huntsman &lt;= 0
-ActiveLink_Huntsman_3: x_Huntsman_3 - 1000000000 z_Huntsman &lt;= 0
-ActiveLink_Huntsman_4: x_Huntsman_4 - 1000000000 z_Huntsman &lt;= 0
-ActiveLink_Huntsman_5: x_Huntsman_5 - 1000000000 z_Huntsman &lt;= 0
-ActiveLink_Wanhua_1: x_Wanhua_1 - 1000000000 z_Wanhua &lt;= 0
-ActiveLink_Wanhua_2: x_Wanhua_2 - 1000000000 z_Wanhua &lt;= 0
-ActiveLink_Wanhua_3: x_Wanhua_3 - 1000000000 z_Wanhua &lt;= 0
-ActiveLink_Wanhua_4: x_Wanhua_4 - 1000000000 z_Wanhua &lt;= 0
-ActiveLink_Wanhua_5: x_Wanhua_5 - 1000000000 z_Wanhua &lt;= 0
-BaseSpend_BASF: S0_BASF - 0.8762 x_BASF_1 - 0.8862 x_BASF_2 - 0.8762 x_BASF_3
- - 0.9372 x_BASF_4 - 0.8762 x_BASF_5 = 0
-BaseSpend_Covestro: S0_Covestro - 0.788 x_Covestro_1 - 0.973 x_Covestro_2
- - 0.863 x_Covestro_3 - 0.983 x_Covestro_4 - 0.813 x_Covestro_5 = 0
-BaseSpend_Dow: S0_Dow - 0.753 x_Dow_1 - 0.823 x_Dow_2 - 0.773 x_Dow_3
- - 0.843 x_Dow_4 - 0.743 x_Dow_5 = 0
-BaseSpend_Huntsman: S0_Huntsman - 0.83 x_Huntsman_1 - 0.83 x_Huntsman_2
- - 0.83 x_Huntsman_3 - 0.83 x_Huntsman_4 - 0.83 x_Huntsman_5 = 0
-BaseSpend_Wanhua: S0_Wanhua - 0.8 x_Wanhua_1 - 0.8 x_Wanhua_2 - 0.8 x_Wanhua_3
- - 0.831 x_Wanhua_4 - 0.8 x_Wanhua_5 = 0
-Capacity_BASF_Bid_ID_1: x_BASF_1 &lt;= 10000000000
-Capacity_BASF_Bid_ID_2: x_BASF_2 &lt;= 10000000000
-Capacity_BASF_Bid_ID_3: x_BASF_3 &lt;= 10000000000
-Capacity_BASF_Bid_ID_4: x_BASF_4 &lt;= 10000000000
-Capacity_BASF_Bid_ID_5: x_BASF_5 &lt;= 10000000000
-Capacity_Covestro_Bid_ID_1: x_Covestro_1 &lt;= 10000000000
-Capacity_Covestro_Bid_ID_2: x_Covestro_2 &lt;= 10000000000
-Capacity_Covestro_Bid_ID_3: x_Covestro_3 &lt;= 10000000000
-Capacity_Covestro_Bid_ID_4: x_Covestro_4 &lt;= 10000000000
-Capacity_Covestro_Bid_ID_5: x_Covestro_5 &lt;= 10000000000
-Capacity_Dow_Bid_ID_1: x_Dow_1 &lt;= 10000000000
-Capacity_Dow_Bid_ID_2: x_Dow_2 &lt;= 10000000000
-Capacity_Dow_Bid_ID_3: x_Dow_3 &lt;= 10000000000
-Capacity_Dow_Bid_ID_4: x_Dow_4 &lt;= 10000000000
-Capacity_Dow_Bid_ID_5: x_Dow_5 &lt;= 10000000000
-Capacity_Huntsman_Bid_ID_1: x_Huntsman_1 &lt;= 10000000000
-Capacity_Huntsman_Bid_ID_2: x_Huntsman_2 &lt;= 10000000000
-Capacity_Huntsman_Bid_ID_3: x_Huntsman_3 &lt;= 10000000000
-Capacity_Huntsman_Bid_ID_4: x_Huntsman_4 &lt;= 10000000000
-Capacity_Huntsman_Bid_ID_5: x_Huntsman_5 &lt;= 10000000000
-Capacity_Wanhua_Bid_ID_1: x_Wanhua_1 &lt;= 10000000000
-Capacity_Wanhua_Bid_ID_2: x_Wanhua_2 &lt;= 10000000000
-Capacity_Wanhua_Bid_ID_3: x_Wanhua_3 &lt;= 10000000000
-Capacity_Wanhua_Bid_ID_4: x_Wanhua_4 &lt;= 10000000000
-Capacity_Wanhua_Bid_ID_5: x_Wanhua_5 &lt;= 10000000000
-Demand_1: x_BASF_1 + x_Covestro_1 + x_Dow_1 + x_Huntsman_1 + x_Wanhua_1
- = 8860493
-Demand_2: x_BASF_2 + x_Covestro_2 + x_Dow_2 + x_Huntsman_2 + x_Wanhua_2
- = 7093293
-Demand_3: x_BASF_3 + x_Covestro_3 + x_Dow_3 + x_Huntsman_3 + x_Wanhua_3
- = 7423090
-Demand_4: x_BASF_4 + x_Covestro_4 + x_Dow_4 + x_Huntsman_4 + x_Wanhua_4
- = 14146424
-Demand_5: x_BASF_5 + x_Covestro_5 + x_Dow_5 + x_Huntsman_5 + x_Wanhua_5
- = 4943948
-EffectiveSpend_BASF: - S0_BASF + S_BASF + d_BASF = 0
-EffectiveSpend_Covestro: - S0_Covestro + S_Covestro + d_Covestro = 0
-EffectiveSpend_Dow: - S0_Dow + S_Dow + d_Dow = 0
-EffectiveSpend_Huntsman: - S0_Huntsman + S_Huntsman + d_Huntsman = 0
-EffectiveSpend_Wanhua: - S0_Wanhua + S_Wanhua + d_Wanhua = 0
-Fix_d_BASF: d_BASF = 0
-Fix_d_Covestro: d_Covestro = 0
-Fix_d_Dow: d_Dow = 0
-Fix_d_Huntsman: d_Huntsman = 0
-Fix_d_Wanhua: d_Wanhua = 0
-Fix_rebate_Dow: rebate_Dow = 0
-Fix_rebate_Wanhua: rebate_Wanhua = 0
-MinAward_BASF: x_BASF_1 + x_BASF_2 + x_BASF_3 + x_BASF_4 + x_BASF_5 - z_BASF
- &gt;= 0
-MinAward_Covestro: x_Covestro_1 + x_Covestro_2 + x_Covestro_3 + x_Covestro_4
- + x_Covestro_5 - z_Covestro &gt;= 0
-MinAward_Dow: x_Dow_1 + x_Dow_2 + x_Dow_3 + x_Dow_4 + x_Dow_5 - z_Dow &gt;= 0
-MinAward_Huntsman: x_Huntsman_1 + x_Huntsman_2 + x_Huntsman_3 + x_Huntsman_4
- + x_Huntsman_5 - z_Huntsman &gt;= 0
-MinAward_Wanhua: x_Wanhua_1 + x_Wanhua_2 + x_Wanhua_3 + x_Wanhua_4
- + x_Wanhua_5 - z_Wanhua &gt;= 0
-RebateTierLower_BASF_0: rebate_BASF - 49150000000 y_rebate_BASF_0
- &gt;= -49150000000
-RebateTierLower_BASF_1: rebate_BASF - 49150000000 y_rebate_BASF_1
- &gt;= -49150000000
-RebateTierLower_Covestro_0: rebate_Covestro - 49150000000 y_rebate_Covestro_0
- &gt;= -49150000000
-RebateTierLower_Covestro_1: rebate_Covestro - 49150000000 y_rebate_Covestro_1
- &gt;= -49150000000
-RebateTierLower_Huntsman_0: rebate_Huntsman - 49150000000 y_rebate_Huntsman_0
- &gt;= -49150000000
-RebateTierLower_Huntsman_1: rebate_Huntsman - 49150000000 y_rebate_Huntsman_1
- &gt;= -49150000000
-RebateTierMax_BASF_0: 49150000000 y_rebate_BASF_0 &lt;= 49150000500
-RebateTierMax_Covestro_0: 49150000000 y_rebate_Covestro_0 &lt;= 49150000500
-RebateTierMax_Huntsman_0: 49150000000 y_rebate_Huntsman_0 &lt;= 49150000700
-_dummy: __dummy = 0
-RebateTierMin_BASF_0: __dummy &gt;= 0
-RebateTierMin_BASF_1: - 500 y_rebate_BASF_1 &gt;= 0
-RebateTierMin_Covestro_0: __dummy &gt;= 0
-RebateTierMin_Covestro_1: x_Covestro_1 + x_Covestro_2 + x_Covestro_3
- + x_Covestro_4 + x_Covestro_5 - 500 y_rebate_Covestro_1 &gt;= 0
-RebateTierMin_Huntsman_0: __dummy &gt;= 0
-RebateTierMin_Huntsman_1: x_Huntsman_1 + x_Huntsman_2 + x_Huntsman_3
- + x_Huntsman_4 + x_Huntsman_5 - 700 y_rebate_Huntsman_1 &gt;= 0
-RebateTierSelect_BASF: y_rebate_BASF_0 + y_rebate_BASF_1 = 1
-RebateTierSelect_Covestro: y_rebate_Covestro_0 + y_rebate_Covestro_1 = 1
-RebateTierSelect_Huntsman: y_rebate_Huntsman_0 + y_rebate_Huntsman_1 = 1
-RebateTierUpper_BASF_0: rebate_BASF + 49150000000 y_rebate_BASF_0
- &lt;= 49150000000
-RebateTierUpper_BASF_1: rebate_BASF + 49150000000 y_rebate_BASF_1
- &lt;= 49150000000
-RebateTierUpper_Covestro_0: rebate_Covestro + 49150000000 y_rebate_Covestro_0
- &lt;= 49150000000
-RebateTierUpper_Covestro_1: rebate_Covestro + 49150000000 y_rebate_Covestro_1
- &lt;= 49150000000
-RebateTierUpper_Huntsman_0: rebate_Huntsman + 49150000000 y_rebate_Huntsman_0
- &lt;= 49150000000
-RebateTierUpper_Huntsman_1: rebate_Huntsman + 49150000000 y_rebate_Huntsman_1
- &lt;= 49150000000
-SupplierExclusion_0_1_BASF: x_BASF_1 = 0
-SupplierExclusion_0_1_Covestro: x_Covestro_1 = 0
-SupplierExclusion_0_1_Huntsman: x_Huntsman_1 = 0
-SupplierExclusion_0_1_Wanhua: x_Wanhua_1 = 0
-SupplierExclusion_0_2_Covestro: x_Covestro_2 = 0
-SupplierExclusion_0_2_Dow: x_Dow_2 = 0
-SupplierExclusion_0_2_Huntsman: x_Huntsman_2 = 0
-SupplierExclusion_0_2_Wanhua: x_Wanhua_2 = 0
-SupplierExclusion_0_3_Covestro: x_Covestro_3 = 0
-SupplierExclusion_0_3_Dow: x_Dow_3 = 0
-SupplierExclusion_0_3_Huntsman: x_Huntsman_3 = 0
-SupplierExclusion_0_3_Wanhua: x_Wanhua_3 = 0
-SupplierExclusion_0_4_Covestro: x_Covestro_4 = 0
-SupplierExclusion_0_4_Dow: x_Dow_4 = 0
-SupplierExclusion_0_4_Huntsman: x_Huntsman_4 = 0
-SupplierExclusion_0_4_Wanhua: x_Wanhua_4 = 0
-SupplierExclusion_0_5_BASF: x_BASF_5 = 0
-SupplierExclusion_0_5_Covestro: x_Covestro_5 = 0
-SupplierExclusion_0_5_Huntsman: x_Huntsman_5 = 0
-SupplierExclusion_0_5_Wanhua: x_Wanhua_5 = 0
-TransitionLower_1_BASF: x_BASF_1 &gt;= 0
-TransitionLower_1_Covestro: x_Covestro_1 &gt;= 0
-TransitionLower_1_Huntsman: x_Huntsman_1 &gt;= 0
-TransitionLower_1_Wanhua: x_Wanhua_1 &gt;= 0
-TransitionLower_2_Covestro: x_Covestro_2 &gt;= 0
-TransitionLower_2_Dow: x_Dow_2 &gt;= 0
-TransitionLower_2_Huntsman: x_Huntsman_2 &gt;= 0
-TransitionLower_2_Wanhua: x_Wanhua_2 &gt;= 0
-TransitionLower_3_Covestro: x_Covestro_3 &gt;= 0
-TransitionLower_3_Dow: x_Dow_3 &gt;= 0
-TransitionLower_3_Huntsman: x_Huntsman_3 &gt;= 0
-TransitionLower_3_Wanhua: x_Wanhua_3 &gt;= 0
-TransitionLower_4_Covestro: x_Covestro_4 &gt;= 0
-TransitionLower_4_Dow: x_Dow_4 &gt;= 0
-TransitionLower_4_Huntsman: x_Huntsman_4 &gt;= 0
-TransitionLower_4_Wanhua: x_Wanhua_4 &gt;= 0
-TransitionLower_5_BASF: x_BASF_5 &gt;= 0
-TransitionLower_5_Covestro: x_Covestro_5 &gt;= 0
-TransitionLower_5_Huntsman: x_Huntsman_5 &gt;= 0
-TransitionLower_5_Wanhua: x_Wanhua_5 &gt;= 0
-Transition_1_BASF: - 8860493 T_1_BASF + x_BASF_1 &lt;= 0
-Transition_1_Covestro: - 8860493 T_1_Covestro + x_Covestro_1 &lt;= 0
-Transition_1_Huntsman: - 8860493 T_1_Huntsman + x_Huntsman_1 &lt;= 0
-Transition_1_Wanhua: - 8860493 T_1_Wanhua + x_Wanhua_1 &lt;= 0
-Transition_2_Covestro: - 7093293 T_2_Covestro + x_Covestro_2 &lt;= 0
-Transition_2_Dow: - 7093293 T_2_Dow + x_Dow_2 &lt;= 0
-Transition_2_Huntsman: - 7093293 T_2_Huntsman + x_Huntsman_2 &lt;= 0
-Transition_2_Wanhua: - 7093293 T_2_Wanhua + x_Wanhua_2 &lt;= 0
-Transition_3_Covestro: - 7423090 T_3_Covestro + x_Covestro_3 &lt;= 0
-Transition_3_Dow: - 7423090 T_3_Dow + x_Dow_3 &lt;= 0
-Transition_3_Huntsman: - 7423090 T_3_Huntsman + x_Huntsman_3 &lt;= 0
-Transition_3_Wanhua: - 7423090 T_3_Wanhua + x_Wanhua_3 &lt;= 0
-Transition_4_Covestro: - 14146424 T_4_Covestro + x_Covestro_4 &lt;= 0
-Transition_4_Dow: - 14146424 T_4_Dow + x_Dow_4 &lt;= 0
-Transition_4_Huntsman: - 14146424 T_4_Huntsman + x_Huntsman_4 &lt;= 0
-Transition_4_Wanhua: - 14146424 T_4_Wanhua + x_Wanhua_4 &lt;= 0
-Transition_5_BASF: - 4943948 T_5_BASF + x_BASF_5 &lt;= 0
-Transition_5_Covestro: - 4943948 T_5_Covestro + x_Covestro_5 &lt;= 0
-Transition_5_Huntsman: - 4943948 T_5_Huntsman + x_Huntsman_5 &lt;= 0
-Transition_5_Wanhua: - 4943948 T_5_Wanhua + x_Wanhua_5 &lt;= 0
-Volume_BASF: V_BASF - x_BASF_1 - x_BASF_2 - x_BASF_3 - x_BASF_4 - x_BASF_5 = 0
-Volume_Covestro: V_Covestro - x_Covestro_1 - x_Covestro_2 - x_Covestro_3
- - x_Covestro_4 - x_Covestro_5 = 0
-Volume_Dow: V_Dow - x_Dow_1 - x_Dow_2 - x_Dow_3 - x_Dow_4 - x_Dow_5 = 0
-Volume_Huntsman: V_Huntsman - x_Huntsman_1 - x_Huntsman_2 - x_Huntsman_3
- - x_Huntsman_4 - x_Huntsman_5 = 0
-Volume_Wanhua: V_Wanhua - x_Wanhua_1 - x_Wanhua_2 - x_Wanhua_3 - x_Wanhua_4
- - x_Wanhua_5 = 0
-Bounds
- __dummy = 0
+ActiveLink_Supplier_1_1: x_Supplier_1_1 - 1000000000 z_Supplier_1 &lt;= 0
+ActiveLink_Supplier_1_2: x_Supplier_1_2 - 1000000000 z_Supplier_1 &lt;= 0
+ActiveLink_Supplier_1_3: x_Supplier_1_3 - 1000000000 z_Supplier_1 &lt;= 0
+ActiveLink_Supplier_1_4: x_Supplier_1_4 - 1000000000 z_Supplier_1 &lt;= 0
+ActiveLink_Supplier_1_5: x_Supplier_1_5 - 1000000000 z_Supplier_1 &lt;= 0
+ActiveLink_Supplier_2_1: x_Supplier_2_1 - 1000000000 z_Supplier_2 &lt;= 0
+ActiveLink_Supplier_2_2: x_Supplier_2_2 - 1000000000 z_Supplier_2 &lt;= 0
+ActiveLink_Supplier_2_3: x_Supplier_2_3 - 1000000000 z_Supplier_2 &lt;= 0
+ActiveLink_Supplier_2_4: x_Supplier_2_4 - 1000000000 z_Supplier_2 &lt;= 0
+ActiveLink_Supplier_2_5: x_Supplier_2_5 - 1000000000 z_Supplier_2 &lt;= 0
+ActiveLink_Supplier_3_1: x_Supplier_3_1 - 1000000000 z_Supplier_3 &lt;= 0
+ActiveLink_Supplier_3_2: x_Supplier_3_2 - 1000000000 z_Supplier_3 &lt;= 0
+ActiveLink_Supplier_3_3: x_Supplier_3_3 - 1000000000 z_Supplier_3 &lt;= 0
+ActiveLink_Supplier_3_4: x_Supplier_3_4 - 1000000000 z_Supplier_3 &lt;= 0
+ActiveLink_Supplier_3_5: x_Supplier_3_5 - 1000000000 z_Supplier_3 &lt;= 0
+ActiveLink_Supplier_4_1: x_Supplier_4_1 - 1000000000 z_Supplier_4 &lt;= 0
+ActiveLink_Supplier_4_2: x_Supplier_4_2 - 1000000000 z_Supplier_4 &lt;= 0
+ActiveLink_Supplier_4_3: x_Supplier_4_3 - 1000000000 z_Supplier_4 &lt;= 0
+ActiveLink_Supplier_4_4: x_Supplier_4_4 - 1000000000 z_Supplier_4 &lt;= 0
+ActiveLink_Supplier_4_5: x_Supplier_4_5 - 1000000000 z_Supplier_4 &lt;= 0
+ActiveLink_Supplier_5_1: x_Supplier_5_1 - 1000000000 z_Supplier_5 &lt;= 0
+ActiveLink_Supplier_5_2: x_Supplier_5_2 - 1000000000 z_Supplier_5 &lt;= 0
+ActiveLink_Supplier_5_3: x_Supplier_5_3 - 1000000000 z_Supplier_5 &lt;= 0
+ActiveLink_Supplier_5_4: x_Supplier_5_4 - 1000000000 z_Supplier_5 &lt;= 0
+ActiveLink_Supplier_5_5: x_Supplier_5_5 - 1000000000 z_Supplier_5 &lt;= 0
+BaseSpend_Supplier_1: S0_Supplier_1 - 34 x_Supplier_1_1 - 15 x_Supplier_1_2
+ - 15 x_Supplier_1_3 - 75 x_Supplier_1_4 - 24 x_Supplier_1_5 = 0
+BaseSpend_Supplier_2: S0_Supplier_2 - 14 x_Supplier_2_1 - 15 x_Supplier_2_2
+ - 78 x_Supplier_2_3 - 34 x_Supplier_2_4 - 15 x_Supplier_2_5 = 0
+BaseSpend_Supplier_3: S0_Supplier_3 - 75 x_Supplier_3_1 - 25 x_Supplier_3_2
+ - 56 x_Supplier_3_3 - 24 x_Supplier_3_4 - 87 x_Supplier_3_5 = 0
+BaseSpend_Supplier_4: S0_Supplier_4 - 93 x_Supplier_4_1 - 24 x_Supplier_4_2
+ - 78 x_Supplier_4_3 - 56 x_Supplier_4_4 - 86 x_Supplier_4_5 = 0
+BaseSpend_Supplier_5: S0_Supplier_5 - 76 x_Supplier_5_1 - 32 x_Supplier_5_2
+ - 89 x_Supplier_5_3 - 13 x_Supplier_5_4 - 68 x_Supplier_5_5 = 0
+BidExclusion_0_1_Supplier_1: x_Supplier_1_1 = 0
+BidExclusion_0_1_Supplier_2: x_Supplier_2_1 = 0
+BidExclusion_0_1_Supplier_3: x_Supplier_3_1 = 0
+BidExclusion_0_1_Supplier_4: x_Supplier_4_1 = 0
+BidExclusion_0_1_Supplier_5: x_Supplier_5_1 = 0
+BidExclusion_0_2_Supplier_1: x_Supplier_1_2 = 0
+BidExclusion_0_2_Supplier_2: x_Supplier_2_2 = 0
+BidExclusion_0_2_Supplier_3: x_Supplier_3_2 = 0
+BidExclusion_0_2_Supplier_5: x_Supplier_5_2 = 0
+BidExclusion_0_3_Supplier_1: x_Supplier_1_3 = 0
+BidExclusion_0_3_Supplier_2: x_Supplier_2_3 = 0
+BidExclusion_0_3_Supplier_3: x_Supplier_3_3 = 0
+BidExclusion_0_3_Supplier_4: x_Supplier_4_3 = 0
+BidExclusion_0_3_Supplier_5: x_Supplier_5_3 = 0
+BidExclusion_0_4_Supplier_1: x_Supplier_1_4 = 0
+BidExclusion_0_4_Supplier_2: x_Supplier_2_4 = 0
+BidExclusion_0_4_Supplier_3: x_Supplier_3_4 = 0
+BidExclusion_0_4_Supplier_4: x_Supplier_4_4 = 0
+BidExclusion_0_5_Supplier_1: x_Supplier_1_5 = 0
+BidExclusion_0_5_Supplier_2: x_Supplier_2_5 = 0
+BidExclusion_0_5_Supplier_3: x_Supplier_3_5 = 0
+Capacity_Supplier_1_Bid_ID_1: x_Supplier_1_1 &lt;= 1457
+Capacity_Supplier_1_Bid_ID_2: x_Supplier_1_2 &lt;= 2422
+Capacity_Supplier_1_Bid_ID_3: x_Supplier_1_3 &lt;= 6463
+Capacity_Supplier_1_Bid_ID_4: x_Supplier_1_4 &lt;= 2358
+Capacity_Supplier_1_Bid_ID_5: x_Supplier_1_5 &lt;= 2422
+Capacity_Supplier_2_Capacity_Group_Category_1: x_Supplier_2_1 + x_Supplier_2_3
+ + x_Supplier_2_4 &lt;= 8001
+Capacity_Supplier_2_Capacity_Group_Category_2: x_Supplier_2_2 &lt;= 2501
+Capacity_Supplier_2_Capacity_Group_Category_3: x_Supplier_2_5 &lt;= 501
+Capacity_Supplier_3_Bid_ID_1: x_Supplier_3_1 &lt;= 1457
+Capacity_Supplier_3_Bid_ID_2: x_Supplier_3_2 &lt;= 2422
+Capacity_Supplier_3_Bid_ID_3: x_Supplier_3_3 &lt;= 6463
+Capacity_Supplier_3_Bid_ID_4: x_Supplier_3_4 &lt;= 2358
+Capacity_Supplier_3_Bid_ID_5: x_Supplier_3_5 &lt;= 2422
+Capacity_Supplier_4_Bid_ID_1: x_Supplier_4_1 &lt;= 1457
+Capacity_Supplier_4_Bid_ID_2: x_Supplier_4_2 &lt;= 2422
+Capacity_Supplier_4_Bid_ID_3: x_Supplier_4_3 &lt;= 6463
+Capacity_Supplier_4_Bid_ID_4: x_Supplier_4_4 &lt;= 2358
+Capacity_Supplier_4_Bid_ID_5: x_Supplier_4_5 &lt;= 2422
+Capacity_Supplier_5_Description_Large_Item: x_Supplier_5_5 &lt;= 5001
+Capacity_Supplier_5_Description_Medium_item: x_Supplier_5_2 &lt;= 2501
+Capacity_Supplier_5_Description_Small_item: x_Supplier_5_1 + x_Supplier_5_3
+ + x_Supplier_5_4 &lt;= 9001
+Demand_1: x_Supplier_1_1 + x_Supplier_2_1 + x_Supplier_3_1 + x_Supplier_4_1
+ + x_Supplier_5_1 = 1456
+Demand_2: x_Supplier_1_2 + x_Supplier_2_2 + x_Supplier_3_2 + x_Supplier_4_2
+ + x_Supplier_5_2 = 2421
+Demand_3: x_Supplier_1_3 + x_Supplier_2_3 + x_Supplier_3_3 + x_Supplier_4_3
+ + x_Supplier_5_3 = 6462
+Demand_4: x_Supplier_1_4 + x_Supplier_2_4 + x_Supplier_3_4 + x_Supplier_4_4
+ + x_Supplier_5_4 = 2357
+Demand_5: x_Supplier_1_5 + x_Supplier_2_5 + x_Supplier_3_5 + x_Supplier_4_5
+ + x_Supplier_5_5 = 2421
+EffectiveSpend_Supplier_1: - S0_Supplier_1 + S_Supplier_1 + d_Supplier_1 = 0
+EffectiveSpend_Supplier_2: - S0_Supplier_2 + S_Supplier_2 + d_Supplier_2 = 0
+EffectiveSpend_Supplier_3: - S0_Supplier_3 + S_Supplier_3 + d_Supplier_3 = 0
+EffectiveSpend_Supplier_4: - S0_Supplier_4 + S_Supplier_4 + d_Supplier_4 = 0
+EffectiveSpend_Supplier_5: - S0_Supplier_5 + S_Supplier_5 + d_Supplier_5 = 0
+Fix_d_Supplier_1: d_Supplier_1 = 0
+Fix_d_Supplier_2: d_Supplier_2 = 0
+Fix_d_Supplier_3: d_Supplier_3 = 0
+Fix_d_Supplier_4: d_Supplier_4 = 0
+Fix_d_Supplier_5: d_Supplier_5 = 0
+Fix_rebate_Supplier_1: rebate_Supplier_1 = 0
+Fix_rebate_Supplier_2: rebate_Supplier_2 = 0
+Fix_rebate_Supplier_3: rebate_Supplier_3 = 0
+Fix_rebate_Supplier_4: rebate_Supplier_4 = 0
+Fix_rebate_Supplier_5: rebate_Supplier_5 = 0
+MinAward_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 - z_Supplier_1 &gt;= 0
+MinAward_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
+ + x_Supplier_2_4 + x_Supplier_2_5 - z_Supplier_2 &gt;= 0
+MinAward_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
+ + x_Supplier_3_4 + x_Supplier_3_5 - z_Supplier_3 &gt;= 0
+MinAward_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
+ + x_Supplier_4_4 + x_Supplier_4_5 - z_Supplier_4 &gt;= 0
+MinAward_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
+ + x_Supplier_5_4 + x_Supplier_5_5 - z_Supplier_5 &gt;= 0
+TransitionLower_1_Supplier_1: x_Supplier_1_1 &gt;= 0
+TransitionLower_1_Supplier_3: x_Supplier_3_1 &gt;= 0
+TransitionLower_1_Supplier_4: x_Supplier_4_1 &gt;= 0
+TransitionLower_1_Supplier_5: x_Supplier_5_1 &gt;= 0
+TransitionLower_2_Supplier_1: x_Supplier_1_2 &gt;= 0
+TransitionLower_2_Supplier_2: x_Supplier_2_2 &gt;= 0
+TransitionLower_2_Supplier_4: x_Supplier_4_2 &gt;= 0
+TransitionLower_2_Supplier_5: x_Supplier_5_2 &gt;= 0
+TransitionLower_3_Supplier_1: x_Supplier_1_3 &gt;= 0
+TransitionLower_3_Supplier_3: x_Supplier_3_3 &gt;= 0
+TransitionLower_3_Supplier_4: x_Supplier_4_3 &gt;= 0
+TransitionLower_3_Supplier_5: x_Supplier_5_3 &gt;= 0
+TransitionLower_4_Supplier_2: x_Supplier_2_4 &gt;= 0
+TransitionLower_4_Supplier_3: x_Supplier_3_4 &gt;= 0
+TransitionLower_4_Supplier_4: x_Supplier_4_4 &gt;= 0
+TransitionLower_4_Supplier_5: x_Supplier_5_4 &gt;= 0
+TransitionLower_5_Supplier_1: x_Supplier_1_5 &gt;= 0
+TransitionLower_5_Supplier_2: x_Supplier_2_5 &gt;= 0
+TransitionLower_5_Supplier_4: x_Supplier_4_5 &gt;= 0
+TransitionLower_5_Supplier_5: x_Supplier_5_5 &gt;= 0
+Transition_1_Supplier_1: - 1456 T_1_Supplier_1 + x_Supplier_1_1 &lt;= 0
+Transition_1_Supplier_3: - 1456 T_1_Supplier_3 + x_Supplier_3_1 &lt;= 0
+Transition_1_Supplier_4: - 1456 T_1_Supplier_4 + x_Supplier_4_1 &lt;= 0
+Transition_1_Supplier_5: - 1456 T_1_Supplier_5 + x_Supplier_5_1 &lt;= 0
+Transition_2_Supplier_1: - 2421 T_2_Supplier_1 + x_Supplier_1_2 &lt;= 0
+Transition_2_Supplier_2: - 2421 T_2_Supplier_2 + x_Supplier_2_2 &lt;= 0
+Transition_2_Supplier_4: - 2421 T_2_Supplier_4 + x_Supplier_4_2 &lt;= 0
+Transition_2_Supplier_5: - 2421 T_2_Supplier_5 + x_Supplier_5_2 &lt;= 0
+Transition_3_Supplier_1: - 6462 T_3_Supplier_1 + x_Supplier_1_3 &lt;= 0
+Transition_3_Supplier_3: - 6462 T_3_Supplier_3 + x_Supplier_3_3 &lt;= 0
+Transition_3_Supplier_4: - 6462 T_3_Supplier_4 + x_Supplier_4_3 &lt;= 0
+Transition_3_Supplier_5: - 6462 T_3_Supplier_5 + x_Supplier_5_3 &lt;= 0
+Transition_4_Supplier_2: - 2357 T_4_Supplier_2 + x_Supplier_2_4 &lt;= 0
+Transition_4_Supplier_3: - 2357 T_4_Supplier_3 + x_Supplier_3_4 &lt;= 0
+Transition_4_Supplier_4: - 2357 T_4_Supplier_4 + x_Supplier_4_4 &lt;= 0
+Transition_4_Supplier_5: - 2357 T_4_Supplier_5 + x_Supplier_5_4 &lt;= 0
+Transition_5_Supplier_1: - 2421 T_5_Supplier_1 + x_Supplier_1_5 &lt;= 0
+Transition_5_Supplier_2: - 2421 T_5_Supplier_2 + x_Supplier_2_5 &lt;= 0
+Transition_5_Supplier_4: - 2421 T_5_Supplier_4 + x_Supplier_4_5 &lt;= 0
+Transition_5_Supplier_5: - 2421 T_5_Supplier_5 + x_Supplier_5_5 &lt;= 0
+Volume_Supplier_1: V_Supplier_1 - x_Supplier_1_1 - x_Supplier_1_2
+ - x_Supplier_1_3 - x_Supplier_1_4 - x_Supplier_1_5 = 0
+Volume_Supplier_2: V_Supplier_2 - x_Supplier_2_1 - x_Supplier_2_2
+ - x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 = 0
+Volume_Supplier_3: V_Supplier_3 - x_Supplier_3_1 - x_Supplier_3_2
+ - x_Supplier_3_3 - x_Supplier_3_4 - x_Supplier_3_5 = 0
+Volume_Supplier_4: V_Supplier_4 - x_Supplier_4_1 - x_Supplier_4_2
+ - x_Supplier_4_3 - x_Supplier_4_4 - x_Supplier_4_5 = 0
+Volume_Supplier_5: V_Supplier_5 - x_Supplier_5_1 - x_Supplier_5_2
+ - x_Supplier_5_3 - x_Supplier_5_4 - x_Supplier_5_5 = 0
 Binaries
-T_1_BASF
-T_1_Covestro
-T_1_Huntsman
-T_1_Wanhua
-T_2_Covestro
-T_2_Dow
-T_2_Huntsman
-T_2_Wanhua
-T_3_Covestro
-T_3_Dow
-T_3_Huntsman
-T_3_Wanhua
-T_4_Covestro
-T_4_Dow
-T_4_Huntsman
-T_4_Wanhua
-T_5_BASF
-T_5_Covestro
-T_5_Huntsman
-T_5_Wanhua
-y_rebate_BASF_0
-y_rebate_BASF_1
-y_rebate_Covestro_0
-y_rebate_Covestro_1
-y_rebate_Huntsman_0
-y_rebate_Huntsman_1
-z_BASF
-z_Covestro
-z_Dow
-z_Huntsman
-z_Wanhua
+T_1_Supplier_1
+T_1_Supplier_3
+T_1_Supplier_4
+T_1_Supplier_5
+T_2_Supplier_1
+T_2_Supplier_2
+T_2_Supplier_4
+T_2_Supplier_5
+T_3_Supplier_1
+T_3_Supplier_3
+T_3_Supplier_4
+T_3_Supplier_5
+T_4_Supplier_2
+T_4_Supplier_3
+T_4_Supplier_4
+T_4_Supplier_5
+T_5_Supplier_1
+T_5_Supplier_2
+T_5_Supplier_4
+T_5_Supplier_5
+z_Supplier_1
+z_Supplier_2
+z_Supplier_3
+z_Supplier_4
+z_Supplier_5
 End
 </t>
         </is>
@@ -1123,7 +1086,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1156,7 +1119,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1170,13 +1133,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10000000000</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Covestro</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1186,17 +1149,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dow</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1206,17 +1169,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>10000000000</v>
+        <v>6463</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Huntsman</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1226,17 +1189,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>10000000000</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Wanhua</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1246,17 +1209,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>10000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1266,17 +1229,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>10000000000</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Covestro</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1290,13 +1253,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dow</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1306,17 +1269,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10000000000</v>
+        <v>6463</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Huntsman</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1326,17 +1289,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>10000000000</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Wanhua</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1346,17 +1309,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>10000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>Supplier 4</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1366,17 +1329,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>10000000000</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Covestro</t>
+          <t>Supplier 4</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1386,17 +1349,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>10000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Dow</t>
+          <t>Supplier 4</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1410,13 +1373,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>10000000000</v>
+        <v>6463</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Huntsman</t>
+          <t>Supplier 4</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1426,17 +1389,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>10000000000</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Wanhua</t>
+          <t>Supplier 4</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1446,211 +1409,131 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>10000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Capacity Group</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Category 1</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>10000000000</v>
+        <v>8001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Covestro</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Capacity Group</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Category 2</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>10000000000</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Dow</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Capacity Group</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Category 3</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>10000000000</v>
+        <v>501</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Huntsman</t>
+          <t>Supplier 5</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Small item</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>10000000000</v>
+        <v>9001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Wanhua</t>
+          <t>Supplier 5</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Medium item</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>10000000000</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BASF</t>
+          <t>Supplier 5</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>Large Item</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Covestro</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Bid ID</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Dow</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Bid ID</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Huntsman</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Bid ID</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Wanhua</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Bid ID</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>10000000000</v>
+        <v>5001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing ability to save scenarios and run them at once
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,15 +536,15 @@
         <v>25</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>36400</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -552,16 +552,16 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>20384</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1456</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>16016</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -595,15 +595,15 @@
         <v>36</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>87156</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -611,16 +611,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>36315</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>2421</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>50841</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -654,15 +654,15 @@
         <v>82</v>
       </c>
       <c r="F4" t="n">
-        <v>529884</v>
+        <v>462357</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Supplier 5</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="K4" t="n">
-        <v>575118</v>
+        <v>84577.5</v>
       </c>
       <c r="L4" t="n">
-        <v>6462</v>
+        <v>5638.5</v>
       </c>
       <c r="M4" t="n">
-        <v>-45234</v>
+        <v>377779.5</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -692,36 +692,36 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Big Island</t>
+          <t>Palatka</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>67527</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>No Bid</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>64233</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>823.5</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>3294</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -751,60 +751,178 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Big Island</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>32</v>
+      </c>
+      <c r="F6" t="n">
+        <v>75424</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Supplier 2</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>34</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>34</v>
+      </c>
+      <c r="K6" t="n">
+        <v>80138</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2357</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-4714</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Huntsville</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Supplier 3</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="E7" t="n">
         <v>75</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F7" t="n">
+        <v>144000</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>24</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>24</v>
+      </c>
+      <c r="K7" t="n">
+        <v>46080</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1920</v>
+      </c>
+      <c r="M7" t="n">
+        <v>97920</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
         <v>0</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>No Bid</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="inlineStr">
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Huntsville</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>75</v>
+      </c>
+      <c r="F8" t="n">
+        <v>37575</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Supplier 2</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>15</v>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="inlineStr">
+      <c r="J8" t="n">
+        <v>15</v>
+      </c>
+      <c r="K8" t="n">
+        <v>7515</v>
+      </c>
+      <c r="L8" t="n">
+        <v>501</v>
+      </c>
+      <c r="M8" t="n">
+        <v>30060</v>
+      </c>
+      <c r="N8" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O6" t="n">
+      <c r="O8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -837,11 +955,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Model is infeasible. Likely causes include:
- - Insufficient supplier capacity relative to demand.
- - Custom rule constraints conflicting with overall volume/demand.
-Detailed Rule Evaluations:
-</t>
+          <t>Model is optimal.</t>
         </is>
       </c>
     </row>
@@ -880,6 +994,56 @@
  - rebate_Supplier_1 - rebate_Supplier_2 - rebate_Supplier_3
  - rebate_Supplier_4 - rebate_Supplier_5
 Subject To
+%VolAwarded_Agg_0_Supplier_1_LB: 0.5 x_Supplier_1_1 + 0.5 x_Supplier_1_2
+ + 0.5 x_Supplier_1_3 + 0.5 x_Supplier_1_4 + 0.5 x_Supplier_1_5
+ - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
+ - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
+ - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
+ - 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
+ - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
+ - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
+ - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_1
+ &gt;= -1000000000
+%VolAwarded_Agg_0_Supplier_2_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
+ - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
+ + 0.5 x_Supplier_2_1 + 0.5 x_Supplier_2_2 + 0.5 x_Supplier_2_3
+ + 0.5 x_Supplier_2_4 + 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
+ - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
+ - 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
+ - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
+ - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
+ - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_2
+ &gt;= -1000000000
+%VolAwarded_Agg_0_Supplier_3_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
+ - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
+ - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
+ - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 + 0.5 x_Supplier_3_1
+ + 0.5 x_Supplier_3_2 + 0.5 x_Supplier_3_3 + 0.5 x_Supplier_3_4
+ + 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
+ - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
+ - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
+ - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_3
+ &gt;= -1000000000
+%VolAwarded_Agg_0_Supplier_4_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
+ - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
+ - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
+ - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
+ - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
+ - 0.5 x_Supplier_3_5 + 0.5 x_Supplier_4_1 + 0.5 x_Supplier_4_2
+ + 0.5 x_Supplier_4_3 + 0.5 x_Supplier_4_4 + 0.5 x_Supplier_4_5
+ - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
+ - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_4
+ &gt;= -1000000000
+%VolAwarded_Agg_0_Supplier_5_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
+ - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
+ - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
+ - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
+ - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
+ - 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
+ - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
+ + 0.5 x_Supplier_5_1 + 0.5 x_Supplier_5_2 + 0.5 x_Supplier_5_3
+ + 0.5 x_Supplier_5_4 + 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_5
+ &gt;= -1000000000
 ActiveLink_Supplier_1_1: x_Supplier_1_1 - 1000000000 z_Supplier_1 &lt;= 0
 ActiveLink_Supplier_1_2: x_Supplier_1_2 - 1000000000 z_Supplier_1 &lt;= 0
 ActiveLink_Supplier_1_3: x_Supplier_1_3 - 1000000000 z_Supplier_1 &lt;= 0
@@ -905,6 +1069,16 @@
 ActiveLink_Supplier_5_3: x_Supplier_5_3 - 1000000000 z_Supplier_5 &lt;= 0
 ActiveLink_Supplier_5_4: x_Supplier_5_4 - 1000000000 z_Supplier_5 &lt;= 0
 ActiveLink_Supplier_5_5: x_Supplier_5_5 - 1000000000 z_Supplier_5 &lt;= 0
+Active_0_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 - 1000000000 y_0_Supplier_1 &lt;= 0
+Active_0_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
+ + x_Supplier_2_4 + x_Supplier_2_5 - 1000000000 y_0_Supplier_2 &lt;= 0
+Active_0_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
+ + x_Supplier_3_4 + x_Supplier_3_5 - 1000000000 y_0_Supplier_3 &lt;= 0
+Active_0_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
+ + x_Supplier_4_4 + x_Supplier_4_5 - 1000000000 y_0_Supplier_4 &lt;= 0
+Active_0_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
+ + x_Supplier_5_4 + x_Supplier_5_5 - 1000000000 y_0_Supplier_5 &lt;= 0
 BaseSpend_Supplier_1: S0_Supplier_1 - 34 x_Supplier_1_1 - 15 x_Supplier_1_2
  - 15 x_Supplier_1_3 - 75 x_Supplier_1_4 - 24 x_Supplier_1_5 = 0
 BaseSpend_Supplier_2: S0_Supplier_2 - 14 x_Supplier_2_1 - 15 x_Supplier_2_2
@@ -915,27 +1089,6 @@
  - 78 x_Supplier_4_3 - 56 x_Supplier_4_4 - 86 x_Supplier_4_5 = 0
 BaseSpend_Supplier_5: S0_Supplier_5 - 76 x_Supplier_5_1 - 32 x_Supplier_5_2
  - 89 x_Supplier_5_3 - 13 x_Supplier_5_4 - 68 x_Supplier_5_5 = 0
-BidExclusion_0_1_Supplier_1: x_Supplier_1_1 = 0
-BidExclusion_0_1_Supplier_2: x_Supplier_2_1 = 0
-BidExclusion_0_1_Supplier_3: x_Supplier_3_1 = 0
-BidExclusion_0_1_Supplier_4: x_Supplier_4_1 = 0
-BidExclusion_0_1_Supplier_5: x_Supplier_5_1 = 0
-BidExclusion_0_2_Supplier_1: x_Supplier_1_2 = 0
-BidExclusion_0_2_Supplier_2: x_Supplier_2_2 = 0
-BidExclusion_0_2_Supplier_3: x_Supplier_3_2 = 0
-BidExclusion_0_2_Supplier_5: x_Supplier_5_2 = 0
-BidExclusion_0_3_Supplier_1: x_Supplier_1_3 = 0
-BidExclusion_0_3_Supplier_2: x_Supplier_2_3 = 0
-BidExclusion_0_3_Supplier_3: x_Supplier_3_3 = 0
-BidExclusion_0_3_Supplier_4: x_Supplier_4_3 = 0
-BidExclusion_0_3_Supplier_5: x_Supplier_5_3 = 0
-BidExclusion_0_4_Supplier_1: x_Supplier_1_4 = 0
-BidExclusion_0_4_Supplier_2: x_Supplier_2_4 = 0
-BidExclusion_0_4_Supplier_3: x_Supplier_3_4 = 0
-BidExclusion_0_4_Supplier_4: x_Supplier_4_4 = 0
-BidExclusion_0_5_Supplier_1: x_Supplier_1_5 = 0
-BidExclusion_0_5_Supplier_2: x_Supplier_2_5 = 0
-BidExclusion_0_5_Supplier_3: x_Supplier_3_5 = 0
 Capacity_Supplier_1_Bid_ID_1: x_Supplier_1_1 &lt;= 1457
 Capacity_Supplier_1_Bid_ID_2: x_Supplier_1_2 &lt;= 2422
 Capacity_Supplier_1_Bid_ID_3: x_Supplier_1_3 &lt;= 6463
@@ -984,6 +1137,16 @@
 Fix_rebate_Supplier_3: rebate_Supplier_3 = 0
 Fix_rebate_Supplier_4: rebate_Supplier_4 = 0
 Fix_rebate_Supplier_5: rebate_Supplier_5 = 0
+MinActive_0_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 &gt;= 0
+MinActive_0_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
+ + x_Supplier_2_4 + x_Supplier_2_5 &gt;= 0
+MinActive_0_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
+ + x_Supplier_3_4 + x_Supplier_3_5 &gt;= 0
+MinActive_0_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
+ + x_Supplier_4_4 + x_Supplier_4_5 &gt;= 0
+MinActive_0_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
+ + x_Supplier_5_4 + x_Supplier_5_5 &gt;= 0
 MinAward_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
  + x_Supplier_1_4 + x_Supplier_1_5 - z_Supplier_1 &gt;= 0
 MinAward_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
@@ -1065,6 +1228,11 @@
 T_5_Supplier_2
 T_5_Supplier_4
 T_5_Supplier_5
+y_0_Supplier_1
+y_0_Supplier_2
+y_0_Supplier_3
+y_0_Supplier_4
+y_0_Supplier_5
 z_Supplier_1
 z_Supplier_2
 z_Supplier_3

</xml_diff>

<commit_message>
Added current price and powerpoint output
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,50 +464,60 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Current Price</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Baseline Spend</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Awarded Supplier</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Original Awarded Supplier Price</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Percentage Volume Discount</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Discounted Awarded Supplier Price</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Awarded Supplier Spend</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Awarded Volume</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Baseline Savings</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Current Price Savings</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Rebate %</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Rebate Savings</t>
         </is>
@@ -536,39 +546,45 @@
         <v>25</v>
       </c>
       <c r="F2" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2" t="n">
         <v>36400</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Supplier 2</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>14</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>14</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>20384</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>1456</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>16016</v>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="n">
+        <v>11648</v>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -595,39 +611,45 @@
         <v>36</v>
       </c>
       <c r="F3" t="n">
+        <v>38</v>
+      </c>
+      <c r="G3" t="n">
         <v>87156</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Supplier 2</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>15</v>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>25</v>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J3" t="n">
-        <v>15</v>
-      </c>
       <c r="K3" t="n">
-        <v>36315</v>
+        <v>25</v>
       </c>
       <c r="L3" t="n">
+        <v>60525</v>
+      </c>
+      <c r="M3" t="n">
         <v>2421</v>
       </c>
-      <c r="M3" t="n">
-        <v>50841</v>
-      </c>
-      <c r="N3" t="inlineStr">
+      <c r="N3" t="n">
+        <v>26631</v>
+      </c>
+      <c r="O3" t="n">
+        <v>31473</v>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -654,104 +676,116 @@
         <v>82</v>
       </c>
       <c r="F4" t="n">
-        <v>462357</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Supplier 1</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>15</v>
-      </c>
-      <c r="I4" t="inlineStr">
+        <v>80</v>
+      </c>
+      <c r="G4" t="n">
+        <v>529884</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Supplier 2</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>78</v>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J4" t="n">
-        <v>15</v>
-      </c>
       <c r="K4" t="n">
-        <v>84577.5</v>
+        <v>78</v>
       </c>
       <c r="L4" t="n">
-        <v>5638.5</v>
+        <v>504036</v>
       </c>
       <c r="M4" t="n">
-        <v>377779.5</v>
-      </c>
-      <c r="N4" t="inlineStr">
+        <v>6462</v>
+      </c>
+      <c r="N4" t="n">
+        <v>25848</v>
+      </c>
+      <c r="O4" t="n">
+        <v>12924</v>
+      </c>
+      <c r="P4" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Palatka</t>
+          <t>Big Island</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="F5" t="n">
-        <v>67527</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Supplier 2</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>78</v>
-      </c>
-      <c r="I5" t="inlineStr">
+        <v>29</v>
+      </c>
+      <c r="G5" t="n">
+        <v>75424</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>75</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J5" t="n">
-        <v>78</v>
-      </c>
       <c r="K5" t="n">
-        <v>64233</v>
+        <v>75</v>
       </c>
       <c r="L5" t="n">
-        <v>823.5</v>
+        <v>176775</v>
       </c>
       <c r="M5" t="n">
-        <v>3294</v>
-      </c>
-      <c r="N5" t="inlineStr">
+        <v>2357</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-101351</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-108422</v>
+      </c>
+      <c r="P5" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,169 +794,57 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Big Island</t>
+          <t>Huntsville</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="F6" t="n">
-        <v>75424</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Supplier 2</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>34</v>
-      </c>
-      <c r="I6" t="inlineStr">
+        <v>70</v>
+      </c>
+      <c r="G6" t="n">
+        <v>181575</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>87</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J6" t="n">
-        <v>34</v>
-      </c>
       <c r="K6" t="n">
-        <v>80138</v>
+        <v>87</v>
       </c>
       <c r="L6" t="n">
-        <v>2357</v>
+        <v>210627</v>
       </c>
       <c r="M6" t="n">
-        <v>-4714</v>
-      </c>
-      <c r="N6" t="inlineStr">
+        <v>2421</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-29052</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-41157</v>
+      </c>
+      <c r="P6" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Huntsville</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Supplier 3</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>75</v>
-      </c>
-      <c r="F7" t="n">
-        <v>144000</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Supplier 1</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>24</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J7" t="n">
-        <v>24</v>
-      </c>
-      <c r="K7" t="n">
-        <v>46080</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1920</v>
-      </c>
-      <c r="M7" t="n">
-        <v>97920</v>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Huntsville</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Supplier 3</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>75</v>
-      </c>
-      <c r="F8" t="n">
-        <v>37575</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Supplier 2</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>15</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>15</v>
-      </c>
-      <c r="K8" t="n">
-        <v>7515</v>
-      </c>
-      <c r="L8" t="n">
-        <v>501</v>
-      </c>
-      <c r="M8" t="n">
-        <v>30060</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O8" t="n">
+      <c r="Q6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -994,56 +916,20 @@
  - rebate_Supplier_1 - rebate_Supplier_2 - rebate_Supplier_3
  - rebate_Supplier_4 - rebate_Supplier_5
 Subject To
-%VolAwarded_Agg_0_Supplier_1_LB: 0.5 x_Supplier_1_1 + 0.5 x_Supplier_1_2
- + 0.5 x_Supplier_1_3 + 0.5 x_Supplier_1_4 + 0.5 x_Supplier_1_5
- - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
- - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
- - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
- - 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
- - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
- - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
- - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_1
- &gt;= -1000000000
-%VolAwarded_Agg_0_Supplier_2_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
- - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
- + 0.5 x_Supplier_2_1 + 0.5 x_Supplier_2_2 + 0.5 x_Supplier_2_3
- + 0.5 x_Supplier_2_4 + 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
- - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
- - 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
- - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
- - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
- - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_2
- &gt;= -1000000000
-%VolAwarded_Agg_0_Supplier_3_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
- - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
- - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
- - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 + 0.5 x_Supplier_3_1
- + 0.5 x_Supplier_3_2 + 0.5 x_Supplier_3_3 + 0.5 x_Supplier_3_4
- + 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
- - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
- - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
- - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_3
- &gt;= -1000000000
-%VolAwarded_Agg_0_Supplier_4_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
- - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
- - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
- - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
- - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
- - 0.5 x_Supplier_3_5 + 0.5 x_Supplier_4_1 + 0.5 x_Supplier_4_2
- + 0.5 x_Supplier_4_3 + 0.5 x_Supplier_4_4 + 0.5 x_Supplier_4_5
- - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
- - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_4
- &gt;= -1000000000
-%VolAwarded_Agg_0_Supplier_5_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
- - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
- - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
- - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
- - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
- - 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
- - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
- + 0.5 x_Supplier_5_1 + 0.5 x_Supplier_5_2 + 0.5 x_Supplier_5_3
- + 0.5 x_Supplier_5_4 + 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_5
- &gt;= -1000000000
+%VolAwarded_Agg_0_incumbent_EQ_LB: - x_Supplier_1_1 - x_Supplier_1_2
+ - x_Supplier_1_3 + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1
+ - x_Supplier_2_2 + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5
+ - x_Supplier_3_1 + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4
+ + 0 x_Supplier_3_5 - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3
+ - x_Supplier_4_4 - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2
+ - x_Supplier_5_3 - x_Supplier_5_4 - x_Supplier_5_5 &gt;= 0
+%VolAwarded_Agg_0_incumbent_EQ_UB: - x_Supplier_1_1 - x_Supplier_1_2
+ - x_Supplier_1_3 + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1
+ - x_Supplier_2_2 + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5
+ - x_Supplier_3_1 + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4
+ + 0 x_Supplier_3_5 - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3
+ - x_Supplier_4_4 - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2
+ - x_Supplier_5_3 - x_Supplier_5_4 - x_Supplier_5_5 &lt;= 0
 ActiveLink_Supplier_1_1: x_Supplier_1_1 - 1000000000 z_Supplier_1 &lt;= 0
 ActiveLink_Supplier_1_2: x_Supplier_1_2 - 1000000000 z_Supplier_1 &lt;= 0
 ActiveLink_Supplier_1_3: x_Supplier_1_3 - 1000000000 z_Supplier_1 &lt;= 0
@@ -1069,16 +955,6 @@
 ActiveLink_Supplier_5_3: x_Supplier_5_3 - 1000000000 z_Supplier_5 &lt;= 0
 ActiveLink_Supplier_5_4: x_Supplier_5_4 - 1000000000 z_Supplier_5 &lt;= 0
 ActiveLink_Supplier_5_5: x_Supplier_5_5 - 1000000000 z_Supplier_5 &lt;= 0
-Active_0_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
- + x_Supplier_1_4 + x_Supplier_1_5 - 1000000000 y_0_Supplier_1 &lt;= 0
-Active_0_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
- + x_Supplier_2_4 + x_Supplier_2_5 - 1000000000 y_0_Supplier_2 &lt;= 0
-Active_0_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
- + x_Supplier_3_4 + x_Supplier_3_5 - 1000000000 y_0_Supplier_3 &lt;= 0
-Active_0_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
- + x_Supplier_4_4 + x_Supplier_4_5 - 1000000000 y_0_Supplier_4 &lt;= 0
-Active_0_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
- + x_Supplier_5_4 + x_Supplier_5_5 - 1000000000 y_0_Supplier_5 &lt;= 0
 BaseSpend_Supplier_1: S0_Supplier_1 - 34 x_Supplier_1_1 - 15 x_Supplier_1_2
  - 15 x_Supplier_1_3 - 75 x_Supplier_1_4 - 24 x_Supplier_1_5 = 0
 BaseSpend_Supplier_2: S0_Supplier_2 - 14 x_Supplier_2_1 - 15 x_Supplier_2_2
@@ -1137,16 +1013,6 @@
 Fix_rebate_Supplier_3: rebate_Supplier_3 = 0
 Fix_rebate_Supplier_4: rebate_Supplier_4 = 0
 Fix_rebate_Supplier_5: rebate_Supplier_5 = 0
-MinActive_0_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
- + x_Supplier_1_4 + x_Supplier_1_5 &gt;= 0
-MinActive_0_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
- + x_Supplier_2_4 + x_Supplier_2_5 &gt;= 0
-MinActive_0_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
- + x_Supplier_3_4 + x_Supplier_3_5 &gt;= 0
-MinActive_0_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
- + x_Supplier_4_4 + x_Supplier_4_5 &gt;= 0
-MinActive_0_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
- + x_Supplier_5_4 + x_Supplier_5_5 &gt;= 0
 MinAward_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
  + x_Supplier_1_4 + x_Supplier_1_5 - z_Supplier_1 &gt;= 0
 MinAward_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
@@ -1228,11 +1094,6 @@
 T_5_Supplier_2
 T_5_Supplier_4
 T_5_Supplier_5
-y_0_Supplier_1
-y_0_Supplier_2
-y_0_Supplier_3
-y_0_Supplier_4
-y_0_Supplier_5
 z_Supplier_1
 z_Supplier_2
 z_Supplier_3

</xml_diff>

<commit_message>
freight logic added to optimizer tool
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,30 +484,45 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Discounted Awarded Supplier Price</t>
+          <t>Discounted Supplier Price</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>Freight Method</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Freight Amount</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Effective Supplier Price</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Awarded Supplier Spend</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Awarded Volume</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Baseline Savings</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Rebate %</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Rebate Savings</t>
         </is>
@@ -554,21 +569,32 @@
       <c r="J2" t="n">
         <v>14</v>
       </c>
-      <c r="K2" t="n">
-        <v>20384</v>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>EXW + KBX</t>
+        </is>
       </c>
       <c r="L2" t="n">
+        <v>18</v>
+      </c>
+      <c r="M2" t="n">
+        <v>32</v>
+      </c>
+      <c r="N2" t="n">
+        <v>46592</v>
+      </c>
+      <c r="O2" t="n">
         <v>1456</v>
       </c>
-      <c r="M2" t="n">
-        <v>16016</v>
-      </c>
-      <c r="N2" t="inlineStr">
+      <c r="P2" t="n">
+        <v>-10192</v>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O2" t="n">
+      <c r="R2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -613,21 +639,32 @@
       <c r="J3" t="n">
         <v>15</v>
       </c>
-      <c r="K3" t="n">
-        <v>36315</v>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>EXW + KBX</t>
+        </is>
       </c>
       <c r="L3" t="n">
+        <v>14</v>
+      </c>
+      <c r="M3" t="n">
+        <v>29</v>
+      </c>
+      <c r="N3" t="n">
+        <v>70209</v>
+      </c>
+      <c r="O3" t="n">
         <v>2421</v>
       </c>
-      <c r="M3" t="n">
-        <v>50841</v>
-      </c>
-      <c r="N3" t="inlineStr">
+      <c r="P3" t="n">
+        <v>16947</v>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O3" t="n">
+      <c r="R3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -654,7 +691,7 @@
         <v>82</v>
       </c>
       <c r="F4" t="n">
-        <v>462357</v>
+        <v>529884</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -672,56 +709,67 @@
       <c r="J4" t="n">
         <v>15</v>
       </c>
-      <c r="K4" t="n">
-        <v>84577.5</v>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>DDP</t>
+        </is>
       </c>
       <c r="L4" t="n">
-        <v>5638.5</v>
+        <v>22</v>
       </c>
       <c r="M4" t="n">
-        <v>377779.5</v>
-      </c>
-      <c r="N4" t="inlineStr">
+        <v>37</v>
+      </c>
+      <c r="N4" t="n">
+        <v>239094</v>
+      </c>
+      <c r="O4" t="n">
+        <v>6462</v>
+      </c>
+      <c r="P4" t="n">
+        <v>290790</v>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O4" t="n">
+      <c r="R4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Palatka</t>
+          <t>Big Island</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="F5" t="n">
-        <v>67527</v>
+        <v>75424</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 5</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -729,29 +777,40 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>78</v>
-      </c>
-      <c r="K5" t="n">
-        <v>64233</v>
+        <v>13</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>DDP</t>
+        </is>
       </c>
       <c r="L5" t="n">
-        <v>823.5</v>
+        <v>32</v>
       </c>
       <c r="M5" t="n">
-        <v>3294</v>
-      </c>
-      <c r="N5" t="inlineStr">
+        <v>45</v>
+      </c>
+      <c r="N5" t="n">
+        <v>106065</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2357</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-30641</v>
+      </c>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O5" t="n">
+      <c r="R5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,27 +819,27 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Big Island</t>
+          <t>Huntsville</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>75</v>
+      </c>
+      <c r="F6" t="n">
+        <v>144000</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Supplier 1</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>32</v>
-      </c>
-      <c r="F6" t="n">
-        <v>75424</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Supplier 2</t>
-        </is>
-      </c>
       <c r="H6" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -788,23 +847,34 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>34</v>
-      </c>
-      <c r="K6" t="n">
-        <v>80138</v>
+        <v>24</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>EXW + KBX</t>
+        </is>
       </c>
       <c r="L6" t="n">
-        <v>2357</v>
+        <v>20</v>
       </c>
       <c r="M6" t="n">
-        <v>-4714</v>
-      </c>
-      <c r="N6" t="inlineStr">
+        <v>44</v>
+      </c>
+      <c r="N6" t="n">
+        <v>84480</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1920</v>
+      </c>
+      <c r="P6" t="n">
+        <v>59520</v>
+      </c>
+      <c r="Q6" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O6" t="n">
+      <c r="R6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -814,7 +884,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -831,15 +901,15 @@
         <v>75</v>
       </c>
       <c r="F7" t="n">
-        <v>144000</v>
+        <v>37575</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -847,82 +917,34 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>24</v>
-      </c>
-      <c r="K7" t="n">
-        <v>46080</v>
+        <v>15</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>EXW + KBX</t>
+        </is>
       </c>
       <c r="L7" t="n">
-        <v>1920</v>
+        <v>14</v>
       </c>
       <c r="M7" t="n">
-        <v>97920</v>
-      </c>
-      <c r="N7" t="inlineStr">
+        <v>29</v>
+      </c>
+      <c r="N7" t="n">
+        <v>14529</v>
+      </c>
+      <c r="O7" t="n">
+        <v>501</v>
+      </c>
+      <c r="P7" t="n">
+        <v>23046</v>
+      </c>
+      <c r="Q7" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Huntsville</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Supplier 3</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>75</v>
-      </c>
-      <c r="F8" t="n">
-        <v>37575</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Supplier 2</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>15</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>15</v>
-      </c>
-      <c r="K8" t="n">
-        <v>7515</v>
-      </c>
-      <c r="L8" t="n">
-        <v>501</v>
-      </c>
-      <c r="M8" t="n">
-        <v>30060</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="O8" t="n">
+      <c r="R7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -994,56 +1016,6 @@
  - rebate_Supplier_1 - rebate_Supplier_2 - rebate_Supplier_3
  - rebate_Supplier_4 - rebate_Supplier_5
 Subject To
-%VolAwarded_Agg_0_Supplier_1_LB: 0.5 x_Supplier_1_1 + 0.5 x_Supplier_1_2
- + 0.5 x_Supplier_1_3 + 0.5 x_Supplier_1_4 + 0.5 x_Supplier_1_5
- - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
- - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
- - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
- - 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
- - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
- - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
- - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_1
- &gt;= -1000000000
-%VolAwarded_Agg_0_Supplier_2_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
- - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
- + 0.5 x_Supplier_2_1 + 0.5 x_Supplier_2_2 + 0.5 x_Supplier_2_3
- + 0.5 x_Supplier_2_4 + 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
- - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
- - 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
- - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
- - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
- - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_2
- &gt;= -1000000000
-%VolAwarded_Agg_0_Supplier_3_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
- - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
- - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
- - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 + 0.5 x_Supplier_3_1
- + 0.5 x_Supplier_3_2 + 0.5 x_Supplier_3_3 + 0.5 x_Supplier_3_4
- + 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
- - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
- - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
- - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_3
- &gt;= -1000000000
-%VolAwarded_Agg_0_Supplier_4_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
- - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
- - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
- - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
- - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
- - 0.5 x_Supplier_3_5 + 0.5 x_Supplier_4_1 + 0.5 x_Supplier_4_2
- + 0.5 x_Supplier_4_3 + 0.5 x_Supplier_4_4 + 0.5 x_Supplier_4_5
- - 0.5 x_Supplier_5_1 - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3
- - 0.5 x_Supplier_5_4 - 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_4
- &gt;= -1000000000
-%VolAwarded_Agg_0_Supplier_5_LB: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2
- - 0.5 x_Supplier_1_3 - 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5
- - 0.5 x_Supplier_2_1 - 0.5 x_Supplier_2_2 - 0.5 x_Supplier_2_3
- - 0.5 x_Supplier_2_4 - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1
- - 0.5 x_Supplier_3_2 - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4
- - 0.5 x_Supplier_3_5 - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2
- - 0.5 x_Supplier_4_3 - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5
- + 0.5 x_Supplier_5_1 + 0.5 x_Supplier_5_2 + 0.5 x_Supplier_5_3
- + 0.5 x_Supplier_5_4 + 0.5 x_Supplier_5_5 - 1000000000 y_0_Supplier_5
- &gt;= -1000000000
 ActiveLink_Supplier_1_1: x_Supplier_1_1 - 1000000000 z_Supplier_1 &lt;= 0
 ActiveLink_Supplier_1_2: x_Supplier_1_2 - 1000000000 z_Supplier_1 &lt;= 0
 ActiveLink_Supplier_1_3: x_Supplier_1_3 - 1000000000 z_Supplier_1 &lt;= 0
@@ -1069,16 +1041,6 @@
 ActiveLink_Supplier_5_3: x_Supplier_5_3 - 1000000000 z_Supplier_5 &lt;= 0
 ActiveLink_Supplier_5_4: x_Supplier_5_4 - 1000000000 z_Supplier_5 &lt;= 0
 ActiveLink_Supplier_5_5: x_Supplier_5_5 - 1000000000 z_Supplier_5 &lt;= 0
-Active_0_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
- + x_Supplier_1_4 + x_Supplier_1_5 - 1000000000 y_0_Supplier_1 &lt;= 0
-Active_0_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
- + x_Supplier_2_4 + x_Supplier_2_5 - 1000000000 y_0_Supplier_2 &lt;= 0
-Active_0_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
- + x_Supplier_3_4 + x_Supplier_3_5 - 1000000000 y_0_Supplier_3 &lt;= 0
-Active_0_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
- + x_Supplier_4_4 + x_Supplier_4_5 - 1000000000 y_0_Supplier_4 &lt;= 0
-Active_0_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
- + x_Supplier_5_4 + x_Supplier_5_5 - 1000000000 y_0_Supplier_5 &lt;= 0
 BaseSpend_Supplier_1: S0_Supplier_1 - 34 x_Supplier_1_1 - 15 x_Supplier_1_2
  - 15 x_Supplier_1_3 - 75 x_Supplier_1_4 - 24 x_Supplier_1_5 = 0
 BaseSpend_Supplier_2: S0_Supplier_2 - 14 x_Supplier_2_1 - 15 x_Supplier_2_2
@@ -1122,11 +1084,16 @@
  + x_Supplier_5_4 = 2357
 Demand_5: x_Supplier_1_5 + x_Supplier_2_5 + x_Supplier_3_5 + x_Supplier_4_5
  + x_Supplier_5_5 = 2421
-EffectiveSpend_Supplier_1: - S0_Supplier_1 + S_Supplier_1 + d_Supplier_1 = 0
-EffectiveSpend_Supplier_2: - S0_Supplier_2 + S_Supplier_2 + d_Supplier_2 = 0
-EffectiveSpend_Supplier_3: - S0_Supplier_3 + S_Supplier_3 + d_Supplier_3 = 0
-EffectiveSpend_Supplier_4: - S0_Supplier_4 + S_Supplier_4 + d_Supplier_4 = 0
-EffectiveSpend_Supplier_5: - S0_Supplier_5 + S_Supplier_5 + d_Supplier_5 = 0
+EffectiveSpend_Supplier_1: - F_Supplier_1 - S0_Supplier_1 + S_Supplier_1
+ + d_Supplier_1 = 0
+EffectiveSpend_Supplier_2: - F_Supplier_2 - S0_Supplier_2 + S_Supplier_2
+ + d_Supplier_2 = 0
+EffectiveSpend_Supplier_3: - F_Supplier_3 - S0_Supplier_3 + S_Supplier_3
+ + d_Supplier_3 = 0
+EffectiveSpend_Supplier_4: - F_Supplier_4 - S0_Supplier_4 + S_Supplier_4
+ + d_Supplier_4 = 0
+EffectiveSpend_Supplier_5: - F_Supplier_5 - S0_Supplier_5 + S_Supplier_5
+ + d_Supplier_5 = 0
 Fix_d_Supplier_1: d_Supplier_1 = 0
 Fix_d_Supplier_2: d_Supplier_2 = 0
 Fix_d_Supplier_3: d_Supplier_3 = 0
@@ -1137,16 +1104,16 @@
 Fix_rebate_Supplier_3: rebate_Supplier_3 = 0
 Fix_rebate_Supplier_4: rebate_Supplier_4 = 0
 Fix_rebate_Supplier_5: rebate_Supplier_5 = 0
-MinActive_0_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
- + x_Supplier_1_4 + x_Supplier_1_5 &gt;= 0
-MinActive_0_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
- + x_Supplier_2_4 + x_Supplier_2_5 &gt;= 0
-MinActive_0_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
- + x_Supplier_3_4 + x_Supplier_3_5 &gt;= 0
-MinActive_0_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
- + x_Supplier_4_4 + x_Supplier_4_5 &gt;= 0
-MinActive_0_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
- + x_Supplier_5_4 + x_Supplier_5_5 &gt;= 0
+Freight_Supplier_1: F_Supplier_1 - 21 x_Supplier_1_1 - 22 x_Supplier_1_2
+ - 22 x_Supplier_1_3 - 22 x_Supplier_1_4 - 20 x_Supplier_1_5 = 0
+Freight_Supplier_2: F_Supplier_2 - 18 x_Supplier_2_1 - 14 x_Supplier_2_2
+ - 19 x_Supplier_2_3 - 19 x_Supplier_2_4 - 14 x_Supplier_2_5 = 0
+Freight_Supplier_3: F_Supplier_3 - 23 x_Supplier_3_1 - 25 x_Supplier_3_2
+ - 27 x_Supplier_3_3 - 27 x_Supplier_3_4 - 27 x_Supplier_3_5 = 0
+Freight_Supplier_4: F_Supplier_4 - 20 x_Supplier_4_1 - 15 x_Supplier_4_2
+ - 18 x_Supplier_4_3 - 20 x_Supplier_4_4 - 19 x_Supplier_4_5 = 0
+Freight_Supplier_5: F_Supplier_5 - 30 x_Supplier_5_1 - 32 x_Supplier_5_2
+ - 32 x_Supplier_5_3 - 32 x_Supplier_5_4 - 27 x_Supplier_5_5 = 0
 MinAward_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
  + x_Supplier_1_4 + x_Supplier_1_5 - z_Supplier_1 &gt;= 0
 MinAward_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
@@ -1228,11 +1195,6 @@
 T_5_Supplier_2
 T_5_Supplier_4
 T_5_Supplier_5
-y_0_Supplier_1
-y_0_Supplier_2
-y_0_Supplier_3
-y_0_Supplier_4
-y_0_Supplier_5
 z_Supplier_1
 z_Supplier_2
 z_Supplier_3

</xml_diff>

<commit_message>
updated zero handling on supplier freight and kbx
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,31 +563,31 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>14</v>
+        <v>12.6</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>EXW + KBX</t>
+          <t>DDP</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>32</v>
+        <v>12.6</v>
       </c>
       <c r="N2" t="n">
-        <v>46592</v>
+        <v>18345.6</v>
       </c>
       <c r="O2" t="n">
         <v>1456</v>
       </c>
       <c r="P2" t="n">
-        <v>-10192</v>
+        <v>18054.4</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -621,15 +621,15 @@
         <v>36</v>
       </c>
       <c r="F3" t="n">
-        <v>87156</v>
+        <v>85608</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 4</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -637,27 +637,27 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>EXW + KBX</t>
+          <t>DDP</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N3" t="n">
-        <v>70209</v>
+        <v>57072</v>
       </c>
       <c r="O3" t="n">
-        <v>2421</v>
+        <v>2378</v>
       </c>
       <c r="P3" t="n">
-        <v>16947</v>
+        <v>28536</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -670,32 +670,32 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Palatka</t>
+          <t>Brunswick</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>36</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1548</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>Supplier 2</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>82</v>
-      </c>
-      <c r="F4" t="n">
-        <v>529884</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Supplier 1</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -703,11 +703,11 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>15</v>
+        <v>13.5</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -715,19 +715,19 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>37</v>
+        <v>13.5</v>
       </c>
       <c r="N4" t="n">
-        <v>239094</v>
+        <v>580.5</v>
       </c>
       <c r="O4" t="n">
-        <v>6462</v>
+        <v>43</v>
       </c>
       <c r="P4" t="n">
-        <v>290790</v>
+        <v>967.5</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -740,7 +740,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -749,27 +749,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Big Island</t>
+          <t>Palatka</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="F5" t="n">
-        <v>75424</v>
+        <v>277324</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Supplier 5</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -785,19 +785,19 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="N5" t="n">
-        <v>106065</v>
+        <v>189392</v>
       </c>
       <c r="O5" t="n">
-        <v>2357</v>
+        <v>3382</v>
       </c>
       <c r="P5" t="n">
-        <v>-30641</v>
+        <v>87932</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -810,28 +810,28 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Huntsville</t>
+          <t>Palatka</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Supplier 3</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F6" t="n">
-        <v>144000</v>
+        <v>252560</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -839,35 +839,35 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>24</v>
+        <v>14.25</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>EXW + KBX</t>
+          <t>DDP</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>44</v>
+        <v>14.25</v>
       </c>
       <c r="N6" t="n">
-        <v>84480</v>
+        <v>43890</v>
       </c>
       <c r="O6" t="n">
-        <v>1920</v>
+        <v>3080</v>
       </c>
       <c r="P6" t="n">
-        <v>59520</v>
+        <v>208670</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -880,71 +880,211 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Big Island</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>32</v>
+      </c>
+      <c r="F7" t="n">
+        <v>75424</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Supplier 5</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>13</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>13</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>DDP</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>13</v>
+      </c>
+      <c r="N7" t="n">
+        <v>30641</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2357</v>
+      </c>
+      <c r="P7" t="n">
+        <v>44783</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Huntsville</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>75</v>
+      </c>
+      <c r="F8" t="n">
+        <v>144000</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>24</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>DDP</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="N8" t="n">
+        <v>43775.99999999999</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1920</v>
+      </c>
+      <c r="P8" t="n">
+        <v>100224</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Huntsville</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Supplier 3</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="E9" t="n">
         <v>75</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F9" t="n">
         <v>37575</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Supplier 2</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="H9" t="n">
         <v>15</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>10%</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>DDP</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="N9" t="n">
+        <v>6763.5</v>
+      </c>
+      <c r="O9" t="n">
+        <v>501</v>
+      </c>
+      <c r="P9" t="n">
+        <v>30811.5</v>
+      </c>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="J7" t="n">
-        <v>15</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>EXW + KBX</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>14</v>
-      </c>
-      <c r="M7" t="n">
-        <v>29</v>
-      </c>
-      <c r="N7" t="n">
-        <v>14529</v>
-      </c>
-      <c r="O7" t="n">
-        <v>501</v>
-      </c>
-      <c r="P7" t="n">
-        <v>23046</v>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="R7" t="n">
+      <c r="R9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1084,6 +1224,26 @@
  + x_Supplier_5_4 = 2357
 Demand_5: x_Supplier_1_5 + x_Supplier_2_5 + x_Supplier_3_5 + x_Supplier_4_5
  + x_Supplier_5_5 = 2421
+DiscountTierLower_Supplier_1_0: - 0.05 S0_Supplier_1 + d_Supplier_1
+ - 1406346 z_discount_Supplier_1_0 &gt;= -1406346
+DiscountTierLower_Supplier_2_0: - 0.1 S0_Supplier_2 + d_Supplier_2
+ - 1023279 z_discount_Supplier_2_0 &gt;= -1023279
+DiscountTierMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 + 1406346 z_discount_Supplier_1_0
+ &lt;= 1411346
+DiscountTierMax_Supplier_2_0: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
+ + x_Supplier_2_4 + x_Supplier_2_5 + 1023279 z_discount_Supplier_2_0
+ &lt;= 1025279
+DiscountTierMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 &gt;= 0
+DiscountTierMin_Supplier_2_0: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
+ + x_Supplier_2_4 + x_Supplier_2_5 &gt;= 0
+DiscountTierSelect_Supplier_1: z_discount_Supplier_1_0 = 1
+DiscountTierSelect_Supplier_2: z_discount_Supplier_2_0 = 1
+DiscountTierUpper_Supplier_1_0: - 0.05 S0_Supplier_1 + d_Supplier_1
+ + 1406346 z_discount_Supplier_1_0 &lt;= 1406346
+DiscountTierUpper_Supplier_2_0: - 0.1 S0_Supplier_2 + d_Supplier_2
+ + 1023279 z_discount_Supplier_2_0 &lt;= 1023279
 EffectiveSpend_Supplier_1: - F_Supplier_1 - S0_Supplier_1 + S_Supplier_1
  + d_Supplier_1 = 0
 EffectiveSpend_Supplier_2: - F_Supplier_2 - S0_Supplier_2 + S_Supplier_2
@@ -1094,8 +1254,6 @@
  + d_Supplier_4 = 0
 EffectiveSpend_Supplier_5: - F_Supplier_5 - S0_Supplier_5 + S_Supplier_5
  + d_Supplier_5 = 0
-Fix_d_Supplier_1: d_Supplier_1 = 0
-Fix_d_Supplier_2: d_Supplier_2 = 0
 Fix_d_Supplier_3: d_Supplier_3 = 0
 Fix_d_Supplier_4: d_Supplier_4 = 0
 Fix_d_Supplier_5: d_Supplier_5 = 0
@@ -1104,16 +1262,11 @@
 Fix_rebate_Supplier_3: rebate_Supplier_3 = 0
 Fix_rebate_Supplier_4: rebate_Supplier_4 = 0
 Fix_rebate_Supplier_5: rebate_Supplier_5 = 0
-Freight_Supplier_1: F_Supplier_1 - 21 x_Supplier_1_1 - 22 x_Supplier_1_2
- - 22 x_Supplier_1_3 - 22 x_Supplier_1_4 - 20 x_Supplier_1_5 = 0
-Freight_Supplier_2: F_Supplier_2 - 18 x_Supplier_2_1 - 14 x_Supplier_2_2
- - 19 x_Supplier_2_3 - 19 x_Supplier_2_4 - 14 x_Supplier_2_5 = 0
-Freight_Supplier_3: F_Supplier_3 - 23 x_Supplier_3_1 - 25 x_Supplier_3_2
- - 27 x_Supplier_3_3 - 27 x_Supplier_3_4 - 27 x_Supplier_3_5 = 0
-Freight_Supplier_4: F_Supplier_4 - 20 x_Supplier_4_1 - 15 x_Supplier_4_2
- - 18 x_Supplier_4_3 - 20 x_Supplier_4_4 - 19 x_Supplier_4_5 = 0
-Freight_Supplier_5: F_Supplier_5 - 30 x_Supplier_5_1 - 32 x_Supplier_5_2
- - 32 x_Supplier_5_3 - 32 x_Supplier_5_4 - 27 x_Supplier_5_5 = 0
+Freight_Supplier_1: F_Supplier_1 = 0
+Freight_Supplier_2: F_Supplier_2 = 0
+Freight_Supplier_3: F_Supplier_3 = 0
+Freight_Supplier_4: F_Supplier_4 = 0
+Freight_Supplier_5: F_Supplier_5 = 0
 MinAward_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
  + x_Supplier_1_4 + x_Supplier_1_5 - z_Supplier_1 &gt;= 0
 MinAward_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
@@ -1200,6 +1353,8 @@
 z_Supplier_3
 z_Supplier_4
 z_Supplier_5
+z_discount_Supplier_1_0
+z_discount_Supplier_2_0
 End
 </t>
         </is>

</xml_diff>

<commit_message>
Updates to fix freight and PPT
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,7 +561,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="G2" t="n">
         <v>36400</v>
@@ -603,7 +603,7 @@
         <v>11648</v>
       </c>
       <c r="R2" t="n">
-        <v>11648</v>
+        <v>-20384</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -637,7 +637,7 @@
         <v>36</v>
       </c>
       <c r="F3" t="n">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="G3" t="n">
         <v>87156</v>
@@ -679,7 +679,7 @@
         <v>19368</v>
       </c>
       <c r="R3" t="n">
-        <v>19368</v>
+        <v>-55683</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -713,7 +713,7 @@
         <v>82</v>
       </c>
       <c r="F4" t="n">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
         <v>529884</v>
@@ -755,7 +755,7 @@
         <v>6462</v>
       </c>
       <c r="R4" t="n">
-        <v>6462</v>
+        <v>-497574</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -789,10 +789,10 @@
         <v>32</v>
       </c>
       <c r="F5" t="n">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>64000</v>
+        <v>75424</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -822,61 +822,61 @@
         <v>78</v>
       </c>
       <c r="O5" t="n">
-        <v>156000</v>
+        <v>183846</v>
       </c>
       <c r="P5" t="n">
-        <v>2000</v>
+        <v>2357</v>
       </c>
       <c r="Q5" t="n">
-        <v>-92000</v>
+        <v>-108422</v>
       </c>
       <c r="R5" t="n">
-        <v>-92000</v>
+        <v>-176775</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>7800</v>
+        <v>174653.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Big Island</t>
+          <t>Huntsville</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="F6" t="n">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>11424</v>
+        <v>181575</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Supplier 5</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -895,19 +895,19 @@
         <v>3</v>
       </c>
       <c r="N6" t="n">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="O6" t="n">
-        <v>5712</v>
+        <v>217890</v>
       </c>
       <c r="P6" t="n">
-        <v>357</v>
+        <v>2421</v>
       </c>
       <c r="Q6" t="n">
-        <v>5712</v>
+        <v>-36315</v>
       </c>
       <c r="R6" t="n">
-        <v>5712</v>
+        <v>-210627</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -915,82 +915,6 @@
         </is>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Huntsville</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Supplier 3</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>75</v>
-      </c>
-      <c r="F7" t="n">
-        <v>75</v>
-      </c>
-      <c r="G7" t="n">
-        <v>208350</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Supplier 3</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>87</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>87</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>DDP</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>3</v>
-      </c>
-      <c r="N7" t="n">
-        <v>90</v>
-      </c>
-      <c r="O7" t="n">
-        <v>250020</v>
-      </c>
-      <c r="P7" t="n">
-        <v>2778</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>-41670</v>
-      </c>
-      <c r="R7" t="n">
-        <v>-41670</v>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="T7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1023,10 +947,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Model is infeasible. Likely causes include:
-- Capacity too low
-- Conflicting custom rules
-</t>
+          <t>Model is optimal.</t>
         </is>
       </c>
     </row>
@@ -1061,7 +982,8 @@
         <is>
           <t xml:space="preserve">\* Sourcing_with_Freight *\
 Minimize
-OBJ: S_Supplier_1 + S_Supplier_2 + S_Supplier_3 + S_Supplier_4 + S_Supplier_5
+OBJ: F_Supplier_1 + F_Supplier_2 + F_Supplier_3 + F_Supplier_4 + F_Supplier_5
+ + S_Supplier_1 + S_Supplier_2 + S_Supplier_3 + S_Supplier_4 + S_Supplier_5
  - reb_Supplier_1 - reb_Supplier_2 - reb_Supplier_3 - reb_Supplier_4
  - reb_Supplier_5
 Subject To
@@ -1085,10 +1007,31 @@
 Cap_Supplier_4_Bid_ID_3: x_Supplier_4_3 &lt;= 100000000000
 Cap_Supplier_4_Bid_ID_4: x_Supplier_4_4 &lt;= 100000000000
 Cap_Supplier_4_Bid_ID_5: x_Supplier_4_5 &lt;= 100000000000
-DMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_3 + x_Supplier_1_4
- + 1000000000 zd_Supplier_1_0 &lt;= 1040000000
-DMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_3 + x_Supplier_1_4
- - 20000000 zd_Supplier_1_0 &gt;= 0
+DDP_ON_Supplier_1_1: - 1000000000 bDDP_Supplier_1_1 + xSF_Supplier_1_1 &lt;= 0
+DDP_ON_Supplier_1_2: - 1000000000 bDDP_Supplier_1_2 + xSF_Supplier_1_2 &lt;= 0
+DDP_ON_Supplier_1_3: - 1000000000 bDDP_Supplier_1_3 + xSF_Supplier_1_3 &lt;= 0
+DDP_ON_Supplier_1_4: - 1000000000 bDDP_Supplier_1_4 + xSF_Supplier_1_4 &lt;= 0
+DDP_ON_Supplier_1_5: - 1000000000 bDDP_Supplier_1_5 + xSF_Supplier_1_5 &lt;= 0
+DDP_ON_Supplier_2_1: - 1000000000 bDDP_Supplier_2_1 + xSF_Supplier_2_1 &lt;= 0
+DDP_ON_Supplier_2_2: - 1000000000 bDDP_Supplier_2_2 + xSF_Supplier_2_2 &lt;= 0
+DDP_ON_Supplier_2_3: - 1000000000 bDDP_Supplier_2_3 + xSF_Supplier_2_3 &lt;= 0
+DDP_ON_Supplier_2_4: - 1000000000 bDDP_Supplier_2_4 + xSF_Supplier_2_4 &lt;= 0
+DDP_ON_Supplier_2_5: - 1000000000 bDDP_Supplier_2_5 + xSF_Supplier_2_5 &lt;= 0
+DDP_ON_Supplier_3_1: - 1000000000 bDDP_Supplier_3_1 + xSF_Supplier_3_1 &lt;= 0
+DDP_ON_Supplier_3_2: - 1000000000 bDDP_Supplier_3_2 + xSF_Supplier_3_2 &lt;= 0
+DDP_ON_Supplier_3_3: - 1000000000 bDDP_Supplier_3_3 + xSF_Supplier_3_3 &lt;= 0
+DDP_ON_Supplier_3_4: - 1000000000 bDDP_Supplier_3_4 + xSF_Supplier_3_4 &lt;= 0
+DDP_ON_Supplier_3_5: - 1000000000 bDDP_Supplier_3_5 + xSF_Supplier_3_5 &lt;= 0
+DDP_ON_Supplier_4_1: - 1000000000 bDDP_Supplier_4_1 + xSF_Supplier_4_1 &lt;= 0
+DDP_ON_Supplier_4_2: - 1000000000 bDDP_Supplier_4_2 + xSF_Supplier_4_2 &lt;= 0
+DDP_ON_Supplier_4_3: - 1000000000 bDDP_Supplier_4_3 + xSF_Supplier_4_3 &lt;= 0
+DDP_ON_Supplier_4_4: - 1000000000 bDDP_Supplier_4_4 + xSF_Supplier_4_4 &lt;= 0
+DDP_ON_Supplier_4_5: - 1000000000 bDDP_Supplier_4_5 + xSF_Supplier_4_5 &lt;= 0
+DDP_ON_Supplier_5_1: - 1000000000 bDDP_Supplier_5_1 + xSF_Supplier_5_1 &lt;= 0
+DDP_ON_Supplier_5_2: - 1000000000 bDDP_Supplier_5_2 + xSF_Supplier_5_2 &lt;= 0
+DDP_ON_Supplier_5_3: - 1000000000 bDDP_Supplier_5_3 + xSF_Supplier_5_3 &lt;= 0
+DDP_ON_Supplier_5_4: - 1000000000 bDDP_Supplier_5_4 + xSF_Supplier_5_4 &lt;= 0
+DDP_ON_Supplier_5_5: - 1000000000 bDDP_Supplier_5_5 + xSF_Supplier_5_5 &lt;= 0
 Demand_1: x_Supplier_1_1 + x_Supplier_2_1 + x_Supplier_3_1 + x_Supplier_4_1
  + x_Supplier_5_1 = 1456
 Demand_2: x_Supplier_1_2 + x_Supplier_2_2 + x_Supplier_3_2 + x_Supplier_4_2
@@ -1099,17 +1042,17 @@
  + x_Supplier_5_4 = 2357
 Demand_5: x_Supplier_1_5 + x_Supplier_2_5 + x_Supplier_3_5 + x_Supplier_4_5
  + x_Supplier_5_5 = 2421
-DisableDisc_Supplier_1_0: zd_Supplier_1_0 = 0
-F_Supplier_1: F_Supplier_1 - 3 x_Supplier_1_1 - 3 x_Supplier_1_2
- - 3 x_Supplier_1_3 - 3 x_Supplier_1_4 - 3 x_Supplier_1_5 = 0
-F_Supplier_2: F_Supplier_2 - 3 x_Supplier_2_1 - 3 x_Supplier_2_2
- - 3 x_Supplier_2_3 - 3 x_Supplier_2_4 - 3 x_Supplier_2_5 = 0
-F_Supplier_3: F_Supplier_3 - 3 x_Supplier_3_1 - 3 x_Supplier_3_2
- - 3 x_Supplier_3_3 - 3 x_Supplier_3_4 - 3 x_Supplier_3_5 = 0
-F_Supplier_4: F_Supplier_4 - 3 x_Supplier_4_1 - 3 x_Supplier_4_2
- - 3 x_Supplier_4_3 - 3 x_Supplier_4_4 - 3 x_Supplier_4_5 = 0
-F_Supplier_5: F_Supplier_5 - 3 x_Supplier_5_1 - 3 x_Supplier_5_2
- - 3 x_Supplier_5_3 - 3 x_Supplier_5_4 - 3 x_Supplier_5_5 = 0
+F_Supplier_1: F_Supplier_1 - 4 xKBX_Supplier_1_1 - 4 xKBX_Supplier_1_2
+ - 4 xKBX_Supplier_1_3 - 4 xKBX_Supplier_1_4 - 4 xKBX_Supplier_1_5 = 0
+F_Supplier_2: F_Supplier_2 - 4 xKBX_Supplier_2_1 - 4 xKBX_Supplier_2_2
+ - 4 xKBX_Supplier_2_3 - 4 xKBX_Supplier_2_4 - 4 xKBX_Supplier_2_5 = 0
+F_Supplier_3: F_Supplier_3 - 4 xKBX_Supplier_3_1 - 4 xKBX_Supplier_3_2
+ - 4 xKBX_Supplier_3_3 - 4 xKBX_Supplier_3_4 - 4 xKBX_Supplier_3_5 = 0
+F_Supplier_4: F_Supplier_4 - 4 xKBX_Supplier_4_1 - 4 xKBX_Supplier_4_2
+ - 4 xKBX_Supplier_4_3 - 4 xKBX_Supplier_4_4 - 4 xKBX_Supplier_4_5 = 0
+F_Supplier_5: F_Supplier_5 - 4 xKBX_Supplier_5_1 - 4 xKBX_Supplier_5_2
+ - 4 xKBX_Supplier_5_3 - 4 xKBX_Supplier_5_4 - 4 xKBX_Supplier_5_5 = 0
+Fixd_Supplier_1: d_Supplier_1 = 0
 Fixd_Supplier_2: d_Supplier_2 = 0
 Fixd_Supplier_3: d_Supplier_3 = 0
 Fixd_Supplier_4: d_Supplier_4 = 0
@@ -1118,6 +1061,106 @@
 Fixreb_Supplier_3: reb_Supplier_3 = 0
 Fixreb_Supplier_4: reb_Supplier_4 = 0
 Fixreb_Supplier_5: reb_Supplier_5 = 0
+KBX_ON_Supplier_1_1: 1000000000 bDDP_Supplier_1_1 + xKBX_Supplier_1_1
+ &lt;= 1000000000
+KBX_ON_Supplier_1_2: 1000000000 bDDP_Supplier_1_2 + xKBX_Supplier_1_2
+ &lt;= 1000000000
+KBX_ON_Supplier_1_3: 1000000000 bDDP_Supplier_1_3 + xKBX_Supplier_1_3
+ &lt;= 1000000000
+KBX_ON_Supplier_1_4: 1000000000 bDDP_Supplier_1_4 + xKBX_Supplier_1_4
+ &lt;= 1000000000
+KBX_ON_Supplier_1_5: 1000000000 bDDP_Supplier_1_5 + xKBX_Supplier_1_5
+ &lt;= 1000000000
+KBX_ON_Supplier_2_1: 1000000000 bDDP_Supplier_2_1 + xKBX_Supplier_2_1
+ &lt;= 1000000000
+KBX_ON_Supplier_2_2: 1000000000 bDDP_Supplier_2_2 + xKBX_Supplier_2_2
+ &lt;= 1000000000
+KBX_ON_Supplier_2_3: 1000000000 bDDP_Supplier_2_3 + xKBX_Supplier_2_3
+ &lt;= 1000000000
+KBX_ON_Supplier_2_4: 1000000000 bDDP_Supplier_2_4 + xKBX_Supplier_2_4
+ &lt;= 1000000000
+KBX_ON_Supplier_2_5: 1000000000 bDDP_Supplier_2_5 + xKBX_Supplier_2_5
+ &lt;= 1000000000
+KBX_ON_Supplier_3_1: 1000000000 bDDP_Supplier_3_1 + xKBX_Supplier_3_1
+ &lt;= 1000000000
+KBX_ON_Supplier_3_2: 1000000000 bDDP_Supplier_3_2 + xKBX_Supplier_3_2
+ &lt;= 1000000000
+KBX_ON_Supplier_3_3: 1000000000 bDDP_Supplier_3_3 + xKBX_Supplier_3_3
+ &lt;= 1000000000
+KBX_ON_Supplier_3_4: 1000000000 bDDP_Supplier_3_4 + xKBX_Supplier_3_4
+ &lt;= 1000000000
+KBX_ON_Supplier_3_5: 1000000000 bDDP_Supplier_3_5 + xKBX_Supplier_3_5
+ &lt;= 1000000000
+KBX_ON_Supplier_4_1: 1000000000 bDDP_Supplier_4_1 + xKBX_Supplier_4_1
+ &lt;= 1000000000
+KBX_ON_Supplier_4_2: 1000000000 bDDP_Supplier_4_2 + xKBX_Supplier_4_2
+ &lt;= 1000000000
+KBX_ON_Supplier_4_3: 1000000000 bDDP_Supplier_4_3 + xKBX_Supplier_4_3
+ &lt;= 1000000000
+KBX_ON_Supplier_4_4: 1000000000 bDDP_Supplier_4_4 + xKBX_Supplier_4_4
+ &lt;= 1000000000
+KBX_ON_Supplier_4_5: 1000000000 bDDP_Supplier_4_5 + xKBX_Supplier_4_5
+ &lt;= 1000000000
+KBX_ON_Supplier_5_1: 1000000000 bDDP_Supplier_5_1 + xKBX_Supplier_5_1
+ &lt;= 1000000000
+KBX_ON_Supplier_5_2: 1000000000 bDDP_Supplier_5_2 + xKBX_Supplier_5_2
+ &lt;= 1000000000
+KBX_ON_Supplier_5_3: 1000000000 bDDP_Supplier_5_3 + xKBX_Supplier_5_3
+ &lt;= 1000000000
+KBX_ON_Supplier_5_4: 1000000000 bDDP_Supplier_5_4 + xKBX_Supplier_5_4
+ &lt;= 1000000000
+KBX_ON_Supplier_5_5: 1000000000 bDDP_Supplier_5_5 + xKBX_Supplier_5_5
+ &lt;= 1000000000
+LinkVol_Supplier_1_1: - xKBX_Supplier_1_1 - xSF_Supplier_1_1 + x_Supplier_1_1
+ = 0
+LinkVol_Supplier_1_2: - xKBX_Supplier_1_2 - xSF_Supplier_1_2 + x_Supplier_1_2
+ = 0
+LinkVol_Supplier_1_3: - xKBX_Supplier_1_3 - xSF_Supplier_1_3 + x_Supplier_1_3
+ = 0
+LinkVol_Supplier_1_4: - xKBX_Supplier_1_4 - xSF_Supplier_1_4 + x_Supplier_1_4
+ = 0
+LinkVol_Supplier_1_5: - xKBX_Supplier_1_5 - xSF_Supplier_1_5 + x_Supplier_1_5
+ = 0
+LinkVol_Supplier_2_1: - xKBX_Supplier_2_1 - xSF_Supplier_2_1 + x_Supplier_2_1
+ = 0
+LinkVol_Supplier_2_2: - xKBX_Supplier_2_2 - xSF_Supplier_2_2 + x_Supplier_2_2
+ = 0
+LinkVol_Supplier_2_3: - xKBX_Supplier_2_3 - xSF_Supplier_2_3 + x_Supplier_2_3
+ = 0
+LinkVol_Supplier_2_4: - xKBX_Supplier_2_4 - xSF_Supplier_2_4 + x_Supplier_2_4
+ = 0
+LinkVol_Supplier_2_5: - xKBX_Supplier_2_5 - xSF_Supplier_2_5 + x_Supplier_2_5
+ = 0
+LinkVol_Supplier_3_1: - xKBX_Supplier_3_1 - xSF_Supplier_3_1 + x_Supplier_3_1
+ = 0
+LinkVol_Supplier_3_2: - xKBX_Supplier_3_2 - xSF_Supplier_3_2 + x_Supplier_3_2
+ = 0
+LinkVol_Supplier_3_3: - xKBX_Supplier_3_3 - xSF_Supplier_3_3 + x_Supplier_3_3
+ = 0
+LinkVol_Supplier_3_4: - xKBX_Supplier_3_4 - xSF_Supplier_3_4 + x_Supplier_3_4
+ = 0
+LinkVol_Supplier_3_5: - xKBX_Supplier_3_5 - xSF_Supplier_3_5 + x_Supplier_3_5
+ = 0
+LinkVol_Supplier_4_1: - xKBX_Supplier_4_1 - xSF_Supplier_4_1 + x_Supplier_4_1
+ = 0
+LinkVol_Supplier_4_2: - xKBX_Supplier_4_2 - xSF_Supplier_4_2 + x_Supplier_4_2
+ = 0
+LinkVol_Supplier_4_3: - xKBX_Supplier_4_3 - xSF_Supplier_4_3 + x_Supplier_4_3
+ = 0
+LinkVol_Supplier_4_4: - xKBX_Supplier_4_4 - xSF_Supplier_4_4 + x_Supplier_4_4
+ = 0
+LinkVol_Supplier_4_5: - xKBX_Supplier_4_5 - xSF_Supplier_4_5 + x_Supplier_4_5
+ = 0
+LinkVol_Supplier_5_1: - xKBX_Supplier_5_1 - xSF_Supplier_5_1 + x_Supplier_5_1
+ = 0
+LinkVol_Supplier_5_2: - xKBX_Supplier_5_2 - xSF_Supplier_5_2 + x_Supplier_5_2
+ = 0
+LinkVol_Supplier_5_3: - xKBX_Supplier_5_3 - xSF_Supplier_5_3 + x_Supplier_5_3
+ = 0
+LinkVol_Supplier_5_4: - xKBX_Supplier_5_4 - xSF_Supplier_5_4 + x_Supplier_5_4
+ = 0
+LinkVol_Supplier_5_5: - xKBX_Supplier_5_5 - xSF_Supplier_5_5 + x_Supplier_5_5
+ = 0
 Link_Supplier_1_1: x_Supplier_1_1 - 1000000000 z_Supplier_1 &lt;= 0
 Link_Supplier_1_2: x_Supplier_1_2 - 1000000000 z_Supplier_1 &lt;= 0
 Link_Supplier_1_3: x_Supplier_1_3 - 1000000000 z_Supplier_1 &lt;= 0
@@ -1153,8 +1196,7 @@
  + x_Supplier_4_4 + x_Supplier_4_5 - z_Supplier_4 &gt;= 0
 MinAward_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
  + x_Supplier_5_4 + x_Supplier_5_5 - z_Supplier_5 &gt;= 0
-NoDisc_Supplier_1: zd_Supplier_1_0 = 0
-OneReb_Supplier_1: yr_Supplier_1_0 = 1
+OneReb_Supplier_1: yr_Supplier_1_0 - z_Supplier_1 = 0
 PctAggEQLB_0: - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
  + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1 - x_Supplier_2_2
  + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 - x_Supplier_3_1
@@ -1169,29 +1211,35 @@
  - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3 - x_Supplier_4_4
  - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
  - x_Supplier_5_4 - x_Supplier_5_5 &lt;= 0
-RMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_3 + x_Supplier_1_4
- + 1000000000 yr_Supplier_1_0 &lt;= 1000002000
-RMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_3 + x_Supplier_1_4 &gt;= 0
-S0_Supplier_1: S0_Supplier_1 - 34 x_Supplier_1_1 - 15 x_Supplier_1_2
- - 15 x_Supplier_1_3 - 75 x_Supplier_1_4 - 24 x_Supplier_1_5 = 0
-S0_Supplier_2: S0_Supplier_2 - 14 x_Supplier_2_1 - 15 x_Supplier_2_2
- - 78 x_Supplier_2_3 - 34 x_Supplier_2_4 - 15 x_Supplier_2_5 = 0
-S0_Supplier_3: S0_Supplier_3 - 75 x_Supplier_3_1 - 25 x_Supplier_3_2
- - 56 x_Supplier_3_3 - 24 x_Supplier_3_4 - 87 x_Supplier_3_5 = 0
-S0_Supplier_4: S0_Supplier_4 - 93 x_Supplier_4_1 - 24 x_Supplier_4_2
- - 78 x_Supplier_4_3 - 56 x_Supplier_4_4 - 86 x_Supplier_4_5 = 0
-S0_Supplier_5: S0_Supplier_5 - 76 x_Supplier_5_1 - 32 x_Supplier_5_2
- - 89 x_Supplier_5_3 - 13 x_Supplier_5_4 - 68 x_Supplier_5_5 = 0
-Spend_Supplier_1: - F_Supplier_1 - S0_Supplier_1 + S_Supplier_1 + d_Supplier_1
- = 0
-Spend_Supplier_2: - F_Supplier_2 - S0_Supplier_2 + S_Supplier_2 + d_Supplier_2
- = 0
-Spend_Supplier_3: - F_Supplier_3 - S0_Supplier_3 + S_Supplier_3 + d_Supplier_3
- = 0
-Spend_Supplier_4: - F_Supplier_4 - S0_Supplier_4 + S_Supplier_4 + d_Supplier_4
- = 0
-Spend_Supplier_5: - F_Supplier_5 - S0_Supplier_5 + S_Supplier_5 + d_Supplier_5
- = 0
+RMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 + 1000000000 yr_Supplier_1_0 &lt;= 1001000000
+RMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 - yr_Supplier_1_0 &gt;= 0
+S0_Supplier_1: S0_Supplier_1 - 34 xKBX_Supplier_1_1 - 15 xKBX_Supplier_1_2
+ - 15 xKBX_Supplier_1_3 - 75 xKBX_Supplier_1_4 - 24 xKBX_Supplier_1_5
+ - 37 xSF_Supplier_1_1 - 18 xSF_Supplier_1_2 - 18 xSF_Supplier_1_3
+ - 78 xSF_Supplier_1_4 - 27 xSF_Supplier_1_5 = 0
+S0_Supplier_2: S0_Supplier_2 - 14 xKBX_Supplier_2_1 - 15 xKBX_Supplier_2_2
+ - 78 xKBX_Supplier_2_3 - 34 xKBX_Supplier_2_4 - 15 xKBX_Supplier_2_5
+ - 17 xSF_Supplier_2_1 - 18 xSF_Supplier_2_2 - 81 xSF_Supplier_2_3
+ - 37 xSF_Supplier_2_4 - 18 xSF_Supplier_2_5 = 0
+S0_Supplier_3: S0_Supplier_3 - 75 xKBX_Supplier_3_1 - 25 xKBX_Supplier_3_2
+ - 56 xKBX_Supplier_3_3 - 24 xKBX_Supplier_3_4 - 87 xKBX_Supplier_3_5
+ - 78 xSF_Supplier_3_1 - 28 xSF_Supplier_3_2 - 59 xSF_Supplier_3_3
+ - 27 xSF_Supplier_3_4 - 90 xSF_Supplier_3_5 = 0
+S0_Supplier_4: S0_Supplier_4 - 93 xKBX_Supplier_4_1 - 24 xKBX_Supplier_4_2
+ - 78 xKBX_Supplier_4_3 - 56 xKBX_Supplier_4_4 - 86 xKBX_Supplier_4_5
+ - 96 xSF_Supplier_4_1 - 27 xSF_Supplier_4_2 - 81 xSF_Supplier_4_3
+ - 59 xSF_Supplier_4_4 - 89 xSF_Supplier_4_5 = 0
+S0_Supplier_5: S0_Supplier_5 - 76 xKBX_Supplier_5_1 - 32 xKBX_Supplier_5_2
+ - 89 xKBX_Supplier_5_3 - 13 xKBX_Supplier_5_4 - 68 xKBX_Supplier_5_5
+ - 79 xSF_Supplier_5_1 - 35 xSF_Supplier_5_2 - 92 xSF_Supplier_5_3
+ - 16 xSF_Supplier_5_4 - 71 xSF_Supplier_5_5 = 0
+Spend_Supplier_1: - S0_Supplier_1 + S_Supplier_1 + d_Supplier_1 = 0
+Spend_Supplier_2: - S0_Supplier_2 + S_Supplier_2 + d_Supplier_2 = 0
+Spend_Supplier_3: - S0_Supplier_3 + S_Supplier_3 + d_Supplier_3 = 0
+Spend_Supplier_4: - S0_Supplier_4 + S_Supplier_4 + d_Supplier_4 = 0
+Spend_Supplier_5: - S0_Supplier_5 + S_Supplier_5 + d_Supplier_5 = 0
 TrLB_1_Supplier_1: x_Supplier_1_1 &gt;= 0
 TrLB_1_Supplier_3: x_Supplier_3_1 &gt;= 0
 TrLB_1_Supplier_4: x_Supplier_4_1 &gt;= 0
@@ -1232,24 +1280,20 @@
 TrUB_5_Supplier_2: - 2421 T_5_Supplier_2 + x_Supplier_2_5 &lt;= 0
 TrUB_5_Supplier_4: - 2421 T_5_Supplier_4 + x_Supplier_4_5 &lt;= 0
 TrUB_5_Supplier_5: - 2421 T_5_Supplier_5 + x_Supplier_5_5 &lt;= 0
-V_Supplier_1: V_Supplier_1 - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
- - x_Supplier_1_4 - x_Supplier_1_5 = 0
-V_Supplier_2: V_Supplier_2 - x_Supplier_2_1 - x_Supplier_2_2 - x_Supplier_2_3
- - x_Supplier_2_4 - x_Supplier_2_5 = 0
-V_Supplier_3: V_Supplier_3 - x_Supplier_3_1 - x_Supplier_3_2 - x_Supplier_3_3
- - x_Supplier_3_4 - x_Supplier_3_5 = 0
-V_Supplier_4: V_Supplier_4 - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3
- - x_Supplier_4_4 - x_Supplier_4_5 = 0
-V_Supplier_5: V_Supplier_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
- - x_Supplier_5_4 - x_Supplier_5_5 = 0
-dLow_Supplier_1_0: - 0.05 S0_Supplier_1 + d_Supplier_1
- - 4.65e+13 zd_Supplier_1_0 &gt;= -4.65e+13
-dUp_Supplier_1_0: - 0.05 S0_Supplier_1 + d_Supplier_1
- + 4.65e+13 zd_Supplier_1_0 &lt;= 4.65e+13
-rLow_Supplier_1_0: - 0.05 S_Supplier_1 + reb_Supplier_1
+dAlwaysZero_Supplier_1: d_Supplier_1 = 0
+dAlwaysZero_Supplier_2: d_Supplier_2 = 0
+dAlwaysZero_Supplier_3: d_Supplier_3 = 0
+dAlwaysZero_Supplier_4: d_Supplier_4 = 0
+dAlwaysZero_Supplier_5: d_Supplier_5 = 0
+rLow_Supplier_1_0: - 0.95 S_Supplier_1 + reb_Supplier_1
  - 4.65e+13 yr_Supplier_1_0 &gt;= -4.65e+13
-rUp_Supplier_1_0: - 0.05 S_Supplier_1 + reb_Supplier_1
+rUp_Supplier_1_0: - 0.95 S_Supplier_1 + reb_Supplier_1
  + 4.65e+13 yr_Supplier_1_0 &lt;= 4.65e+13
+rebAlwaysZero_Supplier_2: reb_Supplier_2 = 0
+rebAlwaysZero_Supplier_3: reb_Supplier_3 = 0
+rebAlwaysZero_Supplier_4: reb_Supplier_4 = 0
+rebAlwaysZero_Supplier_5: reb_Supplier_5 = 0
+rebZeroWhenNoTier_Supplier_1: reb_Supplier_1 - 4.65e+13 yr_Supplier_1_0 &lt;= 0
 Binaries
 T_1_Supplier_1
 T_1_Supplier_3
@@ -1271,13 +1315,37 @@
 T_5_Supplier_2
 T_5_Supplier_4
 T_5_Supplier_5
+bDDP_Supplier_1_1
+bDDP_Supplier_1_2
+bDDP_Supplier_1_3
+bDDP_Supplier_1_4
+bDDP_Supplier_1_5
+bDDP_Supplier_2_1
+bDDP_Supplier_2_2
+bDDP_Supplier_2_3
+bDDP_Supplier_2_4
+bDDP_Supplier_2_5
+bDDP_Supplier_3_1
+bDDP_Supplier_3_2
+bDDP_Supplier_3_3
+bDDP_Supplier_3_4
+bDDP_Supplier_3_5
+bDDP_Supplier_4_1
+bDDP_Supplier_4_2
+bDDP_Supplier_4_3
+bDDP_Supplier_4_4
+bDDP_Supplier_4_5
+bDDP_Supplier_5_1
+bDDP_Supplier_5_2
+bDDP_Supplier_5_3
+bDDP_Supplier_5_4
+bDDP_Supplier_5_5
 yr_Supplier_1_0
 z_Supplier_1
 z_Supplier_2
 z_Supplier_3
 z_Supplier_4
 z_Supplier_5
-zd_Supplier_1_0
 End
 </t>
         </is>

</xml_diff>

<commit_message>
Update freight and ability to not have freight
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -561,49 +561,45 @@
         <v>25</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G2" t="n">
         <v>36400</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>14</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>DDP</t>
-        </is>
-      </c>
+        <v>1.700000000000002</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>17</v>
+        <v>1.700000000000002</v>
       </c>
       <c r="O2" t="n">
-        <v>24752</v>
+        <v>2475.200000000002</v>
       </c>
       <c r="P2" t="n">
         <v>1456</v>
       </c>
       <c r="Q2" t="n">
-        <v>11648</v>
+        <v>33924.8</v>
       </c>
       <c r="R2" t="n">
-        <v>-20384</v>
+        <v>32468.8</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -637,49 +633,45 @@
         <v>36</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="G3" t="n">
         <v>87156</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Supplier 3</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>25</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>DDP</t>
-        </is>
-      </c>
+        <v>0.7500000000000007</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>28</v>
+        <v>0.7500000000000007</v>
       </c>
       <c r="O3" t="n">
-        <v>67788</v>
+        <v>1815.750000000002</v>
       </c>
       <c r="P3" t="n">
         <v>2421</v>
       </c>
       <c r="Q3" t="n">
-        <v>19368</v>
+        <v>85340.25</v>
       </c>
       <c r="R3" t="n">
-        <v>-55683</v>
+        <v>150707.25</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -713,49 +705,45 @@
         <v>82</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G4" t="n">
         <v>529884</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>78</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>DDP</t>
-        </is>
-      </c>
+        <v>0.7500000000000007</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>81</v>
+        <v>0.7500000000000007</v>
       </c>
       <c r="O4" t="n">
-        <v>523422</v>
+        <v>4846.500000000005</v>
       </c>
       <c r="P4" t="n">
         <v>6462</v>
       </c>
       <c r="Q4" t="n">
-        <v>6462</v>
+        <v>525037.5</v>
       </c>
       <c r="R4" t="n">
-        <v>-497574</v>
+        <v>143779.5</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -789,7 +777,7 @@
         <v>32</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="G5" t="n">
         <v>75424</v>
@@ -804,42 +792,38 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>75</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>DDP</t>
-        </is>
-      </c>
+        <v>3.750000000000004</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>78</v>
+        <v>3.750000000000004</v>
       </c>
       <c r="O5" t="n">
-        <v>183846</v>
+        <v>8838.750000000009</v>
       </c>
       <c r="P5" t="n">
         <v>2357</v>
       </c>
       <c r="Q5" t="n">
-        <v>-108422</v>
+        <v>66585.24999999999</v>
       </c>
       <c r="R5" t="n">
-        <v>-176775</v>
+        <v>139652.25</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>174653.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -865,49 +849,45 @@
         <v>75</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G6" t="n">
         <v>181575</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Supplier 3</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>87</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>DDP</t>
-        </is>
-      </c>
+        <v>1.200000000000001</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>90</v>
+        <v>1.200000000000001</v>
       </c>
       <c r="O6" t="n">
-        <v>217890</v>
+        <v>2905.200000000003</v>
       </c>
       <c r="P6" t="n">
         <v>2421</v>
       </c>
       <c r="Q6" t="n">
-        <v>-36315</v>
+        <v>178669.8</v>
       </c>
       <c r="R6" t="n">
-        <v>-210627</v>
+        <v>26146.8</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -987,51 +967,33 @@
  - reb_Supplier_1 - reb_Supplier_2 - reb_Supplier_3 - reb_Supplier_4
  - reb_Supplier_5
 Subject To
-Cap_Supplier_1_Bid_ID_1: x_Supplier_1_1 &lt;= 100000000000
-Cap_Supplier_1_Bid_ID_2: x_Supplier_1_2 &lt;= 100000000000
-Cap_Supplier_1_Bid_ID_3: x_Supplier_1_3 &lt;= 100000000000
-Cap_Supplier_1_Bid_ID_4: x_Supplier_1_4 &lt;= 100000000000
-Cap_Supplier_1_Bid_ID_5: x_Supplier_1_5 &lt;= 100000000000
-Cap_Supplier_2_Bid_ID_1: x_Supplier_2_1 &lt;= 100000000000
-Cap_Supplier_2_Bid_ID_2: x_Supplier_2_2 &lt;= 100000000000
-Cap_Supplier_2_Bid_ID_3: x_Supplier_2_3 &lt;= 100000000000
-Cap_Supplier_2_Bid_ID_4: x_Supplier_2_4 &lt;= 100000000000
-Cap_Supplier_2_Bid_ID_5: x_Supplier_2_5 &lt;= 100000000000
-Cap_Supplier_3_Bid_ID_1: x_Supplier_3_1 &lt;= 100000000000
-Cap_Supplier_3_Bid_ID_2: x_Supplier_3_2 &lt;= 100000000000
-Cap_Supplier_3_Bid_ID_3: x_Supplier_3_3 &lt;= 100000000000
-Cap_Supplier_3_Bid_ID_4: x_Supplier_3_4 &lt;= 100000000000
-Cap_Supplier_3_Bid_ID_5: x_Supplier_3_5 &lt;= 100000000000
-Cap_Supplier_4_Bid_ID_1: x_Supplier_4_1 &lt;= 100000000000
-Cap_Supplier_4_Bid_ID_2: x_Supplier_4_2 &lt;= 100000000000
-Cap_Supplier_4_Bid_ID_3: x_Supplier_4_3 &lt;= 100000000000
-Cap_Supplier_4_Bid_ID_4: x_Supplier_4_4 &lt;= 100000000000
-Cap_Supplier_4_Bid_ID_5: x_Supplier_4_5 &lt;= 100000000000
-DDP_ON_Supplier_1_1: - 1000000000 bDDP_Supplier_1_1 + xSF_Supplier_1_1 &lt;= 0
-DDP_ON_Supplier_1_2: - 1000000000 bDDP_Supplier_1_2 + xSF_Supplier_1_2 &lt;= 0
-DDP_ON_Supplier_1_3: - 1000000000 bDDP_Supplier_1_3 + xSF_Supplier_1_3 &lt;= 0
-DDP_ON_Supplier_1_4: - 1000000000 bDDP_Supplier_1_4 + xSF_Supplier_1_4 &lt;= 0
-DDP_ON_Supplier_1_5: - 1000000000 bDDP_Supplier_1_5 + xSF_Supplier_1_5 &lt;= 0
-DDP_ON_Supplier_2_1: - 1000000000 bDDP_Supplier_2_1 + xSF_Supplier_2_1 &lt;= 0
-DDP_ON_Supplier_2_2: - 1000000000 bDDP_Supplier_2_2 + xSF_Supplier_2_2 &lt;= 0
-DDP_ON_Supplier_2_3: - 1000000000 bDDP_Supplier_2_3 + xSF_Supplier_2_3 &lt;= 0
-DDP_ON_Supplier_2_4: - 1000000000 bDDP_Supplier_2_4 + xSF_Supplier_2_4 &lt;= 0
-DDP_ON_Supplier_2_5: - 1000000000 bDDP_Supplier_2_5 + xSF_Supplier_2_5 &lt;= 0
-DDP_ON_Supplier_3_1: - 1000000000 bDDP_Supplier_3_1 + xSF_Supplier_3_1 &lt;= 0
-DDP_ON_Supplier_3_2: - 1000000000 bDDP_Supplier_3_2 + xSF_Supplier_3_2 &lt;= 0
-DDP_ON_Supplier_3_3: - 1000000000 bDDP_Supplier_3_3 + xSF_Supplier_3_3 &lt;= 0
-DDP_ON_Supplier_3_4: - 1000000000 bDDP_Supplier_3_4 + xSF_Supplier_3_4 &lt;= 0
-DDP_ON_Supplier_3_5: - 1000000000 bDDP_Supplier_3_5 + xSF_Supplier_3_5 &lt;= 0
-DDP_ON_Supplier_4_1: - 1000000000 bDDP_Supplier_4_1 + xSF_Supplier_4_1 &lt;= 0
-DDP_ON_Supplier_4_2: - 1000000000 bDDP_Supplier_4_2 + xSF_Supplier_4_2 &lt;= 0
-DDP_ON_Supplier_4_3: - 1000000000 bDDP_Supplier_4_3 + xSF_Supplier_4_3 &lt;= 0
-DDP_ON_Supplier_4_4: - 1000000000 bDDP_Supplier_4_4 + xSF_Supplier_4_4 &lt;= 0
-DDP_ON_Supplier_4_5: - 1000000000 bDDP_Supplier_4_5 + xSF_Supplier_4_5 &lt;= 0
-DDP_ON_Supplier_5_1: - 1000000000 bDDP_Supplier_5_1 + xSF_Supplier_5_1 &lt;= 0
-DDP_ON_Supplier_5_2: - 1000000000 bDDP_Supplier_5_2 + xSF_Supplier_5_2 &lt;= 0
-DDP_ON_Supplier_5_3: - 1000000000 bDDP_Supplier_5_3 + xSF_Supplier_5_3 &lt;= 0
-DDP_ON_Supplier_5_4: - 1000000000 bDDP_Supplier_5_4 + xSF_Supplier_5_4 &lt;= 0
-DDP_ON_Supplier_5_5: - 1000000000 bDDP_Supplier_5_5 + xSF_Supplier_5_5 &lt;= 0
+Cap_Supplier_1_Bid_ID_1: x_Supplier_1_1 &lt;= 1457
+Cap_Supplier_1_Bid_ID_2: x_Supplier_1_2 &lt;= 2422
+Cap_Supplier_1_Bid_ID_3: x_Supplier_1_3 &lt;= 6463
+Cap_Supplier_1_Bid_ID_4: x_Supplier_1_4 &lt;= 2358
+Cap_Supplier_1_Bid_ID_5: x_Supplier_1_5 &lt;= 2422
+Cap_Supplier_2_Capacity_Group_Category_1: x_Supplier_2_1 + x_Supplier_2_3
+ + x_Supplier_2_4 &lt;= 8001
+Cap_Supplier_2_Capacity_Group_Category_2: x_Supplier_2_2 &lt;= 2501
+Cap_Supplier_2_Capacity_Group_Category_3: x_Supplier_2_5 &lt;= 501
+Cap_Supplier_3_Bid_ID_1: x_Supplier_3_1 &lt;= 1457
+Cap_Supplier_3_Bid_ID_2: x_Supplier_3_2 &lt;= 2422
+Cap_Supplier_3_Bid_ID_3: x_Supplier_3_3 &lt;= 6463
+Cap_Supplier_3_Bid_ID_4: x_Supplier_3_4 &lt;= 2358
+Cap_Supplier_3_Bid_ID_5: x_Supplier_3_5 &lt;= 2422
+Cap_Supplier_4_Bid_ID_1: x_Supplier_4_1 &lt;= 1457
+Cap_Supplier_4_Bid_ID_2: x_Supplier_4_2 &lt;= 2422
+Cap_Supplier_4_Bid_ID_3: x_Supplier_4_3 &lt;= 6463
+Cap_Supplier_4_Bid_ID_4: x_Supplier_4_4 &lt;= 2358
+Cap_Supplier_4_Bid_ID_5: x_Supplier_4_5 &lt;= 2422
+Cap_Supplier_5_Description_Large_Item: x_Supplier_5_5 &lt;= 5001
+Cap_Supplier_5_Description_Medium_item: x_Supplier_5_2 &lt;= 2501
+Cap_Supplier_5_Description_Small_item: x_Supplier_5_1 + x_Supplier_5_3
+ + x_Supplier_5_4 &lt;= 9001
+DMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 + 1000000000 zd_Supplier_1_0 &lt;= 1001000000
+DMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 - zd_Supplier_1_0 &gt;= 0
 Demand_1: x_Supplier_1_1 + x_Supplier_2_1 + x_Supplier_3_1 + x_Supplier_4_1
  + x_Supplier_5_1 = 1456
 Demand_2: x_Supplier_1_2 + x_Supplier_2_2 + x_Supplier_3_2 + x_Supplier_4_2
@@ -1042,125 +1004,25 @@
  + x_Supplier_5_4 = 2357
 Demand_5: x_Supplier_1_5 + x_Supplier_2_5 + x_Supplier_3_5 + x_Supplier_4_5
  + x_Supplier_5_5 = 2421
-F_Supplier_1: F_Supplier_1 - 4 xKBX_Supplier_1_1 - 4 xKBX_Supplier_1_2
- - 4 xKBX_Supplier_1_3 - 4 xKBX_Supplier_1_4 - 4 xKBX_Supplier_1_5 = 0
-F_Supplier_2: F_Supplier_2 - 4 xKBX_Supplier_2_1 - 4 xKBX_Supplier_2_2
- - 4 xKBX_Supplier_2_3 - 4 xKBX_Supplier_2_4 - 4 xKBX_Supplier_2_5 = 0
-F_Supplier_3: F_Supplier_3 - 4 xKBX_Supplier_3_1 - 4 xKBX_Supplier_3_2
- - 4 xKBX_Supplier_3_3 - 4 xKBX_Supplier_3_4 - 4 xKBX_Supplier_3_5 = 0
-F_Supplier_4: F_Supplier_4 - 4 xKBX_Supplier_4_1 - 4 xKBX_Supplier_4_2
- - 4 xKBX_Supplier_4_3 - 4 xKBX_Supplier_4_4 - 4 xKBX_Supplier_4_5 = 0
-F_Supplier_5: F_Supplier_5 - 4 xKBX_Supplier_5_1 - 4 xKBX_Supplier_5_2
- - 4 xKBX_Supplier_5_3 - 4 xKBX_Supplier_5_4 - 4 xKBX_Supplier_5_5 = 0
-Fixd_Supplier_1: d_Supplier_1 = 0
+F_Supplier_1: F_Supplier_1 = 0
+F_Supplier_2: F_Supplier_2 = 0
+F_Supplier_3: F_Supplier_3 = 0
+F_Supplier_4: F_Supplier_4 = 0
+F_Supplier_5: F_Supplier_5 = 0
 Fixd_Supplier_2: d_Supplier_2 = 0
 Fixd_Supplier_3: d_Supplier_3 = 0
 Fixd_Supplier_4: d_Supplier_4 = 0
 Fixd_Supplier_5: d_Supplier_5 = 0
+Fixreb_Supplier_1: reb_Supplier_1 = 0
 Fixreb_Supplier_2: reb_Supplier_2 = 0
 Fixreb_Supplier_3: reb_Supplier_3 = 0
 Fixreb_Supplier_4: reb_Supplier_4 = 0
 Fixreb_Supplier_5: reb_Supplier_5 = 0
-KBX_ON_Supplier_1_1: 1000000000 bDDP_Supplier_1_1 + xKBX_Supplier_1_1
- &lt;= 1000000000
-KBX_ON_Supplier_1_2: 1000000000 bDDP_Supplier_1_2 + xKBX_Supplier_1_2
- &lt;= 1000000000
-KBX_ON_Supplier_1_3: 1000000000 bDDP_Supplier_1_3 + xKBX_Supplier_1_3
- &lt;= 1000000000
-KBX_ON_Supplier_1_4: 1000000000 bDDP_Supplier_1_4 + xKBX_Supplier_1_4
- &lt;= 1000000000
-KBX_ON_Supplier_1_5: 1000000000 bDDP_Supplier_1_5 + xKBX_Supplier_1_5
- &lt;= 1000000000
-KBX_ON_Supplier_2_1: 1000000000 bDDP_Supplier_2_1 + xKBX_Supplier_2_1
- &lt;= 1000000000
-KBX_ON_Supplier_2_2: 1000000000 bDDP_Supplier_2_2 + xKBX_Supplier_2_2
- &lt;= 1000000000
-KBX_ON_Supplier_2_3: 1000000000 bDDP_Supplier_2_3 + xKBX_Supplier_2_3
- &lt;= 1000000000
-KBX_ON_Supplier_2_4: 1000000000 bDDP_Supplier_2_4 + xKBX_Supplier_2_4
- &lt;= 1000000000
-KBX_ON_Supplier_2_5: 1000000000 bDDP_Supplier_2_5 + xKBX_Supplier_2_5
- &lt;= 1000000000
-KBX_ON_Supplier_3_1: 1000000000 bDDP_Supplier_3_1 + xKBX_Supplier_3_1
- &lt;= 1000000000
-KBX_ON_Supplier_3_2: 1000000000 bDDP_Supplier_3_2 + xKBX_Supplier_3_2
- &lt;= 1000000000
-KBX_ON_Supplier_3_3: 1000000000 bDDP_Supplier_3_3 + xKBX_Supplier_3_3
- &lt;= 1000000000
-KBX_ON_Supplier_3_4: 1000000000 bDDP_Supplier_3_4 + xKBX_Supplier_3_4
- &lt;= 1000000000
-KBX_ON_Supplier_3_5: 1000000000 bDDP_Supplier_3_5 + xKBX_Supplier_3_5
- &lt;= 1000000000
-KBX_ON_Supplier_4_1: 1000000000 bDDP_Supplier_4_1 + xKBX_Supplier_4_1
- &lt;= 1000000000
-KBX_ON_Supplier_4_2: 1000000000 bDDP_Supplier_4_2 + xKBX_Supplier_4_2
- &lt;= 1000000000
-KBX_ON_Supplier_4_3: 1000000000 bDDP_Supplier_4_3 + xKBX_Supplier_4_3
- &lt;= 1000000000
-KBX_ON_Supplier_4_4: 1000000000 bDDP_Supplier_4_4 + xKBX_Supplier_4_4
- &lt;= 1000000000
-KBX_ON_Supplier_4_5: 1000000000 bDDP_Supplier_4_5 + xKBX_Supplier_4_5
- &lt;= 1000000000
-KBX_ON_Supplier_5_1: 1000000000 bDDP_Supplier_5_1 + xKBX_Supplier_5_1
- &lt;= 1000000000
-KBX_ON_Supplier_5_2: 1000000000 bDDP_Supplier_5_2 + xKBX_Supplier_5_2
- &lt;= 1000000000
-KBX_ON_Supplier_5_3: 1000000000 bDDP_Supplier_5_3 + xKBX_Supplier_5_3
- &lt;= 1000000000
-KBX_ON_Supplier_5_4: 1000000000 bDDP_Supplier_5_4 + xKBX_Supplier_5_4
- &lt;= 1000000000
-KBX_ON_Supplier_5_5: 1000000000 bDDP_Supplier_5_5 + xKBX_Supplier_5_5
- &lt;= 1000000000
-LinkVol_Supplier_1_1: - xKBX_Supplier_1_1 - xSF_Supplier_1_1 + x_Supplier_1_1
- = 0
-LinkVol_Supplier_1_2: - xKBX_Supplier_1_2 - xSF_Supplier_1_2 + x_Supplier_1_2
- = 0
-LinkVol_Supplier_1_3: - xKBX_Supplier_1_3 - xSF_Supplier_1_3 + x_Supplier_1_3
- = 0
-LinkVol_Supplier_1_4: - xKBX_Supplier_1_4 - xSF_Supplier_1_4 + x_Supplier_1_4
- = 0
-LinkVol_Supplier_1_5: - xKBX_Supplier_1_5 - xSF_Supplier_1_5 + x_Supplier_1_5
- = 0
-LinkVol_Supplier_2_1: - xKBX_Supplier_2_1 - xSF_Supplier_2_1 + x_Supplier_2_1
- = 0
-LinkVol_Supplier_2_2: - xKBX_Supplier_2_2 - xSF_Supplier_2_2 + x_Supplier_2_2
- = 0
-LinkVol_Supplier_2_3: - xKBX_Supplier_2_3 - xSF_Supplier_2_3 + x_Supplier_2_3
- = 0
-LinkVol_Supplier_2_4: - xKBX_Supplier_2_4 - xSF_Supplier_2_4 + x_Supplier_2_4
- = 0
-LinkVol_Supplier_2_5: - xKBX_Supplier_2_5 - xSF_Supplier_2_5 + x_Supplier_2_5
- = 0
-LinkVol_Supplier_3_1: - xKBX_Supplier_3_1 - xSF_Supplier_3_1 + x_Supplier_3_1
- = 0
-LinkVol_Supplier_3_2: - xKBX_Supplier_3_2 - xSF_Supplier_3_2 + x_Supplier_3_2
- = 0
-LinkVol_Supplier_3_3: - xKBX_Supplier_3_3 - xSF_Supplier_3_3 + x_Supplier_3_3
- = 0
-LinkVol_Supplier_3_4: - xKBX_Supplier_3_4 - xSF_Supplier_3_4 + x_Supplier_3_4
- = 0
-LinkVol_Supplier_3_5: - xKBX_Supplier_3_5 - xSF_Supplier_3_5 + x_Supplier_3_5
- = 0
-LinkVol_Supplier_4_1: - xKBX_Supplier_4_1 - xSF_Supplier_4_1 + x_Supplier_4_1
- = 0
-LinkVol_Supplier_4_2: - xKBX_Supplier_4_2 - xSF_Supplier_4_2 + x_Supplier_4_2
- = 0
-LinkVol_Supplier_4_3: - xKBX_Supplier_4_3 - xSF_Supplier_4_3 + x_Supplier_4_3
- = 0
-LinkVol_Supplier_4_4: - xKBX_Supplier_4_4 - xSF_Supplier_4_4 + x_Supplier_4_4
- = 0
-LinkVol_Supplier_4_5: - xKBX_Supplier_4_5 - xSF_Supplier_4_5 + x_Supplier_4_5
- = 0
-LinkVol_Supplier_5_1: - xKBX_Supplier_5_1 - xSF_Supplier_5_1 + x_Supplier_5_1
- = 0
-LinkVol_Supplier_5_2: - xKBX_Supplier_5_2 - xSF_Supplier_5_2 + x_Supplier_5_2
- = 0
-LinkVol_Supplier_5_3: - xKBX_Supplier_5_3 - xSF_Supplier_5_3 + x_Supplier_5_3
- = 0
-LinkVol_Supplier_5_4: - xKBX_Supplier_5_4 - xSF_Supplier_5_4 + x_Supplier_5_4
- = 0
-LinkVol_Supplier_5_5: - xKBX_Supplier_5_5 - xSF_Supplier_5_5 + x_Supplier_5_5
- = 0
+FreightOff_Supplier_1: F_Supplier_1 = 0
+FreightOff_Supplier_2: F_Supplier_2 = 0
+FreightOff_Supplier_3: F_Supplier_3 = 0
+FreightOff_Supplier_4: F_Supplier_4 = 0
+FreightOff_Supplier_5: F_Supplier_5 = 0
 Link_Supplier_1_1: x_Supplier_1_1 - 1000000000 z_Supplier_1 &lt;= 0
 Link_Supplier_1_2: x_Supplier_1_2 - 1000000000 z_Supplier_1 &lt;= 0
 Link_Supplier_1_3: x_Supplier_1_3 - 1000000000 z_Supplier_1 &lt;= 0
@@ -1196,50 +1058,32 @@
  + x_Supplier_4_4 + x_Supplier_4_5 - z_Supplier_4 &gt;= 0
 MinAward_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
  + x_Supplier_5_4 + x_Supplier_5_5 - z_Supplier_5 &gt;= 0
-OneReb_Supplier_1: yr_Supplier_1_0 - z_Supplier_1 = 0
-PctAggEQLB_0: - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
- + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1 - x_Supplier_2_2
- + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 - x_Supplier_3_1
- + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4 + 0 x_Supplier_3_5
- - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3 - x_Supplier_4_4
- - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
- - x_Supplier_5_4 - x_Supplier_5_5 &gt;= 0
-PctAggEQUB_0: - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
- + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1 - x_Supplier_2_2
- + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 - x_Supplier_3_1
- + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4 + 0 x_Supplier_3_5
- - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3 - x_Supplier_4_4
- - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
- - x_Supplier_5_4 - x_Supplier_5_5 &lt;= 0
-RMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
- + x_Supplier_1_4 + x_Supplier_1_5 + 1000000000 yr_Supplier_1_0 &lt;= 1001000000
-RMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
- + x_Supplier_1_4 + x_Supplier_1_5 - yr_Supplier_1_0 &gt;= 0
-S0_Supplier_1: S0_Supplier_1 - 34 xKBX_Supplier_1_1 - 15 xKBX_Supplier_1_2
- - 15 xKBX_Supplier_1_3 - 75 xKBX_Supplier_1_4 - 24 xKBX_Supplier_1_5
- - 37 xSF_Supplier_1_1 - 18 xSF_Supplier_1_2 - 18 xSF_Supplier_1_3
- - 78 xSF_Supplier_1_4 - 27 xSF_Supplier_1_5 = 0
-S0_Supplier_2: S0_Supplier_2 - 14 xKBX_Supplier_2_1 - 15 xKBX_Supplier_2_2
- - 78 xKBX_Supplier_2_3 - 34 xKBX_Supplier_2_4 - 15 xKBX_Supplier_2_5
- - 17 xSF_Supplier_2_1 - 18 xSF_Supplier_2_2 - 81 xSF_Supplier_2_3
- - 37 xSF_Supplier_2_4 - 18 xSF_Supplier_2_5 = 0
-S0_Supplier_3: S0_Supplier_3 - 75 xKBX_Supplier_3_1 - 25 xKBX_Supplier_3_2
- - 56 xKBX_Supplier_3_3 - 24 xKBX_Supplier_3_4 - 87 xKBX_Supplier_3_5
- - 78 xSF_Supplier_3_1 - 28 xSF_Supplier_3_2 - 59 xSF_Supplier_3_3
- - 27 xSF_Supplier_3_4 - 90 xSF_Supplier_3_5 = 0
-S0_Supplier_4: S0_Supplier_4 - 93 xKBX_Supplier_4_1 - 24 xKBX_Supplier_4_2
- - 78 xKBX_Supplier_4_3 - 56 xKBX_Supplier_4_4 - 86 xKBX_Supplier_4_5
- - 96 xSF_Supplier_4_1 - 27 xSF_Supplier_4_2 - 81 xSF_Supplier_4_3
- - 59 xSF_Supplier_4_4 - 89 xSF_Supplier_4_5 = 0
-S0_Supplier_5: S0_Supplier_5 - 76 xKBX_Supplier_5_1 - 32 xKBX_Supplier_5_2
- - 89 xKBX_Supplier_5_3 - 13 xKBX_Supplier_5_4 - 68 xKBX_Supplier_5_5
- - 79 xSF_Supplier_5_1 - 35 xSF_Supplier_5_2 - 92 xSF_Supplier_5_3
- - 16 xSF_Supplier_5_4 - 71 xSF_Supplier_5_5 = 0
+OneDisc_Supplier_1: - z_Supplier_1 + zd_Supplier_1_0 = 0
+S0_Supplier_1: S0_Supplier_1 - 34 x_Supplier_1_1 - 15 x_Supplier_1_2
+ - 15 x_Supplier_1_3 - 75 x_Supplier_1_4 - 24 x_Supplier_1_5 = 0
+S0_Supplier_2: S0_Supplier_2 - 14 x_Supplier_2_1 - 15 x_Supplier_2_2
+ - 78 x_Supplier_2_3 - 34 x_Supplier_2_4 - 15 x_Supplier_2_5 = 0
+S0_Supplier_3: S0_Supplier_3 - 75 x_Supplier_3_1 - 25 x_Supplier_3_2
+ - 56 x_Supplier_3_3 - 24 x_Supplier_3_4 - 87 x_Supplier_3_5 = 0
+S0_Supplier_4: S0_Supplier_4 - 93 x_Supplier_4_1 - 24 x_Supplier_4_2
+ - 78 x_Supplier_4_3 - 56 x_Supplier_4_4 - 86 x_Supplier_4_5 = 0
+S0_Supplier_5: S0_Supplier_5 - 76 x_Supplier_5_1 - 32 x_Supplier_5_2
+ - 89 x_Supplier_5_3 - 13 x_Supplier_5_4 - 68 x_Supplier_5_5 = 0
 Spend_Supplier_1: - S0_Supplier_1 + S_Supplier_1 + d_Supplier_1 = 0
 Spend_Supplier_2: - S0_Supplier_2 + S_Supplier_2 + d_Supplier_2 = 0
 Spend_Supplier_3: - S0_Supplier_3 + S_Supplier_3 + d_Supplier_3 = 0
 Spend_Supplier_4: - S0_Supplier_4 + S_Supplier_4 + d_Supplier_4 = 0
 Spend_Supplier_5: - S0_Supplier_5 + S_Supplier_5 + d_Supplier_5 = 0
+SupCntEQ_0: Y_sup_0_Supplier_1 + Y_sup_0_Supplier_2 + Y_sup_0_Supplier_3
+ + Y_sup_0_Supplier_4 + Y_sup_0_Supplier_5 = 1
+SupCntEQ_1: Y_sup_1_Supplier_1 + Y_sup_1_Supplier_2 + Y_sup_1_Supplier_3
+ + Y_sup_1_Supplier_4 + Y_sup_1_Supplier_5 = 1
+SupCntEQ_2: Y_sup_2_Supplier_1 + Y_sup_2_Supplier_2 + Y_sup_2_Supplier_3
+ + Y_sup_2_Supplier_4 + Y_sup_2_Supplier_5 = 1
+SupCntEQ_3: Y_sup_3_Supplier_1 + Y_sup_3_Supplier_2 + Y_sup_3_Supplier_3
+ + Y_sup_3_Supplier_4 + Y_sup_3_Supplier_5 = 1
+SupCntEQ_4: Y_sup_4_Supplier_1 + Y_sup_4_Supplier_2 + Y_sup_4_Supplier_3
+ + Y_sup_4_Supplier_4 + Y_sup_4_Supplier_5 = 1
 TrLB_1_Supplier_1: x_Supplier_1_1 &gt;= 0
 TrLB_1_Supplier_3: x_Supplier_3_1 &gt;= 0
 TrLB_1_Supplier_4: x_Supplier_4_1 &gt;= 0
@@ -1280,20 +1124,70 @@
 TrUB_5_Supplier_2: - 2421 T_5_Supplier_2 + x_Supplier_2_5 &lt;= 0
 TrUB_5_Supplier_4: - 2421 T_5_Supplier_4 + x_Supplier_4_5 &lt;= 0
 TrUB_5_Supplier_5: - 2421 T_5_Supplier_5 + x_Supplier_5_5 &lt;= 0
-dAlwaysZero_Supplier_1: d_Supplier_1 = 0
-dAlwaysZero_Supplier_2: d_Supplier_2 = 0
-dAlwaysZero_Supplier_3: d_Supplier_3 = 0
-dAlwaysZero_Supplier_4: d_Supplier_4 = 0
-dAlwaysZero_Supplier_5: d_Supplier_5 = 0
-rLow_Supplier_1_0: - 0.95 S_Supplier_1 + reb_Supplier_1
- - 4.65e+13 yr_Supplier_1_0 &gt;= -4.65e+13
-rUp_Supplier_1_0: - 0.95 S_Supplier_1 + reb_Supplier_1
- + 4.65e+13 yr_Supplier_1_0 &lt;= 4.65e+13
-rebAlwaysZero_Supplier_2: reb_Supplier_2 = 0
-rebAlwaysZero_Supplier_3: reb_Supplier_3 = 0
-rebAlwaysZero_Supplier_4: reb_Supplier_4 = 0
-rebAlwaysZero_Supplier_5: reb_Supplier_5 = 0
-rebZeroWhenNoTier_Supplier_1: reb_Supplier_1 - 4.65e+13 yr_Supplier_1_0 &lt;= 0
+Ylb_0_Supplier_1: - 1e-06 Y_sup_0_Supplier_1 + x_Supplier_1_1 &gt;= 0
+Ylb_0_Supplier_2: - 1e-06 Y_sup_0_Supplier_2 + x_Supplier_2_1 &gt;= 0
+Ylb_0_Supplier_3: - 1e-06 Y_sup_0_Supplier_3 + x_Supplier_3_1 &gt;= 0
+Ylb_0_Supplier_4: - 1e-06 Y_sup_0_Supplier_4 + x_Supplier_4_1 &gt;= 0
+Ylb_0_Supplier_5: - 1e-06 Y_sup_0_Supplier_5 + x_Supplier_5_1 &gt;= 0
+Ylb_1_Supplier_1: - 1e-06 Y_sup_1_Supplier_1 + x_Supplier_1_2 &gt;= 0
+Ylb_1_Supplier_2: - 1e-06 Y_sup_1_Supplier_2 + x_Supplier_2_2 &gt;= 0
+Ylb_1_Supplier_3: - 1e-06 Y_sup_1_Supplier_3 + x_Supplier_3_2 &gt;= 0
+Ylb_1_Supplier_4: - 1e-06 Y_sup_1_Supplier_4 + x_Supplier_4_2 &gt;= 0
+Ylb_1_Supplier_5: - 1e-06 Y_sup_1_Supplier_5 + x_Supplier_5_2 &gt;= 0
+Ylb_2_Supplier_1: - 1e-06 Y_sup_2_Supplier_1 + x_Supplier_1_3 &gt;= 0
+Ylb_2_Supplier_2: - 1e-06 Y_sup_2_Supplier_2 + x_Supplier_2_3 &gt;= 0
+Ylb_2_Supplier_3: - 1e-06 Y_sup_2_Supplier_3 + x_Supplier_3_3 &gt;= 0
+Ylb_2_Supplier_4: - 1e-06 Y_sup_2_Supplier_4 + x_Supplier_4_3 &gt;= 0
+Ylb_2_Supplier_5: - 1e-06 Y_sup_2_Supplier_5 + x_Supplier_5_3 &gt;= 0
+Ylb_3_Supplier_1: - 1e-06 Y_sup_3_Supplier_1 + x_Supplier_1_4 &gt;= 0
+Ylb_3_Supplier_2: - 1e-06 Y_sup_3_Supplier_2 + x_Supplier_2_4 &gt;= 0
+Ylb_3_Supplier_3: - 1e-06 Y_sup_3_Supplier_3 + x_Supplier_3_4 &gt;= 0
+Ylb_3_Supplier_4: - 1e-06 Y_sup_3_Supplier_4 + x_Supplier_4_4 &gt;= 0
+Ylb_3_Supplier_5: - 1e-06 Y_sup_3_Supplier_5 + x_Supplier_5_4 &gt;= 0
+Ylb_4_Supplier_1: - 1e-06 Y_sup_4_Supplier_1 + x_Supplier_1_5 &gt;= 0
+Ylb_4_Supplier_2: - 1e-06 Y_sup_4_Supplier_2 + x_Supplier_2_5 &gt;= 0
+Ylb_4_Supplier_3: - 1e-06 Y_sup_4_Supplier_3 + x_Supplier_3_5 &gt;= 0
+Ylb_4_Supplier_4: - 1e-06 Y_sup_4_Supplier_4 + x_Supplier_4_5 &gt;= 0
+Ylb_4_Supplier_5: - 1e-06 Y_sup_4_Supplier_5 + x_Supplier_5_5 &gt;= 0
+Yub_0_Supplier_1: - 1000000000 Y_sup_0_Supplier_1 + x_Supplier_1_1 &lt;= 0
+Yub_0_Supplier_2: - 1000000000 Y_sup_0_Supplier_2 + x_Supplier_2_1 &lt;= 0
+Yub_0_Supplier_3: - 1000000000 Y_sup_0_Supplier_3 + x_Supplier_3_1 &lt;= 0
+Yub_0_Supplier_4: - 1000000000 Y_sup_0_Supplier_4 + x_Supplier_4_1 &lt;= 0
+Yub_0_Supplier_5: - 1000000000 Y_sup_0_Supplier_5 + x_Supplier_5_1 &lt;= 0
+Yub_1_Supplier_1: - 1000000000 Y_sup_1_Supplier_1 + x_Supplier_1_2 &lt;= 0
+Yub_1_Supplier_2: - 1000000000 Y_sup_1_Supplier_2 + x_Supplier_2_2 &lt;= 0
+Yub_1_Supplier_3: - 1000000000 Y_sup_1_Supplier_3 + x_Supplier_3_2 &lt;= 0
+Yub_1_Supplier_4: - 1000000000 Y_sup_1_Supplier_4 + x_Supplier_4_2 &lt;= 0
+Yub_1_Supplier_5: - 1000000000 Y_sup_1_Supplier_5 + x_Supplier_5_2 &lt;= 0
+Yub_2_Supplier_1: - 1000000000 Y_sup_2_Supplier_1 + x_Supplier_1_3 &lt;= 0
+Yub_2_Supplier_2: - 1000000000 Y_sup_2_Supplier_2 + x_Supplier_2_3 &lt;= 0
+Yub_2_Supplier_3: - 1000000000 Y_sup_2_Supplier_3 + x_Supplier_3_3 &lt;= 0
+Yub_2_Supplier_4: - 1000000000 Y_sup_2_Supplier_4 + x_Supplier_4_3 &lt;= 0
+Yub_2_Supplier_5: - 1000000000 Y_sup_2_Supplier_5 + x_Supplier_5_3 &lt;= 0
+Yub_3_Supplier_1: - 1000000000 Y_sup_3_Supplier_1 + x_Supplier_1_4 &lt;= 0
+Yub_3_Supplier_2: - 1000000000 Y_sup_3_Supplier_2 + x_Supplier_2_4 &lt;= 0
+Yub_3_Supplier_3: - 1000000000 Y_sup_3_Supplier_3 + x_Supplier_3_4 &lt;= 0
+Yub_3_Supplier_4: - 1000000000 Y_sup_3_Supplier_4 + x_Supplier_4_4 &lt;= 0
+Yub_3_Supplier_5: - 1000000000 Y_sup_3_Supplier_5 + x_Supplier_5_4 &lt;= 0
+Yub_4_Supplier_1: - 1000000000 Y_sup_4_Supplier_1 + x_Supplier_1_5 &lt;= 0
+Yub_4_Supplier_2: - 1000000000 Y_sup_4_Supplier_2 + x_Supplier_2_5 &lt;= 0
+Yub_4_Supplier_3: - 1000000000 Y_sup_4_Supplier_3 + x_Supplier_3_5 &lt;= 0
+Yub_4_Supplier_4: - 1000000000 Y_sup_4_Supplier_4 + x_Supplier_4_5 &lt;= 0
+Yub_4_Supplier_5: - 1000000000 Y_sup_4_Supplier_5 + x_Supplier_5_5 &lt;= 0
+dLow_Supplier_1_0: - 0.95 S0_Supplier_1 + d_Supplier_1
+ - 1406346 zd_Supplier_1_0 &gt;= -1406346
+dUp_Supplier_1_0: - 0.95 S0_Supplier_1 + d_Supplier_1
+ + 1406346 zd_Supplier_1_0 &lt;= 1406346
+dZeroNoTier_Supplier_2: d_Supplier_2 = 0
+dZeroNoTier_Supplier_3: d_Supplier_3 = 0
+dZeroNoTier_Supplier_4: d_Supplier_4 = 0
+dZeroNoTier_Supplier_5: d_Supplier_5 = 0
+dZero_Supplier_1: d_Supplier_1 - 1406346 zd_Supplier_1_0 &lt;= 0
+rZeroNoTier_Supplier_1: reb_Supplier_1 = 0
+rZeroNoTier_Supplier_2: reb_Supplier_2 = 0
+rZeroNoTier_Supplier_3: reb_Supplier_3 = 0
+rZeroNoTier_Supplier_4: reb_Supplier_4 = 0
+rZeroNoTier_Supplier_5: reb_Supplier_5 = 0
 Binaries
 T_1_Supplier_1
 T_1_Supplier_3
@@ -1315,37 +1209,37 @@
 T_5_Supplier_2
 T_5_Supplier_4
 T_5_Supplier_5
-bDDP_Supplier_1_1
-bDDP_Supplier_1_2
-bDDP_Supplier_1_3
-bDDP_Supplier_1_4
-bDDP_Supplier_1_5
-bDDP_Supplier_2_1
-bDDP_Supplier_2_2
-bDDP_Supplier_2_3
-bDDP_Supplier_2_4
-bDDP_Supplier_2_5
-bDDP_Supplier_3_1
-bDDP_Supplier_3_2
-bDDP_Supplier_3_3
-bDDP_Supplier_3_4
-bDDP_Supplier_3_5
-bDDP_Supplier_4_1
-bDDP_Supplier_4_2
-bDDP_Supplier_4_3
-bDDP_Supplier_4_4
-bDDP_Supplier_4_5
-bDDP_Supplier_5_1
-bDDP_Supplier_5_2
-bDDP_Supplier_5_3
-bDDP_Supplier_5_4
-bDDP_Supplier_5_5
-yr_Supplier_1_0
+Y_sup_0_Supplier_1
+Y_sup_0_Supplier_2
+Y_sup_0_Supplier_3
+Y_sup_0_Supplier_4
+Y_sup_0_Supplier_5
+Y_sup_1_Supplier_1
+Y_sup_1_Supplier_2
+Y_sup_1_Supplier_3
+Y_sup_1_Supplier_4
+Y_sup_1_Supplier_5
+Y_sup_2_Supplier_1
+Y_sup_2_Supplier_2
+Y_sup_2_Supplier_3
+Y_sup_2_Supplier_4
+Y_sup_2_Supplier_5
+Y_sup_3_Supplier_1
+Y_sup_3_Supplier_2
+Y_sup_3_Supplier_3
+Y_sup_3_Supplier_4
+Y_sup_3_Supplier_5
+Y_sup_4_Supplier_1
+Y_sup_4_Supplier_2
+Y_sup_4_Supplier_3
+Y_sup_4_Supplier_4
+Y_sup_4_Supplier_5
 z_Supplier_1
 z_Supplier_2
 z_Supplier_3
 z_Supplier_4
 z_Supplier_5
+zd_Supplier_1_0
 End
 </t>
         </is>
@@ -1362,7 +1256,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1409,7 +1303,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>100000000000</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="3">
@@ -1429,7 +1323,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>100000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="4">
@@ -1449,7 +1343,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>100000000000</v>
+        <v>6463</v>
       </c>
     </row>
     <row r="5">
@@ -1469,7 +1363,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>100000000000</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="6">
@@ -1489,7 +1383,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>100000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="7">
@@ -1509,7 +1403,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>100000000000</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="8">
@@ -1529,7 +1423,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>100000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="9">
@@ -1549,7 +1443,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>100000000000</v>
+        <v>6463</v>
       </c>
     </row>
     <row r="10">
@@ -1569,7 +1463,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>100000000000</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="11">
@@ -1589,7 +1483,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>100000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="12">
@@ -1609,7 +1503,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>100000000000</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="13">
@@ -1629,7 +1523,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>100000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="14">
@@ -1649,7 +1543,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>100000000000</v>
+        <v>6463</v>
       </c>
     </row>
     <row r="15">
@@ -1669,7 +1563,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>100000000000</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="16">
@@ -1689,7 +1583,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>100000000000</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="17">
@@ -1700,16 +1594,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Capacity Group</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Category 1</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>100000000000</v>
+        <v>8001</v>
       </c>
     </row>
     <row r="18">
@@ -1720,16 +1614,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Capacity Group</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Category 2</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>100000000000</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="19">
@@ -1740,56 +1634,76 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Capacity Group</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Category 3</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>100000000000</v>
+        <v>501</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 5</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Small item</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>100000000000</v>
+        <v>9001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 5</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bid ID</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>Medium item</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>100000000000</v>
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Supplier 5</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Large Item</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed input template to be simplier
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -576,38 +576,38 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>1.700000000000002</v>
+        <v>33.32</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>1.700000000000002</v>
+        <v>33.32</v>
       </c>
       <c r="O2" t="n">
-        <v>2475.200000000002</v>
+        <v>48513.92</v>
       </c>
       <c r="P2" t="n">
         <v>1456</v>
       </c>
       <c r="Q2" t="n">
-        <v>33924.8</v>
+        <v>-12113.92</v>
       </c>
       <c r="R2" t="n">
-        <v>32468.8</v>
+        <v>-13569.92</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>46088.22399999999</v>
       </c>
     </row>
     <row r="3">
@@ -648,38 +648,38 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0.7500000000000007</v>
+        <v>14.7</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7500000000000007</v>
+        <v>14.7</v>
       </c>
       <c r="O3" t="n">
-        <v>1815.750000000002</v>
+        <v>35588.7</v>
       </c>
       <c r="P3" t="n">
         <v>2421</v>
       </c>
       <c r="Q3" t="n">
-        <v>85340.25</v>
+        <v>51567.3</v>
       </c>
       <c r="R3" t="n">
-        <v>150707.25</v>
+        <v>116934.3</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>33809.26499999999</v>
       </c>
     </row>
     <row r="4">
@@ -712,38 +712,38 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0.7500000000000007</v>
+        <v>78</v>
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0.7500000000000007</v>
+        <v>78</v>
       </c>
       <c r="O4" t="n">
-        <v>4846.500000000005</v>
+        <v>504036</v>
       </c>
       <c r="P4" t="n">
         <v>6462</v>
       </c>
       <c r="Q4" t="n">
-        <v>525037.5</v>
+        <v>25848</v>
       </c>
       <c r="R4" t="n">
-        <v>143779.5</v>
+        <v>-355410</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -792,38 +792,38 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>3.750000000000004</v>
+        <v>73.5</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>3.750000000000004</v>
+        <v>73.5</v>
       </c>
       <c r="O5" t="n">
-        <v>8838.750000000009</v>
+        <v>173239.5</v>
       </c>
       <c r="P5" t="n">
         <v>2357</v>
       </c>
       <c r="Q5" t="n">
-        <v>66585.24999999999</v>
+        <v>-97815.5</v>
       </c>
       <c r="R5" t="n">
-        <v>139652.25</v>
+        <v>-24748.5</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
+        <v>164577.525</v>
       </c>
     </row>
     <row r="6">
@@ -864,38 +864,38 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>1.200000000000001</v>
+        <v>23.52</v>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>1.200000000000001</v>
+        <v>23.52</v>
       </c>
       <c r="O6" t="n">
-        <v>2905.200000000003</v>
+        <v>56941.92</v>
       </c>
       <c r="P6" t="n">
         <v>2421</v>
       </c>
       <c r="Q6" t="n">
-        <v>178669.8</v>
+        <v>124633.08</v>
       </c>
       <c r="R6" t="n">
-        <v>26146.8</v>
+        <v>-27889.92</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>54094.82399999999</v>
       </c>
     </row>
   </sheetData>
@@ -967,6 +967,76 @@
  - reb_Supplier_1 - reb_Supplier_2 - reb_Supplier_3 - reb_Supplier_4
  - reb_Supplier_5
 Subject To
+AllPctLB_1_Supplier_1: 0.8 x_Supplier_1_1 + 0.8 x_Supplier_1_2
+ + 0.8 x_Supplier_1_3 + 0.8 x_Supplier_1_4 + 0.8 x_Supplier_1_5
+ - 0.2 x_Supplier_2_1 - 0.2 x_Supplier_2_2 - 0.2 x_Supplier_2_3
+ - 0.2 x_Supplier_2_4 - 0.2 x_Supplier_2_5 - 0.2 x_Supplier_3_1
+ - 0.2 x_Supplier_3_2 - 0.2 x_Supplier_3_3 - 0.2 x_Supplier_3_4
+ - 0.2 x_Supplier_3_5 - 0.2 x_Supplier_4_1 - 0.2 x_Supplier_4_2
+ - 0.2 x_Supplier_4_3 - 0.2 x_Supplier_4_4 - 0.2 x_Supplier_4_5
+ - 0.2 x_Supplier_5_1 - 0.2 x_Supplier_5_2 - 0.2 x_Supplier_5_3
+ - 0.2 x_Supplier_5_4 - 0.2 x_Supplier_5_5 - 1000000000 y_1_Supplier_1
+ &gt;= -1000000000
+AllPctLB_1_Supplier_2: - 0.2 x_Supplier_1_1 - 0.2 x_Supplier_1_2
+ - 0.2 x_Supplier_1_3 - 0.2 x_Supplier_1_4 - 0.2 x_Supplier_1_5
+ + 0.8 x_Supplier_2_1 + 0.8 x_Supplier_2_2 + 0.8 x_Supplier_2_3
+ + 0.8 x_Supplier_2_4 + 0.8 x_Supplier_2_5 - 0.2 x_Supplier_3_1
+ - 0.2 x_Supplier_3_2 - 0.2 x_Supplier_3_3 - 0.2 x_Supplier_3_4
+ - 0.2 x_Supplier_3_5 - 0.2 x_Supplier_4_1 - 0.2 x_Supplier_4_2
+ - 0.2 x_Supplier_4_3 - 0.2 x_Supplier_4_4 - 0.2 x_Supplier_4_5
+ - 0.2 x_Supplier_5_1 - 0.2 x_Supplier_5_2 - 0.2 x_Supplier_5_3
+ - 0.2 x_Supplier_5_4 - 0.2 x_Supplier_5_5 - 1000000000 y_1_Supplier_2
+ &gt;= -1000000000
+AllPctLB_1_Supplier_3: - 0.2 x_Supplier_1_1 - 0.2 x_Supplier_1_2
+ - 0.2 x_Supplier_1_3 - 0.2 x_Supplier_1_4 - 0.2 x_Supplier_1_5
+ - 0.2 x_Supplier_2_1 - 0.2 x_Supplier_2_2 - 0.2 x_Supplier_2_3
+ - 0.2 x_Supplier_2_4 - 0.2 x_Supplier_2_5 + 0.8 x_Supplier_3_1
+ + 0.8 x_Supplier_3_2 + 0.8 x_Supplier_3_3 + 0.8 x_Supplier_3_4
+ + 0.8 x_Supplier_3_5 - 0.2 x_Supplier_4_1 - 0.2 x_Supplier_4_2
+ - 0.2 x_Supplier_4_3 - 0.2 x_Supplier_4_4 - 0.2 x_Supplier_4_5
+ - 0.2 x_Supplier_5_1 - 0.2 x_Supplier_5_2 - 0.2 x_Supplier_5_3
+ - 0.2 x_Supplier_5_4 - 0.2 x_Supplier_5_5 - 1000000000 y_1_Supplier_3
+ &gt;= -1000000000
+AllPctLB_1_Supplier_4: - 0.2 x_Supplier_1_1 - 0.2 x_Supplier_1_2
+ - 0.2 x_Supplier_1_3 - 0.2 x_Supplier_1_4 - 0.2 x_Supplier_1_5
+ - 0.2 x_Supplier_2_1 - 0.2 x_Supplier_2_2 - 0.2 x_Supplier_2_3
+ - 0.2 x_Supplier_2_4 - 0.2 x_Supplier_2_5 - 0.2 x_Supplier_3_1
+ - 0.2 x_Supplier_3_2 - 0.2 x_Supplier_3_3 - 0.2 x_Supplier_3_4
+ - 0.2 x_Supplier_3_5 + 0.8 x_Supplier_4_1 + 0.8 x_Supplier_4_2
+ + 0.8 x_Supplier_4_3 + 0.8 x_Supplier_4_4 + 0.8 x_Supplier_4_5
+ - 0.2 x_Supplier_5_1 - 0.2 x_Supplier_5_2 - 0.2 x_Supplier_5_3
+ - 0.2 x_Supplier_5_4 - 0.2 x_Supplier_5_5 - 1000000000 y_1_Supplier_4
+ &gt;= -1000000000
+AllPctLB_1_Supplier_5: - 0.2 x_Supplier_1_1 - 0.2 x_Supplier_1_2
+ - 0.2 x_Supplier_1_3 - 0.2 x_Supplier_1_4 - 0.2 x_Supplier_1_5
+ - 0.2 x_Supplier_2_1 - 0.2 x_Supplier_2_2 - 0.2 x_Supplier_2_3
+ - 0.2 x_Supplier_2_4 - 0.2 x_Supplier_2_5 - 0.2 x_Supplier_3_1
+ - 0.2 x_Supplier_3_2 - 0.2 x_Supplier_3_3 - 0.2 x_Supplier_3_4
+ - 0.2 x_Supplier_3_5 - 0.2 x_Supplier_4_1 - 0.2 x_Supplier_4_2
+ - 0.2 x_Supplier_4_3 - 0.2 x_Supplier_4_4 - 0.2 x_Supplier_4_5
+ + 0.8 x_Supplier_5_1 + 0.8 x_Supplier_5_2 + 0.8 x_Supplier_5_3
+ + 0.8 x_Supplier_5_4 + 0.8 x_Supplier_5_5 - 1000000000 y_1_Supplier_5
+ &gt;= -1000000000
+AllYlb_1_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 &gt;= 0
+AllYlb_1_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
+ + x_Supplier_2_4 + x_Supplier_2_5 &gt;= 0
+AllYlb_1_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
+ + x_Supplier_3_4 + x_Supplier_3_5 &gt;= 0
+AllYlb_1_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
+ + x_Supplier_4_4 + x_Supplier_4_5 &gt;= 0
+AllYlb_1_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
+ + x_Supplier_5_4 + x_Supplier_5_5 &gt;= 0
+AllYub_1_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 - 1000000000 y_1_Supplier_1 &lt;= 0
+AllYub_1_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
+ + x_Supplier_2_4 + x_Supplier_2_5 - 1000000000 y_1_Supplier_2 &lt;= 0
+AllYub_1_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
+ + x_Supplier_3_4 + x_Supplier_3_5 - 1000000000 y_1_Supplier_3 &lt;= 0
+AllYub_1_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
+ + x_Supplier_4_4 + x_Supplier_4_5 - 1000000000 y_1_Supplier_4 &lt;= 0
+AllYub_1_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
+ + x_Supplier_5_4 + x_Supplier_5_5 - 1000000000 y_1_Supplier_5 &lt;= 0
 Cap_Supplier_1_Bid_ID_1: x_Supplier_1_1 &lt;= 1457
 Cap_Supplier_1_Bid_ID_2: x_Supplier_1_2 &lt;= 2422
 Cap_Supplier_1_Bid_ID_3: x_Supplier_1_3 &lt;= 6463
@@ -1013,7 +1083,6 @@
 Fixd_Supplier_3: d_Supplier_3 = 0
 Fixd_Supplier_4: d_Supplier_4 = 0
 Fixd_Supplier_5: d_Supplier_5 = 0
-Fixreb_Supplier_1: reb_Supplier_1 = 0
 Fixreb_Supplier_2: reb_Supplier_2 = 0
 Fixreb_Supplier_3: reb_Supplier_3 = 0
 Fixreb_Supplier_4: reb_Supplier_4 = 0
@@ -1059,6 +1128,20 @@
 MinAward_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
  + x_Supplier_5_4 + x_Supplier_5_5 - z_Supplier_5 &gt;= 0
 OneDisc_Supplier_1: - z_Supplier_1 + zd_Supplier_1_0 = 0
+OneReb_Supplier_1: yr_Supplier_1_0 - z_Supplier_1 = 0
+PctAggLB_2: - 0.5 x_Supplier_1_1 - 0.5 x_Supplier_1_2 - 0.5 x_Supplier_1_3
+ + 0.5 x_Supplier_1_4 - 0.5 x_Supplier_1_5 + 0.5 x_Supplier_2_1
+ - 0.5 x_Supplier_2_2 + 0.5 x_Supplier_2_3 - 0.5 x_Supplier_2_4
+ - 0.5 x_Supplier_2_5 - 0.5 x_Supplier_3_1 + 0.5 x_Supplier_3_2
+ - 0.5 x_Supplier_3_3 - 0.5 x_Supplier_3_4 + 0.5 x_Supplier_3_5
+ - 0.5 x_Supplier_4_1 - 0.5 x_Supplier_4_2 - 0.5 x_Supplier_4_3
+ - 0.5 x_Supplier_4_4 - 0.5 x_Supplier_4_5 - 0.5 x_Supplier_5_1
+ - 0.5 x_Supplier_5_2 - 0.5 x_Supplier_5_3 - 0.5 x_Supplier_5_4
+ - 0.5 x_Supplier_5_5 &gt;= 0
+RMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 + 1000000000 yr_Supplier_1_0 &lt;= 1001000000
+RMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 - yr_Supplier_1_0 &gt;= 0
 S0_Supplier_1: S0_Supplier_1 - 34 x_Supplier_1_1 - 15 x_Supplier_1_2
  - 15 x_Supplier_1_3 - 75 x_Supplier_1_4 - 24 x_Supplier_1_5 = 0
 S0_Supplier_2: S0_Supplier_2 - 14 x_Supplier_2_1 - 15 x_Supplier_2_2
@@ -1074,16 +1157,18 @@
 Spend_Supplier_3: - S0_Supplier_3 + S_Supplier_3 + d_Supplier_3 = 0
 Spend_Supplier_4: - S0_Supplier_4 + S_Supplier_4 + d_Supplier_4 = 0
 Spend_Supplier_5: - S0_Supplier_5 + S_Supplier_5 + d_Supplier_5 = 0
-SupCntEQ_0: Y_sup_0_Supplier_1 + Y_sup_0_Supplier_2 + Y_sup_0_Supplier_3
- + Y_sup_0_Supplier_4 + Y_sup_0_Supplier_5 = 1
-SupCntEQ_1: Y_sup_1_Supplier_1 + Y_sup_1_Supplier_2 + Y_sup_1_Supplier_3
- + Y_sup_1_Supplier_4 + Y_sup_1_Supplier_5 = 1
-SupCntEQ_2: Y_sup_2_Supplier_1 + Y_sup_2_Supplier_2 + Y_sup_2_Supplier_3
- + Y_sup_2_Supplier_4 + Y_sup_2_Supplier_5 = 1
 SupCntEQ_3: Y_sup_3_Supplier_1 + Y_sup_3_Supplier_2 + Y_sup_3_Supplier_3
  + Y_sup_3_Supplier_4 + Y_sup_3_Supplier_5 = 1
 SupCntEQ_4: Y_sup_4_Supplier_1 + Y_sup_4_Supplier_2 + Y_sup_4_Supplier_3
  + Y_sup_4_Supplier_4 + Y_sup_4_Supplier_5 = 1
+SupCntEQ_5: Y_sup_5_Supplier_1 + Y_sup_5_Supplier_2 + Y_sup_5_Supplier_3
+ + Y_sup_5_Supplier_4 + Y_sup_5_Supplier_5 = 1
+SupCntEQ_6: Y_sup_6_Supplier_1 + Y_sup_6_Supplier_2 + Y_sup_6_Supplier_3
+ + Y_sup_6_Supplier_4 + Y_sup_6_Supplier_5 = 1
+SupCntEQ_7: Y_sup_7_Supplier_1 + Y_sup_7_Supplier_2 + Y_sup_7_Supplier_3
+ + Y_sup_7_Supplier_4 + Y_sup_7_Supplier_5 = 1
+SupCntLB_0: Y_sup_0_Supplier_1 + Y_sup_0_Supplier_2 + Y_sup_0_Supplier_3
+ + Y_sup_0_Supplier_4 + Y_sup_0_Supplier_5 &gt;= 2
 TrLB_1_Supplier_1: x_Supplier_1_1 &gt;= 0
 TrLB_1_Supplier_3: x_Supplier_3_1 &gt;= 0
 TrLB_1_Supplier_4: x_Supplier_4_1 &gt;= 0
@@ -1124,70 +1209,94 @@
 TrUB_5_Supplier_2: - 2421 T_5_Supplier_2 + x_Supplier_2_5 &lt;= 0
 TrUB_5_Supplier_4: - 2421 T_5_Supplier_4 + x_Supplier_4_5 &lt;= 0
 TrUB_5_Supplier_5: - 2421 T_5_Supplier_5 + x_Supplier_5_5 &lt;= 0
-Ylb_0_Supplier_1: - 1e-06 Y_sup_0_Supplier_1 + x_Supplier_1_1 &gt;= 0
-Ylb_0_Supplier_2: - 1e-06 Y_sup_0_Supplier_2 + x_Supplier_2_1 &gt;= 0
-Ylb_0_Supplier_3: - 1e-06 Y_sup_0_Supplier_3 + x_Supplier_3_1 &gt;= 0
-Ylb_0_Supplier_4: - 1e-06 Y_sup_0_Supplier_4 + x_Supplier_4_1 &gt;= 0
-Ylb_0_Supplier_5: - 1e-06 Y_sup_0_Supplier_5 + x_Supplier_5_1 &gt;= 0
-Ylb_1_Supplier_1: - 1e-06 Y_sup_1_Supplier_1 + x_Supplier_1_2 &gt;= 0
-Ylb_1_Supplier_2: - 1e-06 Y_sup_1_Supplier_2 + x_Supplier_2_2 &gt;= 0
-Ylb_1_Supplier_3: - 1e-06 Y_sup_1_Supplier_3 + x_Supplier_3_2 &gt;= 0
-Ylb_1_Supplier_4: - 1e-06 Y_sup_1_Supplier_4 + x_Supplier_4_2 &gt;= 0
-Ylb_1_Supplier_5: - 1e-06 Y_sup_1_Supplier_5 + x_Supplier_5_2 &gt;= 0
-Ylb_2_Supplier_1: - 1e-06 Y_sup_2_Supplier_1 + x_Supplier_1_3 &gt;= 0
-Ylb_2_Supplier_2: - 1e-06 Y_sup_2_Supplier_2 + x_Supplier_2_3 &gt;= 0
-Ylb_2_Supplier_3: - 1e-06 Y_sup_2_Supplier_3 + x_Supplier_3_3 &gt;= 0
-Ylb_2_Supplier_4: - 1e-06 Y_sup_2_Supplier_4 + x_Supplier_4_3 &gt;= 0
-Ylb_2_Supplier_5: - 1e-06 Y_sup_2_Supplier_5 + x_Supplier_5_3 &gt;= 0
-Ylb_3_Supplier_1: - 1e-06 Y_sup_3_Supplier_1 + x_Supplier_1_4 &gt;= 0
-Ylb_3_Supplier_2: - 1e-06 Y_sup_3_Supplier_2 + x_Supplier_2_4 &gt;= 0
-Ylb_3_Supplier_3: - 1e-06 Y_sup_3_Supplier_3 + x_Supplier_3_4 &gt;= 0
-Ylb_3_Supplier_4: - 1e-06 Y_sup_3_Supplier_4 + x_Supplier_4_4 &gt;= 0
-Ylb_3_Supplier_5: - 1e-06 Y_sup_3_Supplier_5 + x_Supplier_5_4 &gt;= 0
-Ylb_4_Supplier_1: - 1e-06 Y_sup_4_Supplier_1 + x_Supplier_1_5 &gt;= 0
-Ylb_4_Supplier_2: - 1e-06 Y_sup_4_Supplier_2 + x_Supplier_2_5 &gt;= 0
-Ylb_4_Supplier_3: - 1e-06 Y_sup_4_Supplier_3 + x_Supplier_3_5 &gt;= 0
-Ylb_4_Supplier_4: - 1e-06 Y_sup_4_Supplier_4 + x_Supplier_4_5 &gt;= 0
-Ylb_4_Supplier_5: - 1e-06 Y_sup_4_Supplier_5 + x_Supplier_5_5 &gt;= 0
-Yub_0_Supplier_1: - 1000000000 Y_sup_0_Supplier_1 + x_Supplier_1_1 &lt;= 0
-Yub_0_Supplier_2: - 1000000000 Y_sup_0_Supplier_2 + x_Supplier_2_1 &lt;= 0
-Yub_0_Supplier_3: - 1000000000 Y_sup_0_Supplier_3 + x_Supplier_3_1 &lt;= 0
-Yub_0_Supplier_4: - 1000000000 Y_sup_0_Supplier_4 + x_Supplier_4_1 &lt;= 0
-Yub_0_Supplier_5: - 1000000000 Y_sup_0_Supplier_5 + x_Supplier_5_1 &lt;= 0
-Yub_1_Supplier_1: - 1000000000 Y_sup_1_Supplier_1 + x_Supplier_1_2 &lt;= 0
-Yub_1_Supplier_2: - 1000000000 Y_sup_1_Supplier_2 + x_Supplier_2_2 &lt;= 0
-Yub_1_Supplier_3: - 1000000000 Y_sup_1_Supplier_3 + x_Supplier_3_2 &lt;= 0
-Yub_1_Supplier_4: - 1000000000 Y_sup_1_Supplier_4 + x_Supplier_4_2 &lt;= 0
-Yub_1_Supplier_5: - 1000000000 Y_sup_1_Supplier_5 + x_Supplier_5_2 &lt;= 0
-Yub_2_Supplier_1: - 1000000000 Y_sup_2_Supplier_1 + x_Supplier_1_3 &lt;= 0
-Yub_2_Supplier_2: - 1000000000 Y_sup_2_Supplier_2 + x_Supplier_2_3 &lt;= 0
-Yub_2_Supplier_3: - 1000000000 Y_sup_2_Supplier_3 + x_Supplier_3_3 &lt;= 0
-Yub_2_Supplier_4: - 1000000000 Y_sup_2_Supplier_4 + x_Supplier_4_3 &lt;= 0
-Yub_2_Supplier_5: - 1000000000 Y_sup_2_Supplier_5 + x_Supplier_5_3 &lt;= 0
-Yub_3_Supplier_1: - 1000000000 Y_sup_3_Supplier_1 + x_Supplier_1_4 &lt;= 0
-Yub_3_Supplier_2: - 1000000000 Y_sup_3_Supplier_2 + x_Supplier_2_4 &lt;= 0
-Yub_3_Supplier_3: - 1000000000 Y_sup_3_Supplier_3 + x_Supplier_3_4 &lt;= 0
-Yub_3_Supplier_4: - 1000000000 Y_sup_3_Supplier_4 + x_Supplier_4_4 &lt;= 0
-Yub_3_Supplier_5: - 1000000000 Y_sup_3_Supplier_5 + x_Supplier_5_4 &lt;= 0
-Yub_4_Supplier_1: - 1000000000 Y_sup_4_Supplier_1 + x_Supplier_1_5 &lt;= 0
-Yub_4_Supplier_2: - 1000000000 Y_sup_4_Supplier_2 + x_Supplier_2_5 &lt;= 0
-Yub_4_Supplier_3: - 1000000000 Y_sup_4_Supplier_3 + x_Supplier_3_5 &lt;= 0
-Yub_4_Supplier_4: - 1000000000 Y_sup_4_Supplier_4 + x_Supplier_4_5 &lt;= 0
-Yub_4_Supplier_5: - 1000000000 Y_sup_4_Supplier_5 + x_Supplier_5_5 &lt;= 0
-dLow_Supplier_1_0: - 0.95 S0_Supplier_1 + d_Supplier_1
+Ylb_0_Supplier_1: - 1e-06 Y_sup_0_Supplier_1 + x_Supplier_1_1 + x_Supplier_1_2
+ + x_Supplier_1_3 + x_Supplier_1_4 + x_Supplier_1_5 &gt;= 0
+Ylb_0_Supplier_2: - 1e-06 Y_sup_0_Supplier_2 + x_Supplier_2_1 + x_Supplier_2_2
+ + x_Supplier_2_3 + x_Supplier_2_4 + x_Supplier_2_5 &gt;= 0
+Ylb_0_Supplier_3: - 1e-06 Y_sup_0_Supplier_3 + x_Supplier_3_1 + x_Supplier_3_2
+ + x_Supplier_3_3 + x_Supplier_3_4 + x_Supplier_3_5 &gt;= 0
+Ylb_0_Supplier_4: - 1e-06 Y_sup_0_Supplier_4 + x_Supplier_4_1 + x_Supplier_4_2
+ + x_Supplier_4_3 + x_Supplier_4_4 + x_Supplier_4_5 &gt;= 0
+Ylb_0_Supplier_5: - 1e-06 Y_sup_0_Supplier_5 + x_Supplier_5_1 + x_Supplier_5_2
+ + x_Supplier_5_3 + x_Supplier_5_4 + x_Supplier_5_5 &gt;= 0
+Ylb_3_Supplier_1: - 1e-06 Y_sup_3_Supplier_1 + x_Supplier_1_1 &gt;= 0
+Ylb_3_Supplier_2: - 1e-06 Y_sup_3_Supplier_2 + x_Supplier_2_1 &gt;= 0
+Ylb_3_Supplier_3: - 1e-06 Y_sup_3_Supplier_3 + x_Supplier_3_1 &gt;= 0
+Ylb_3_Supplier_4: - 1e-06 Y_sup_3_Supplier_4 + x_Supplier_4_1 &gt;= 0
+Ylb_3_Supplier_5: - 1e-06 Y_sup_3_Supplier_5 + x_Supplier_5_1 &gt;= 0
+Ylb_4_Supplier_1: - 1e-06 Y_sup_4_Supplier_1 + x_Supplier_1_2 &gt;= 0
+Ylb_4_Supplier_2: - 1e-06 Y_sup_4_Supplier_2 + x_Supplier_2_2 &gt;= 0
+Ylb_4_Supplier_3: - 1e-06 Y_sup_4_Supplier_3 + x_Supplier_3_2 &gt;= 0
+Ylb_4_Supplier_4: - 1e-06 Y_sup_4_Supplier_4 + x_Supplier_4_2 &gt;= 0
+Ylb_4_Supplier_5: - 1e-06 Y_sup_4_Supplier_5 + x_Supplier_5_2 &gt;= 0
+Ylb_5_Supplier_1: - 1e-06 Y_sup_5_Supplier_1 + x_Supplier_1_3 &gt;= 0
+Ylb_5_Supplier_2: - 1e-06 Y_sup_5_Supplier_2 + x_Supplier_2_3 &gt;= 0
+Ylb_5_Supplier_3: - 1e-06 Y_sup_5_Supplier_3 + x_Supplier_3_3 &gt;= 0
+Ylb_5_Supplier_4: - 1e-06 Y_sup_5_Supplier_4 + x_Supplier_4_3 &gt;= 0
+Ylb_5_Supplier_5: - 1e-06 Y_sup_5_Supplier_5 + x_Supplier_5_3 &gt;= 0
+Ylb_6_Supplier_1: - 1e-06 Y_sup_6_Supplier_1 + x_Supplier_1_4 &gt;= 0
+Ylb_6_Supplier_2: - 1e-06 Y_sup_6_Supplier_2 + x_Supplier_2_4 &gt;= 0
+Ylb_6_Supplier_3: - 1e-06 Y_sup_6_Supplier_3 + x_Supplier_3_4 &gt;= 0
+Ylb_6_Supplier_4: - 1e-06 Y_sup_6_Supplier_4 + x_Supplier_4_4 &gt;= 0
+Ylb_6_Supplier_5: - 1e-06 Y_sup_6_Supplier_5 + x_Supplier_5_4 &gt;= 0
+Ylb_7_Supplier_1: - 1e-06 Y_sup_7_Supplier_1 + x_Supplier_1_5 &gt;= 0
+Ylb_7_Supplier_2: - 1e-06 Y_sup_7_Supplier_2 + x_Supplier_2_5 &gt;= 0
+Ylb_7_Supplier_3: - 1e-06 Y_sup_7_Supplier_3 + x_Supplier_3_5 &gt;= 0
+Ylb_7_Supplier_4: - 1e-06 Y_sup_7_Supplier_4 + x_Supplier_4_5 &gt;= 0
+Ylb_7_Supplier_5: - 1e-06 Y_sup_7_Supplier_5 + x_Supplier_5_5 &gt;= 0
+Yub_0_Supplier_1: - 1000000000 Y_sup_0_Supplier_1 + x_Supplier_1_1
+ + x_Supplier_1_2 + x_Supplier_1_3 + x_Supplier_1_4 + x_Supplier_1_5 &lt;= 0
+Yub_0_Supplier_2: - 1000000000 Y_sup_0_Supplier_2 + x_Supplier_2_1
+ + x_Supplier_2_2 + x_Supplier_2_3 + x_Supplier_2_4 + x_Supplier_2_5 &lt;= 0
+Yub_0_Supplier_3: - 1000000000 Y_sup_0_Supplier_3 + x_Supplier_3_1
+ + x_Supplier_3_2 + x_Supplier_3_3 + x_Supplier_3_4 + x_Supplier_3_5 &lt;= 0
+Yub_0_Supplier_4: - 1000000000 Y_sup_0_Supplier_4 + x_Supplier_4_1
+ + x_Supplier_4_2 + x_Supplier_4_3 + x_Supplier_4_4 + x_Supplier_4_5 &lt;= 0
+Yub_0_Supplier_5: - 1000000000 Y_sup_0_Supplier_5 + x_Supplier_5_1
+ + x_Supplier_5_2 + x_Supplier_5_3 + x_Supplier_5_4 + x_Supplier_5_5 &lt;= 0
+Yub_3_Supplier_1: - 1000000000 Y_sup_3_Supplier_1 + x_Supplier_1_1 &lt;= 0
+Yub_3_Supplier_2: - 1000000000 Y_sup_3_Supplier_2 + x_Supplier_2_1 &lt;= 0
+Yub_3_Supplier_3: - 1000000000 Y_sup_3_Supplier_3 + x_Supplier_3_1 &lt;= 0
+Yub_3_Supplier_4: - 1000000000 Y_sup_3_Supplier_4 + x_Supplier_4_1 &lt;= 0
+Yub_3_Supplier_5: - 1000000000 Y_sup_3_Supplier_5 + x_Supplier_5_1 &lt;= 0
+Yub_4_Supplier_1: - 1000000000 Y_sup_4_Supplier_1 + x_Supplier_1_2 &lt;= 0
+Yub_4_Supplier_2: - 1000000000 Y_sup_4_Supplier_2 + x_Supplier_2_2 &lt;= 0
+Yub_4_Supplier_3: - 1000000000 Y_sup_4_Supplier_3 + x_Supplier_3_2 &lt;= 0
+Yub_4_Supplier_4: - 1000000000 Y_sup_4_Supplier_4 + x_Supplier_4_2 &lt;= 0
+Yub_4_Supplier_5: - 1000000000 Y_sup_4_Supplier_5 + x_Supplier_5_2 &lt;= 0
+Yub_5_Supplier_1: - 1000000000 Y_sup_5_Supplier_1 + x_Supplier_1_3 &lt;= 0
+Yub_5_Supplier_2: - 1000000000 Y_sup_5_Supplier_2 + x_Supplier_2_3 &lt;= 0
+Yub_5_Supplier_3: - 1000000000 Y_sup_5_Supplier_3 + x_Supplier_3_3 &lt;= 0
+Yub_5_Supplier_4: - 1000000000 Y_sup_5_Supplier_4 + x_Supplier_4_3 &lt;= 0
+Yub_5_Supplier_5: - 1000000000 Y_sup_5_Supplier_5 + x_Supplier_5_3 &lt;= 0
+Yub_6_Supplier_1: - 1000000000 Y_sup_6_Supplier_1 + x_Supplier_1_4 &lt;= 0
+Yub_6_Supplier_2: - 1000000000 Y_sup_6_Supplier_2 + x_Supplier_2_4 &lt;= 0
+Yub_6_Supplier_3: - 1000000000 Y_sup_6_Supplier_3 + x_Supplier_3_4 &lt;= 0
+Yub_6_Supplier_4: - 1000000000 Y_sup_6_Supplier_4 + x_Supplier_4_4 &lt;= 0
+Yub_6_Supplier_5: - 1000000000 Y_sup_6_Supplier_5 + x_Supplier_5_4 &lt;= 0
+Yub_7_Supplier_1: - 1000000000 Y_sup_7_Supplier_1 + x_Supplier_1_5 &lt;= 0
+Yub_7_Supplier_2: - 1000000000 Y_sup_7_Supplier_2 + x_Supplier_2_5 &lt;= 0
+Yub_7_Supplier_3: - 1000000000 Y_sup_7_Supplier_3 + x_Supplier_3_5 &lt;= 0
+Yub_7_Supplier_4: - 1000000000 Y_sup_7_Supplier_4 + x_Supplier_4_5 &lt;= 0
+Yub_7_Supplier_5: - 1000000000 Y_sup_7_Supplier_5 + x_Supplier_5_5 &lt;= 0
+dLow_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1
  - 1406346 zd_Supplier_1_0 &gt;= -1406346
-dUp_Supplier_1_0: - 0.95 S0_Supplier_1 + d_Supplier_1
+dUp_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1
  + 1406346 zd_Supplier_1_0 &lt;= 1406346
 dZeroNoTier_Supplier_2: d_Supplier_2 = 0
 dZeroNoTier_Supplier_3: d_Supplier_3 = 0
 dZeroNoTier_Supplier_4: d_Supplier_4 = 0
 dZeroNoTier_Supplier_5: d_Supplier_5 = 0
 dZero_Supplier_1: d_Supplier_1 - 1406346 zd_Supplier_1_0 &lt;= 0
-rZeroNoTier_Supplier_1: reb_Supplier_1 = 0
+rLow_Supplier_1_0: - 0.95 S_Supplier_1 + reb_Supplier_1
+ - 1406346 yr_Supplier_1_0 &gt;= -1406346
+rUp_Supplier_1_0: - 0.95 S_Supplier_1 + reb_Supplier_1
+ + 1406346 yr_Supplier_1_0 &lt;= 1406346
 rZeroNoTier_Supplier_2: reb_Supplier_2 = 0
 rZeroNoTier_Supplier_3: reb_Supplier_3 = 0
 rZeroNoTier_Supplier_4: reb_Supplier_4 = 0
 rZeroNoTier_Supplier_5: reb_Supplier_5 = 0
+rZero_Supplier_1: reb_Supplier_1 - 1406346 yr_Supplier_1_0 &lt;= 0
 Binaries
 T_1_Supplier_1
 T_1_Supplier_3
@@ -1214,16 +1323,6 @@
 Y_sup_0_Supplier_3
 Y_sup_0_Supplier_4
 Y_sup_0_Supplier_5
-Y_sup_1_Supplier_1
-Y_sup_1_Supplier_2
-Y_sup_1_Supplier_3
-Y_sup_1_Supplier_4
-Y_sup_1_Supplier_5
-Y_sup_2_Supplier_1
-Y_sup_2_Supplier_2
-Y_sup_2_Supplier_3
-Y_sup_2_Supplier_4
-Y_sup_2_Supplier_5
 Y_sup_3_Supplier_1
 Y_sup_3_Supplier_2
 Y_sup_3_Supplier_3
@@ -1234,6 +1333,27 @@
 Y_sup_4_Supplier_3
 Y_sup_4_Supplier_4
 Y_sup_4_Supplier_5
+Y_sup_5_Supplier_1
+Y_sup_5_Supplier_2
+Y_sup_5_Supplier_3
+Y_sup_5_Supplier_4
+Y_sup_5_Supplier_5
+Y_sup_6_Supplier_1
+Y_sup_6_Supplier_2
+Y_sup_6_Supplier_3
+Y_sup_6_Supplier_4
+Y_sup_6_Supplier_5
+Y_sup_7_Supplier_1
+Y_sup_7_Supplier_2
+Y_sup_7_Supplier_3
+Y_sup_7_Supplier_4
+Y_sup_7_Supplier_5
+y_1_Supplier_1
+y_1_Supplier_2
+y_1_Supplier_3
+y_1_Supplier_4
+y_1_Supplier_5
+yr_Supplier_1_0
 z_Supplier_1
 z_Supplier_2
 z_Supplier_3

</xml_diff>

<commit_message>
Added Sceario Summary to Powerpoint output for Optimization
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -561,57 +561,57 @@
         <v>25</v>
       </c>
       <c r="F2" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>36400</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>14</v>
+        <v>33.32</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>GP Pickup (KBX)</t>
+          <t>DDP</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2" t="n">
-        <v>15</v>
+        <v>35.32</v>
       </c>
       <c r="O2" t="n">
-        <v>21840</v>
+        <v>51425.92</v>
       </c>
       <c r="P2" t="n">
         <v>1456</v>
       </c>
       <c r="Q2" t="n">
-        <v>14560</v>
+        <v>-15025.92</v>
       </c>
       <c r="R2" t="n">
-        <v>13104</v>
+        <v>-49969.92</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>48854.624</v>
       </c>
     </row>
     <row r="3">
@@ -637,57 +637,57 @@
         <v>36</v>
       </c>
       <c r="F3" t="n">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>87156</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Supplier 3</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>25</v>
+        <v>14.7</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>GP Pickup (KBX)</t>
+          <t>DDP</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3" t="n">
-        <v>26</v>
+        <v>16.7</v>
       </c>
       <c r="O3" t="n">
-        <v>62946</v>
+        <v>40430.7</v>
       </c>
       <c r="P3" t="n">
         <v>2421</v>
       </c>
       <c r="Q3" t="n">
-        <v>24210</v>
+        <v>46725.3</v>
       </c>
       <c r="R3" t="n">
-        <v>89577</v>
+        <v>-38009.7</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>38409.16499999999</v>
       </c>
     </row>
     <row r="4">
@@ -713,57 +713,57 @@
         <v>82</v>
       </c>
       <c r="F4" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
         <v>529884</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Supplier 2</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>78</v>
+        <v>14.7</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>GP Pickup (KBX)</t>
+          <t>DDP</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4" t="n">
-        <v>79</v>
+        <v>16.7</v>
       </c>
       <c r="O4" t="n">
-        <v>510498</v>
+        <v>107915.4</v>
       </c>
       <c r="P4" t="n">
         <v>6462</v>
       </c>
       <c r="Q4" t="n">
-        <v>19386</v>
+        <v>421968.6</v>
       </c>
       <c r="R4" t="n">
-        <v>-361872</v>
+        <v>-101453.4</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>102519.63</v>
       </c>
     </row>
     <row r="5">
@@ -789,7 +789,7 @@
         <v>32</v>
       </c>
       <c r="F5" t="n">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>75424</v>
@@ -831,7 +831,7 @@
         <v>-102529.5</v>
       </c>
       <c r="R5" t="n">
-        <v>-29462.5</v>
+        <v>-175596.5</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
@@ -865,57 +865,57 @@
         <v>75</v>
       </c>
       <c r="F6" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
         <v>181575</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Supplier 3</t>
+          <t>Supplier 1</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>87</v>
+        <v>23.52</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>GP Pickup (KBX)</t>
+          <t>DDP</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6" t="n">
-        <v>88</v>
+        <v>25.52</v>
       </c>
       <c r="O6" t="n">
-        <v>213048</v>
+        <v>61783.92</v>
       </c>
       <c r="P6" t="n">
         <v>2421</v>
       </c>
       <c r="Q6" t="n">
-        <v>-31473</v>
+        <v>119791.08</v>
       </c>
       <c r="R6" t="n">
-        <v>-183996</v>
+        <v>-59362.92</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>58694.72399999999</v>
       </c>
     </row>
   </sheetData>
@@ -1204,20 +1204,6 @@
  + x_Supplier_5_4 + x_Supplier_5_5 - z_Supplier_5 &gt;= 0
 OneDisc_Supplier_1: - z_Supplier_1 + zd_Supplier_1_0 = 0
 OneReb_Supplier_1: yr_Supplier_1_0 - z_Supplier_1 = 0
-PctAggEQLB_0: - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
- + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1 - x_Supplier_2_2
- + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 - x_Supplier_3_1
- + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4 + 0 x_Supplier_3_5
- - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3 - x_Supplier_4_4
- - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
- - x_Supplier_5_4 - x_Supplier_5_5 &gt;= 0
-PctAggEQUB_0: - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
- + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1 - x_Supplier_2_2
- + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 - x_Supplier_3_1
- + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4 + 0 x_Supplier_3_5
- - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3 - x_Supplier_4_4
- - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
- - x_Supplier_5_4 - x_Supplier_5_5 &lt;= 0
 RMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
  + x_Supplier_1_4 + x_Supplier_1_5 + 1000000000 yr_Supplier_1_0 &lt;= 1001000000
 RMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
@@ -1247,6 +1233,8 @@
 Spend_Supplier_3: - S0_Supplier_3 + S_Supplier_3 + d_Supplier_3 = 0
 Spend_Supplier_4: - S0_Supplier_4 + S_Supplier_4 + d_Supplier_4 = 0
 Spend_Supplier_5: - S0_Supplier_5 + S_Supplier_5 + d_Supplier_5 = 0
+SupCntUB_0: Y_sup_0_Supplier_1 + Y_sup_0_Supplier_2 + Y_sup_0_Supplier_3
+ + Y_sup_0_Supplier_4 + Y_sup_0_Supplier_5 &lt;= 2
 TrLB_1_Supplier_1: x_Supplier_1_1 &gt;= 0
 TrLB_1_Supplier_3: x_Supplier_3_1 &gt;= 0
 TrLB_1_Supplier_4: x_Supplier_4_1 &gt;= 0
@@ -1287,6 +1275,26 @@
 TrUB_5_Supplier_2: - 2421 T_5_Supplier_2 + x_Supplier_2_5 &lt;= 0
 TrUB_5_Supplier_4: - 2421 T_5_Supplier_4 + x_Supplier_4_5 &lt;= 0
 TrUB_5_Supplier_5: - 2421 T_5_Supplier_5 + x_Supplier_5_5 &lt;= 0
+Ylb_0_Supplier_1: - 1e-06 Y_sup_0_Supplier_1 + x_Supplier_1_1 + x_Supplier_1_2
+ + x_Supplier_1_3 + x_Supplier_1_4 + x_Supplier_1_5 &gt;= 0
+Ylb_0_Supplier_2: - 1e-06 Y_sup_0_Supplier_2 + x_Supplier_2_1 + x_Supplier_2_2
+ + x_Supplier_2_3 + x_Supplier_2_4 + x_Supplier_2_5 &gt;= 0
+Ylb_0_Supplier_3: - 1e-06 Y_sup_0_Supplier_3 + x_Supplier_3_1 + x_Supplier_3_2
+ + x_Supplier_3_3 + x_Supplier_3_4 + x_Supplier_3_5 &gt;= 0
+Ylb_0_Supplier_4: - 1e-06 Y_sup_0_Supplier_4 + x_Supplier_4_1 + x_Supplier_4_2
+ + x_Supplier_4_3 + x_Supplier_4_4 + x_Supplier_4_5 &gt;= 0
+Ylb_0_Supplier_5: - 1e-06 Y_sup_0_Supplier_5 + x_Supplier_5_1 + x_Supplier_5_2
+ + x_Supplier_5_3 + x_Supplier_5_4 + x_Supplier_5_5 &gt;= 0
+Yub_0_Supplier_1: - 1000000000 Y_sup_0_Supplier_1 + x_Supplier_1_1
+ + x_Supplier_1_2 + x_Supplier_1_3 + x_Supplier_1_4 + x_Supplier_1_5 &lt;= 0
+Yub_0_Supplier_2: - 1000000000 Y_sup_0_Supplier_2 + x_Supplier_2_1
+ + x_Supplier_2_2 + x_Supplier_2_3 + x_Supplier_2_4 + x_Supplier_2_5 &lt;= 0
+Yub_0_Supplier_3: - 1000000000 Y_sup_0_Supplier_3 + x_Supplier_3_1
+ + x_Supplier_3_2 + x_Supplier_3_3 + x_Supplier_3_4 + x_Supplier_3_5 &lt;= 0
+Yub_0_Supplier_4: - 1000000000 Y_sup_0_Supplier_4 + x_Supplier_4_1
+ + x_Supplier_4_2 + x_Supplier_4_3 + x_Supplier_4_4 + x_Supplier_4_5 &lt;= 0
+Yub_0_Supplier_5: - 1000000000 Y_sup_0_Supplier_5 + x_Supplier_5_1
+ + x_Supplier_5_2 + x_Supplier_5_3 + x_Supplier_5_4 + x_Supplier_5_5 &lt;= 0
 dLow_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1
  - 1406346 zd_Supplier_1_0 &gt;= -1406346
 dUp_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1
@@ -1326,6 +1334,11 @@
 T_5_Supplier_2
 T_5_Supplier_4
 T_5_Supplier_5
+Y_sup_0_Supplier_1
+Y_sup_0_Supplier_2
+Y_sup_0_Supplier_3
+Y_sup_0_Supplier_4
+Y_sup_0_Supplier_5
 bDDP_Supplier_1_1
 bDDP_Supplier_1_2
 bDDP_Supplier_1_3

</xml_diff>

<commit_message>
may 19 updates still not working
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -568,50 +568,50 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>33.32</v>
+        <v>14</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>DDP</t>
+          <t>GP Pickup (KBX)</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>35.32</v>
+        <v>15</v>
       </c>
       <c r="O2" t="n">
-        <v>51425.92</v>
+        <v>21840</v>
       </c>
       <c r="P2" t="n">
         <v>1456</v>
       </c>
       <c r="Q2" t="n">
-        <v>-15025.92</v>
+        <v>14560</v>
       </c>
       <c r="R2" t="n">
-        <v>-49969.92</v>
+        <v>-20384</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>48854.624</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -644,50 +644,50 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>14.7</v>
+        <v>25</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>DDP</t>
+          <t>GP Pickup (KBX)</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>16.7</v>
+        <v>26</v>
       </c>
       <c r="O3" t="n">
-        <v>40430.7</v>
+        <v>62946</v>
       </c>
       <c r="P3" t="n">
         <v>2421</v>
       </c>
       <c r="Q3" t="n">
-        <v>46725.3</v>
+        <v>24210</v>
       </c>
       <c r="R3" t="n">
-        <v>-38009.7</v>
+        <v>-60525</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>38409.16499999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -720,50 +720,50 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>14.7</v>
+        <v>78</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>DDP</t>
+          <t>GP Pickup (KBX)</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>16.7</v>
+        <v>79</v>
       </c>
       <c r="O4" t="n">
-        <v>107915.4</v>
+        <v>510498</v>
       </c>
       <c r="P4" t="n">
         <v>6462</v>
       </c>
       <c r="Q4" t="n">
-        <v>421968.6</v>
+        <v>19386</v>
       </c>
       <c r="R4" t="n">
-        <v>-101453.4</v>
+        <v>-504036</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>102519.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -872,50 +872,50 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 3</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>23.52</v>
+        <v>87</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>DDP</t>
+          <t>GP Pickup (KBX)</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
-        <v>25.52</v>
+        <v>88</v>
       </c>
       <c r="O6" t="n">
-        <v>61783.92</v>
+        <v>213048</v>
       </c>
       <c r="P6" t="n">
         <v>2421</v>
       </c>
       <c r="Q6" t="n">
-        <v>119791.08</v>
+        <v>-31473</v>
       </c>
       <c r="R6" t="n">
-        <v>-59362.92</v>
+        <v>-210627</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>58694.72399999999</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1204,6 +1204,20 @@
  + x_Supplier_5_4 + x_Supplier_5_5 - z_Supplier_5 &gt;= 0
 OneDisc_Supplier_1: - z_Supplier_1 + zd_Supplier_1_0 = 0
 OneReb_Supplier_1: yr_Supplier_1_0 - z_Supplier_1 = 0
+PctAggEQLB_0: - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
+ + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1 - x_Supplier_2_2
+ + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 - x_Supplier_3_1
+ + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4 + 0 x_Supplier_3_5
+ - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3 - x_Supplier_4_4
+ - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
+ - x_Supplier_5_4 - x_Supplier_5_5 &gt;= 0
+PctAggEQUB_0: - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
+ + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1 - x_Supplier_2_2
+ + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 - x_Supplier_3_1
+ + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4 + 0 x_Supplier_3_5
+ - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3 - x_Supplier_4_4
+ - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
+ - x_Supplier_5_4 - x_Supplier_5_5 &lt;= 0
 RMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
  + x_Supplier_1_4 + x_Supplier_1_5 + 1000000000 yr_Supplier_1_0 &lt;= 1001000000
 RMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
@@ -1233,8 +1247,6 @@
 Spend_Supplier_3: - S0_Supplier_3 + S_Supplier_3 + d_Supplier_3 = 0
 Spend_Supplier_4: - S0_Supplier_4 + S_Supplier_4 + d_Supplier_4 = 0
 Spend_Supplier_5: - S0_Supplier_5 + S_Supplier_5 + d_Supplier_5 = 0
-SupCntUB_0: Y_sup_0_Supplier_1 + Y_sup_0_Supplier_2 + Y_sup_0_Supplier_3
- + Y_sup_0_Supplier_4 + Y_sup_0_Supplier_5 &lt;= 2
 TrLB_1_Supplier_1: x_Supplier_1_1 &gt;= 0
 TrLB_1_Supplier_3: x_Supplier_3_1 &gt;= 0
 TrLB_1_Supplier_4: x_Supplier_4_1 &gt;= 0
@@ -1275,26 +1287,6 @@
 TrUB_5_Supplier_2: - 2421 T_5_Supplier_2 + x_Supplier_2_5 &lt;= 0
 TrUB_5_Supplier_4: - 2421 T_5_Supplier_4 + x_Supplier_4_5 &lt;= 0
 TrUB_5_Supplier_5: - 2421 T_5_Supplier_5 + x_Supplier_5_5 &lt;= 0
-Ylb_0_Supplier_1: - 1e-06 Y_sup_0_Supplier_1 + x_Supplier_1_1 + x_Supplier_1_2
- + x_Supplier_1_3 + x_Supplier_1_4 + x_Supplier_1_5 &gt;= 0
-Ylb_0_Supplier_2: - 1e-06 Y_sup_0_Supplier_2 + x_Supplier_2_1 + x_Supplier_2_2
- + x_Supplier_2_3 + x_Supplier_2_4 + x_Supplier_2_5 &gt;= 0
-Ylb_0_Supplier_3: - 1e-06 Y_sup_0_Supplier_3 + x_Supplier_3_1 + x_Supplier_3_2
- + x_Supplier_3_3 + x_Supplier_3_4 + x_Supplier_3_5 &gt;= 0
-Ylb_0_Supplier_4: - 1e-06 Y_sup_0_Supplier_4 + x_Supplier_4_1 + x_Supplier_4_2
- + x_Supplier_4_3 + x_Supplier_4_4 + x_Supplier_4_5 &gt;= 0
-Ylb_0_Supplier_5: - 1e-06 Y_sup_0_Supplier_5 + x_Supplier_5_1 + x_Supplier_5_2
- + x_Supplier_5_3 + x_Supplier_5_4 + x_Supplier_5_5 &gt;= 0
-Yub_0_Supplier_1: - 1000000000 Y_sup_0_Supplier_1 + x_Supplier_1_1
- + x_Supplier_1_2 + x_Supplier_1_3 + x_Supplier_1_4 + x_Supplier_1_5 &lt;= 0
-Yub_0_Supplier_2: - 1000000000 Y_sup_0_Supplier_2 + x_Supplier_2_1
- + x_Supplier_2_2 + x_Supplier_2_3 + x_Supplier_2_4 + x_Supplier_2_5 &lt;= 0
-Yub_0_Supplier_3: - 1000000000 Y_sup_0_Supplier_3 + x_Supplier_3_1
- + x_Supplier_3_2 + x_Supplier_3_3 + x_Supplier_3_4 + x_Supplier_3_5 &lt;= 0
-Yub_0_Supplier_4: - 1000000000 Y_sup_0_Supplier_4 + x_Supplier_4_1
- + x_Supplier_4_2 + x_Supplier_4_3 + x_Supplier_4_4 + x_Supplier_4_5 &lt;= 0
-Yub_0_Supplier_5: - 1000000000 Y_sup_0_Supplier_5 + x_Supplier_5_1
- + x_Supplier_5_2 + x_Supplier_5_3 + x_Supplier_5_4 + x_Supplier_5_5 &lt;= 0
 dLow_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1
  - 1406346 zd_Supplier_1_0 &gt;= -1406346
 dUp_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1
@@ -1334,11 +1326,6 @@
 T_5_Supplier_2
 T_5_Supplier_4
 T_5_Supplier_5
-Y_sup_0_Supplier_1
-Y_sup_0_Supplier_2
-Y_sup_0_Supplier_3
-Y_sup_0_Supplier_4
-Y_sup_0_Supplier_5
 bDDP_Supplier_1_1
 bDDP_Supplier_1_2
 bDDP_Supplier_1_3

</xml_diff>

<commit_message>
Final Optimization version without rebates included in presentation sumamry
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,19 +568,19 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Supplier 1</t>
+          <t>Supplier 2</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>33.32</v>
+        <v>14</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -588,30 +588,334 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>2</v>
+        <v>0.4996874378925605</v>
       </c>
       <c r="N2" t="n">
-        <v>35.32</v>
+        <v>14.49968743789256</v>
       </c>
       <c r="O2" t="n">
-        <v>51425.92</v>
+        <v>21111.54490957157</v>
       </c>
       <c r="P2" t="n">
         <v>1456</v>
       </c>
       <c r="Q2" t="n">
-        <v>-15025.92</v>
+        <v>15288.45509042843</v>
       </c>
       <c r="R2" t="n">
-        <v>-49969.92</v>
+        <v>-19655.54490957157</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Brunswick</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>36</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>87156</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>25</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>25</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>DDP</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>0.273169314994002</v>
+      </c>
+      <c r="N3" t="n">
+        <v>25.273169314994</v>
+      </c>
+      <c r="O3" t="n">
+        <v>61186.34291160048</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2421</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>25969.65708839952</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-58765.34291160048</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Palatka</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Supplier 2</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>82</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>529884</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Supplier 2</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>78</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>78</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>DDP</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>0.5839923450148741</v>
+      </c>
+      <c r="N4" t="n">
+        <v>78.58399234501488</v>
+      </c>
+      <c r="O4" t="n">
+        <v>507809.7585334862</v>
+      </c>
+      <c r="P4" t="n">
+        <v>6462</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>22074.24146651383</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-501347.7585334862</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Big Island</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>32</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>75424</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>75</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>DDP</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>0.3658246386205851</v>
+      </c>
+      <c r="N5" t="n">
+        <v>73.86582463862058</v>
+      </c>
+      <c r="O5" t="n">
+        <v>174101.7486732287</v>
+      </c>
+      <c r="P5" t="n">
+        <v>2357</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-98677.74867322872</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-171744.7486732287</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
           <t>95%</t>
         </is>
       </c>
-      <c r="T2" t="n">
-        <v>48854.624</v>
+      <c r="T5" t="n">
+        <v>165396.6612395673</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Huntsville</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>75</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>181575</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>87</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>87</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>DDP</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>0.06361691861653185</v>
+      </c>
+      <c r="N6" t="n">
+        <v>87.06361691861653</v>
+      </c>
+      <c r="O6" t="n">
+        <v>210781.0165599706</v>
+      </c>
+      <c r="P6" t="n">
+        <v>2421</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-29206.01655997062</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-208360.0165599706</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -678,43 +982,391 @@
         <is>
           <t xml:space="preserve">\* Sourcing_with_Freight *\
 Minimize
-OBJ: F_Supplier_1 + S_Supplier_1 - reb_Supplier_1
+OBJ: F_Supplier_1 + F_Supplier_2 + F_Supplier_3 + F_Supplier_4 + F_Supplier_5
+ + S_Supplier_1 + S_Supplier_2 + S_Supplier_3 + S_Supplier_4 + S_Supplier_5
+ - reb_Supplier_1 - reb_Supplier_2 - reb_Supplier_3 - reb_Supplier_4
+ - reb_Supplier_5
 Subject To
 Cap_Supplier_1_Bid_ID_1: x_Supplier_1_1 &lt;= 1457
+Cap_Supplier_1_Bid_ID_2: x_Supplier_1_2 &lt;= 2422
+Cap_Supplier_1_Bid_ID_3: x_Supplier_1_3 &lt;= 6463
+Cap_Supplier_1_Bid_ID_4: x_Supplier_1_4 &lt;= 2358
+Cap_Supplier_1_Bid_ID_5: x_Supplier_1_5 &lt;= 2422
+Cap_Supplier_2_Capacity_Group_Category_1: x_Supplier_2_1 + x_Supplier_2_3
+ + x_Supplier_2_4 &lt;= 8001
+Cap_Supplier_2_Capacity_Group_Category_2: x_Supplier_2_2 &lt;= 2501
+Cap_Supplier_2_Capacity_Group_Category_3: x_Supplier_2_5 &lt;= 501
+Cap_Supplier_3_Bid_ID_1: x_Supplier_3_1 &lt;= 1457
+Cap_Supplier_3_Bid_ID_2: x_Supplier_3_2 &lt;= 2422
+Cap_Supplier_3_Bid_ID_3: x_Supplier_3_3 &lt;= 6463
+Cap_Supplier_3_Bid_ID_4: x_Supplier_3_4 &lt;= 2358
+Cap_Supplier_3_Bid_ID_5: x_Supplier_3_5 &lt;= 2422
+Cap_Supplier_4_Bid_ID_1: x_Supplier_4_1 &lt;= 1457
+Cap_Supplier_4_Bid_ID_2: x_Supplier_4_2 &lt;= 2422
+Cap_Supplier_4_Bid_ID_3: x_Supplier_4_3 &lt;= 6463
+Cap_Supplier_4_Bid_ID_4: x_Supplier_4_4 &lt;= 2358
+Cap_Supplier_4_Bid_ID_5: x_Supplier_4_5 &lt;= 2422
+Cap_Supplier_5_Description_Large_Item: x_Supplier_5_5 &lt;= 5001
+Cap_Supplier_5_Description_Medium_item: x_Supplier_5_2 &lt;= 2501
+Cap_Supplier_5_Description_Small_item: x_Supplier_5_1 + x_Supplier_5_3
+ + x_Supplier_5_4 &lt;= 9001
 DDP_ON_Supplier_1_1: - 1000000000 bDDP_Supplier_1_1 + xSF_Supplier_1_1 &lt;= 0
-DMax_Supplier_1_0: x_Supplier_1_1 + 1000000000 zd_Supplier_1_0 &lt;= 1001000000
-DMin_Supplier_1_0: x_Supplier_1_1 - zd_Supplier_1_0 &gt;= 0
-Demand_1: x_Supplier_1_1 = 1456
-F_Supplier_1: F_Supplier_1 - xKBX_Supplier_1_1 = 0
+DDP_ON_Supplier_1_2: - 1000000000 bDDP_Supplier_1_2 + xSF_Supplier_1_2 &lt;= 0
+DDP_ON_Supplier_1_3: - 1000000000 bDDP_Supplier_1_3 + xSF_Supplier_1_3 &lt;= 0
+DDP_ON_Supplier_1_4: - 1000000000 bDDP_Supplier_1_4 + xSF_Supplier_1_4 &lt;= 0
+DDP_ON_Supplier_1_5: - 1000000000 bDDP_Supplier_1_5 + xSF_Supplier_1_5 &lt;= 0
+DDP_ON_Supplier_2_1: - 1000000000 bDDP_Supplier_2_1 + xSF_Supplier_2_1 &lt;= 0
+DDP_ON_Supplier_2_2: - 1000000000 bDDP_Supplier_2_2 + xSF_Supplier_2_2 &lt;= 0
+DDP_ON_Supplier_2_3: - 1000000000 bDDP_Supplier_2_3 + xSF_Supplier_2_3 &lt;= 0
+DDP_ON_Supplier_2_4: - 1000000000 bDDP_Supplier_2_4 + xSF_Supplier_2_4 &lt;= 0
+DDP_ON_Supplier_2_5: - 1000000000 bDDP_Supplier_2_5 + xSF_Supplier_2_5 &lt;= 0
+DDP_ON_Supplier_3_1: - 1000000000 bDDP_Supplier_3_1 + xSF_Supplier_3_1 &lt;= 0
+DDP_ON_Supplier_3_2: - 1000000000 bDDP_Supplier_3_2 + xSF_Supplier_3_2 &lt;= 0
+DDP_ON_Supplier_3_3: - 1000000000 bDDP_Supplier_3_3 + xSF_Supplier_3_3 &lt;= 0
+DDP_ON_Supplier_3_4: - 1000000000 bDDP_Supplier_3_4 + xSF_Supplier_3_4 &lt;= 0
+DDP_ON_Supplier_3_5: - 1000000000 bDDP_Supplier_3_5 + xSF_Supplier_3_5 &lt;= 0
+DDP_ON_Supplier_4_1: - 1000000000 bDDP_Supplier_4_1 + xSF_Supplier_4_1 &lt;= 0
+DDP_ON_Supplier_4_2: - 1000000000 bDDP_Supplier_4_2 + xSF_Supplier_4_2 &lt;= 0
+DDP_ON_Supplier_4_3: - 1000000000 bDDP_Supplier_4_3 + xSF_Supplier_4_3 &lt;= 0
+DDP_ON_Supplier_4_4: - 1000000000 bDDP_Supplier_4_4 + xSF_Supplier_4_4 &lt;= 0
+DDP_ON_Supplier_4_5: - 1000000000 bDDP_Supplier_4_5 + xSF_Supplier_4_5 &lt;= 0
+DDP_ON_Supplier_5_1: - 1000000000 bDDP_Supplier_5_1 + xSF_Supplier_5_1 &lt;= 0
+DDP_ON_Supplier_5_2: - 1000000000 bDDP_Supplier_5_2 + xSF_Supplier_5_2 &lt;= 0
+DDP_ON_Supplier_5_3: - 1000000000 bDDP_Supplier_5_3 + xSF_Supplier_5_3 &lt;= 0
+DDP_ON_Supplier_5_4: - 1000000000 bDDP_Supplier_5_4 + xSF_Supplier_5_4 &lt;= 0
+DDP_ON_Supplier_5_5: - 1000000000 bDDP_Supplier_5_5 + xSF_Supplier_5_5 &lt;= 0
+DMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 + 1000000000 zd_Supplier_1_0 &lt;= 1001000000
+DMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 - zd_Supplier_1_0 &gt;= 0
+Demand_1: x_Supplier_1_1 + x_Supplier_2_1 + x_Supplier_3_1 + x_Supplier_4_1
+ + x_Supplier_5_1 = 1456
+Demand_2: x_Supplier_1_2 + x_Supplier_2_2 + x_Supplier_3_2 + x_Supplier_4_2
+ + x_Supplier_5_2 = 2421
+Demand_3: x_Supplier_1_3 + x_Supplier_2_3 + x_Supplier_3_3 + x_Supplier_4_3
+ + x_Supplier_5_3 = 6462
+Demand_4: x_Supplier_1_4 + x_Supplier_2_4 + x_Supplier_3_4 + x_Supplier_4_4
+ + x_Supplier_5_4 = 2357
+Demand_5: x_Supplier_1_5 + x_Supplier_2_5 + x_Supplier_3_5 + x_Supplier_4_5
+ + x_Supplier_5_5 = 2421
+F_Supplier_1: F_Supplier_1 - 0.412162289871 xKBX_Supplier_1_1
+ - 0.22235953793 xKBX_Supplier_1_2 - 0.512780804906 xKBX_Supplier_1_3
+ - 0.394681495501 xKBX_Supplier_1_4 - 0.0753850747199 xKBX_Supplier_1_5 = 0
+F_Supplier_2: F_Supplier_2 - 0.757107072844 xKBX_Supplier_2_1
+ - 0.356630788891 xKBX_Supplier_2_2 - 0.858608241067 xKBX_Supplier_2_3
+ - 0.917768682562 xKBX_Supplier_2_4 - 0.967175460043 xKBX_Supplier_2_5 = 0
+F_Supplier_3: F_Supplier_3 - 0.241023405628 xKBX_Supplier_3_1
+ - 0.454237724257 xKBX_Supplier_3_2 - 0.129107439223 xKBX_Supplier_3_3
+ - 0.451698077422 xKBX_Supplier_3_4 - 0.45801791591 xKBX_Supplier_3_5 = 0
+F_Supplier_4: F_Supplier_4 - 0.255919123062 xKBX_Supplier_4_1
+ - 0.559049287841 xKBX_Supplier_4_2 - 0.479616530055 xKBX_Supplier_4_3
+ - 0.593669220863 xKBX_Supplier_4_4 - 0.33835492882 xKBX_Supplier_4_5 = 0
+F_Supplier_5: F_Supplier_5 - 0.182453952076 xKBX_Supplier_5_1
+ - 0.409663732116 xKBX_Supplier_5_2 - 0.770440355959 xKBX_Supplier_5_3
+ - 0.0145714073022 xKBX_Supplier_5_4 - 0.728726258075 xKBX_Supplier_5_5 = 0
+Fixd_Supplier_2: d_Supplier_2 = 0
+Fixd_Supplier_3: d_Supplier_3 = 0
+Fixd_Supplier_4: d_Supplier_4 = 0
+Fixd_Supplier_5: d_Supplier_5 = 0
+Fixreb_Supplier_2: reb_Supplier_2 = 0
+Fixreb_Supplier_3: reb_Supplier_3 = 0
+Fixreb_Supplier_4: reb_Supplier_4 = 0
+Fixreb_Supplier_5: reb_Supplier_5 = 0
 KBX_ON_Supplier_1_1: 1000000000 bDDP_Supplier_1_1 + xKBX_Supplier_1_1
  &lt;= 1000000000
+KBX_ON_Supplier_1_2: 1000000000 bDDP_Supplier_1_2 + xKBX_Supplier_1_2
+ &lt;= 1000000000
+KBX_ON_Supplier_1_3: 1000000000 bDDP_Supplier_1_3 + xKBX_Supplier_1_3
+ &lt;= 1000000000
+KBX_ON_Supplier_1_4: 1000000000 bDDP_Supplier_1_4 + xKBX_Supplier_1_4
+ &lt;= 1000000000
+KBX_ON_Supplier_1_5: 1000000000 bDDP_Supplier_1_5 + xKBX_Supplier_1_5
+ &lt;= 1000000000
+KBX_ON_Supplier_2_1: 1000000000 bDDP_Supplier_2_1 + xKBX_Supplier_2_1
+ &lt;= 1000000000
+KBX_ON_Supplier_2_2: 1000000000 bDDP_Supplier_2_2 + xKBX_Supplier_2_2
+ &lt;= 1000000000
+KBX_ON_Supplier_2_3: 1000000000 bDDP_Supplier_2_3 + xKBX_Supplier_2_3
+ &lt;= 1000000000
+KBX_ON_Supplier_2_4: 1000000000 bDDP_Supplier_2_4 + xKBX_Supplier_2_4
+ &lt;= 1000000000
+KBX_ON_Supplier_2_5: 1000000000 bDDP_Supplier_2_5 + xKBX_Supplier_2_5
+ &lt;= 1000000000
+KBX_ON_Supplier_3_1: 1000000000 bDDP_Supplier_3_1 + xKBX_Supplier_3_1
+ &lt;= 1000000000
+KBX_ON_Supplier_3_2: 1000000000 bDDP_Supplier_3_2 + xKBX_Supplier_3_2
+ &lt;= 1000000000
+KBX_ON_Supplier_3_3: 1000000000 bDDP_Supplier_3_3 + xKBX_Supplier_3_3
+ &lt;= 1000000000
+KBX_ON_Supplier_3_4: 1000000000 bDDP_Supplier_3_4 + xKBX_Supplier_3_4
+ &lt;= 1000000000
+KBX_ON_Supplier_3_5: 1000000000 bDDP_Supplier_3_5 + xKBX_Supplier_3_5
+ &lt;= 1000000000
+KBX_ON_Supplier_4_1: 1000000000 bDDP_Supplier_4_1 + xKBX_Supplier_4_1
+ &lt;= 1000000000
+KBX_ON_Supplier_4_2: 1000000000 bDDP_Supplier_4_2 + xKBX_Supplier_4_2
+ &lt;= 1000000000
+KBX_ON_Supplier_4_3: 1000000000 bDDP_Supplier_4_3 + xKBX_Supplier_4_3
+ &lt;= 1000000000
+KBX_ON_Supplier_4_4: 1000000000 bDDP_Supplier_4_4 + xKBX_Supplier_4_4
+ &lt;= 1000000000
+KBX_ON_Supplier_4_5: 1000000000 bDDP_Supplier_4_5 + xKBX_Supplier_4_5
+ &lt;= 1000000000
+KBX_ON_Supplier_5_1: 1000000000 bDDP_Supplier_5_1 + xKBX_Supplier_5_1
+ &lt;= 1000000000
+KBX_ON_Supplier_5_2: 1000000000 bDDP_Supplier_5_2 + xKBX_Supplier_5_2
+ &lt;= 1000000000
+KBX_ON_Supplier_5_3: 1000000000 bDDP_Supplier_5_3 + xKBX_Supplier_5_3
+ &lt;= 1000000000
+KBX_ON_Supplier_5_4: 1000000000 bDDP_Supplier_5_4 + xKBX_Supplier_5_4
+ &lt;= 1000000000
+KBX_ON_Supplier_5_5: 1000000000 bDDP_Supplier_5_5 + xKBX_Supplier_5_5
+ &lt;= 1000000000
 LinkVol_Supplier_1_1: - xKBX_Supplier_1_1 - xSF_Supplier_1_1 + x_Supplier_1_1
  = 0
+LinkVol_Supplier_1_2: - xKBX_Supplier_1_2 - xSF_Supplier_1_2 + x_Supplier_1_2
+ = 0
+LinkVol_Supplier_1_3: - xKBX_Supplier_1_3 - xSF_Supplier_1_3 + x_Supplier_1_3
+ = 0
+LinkVol_Supplier_1_4: - xKBX_Supplier_1_4 - xSF_Supplier_1_4 + x_Supplier_1_4
+ = 0
+LinkVol_Supplier_1_5: - xKBX_Supplier_1_5 - xSF_Supplier_1_5 + x_Supplier_1_5
+ = 0
+LinkVol_Supplier_2_1: - xKBX_Supplier_2_1 - xSF_Supplier_2_1 + x_Supplier_2_1
+ = 0
+LinkVol_Supplier_2_2: - xKBX_Supplier_2_2 - xSF_Supplier_2_2 + x_Supplier_2_2
+ = 0
+LinkVol_Supplier_2_3: - xKBX_Supplier_2_3 - xSF_Supplier_2_3 + x_Supplier_2_3
+ = 0
+LinkVol_Supplier_2_4: - xKBX_Supplier_2_4 - xSF_Supplier_2_4 + x_Supplier_2_4
+ = 0
+LinkVol_Supplier_2_5: - xKBX_Supplier_2_5 - xSF_Supplier_2_5 + x_Supplier_2_5
+ = 0
+LinkVol_Supplier_3_1: - xKBX_Supplier_3_1 - xSF_Supplier_3_1 + x_Supplier_3_1
+ = 0
+LinkVol_Supplier_3_2: - xKBX_Supplier_3_2 - xSF_Supplier_3_2 + x_Supplier_3_2
+ = 0
+LinkVol_Supplier_3_3: - xKBX_Supplier_3_3 - xSF_Supplier_3_3 + x_Supplier_3_3
+ = 0
+LinkVol_Supplier_3_4: - xKBX_Supplier_3_4 - xSF_Supplier_3_4 + x_Supplier_3_4
+ = 0
+LinkVol_Supplier_3_5: - xKBX_Supplier_3_5 - xSF_Supplier_3_5 + x_Supplier_3_5
+ = 0
+LinkVol_Supplier_4_1: - xKBX_Supplier_4_1 - xSF_Supplier_4_1 + x_Supplier_4_1
+ = 0
+LinkVol_Supplier_4_2: - xKBX_Supplier_4_2 - xSF_Supplier_4_2 + x_Supplier_4_2
+ = 0
+LinkVol_Supplier_4_3: - xKBX_Supplier_4_3 - xSF_Supplier_4_3 + x_Supplier_4_3
+ = 0
+LinkVol_Supplier_4_4: - xKBX_Supplier_4_4 - xSF_Supplier_4_4 + x_Supplier_4_4
+ = 0
+LinkVol_Supplier_4_5: - xKBX_Supplier_4_5 - xSF_Supplier_4_5 + x_Supplier_4_5
+ = 0
+LinkVol_Supplier_5_1: - xKBX_Supplier_5_1 - xSF_Supplier_5_1 + x_Supplier_5_1
+ = 0
+LinkVol_Supplier_5_2: - xKBX_Supplier_5_2 - xSF_Supplier_5_2 + x_Supplier_5_2
+ = 0
+LinkVol_Supplier_5_3: - xKBX_Supplier_5_3 - xSF_Supplier_5_3 + x_Supplier_5_3
+ = 0
+LinkVol_Supplier_5_4: - xKBX_Supplier_5_4 - xSF_Supplier_5_4 + x_Supplier_5_4
+ = 0
+LinkVol_Supplier_5_5: - xKBX_Supplier_5_5 - xSF_Supplier_5_5 + x_Supplier_5_5
+ = 0
 Link_Supplier_1_1: x_Supplier_1_1 - 1000000000 z_Supplier_1 &lt;= 0
-MinAward_Supplier_1: x_Supplier_1_1 - z_Supplier_1 &gt;= 0
+Link_Supplier_1_2: x_Supplier_1_2 - 1000000000 z_Supplier_1 &lt;= 0
+Link_Supplier_1_3: x_Supplier_1_3 - 1000000000 z_Supplier_1 &lt;= 0
+Link_Supplier_1_4: x_Supplier_1_4 - 1000000000 z_Supplier_1 &lt;= 0
+Link_Supplier_1_5: x_Supplier_1_5 - 1000000000 z_Supplier_1 &lt;= 0
+Link_Supplier_2_1: x_Supplier_2_1 - 1000000000 z_Supplier_2 &lt;= 0
+Link_Supplier_2_2: x_Supplier_2_2 - 1000000000 z_Supplier_2 &lt;= 0
+Link_Supplier_2_3: x_Supplier_2_3 - 1000000000 z_Supplier_2 &lt;= 0
+Link_Supplier_2_4: x_Supplier_2_4 - 1000000000 z_Supplier_2 &lt;= 0
+Link_Supplier_2_5: x_Supplier_2_5 - 1000000000 z_Supplier_2 &lt;= 0
+Link_Supplier_3_1: x_Supplier_3_1 - 1000000000 z_Supplier_3 &lt;= 0
+Link_Supplier_3_2: x_Supplier_3_2 - 1000000000 z_Supplier_3 &lt;= 0
+Link_Supplier_3_3: x_Supplier_3_3 - 1000000000 z_Supplier_3 &lt;= 0
+Link_Supplier_3_4: x_Supplier_3_4 - 1000000000 z_Supplier_3 &lt;= 0
+Link_Supplier_3_5: x_Supplier_3_5 - 1000000000 z_Supplier_3 &lt;= 0
+Link_Supplier_4_1: x_Supplier_4_1 - 1000000000 z_Supplier_4 &lt;= 0
+Link_Supplier_4_2: x_Supplier_4_2 - 1000000000 z_Supplier_4 &lt;= 0
+Link_Supplier_4_3: x_Supplier_4_3 - 1000000000 z_Supplier_4 &lt;= 0
+Link_Supplier_4_4: x_Supplier_4_4 - 1000000000 z_Supplier_4 &lt;= 0
+Link_Supplier_4_5: x_Supplier_4_5 - 1000000000 z_Supplier_4 &lt;= 0
+Link_Supplier_5_1: x_Supplier_5_1 - 1000000000 z_Supplier_5 &lt;= 0
+Link_Supplier_5_2: x_Supplier_5_2 - 1000000000 z_Supplier_5 &lt;= 0
+Link_Supplier_5_3: x_Supplier_5_3 - 1000000000 z_Supplier_5 &lt;= 0
+Link_Supplier_5_4: x_Supplier_5_4 - 1000000000 z_Supplier_5 &lt;= 0
+Link_Supplier_5_5: x_Supplier_5_5 - 1000000000 z_Supplier_5 &lt;= 0
+MinAward_Supplier_1: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 - z_Supplier_1 &gt;= 0
+MinAward_Supplier_2: x_Supplier_2_1 + x_Supplier_2_2 + x_Supplier_2_3
+ + x_Supplier_2_4 + x_Supplier_2_5 - z_Supplier_2 &gt;= 0
+MinAward_Supplier_3: x_Supplier_3_1 + x_Supplier_3_2 + x_Supplier_3_3
+ + x_Supplier_3_4 + x_Supplier_3_5 - z_Supplier_3 &gt;= 0
+MinAward_Supplier_4: x_Supplier_4_1 + x_Supplier_4_2 + x_Supplier_4_3
+ + x_Supplier_4_4 + x_Supplier_4_5 - z_Supplier_4 &gt;= 0
+MinAward_Supplier_5: x_Supplier_5_1 + x_Supplier_5_2 + x_Supplier_5_3
+ + x_Supplier_5_4 + x_Supplier_5_5 - z_Supplier_5 &gt;= 0
 OneDisc_Supplier_1: - z_Supplier_1 + zd_Supplier_1_0 = 0
 OneReb_Supplier_1: yr_Supplier_1_0 - z_Supplier_1 = 0
-RMax_Supplier_1_0: x_Supplier_1_1 + 1000000000 yr_Supplier_1_0 &lt;= 1001000000
-RMin_Supplier_1_0: x_Supplier_1_1 - yr_Supplier_1_0 &gt;= 0
-S0_Supplier_1: S0_Supplier_1 - 34 xKBX_Supplier_1_1 - 36 xSF_Supplier_1_1 = 0
+PctAggEQLB_0: - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
+ + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1 - x_Supplier_2_2
+ + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 - x_Supplier_3_1
+ + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4 + 0 x_Supplier_3_5
+ - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3 - x_Supplier_4_4
+ - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
+ - x_Supplier_5_4 - x_Supplier_5_5 &gt;= 0
+PctAggEQUB_0: - x_Supplier_1_1 - x_Supplier_1_2 - x_Supplier_1_3
+ + 0 x_Supplier_1_4 - x_Supplier_1_5 + 0 x_Supplier_2_1 - x_Supplier_2_2
+ + 0 x_Supplier_2_3 - x_Supplier_2_4 - x_Supplier_2_5 - x_Supplier_3_1
+ + 0 x_Supplier_3_2 - x_Supplier_3_3 - x_Supplier_3_4 + 0 x_Supplier_3_5
+ - x_Supplier_4_1 - x_Supplier_4_2 - x_Supplier_4_3 - x_Supplier_4_4
+ - x_Supplier_4_5 - x_Supplier_5_1 - x_Supplier_5_2 - x_Supplier_5_3
+ - x_Supplier_5_4 - x_Supplier_5_5 &lt;= 0
+RMax_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 + 1000000000 yr_Supplier_1_0 &lt;= 1001000000
+RMin_Supplier_1_0: x_Supplier_1_1 + x_Supplier_1_2 + x_Supplier_1_3
+ + x_Supplier_1_4 + x_Supplier_1_5 - yr_Supplier_1_0 &gt;= 0
+S0_Supplier_1: S0_Supplier_1 - 34 xKBX_Supplier_1_1 - 15 xKBX_Supplier_1_2
+ - 15 xKBX_Supplier_1_3 - 75 xKBX_Supplier_1_4 - 24 xKBX_Supplier_1_5
+ - 34.0453508742 xSF_Supplier_1_1 - 15.5713844108 xSF_Supplier_1_2
+ - 15.6132383629 xSF_Supplier_1_3 - 75.3658246386 xSF_Supplier_1_4
+ - 24.5552993592 xSF_Supplier_1_5 = 0
+S0_Supplier_2: S0_Supplier_2 - 14 xKBX_Supplier_2_1 - 15 xKBX_Supplier_2_2
+ - 78 xKBX_Supplier_2_3 - 34 xKBX_Supplier_2_4 - 15 xKBX_Supplier_2_5
+ - 14.4996874379 xSF_Supplier_2_1 - 15.6610023131 xSF_Supplier_2_2
+ - 78.583992345 xSF_Supplier_2_3 - 34.245663609 xSF_Supplier_2_4
+ - 15.4376357648 xSF_Supplier_2_5 = 0
+S0_Supplier_3: S0_Supplier_3 - 75 xKBX_Supplier_3_1 - 25 xKBX_Supplier_3_2
+ - 56 xKBX_Supplier_3_3 - 24 xKBX_Supplier_3_4 - 87 xKBX_Supplier_3_5
+ - 75.7343467169 xSF_Supplier_3_1 - 25.273169315 xSF_Supplier_3_2
+ - 56.1815020183 xSF_Supplier_3_3 - 24.660791839 xSF_Supplier_3_4
+ - 87.0636169186 xSF_Supplier_3_5 = 0
+S0_Supplier_4: S0_Supplier_4 - 93 xKBX_Supplier_4_1 - 24 xKBX_Supplier_4_2
+ - 78 xKBX_Supplier_4_3 - 56 xKBX_Supplier_4_4 - 86 xKBX_Supplier_4_5
+ - 93.9042837523 xSF_Supplier_4_1 - 24.4606874043 xSF_Supplier_4_2
+ - 78.4896300664 xSF_Supplier_4_3 - 56.3562030322 xSF_Supplier_4_4
+ - 86.618544981 xSF_Supplier_4_5 = 0
+S0_Supplier_5: S0_Supplier_5 - 76 xKBX_Supplier_5_1 - 32 xKBX_Supplier_5_2
+ - 89 xKBX_Supplier_5_3 - 13 xKBX_Supplier_5_4 - 68 xKBX_Supplier_5_5
+ - 76.022766062 xSF_Supplier_5_1 - 32.3245140214 xSF_Supplier_5_2
+ - 89.583153403 xSF_Supplier_5_3 - 13.2006886512 xSF_Supplier_5_4
+ - 68.7967611263 xSF_Supplier_5_5 = 0
 Spend_Supplier_1: - S0_Supplier_1 + S_Supplier_1 + d_Supplier_1 = 0
+Spend_Supplier_2: - S0_Supplier_2 + S_Supplier_2 + d_Supplier_2 = 0
+Spend_Supplier_3: - S0_Supplier_3 + S_Supplier_3 + d_Supplier_3 = 0
+Spend_Supplier_4: - S0_Supplier_4 + S_Supplier_4 + d_Supplier_4 = 0
+Spend_Supplier_5: - S0_Supplier_5 + S_Supplier_5 + d_Supplier_5 = 0
 TrLB_1_Supplier_1: x_Supplier_1_1 &gt;= 0
+TrLB_1_Supplier_3: x_Supplier_3_1 &gt;= 0
+TrLB_1_Supplier_4: x_Supplier_4_1 &gt;= 0
+TrLB_1_Supplier_5: x_Supplier_5_1 &gt;= 0
+TrLB_2_Supplier_1: x_Supplier_1_2 &gt;= 0
+TrLB_2_Supplier_2: x_Supplier_2_2 &gt;= 0
+TrLB_2_Supplier_4: x_Supplier_4_2 &gt;= 0
+TrLB_2_Supplier_5: x_Supplier_5_2 &gt;= 0
+TrLB_3_Supplier_1: x_Supplier_1_3 &gt;= 0
+TrLB_3_Supplier_3: x_Supplier_3_3 &gt;= 0
+TrLB_3_Supplier_4: x_Supplier_4_3 &gt;= 0
+TrLB_3_Supplier_5: x_Supplier_5_3 &gt;= 0
+TrLB_4_Supplier_2: x_Supplier_2_4 &gt;= 0
+TrLB_4_Supplier_3: x_Supplier_3_4 &gt;= 0
+TrLB_4_Supplier_4: x_Supplier_4_4 &gt;= 0
+TrLB_4_Supplier_5: x_Supplier_5_4 &gt;= 0
+TrLB_5_Supplier_1: x_Supplier_1_5 &gt;= 0
+TrLB_5_Supplier_2: x_Supplier_2_5 &gt;= 0
+TrLB_5_Supplier_4: x_Supplier_4_5 &gt;= 0
+TrLB_5_Supplier_5: x_Supplier_5_5 &gt;= 0
 TrUB_1_Supplier_1: - 1456 T_1_Supplier_1 + x_Supplier_1_1 &lt;= 0
-dLow_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1 - 49538 zd_Supplier_1_0
- &gt;= -49538
-dUp_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1 + 49538 zd_Supplier_1_0
- &lt;= 49538
-dZero_Supplier_1: d_Supplier_1 - 49538 zd_Supplier_1_0 &lt;= 0
+TrUB_1_Supplier_3: - 1456 T_1_Supplier_3 + x_Supplier_3_1 &lt;= 0
+TrUB_1_Supplier_4: - 1456 T_1_Supplier_4 + x_Supplier_4_1 &lt;= 0
+TrUB_1_Supplier_5: - 1456 T_1_Supplier_5 + x_Supplier_5_1 &lt;= 0
+TrUB_2_Supplier_1: - 2421 T_2_Supplier_1 + x_Supplier_1_2 &lt;= 0
+TrUB_2_Supplier_2: - 2421 T_2_Supplier_2 + x_Supplier_2_2 &lt;= 0
+TrUB_2_Supplier_4: - 2421 T_2_Supplier_4 + x_Supplier_4_2 &lt;= 0
+TrUB_2_Supplier_5: - 2421 T_2_Supplier_5 + x_Supplier_5_2 &lt;= 0
+TrUB_3_Supplier_1: - 6462 T_3_Supplier_1 + x_Supplier_1_3 &lt;= 0
+TrUB_3_Supplier_3: - 6462 T_3_Supplier_3 + x_Supplier_3_3 &lt;= 0
+TrUB_3_Supplier_4: - 6462 T_3_Supplier_4 + x_Supplier_4_3 &lt;= 0
+TrUB_3_Supplier_5: - 6462 T_3_Supplier_5 + x_Supplier_5_3 &lt;= 0
+TrUB_4_Supplier_2: - 2357 T_4_Supplier_2 + x_Supplier_2_4 &lt;= 0
+TrUB_4_Supplier_3: - 2357 T_4_Supplier_3 + x_Supplier_3_4 &lt;= 0
+TrUB_4_Supplier_4: - 2357 T_4_Supplier_4 + x_Supplier_4_4 &lt;= 0
+TrUB_4_Supplier_5: - 2357 T_4_Supplier_5 + x_Supplier_5_4 &lt;= 0
+TrUB_5_Supplier_1: - 2421 T_5_Supplier_1 + x_Supplier_1_5 &lt;= 0
+TrUB_5_Supplier_2: - 2421 T_5_Supplier_2 + x_Supplier_2_5 &lt;= 0
+TrUB_5_Supplier_4: - 2421 T_5_Supplier_4 + x_Supplier_4_5 &lt;= 0
+TrUB_5_Supplier_5: - 2421 T_5_Supplier_5 + x_Supplier_5_5 &lt;= 0
+dLow_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1
+ - 1406346 zd_Supplier_1_0 &gt;= -1406346
+dUp_Supplier_1_0: - 0.02 S0_Supplier_1 + d_Supplier_1
+ + 1406346 zd_Supplier_1_0 &lt;= 1406346
+dZeroNoTier_Supplier_2: d_Supplier_2 = 0
+dZeroNoTier_Supplier_3: d_Supplier_3 = 0
+dZeroNoTier_Supplier_4: d_Supplier_4 = 0
+dZeroNoTier_Supplier_5: d_Supplier_5 = 0
+dZero_Supplier_1: d_Supplier_1 - 1406346 zd_Supplier_1_0 &lt;= 0
 rLow_Supplier_1_0: - 0.95 S_Supplier_1 + reb_Supplier_1
- - 49538 yr_Supplier_1_0 &gt;= -49538
-rUp_Supplier_1_0: - 0.95 S_Supplier_1 + reb_Supplier_1 + 49538 yr_Supplier_1_0
- &lt;= 49538
-rZero_Supplier_1: reb_Supplier_1 - 49538 yr_Supplier_1_0 &lt;= 0
+ - 1406346 yr_Supplier_1_0 &gt;= -1406346
+rUp_Supplier_1_0: - 0.95 S_Supplier_1 + reb_Supplier_1
+ + 1406346 yr_Supplier_1_0 &lt;= 1406346
+rZeroNoTier_Supplier_2: reb_Supplier_2 = 0
+rZeroNoTier_Supplier_3: reb_Supplier_3 = 0
+rZeroNoTier_Supplier_4: reb_Supplier_4 = 0
+rZeroNoTier_Supplier_5: reb_Supplier_5 = 0
+rZero_Supplier_1: reb_Supplier_1 - 1406346 yr_Supplier_1_0 &lt;= 0
 Binaries
 T_1_Supplier_1
+T_1_Supplier_3
+T_1_Supplier_4
+T_1_Supplier_5
+T_2_Supplier_1
+T_2_Supplier_2
+T_2_Supplier_4
+T_2_Supplier_5
+T_3_Supplier_1
+T_3_Supplier_3
+T_3_Supplier_4
+T_3_Supplier_5
+T_4_Supplier_2
+T_4_Supplier_3
+T_4_Supplier_4
+T_4_Supplier_5
+T_5_Supplier_1
+T_5_Supplier_2
+T_5_Supplier_4
+T_5_Supplier_5
 bDDP_Supplier_1_1
+bDDP_Supplier_1_2
+bDDP_Supplier_1_3
+bDDP_Supplier_1_4
+bDDP_Supplier_1_5
+bDDP_Supplier_2_1
+bDDP_Supplier_2_2
+bDDP_Supplier_2_3
+bDDP_Supplier_2_4
+bDDP_Supplier_2_5
+bDDP_Supplier_3_1
+bDDP_Supplier_3_2
+bDDP_Supplier_3_3
+bDDP_Supplier_3_4
+bDDP_Supplier_3_5
+bDDP_Supplier_4_1
+bDDP_Supplier_4_2
+bDDP_Supplier_4_3
+bDDP_Supplier_4_4
+bDDP_Supplier_4_5
+bDDP_Supplier_5_1
+bDDP_Supplier_5_2
+bDDP_Supplier_5_3
+bDDP_Supplier_5_4
+bDDP_Supplier_5_5
 yr_Supplier_1_0
 z_Supplier_1
+z_Supplier_2
+z_Supplier_3
+z_Supplier_4
+z_Supplier_5
 zd_Supplier_1_0
 End
 </t>
@@ -732,7 +1384,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,6 +1434,406 @@
         <v>1457</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>6463</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Supplier 1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>6463</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Supplier 3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Supplier 4</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Supplier 4</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Supplier 4</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>6463</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Supplier 4</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Supplier 4</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bid ID</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Supplier 2</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Capacity Group</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Category 1</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>8001</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Supplier 2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Capacity Group</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Category 2</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Supplier 2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Capacity Group</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Category 3</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Supplier 5</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Small item</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Supplier 5</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Medium item</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Supplier 5</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Large Item</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>